<commit_message>
Irrelevent members lose experiment
</commit_message>
<xml_diff>
--- a/benchmark/Configuration.xlsx
+++ b/benchmark/Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\autem\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B613F2-89A9-474D-B796-EB87763E7BE8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850B7DDF-3664-4451-9434-7DCB7DF43E6A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10620" yWindow="2310" windowWidth="15360" windowHeight="10605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12150" yWindow="1770" windowWidth="15360" windowHeight="10605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openml_100" sheetId="1" r:id="rId1"/>
@@ -1208,10 +1208,10 @@
   <dimension ref="A1:M93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,10 +1272,13 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
         <v>104</v>
@@ -1287,19 +1290,19 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="H2">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="I2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K2">
-        <v>1473</v>
+        <v>768</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -1310,10 +1313,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D3" t="s">
         <v>104</v>
@@ -1325,33 +1328,33 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="H3">
-        <v>1788</v>
+        <v>53</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J3">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K3">
-        <v>8124</v>
+        <v>846</v>
       </c>
       <c r="L3">
-        <v>2480</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>2480</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
         <v>104</v>
@@ -1363,19 +1366,19 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="H4">
-        <v>28</v>
+        <v>145804</v>
       </c>
       <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
         <v>10</v>
       </c>
-      <c r="J4">
-        <v>65</v>
-      </c>
       <c r="K4">
-        <v>5620</v>
+        <v>958</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -1386,10 +1389,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D5" t="s">
         <v>104</v>
@@ -1401,33 +1404,33 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="H5">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J5">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="K5">
-        <v>690</v>
+        <v>2000</v>
       </c>
       <c r="L5">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="M5">
-        <v>67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
         <v>104</v>
@@ -1439,19 +1442,19 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="H6">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J6">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="K6">
-        <v>1000</v>
+        <v>625</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -1462,10 +1465,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D7" t="s">
         <v>104</v>
@@ -1477,33 +1480,33 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H7">
-        <v>32</v>
+        <v>3021</v>
       </c>
       <c r="I7">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J7">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="K7">
-        <v>10992</v>
+        <v>3772</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>3772</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>6064</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D8" t="s">
         <v>104</v>
@@ -1515,33 +1518,33 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="H8">
-        <v>1779</v>
+        <v>29</v>
       </c>
       <c r="I8">
         <v>2</v>
       </c>
       <c r="J8">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="K8">
-        <v>699</v>
+        <v>690</v>
       </c>
       <c r="L8">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="M8">
-        <v>16</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D9" t="s">
         <v>104</v>
@@ -1553,33 +1556,33 @@
         <v>1</v>
       </c>
       <c r="G9">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="H9">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="I9">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="J9">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K9">
-        <v>3196</v>
+        <v>683</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>121</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>2337</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D10" t="s">
         <v>104</v>
@@ -1591,33 +1594,33 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="H10">
-        <v>6</v>
+        <v>1779</v>
       </c>
       <c r="I10">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="J10">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="K10">
-        <v>20000</v>
+        <v>699</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D11" t="s">
         <v>104</v>
@@ -1629,19 +1632,19 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="H11">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="I11">
         <v>3</v>
       </c>
       <c r="J11">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K11">
-        <v>625</v>
+        <v>1473</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1652,10 +1655,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D12" t="s">
         <v>104</v>
@@ -1667,33 +1670,33 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="H12">
-        <v>12</v>
+        <v>1788</v>
       </c>
       <c r="I12">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J12">
-        <v>217</v>
+        <v>23</v>
       </c>
       <c r="K12">
-        <v>2000</v>
+        <v>8124</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>2480</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>2480</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D13" t="s">
         <v>104</v>
@@ -1705,19 +1708,19 @@
         <v>1</v>
       </c>
       <c r="G13">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="H13">
-        <v>1778</v>
+        <v>28</v>
       </c>
       <c r="I13">
         <v>10</v>
       </c>
       <c r="J13">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="K13">
-        <v>2000</v>
+        <v>5620</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -1728,10 +1731,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D14" t="s">
         <v>104</v>
@@ -1743,19 +1746,19 @@
         <v>1</v>
       </c>
       <c r="G14">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="H14">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="I14">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J14">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="K14">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -1766,7 +1769,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
         <v>104</v>
@@ -1781,19 +1784,19 @@
         <v>1</v>
       </c>
       <c r="G15">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="H15">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="I15">
         <v>10</v>
       </c>
       <c r="J15">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="K15">
-        <v>2000</v>
+        <v>10992</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1804,10 +1807,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D16" t="s">
         <v>104</v>
@@ -1819,19 +1822,19 @@
         <v>1</v>
       </c>
       <c r="G16">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="H16">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="I16">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J16">
-        <v>241</v>
+        <v>37</v>
       </c>
       <c r="K16">
-        <v>2000</v>
+        <v>3196</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -1842,10 +1845,10 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D17" t="s">
         <v>104</v>
@@ -1857,19 +1860,19 @@
         <v>1</v>
       </c>
       <c r="G17">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="H17">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="I17">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="J17">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="K17">
-        <v>2000</v>
+        <v>20000</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -1880,10 +1883,10 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D18" t="s">
         <v>104</v>
@@ -1895,19 +1898,19 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="H18">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="I18">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J18">
-        <v>20</v>
+        <v>217</v>
       </c>
       <c r="K18">
-        <v>2310</v>
+        <v>2000</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1918,13 +1921,10 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>104</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D19" t="s">
         <v>104</v>
@@ -1936,19 +1936,19 @@
         <v>1</v>
       </c>
       <c r="G19">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="H19">
-        <v>37</v>
+        <v>1778</v>
       </c>
       <c r="I19">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J19">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="K19">
-        <v>768</v>
+        <v>2000</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -1959,10 +1959,10 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D20" t="s">
         <v>104</v>
@@ -1974,71 +1974,71 @@
         <v>1</v>
       </c>
       <c r="G20">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="H20">
-        <v>3021</v>
+        <v>16</v>
       </c>
       <c r="I20">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J20">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="K20">
-        <v>3772</v>
+        <v>2000</v>
       </c>
       <c r="L20">
-        <v>3772</v>
+        <v>0</v>
       </c>
       <c r="M20">
-        <v>6064</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21">
         <v>20</v>
       </c>
-      <c r="C21" t="s">
-        <v>104</v>
-      </c>
-      <c r="D21" t="s">
-        <v>104</v>
-      </c>
-      <c r="E21" t="s">
-        <v>104</v>
-      </c>
-      <c r="F21" t="s">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>42</v>
-      </c>
       <c r="H21">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I21">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J21">
-        <v>36</v>
+        <v>241</v>
       </c>
       <c r="K21">
-        <v>683</v>
+        <v>2000</v>
       </c>
       <c r="L21">
-        <v>121</v>
+        <v>0</v>
       </c>
       <c r="M21">
-        <v>2337</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D22" t="s">
         <v>104</v>
@@ -2050,19 +2050,19 @@
         <v>1</v>
       </c>
       <c r="G22">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="H22">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="I22">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J22">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="K22">
-        <v>4601</v>
+        <v>2000</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -2073,10 +2073,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D23" t="s">
         <v>104</v>
@@ -2088,19 +2088,19 @@
         <v>1</v>
       </c>
       <c r="G23">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="H23">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="I23">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J23">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="K23">
-        <v>3190</v>
+        <v>2310</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -2111,7 +2111,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
         <v>104</v>
@@ -2126,19 +2126,19 @@
         <v>1</v>
       </c>
       <c r="G24">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H24">
-        <v>145804</v>
+        <v>43</v>
       </c>
       <c r="I24">
         <v>2</v>
       </c>
       <c r="J24">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="K24">
-        <v>958</v>
+        <v>4601</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -2149,10 +2149,10 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="D25" t="s">
         <v>104</v>
@@ -2164,19 +2164,19 @@
         <v>1</v>
       </c>
       <c r="G25">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="H25">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="I25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J25">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="K25">
-        <v>846</v>
+        <v>3190</v>
       </c>
       <c r="L25">
         <v>0</v>

</xml_diff>

<commit_message>
2nd block of datasets
</commit_message>
<xml_diff>
--- a/benchmark/Configuration.xlsx
+++ b/benchmark/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\autem\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DFBE82-215E-4955-ABA7-DE0E117E63DF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46596795-FA5F-40FB-A05C-1679AA855A8F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="114">
   <si>
     <t>kr-vs-kp</t>
   </si>
@@ -348,7 +348,28 @@
     <t>Select</t>
   </si>
   <si>
-    <t>Performance</t>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Wrong config</t>
+  </si>
+  <si>
+    <t>Baseline missing</t>
+  </si>
+  <si>
+    <t>Problem</t>
+  </si>
+  <si>
+    <t>Long runtime</t>
+  </si>
+  <si>
+    <t>Wide</t>
+  </si>
+  <si>
+    <t>Very wide</t>
+  </si>
+  <si>
+    <t>Wide, Long</t>
   </si>
 </sst>
 </file>
@@ -832,12 +853,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1196,10 +1218,10 @@
   <dimension ref="A1:J93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,7 +1275,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -1285,7 +1307,7 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -1317,7 +1339,7 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -1349,7 +1371,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
@@ -1381,7 +1403,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -1413,7 +1435,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
@@ -1445,7 +1467,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -1477,7 +1499,7 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -1509,7 +1531,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -1541,7 +1563,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -1573,7 +1595,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -1605,7 +1627,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -1637,7 +1659,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
@@ -1669,7 +1691,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
@@ -1701,7 +1723,7 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
@@ -1733,7 +1755,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
@@ -1765,10 +1787,10 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C18" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="D18">
         <v>12</v>
@@ -1797,7 +1819,7 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
@@ -1829,7 +1851,7 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
@@ -1861,7 +1883,7 @@
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
@@ -1893,7 +1915,7 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
@@ -1925,7 +1947,7 @@
         <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
@@ -1957,7 +1979,7 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C24" t="s">
         <v>1</v>
@@ -1989,7 +2011,7 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
@@ -2021,7 +2043,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -2053,7 +2075,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
@@ -2084,14 +2106,17 @@
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="B28" t="s">
+        <v>106</v>
+      </c>
       <c r="C28" t="s">
         <v>1</v>
       </c>
       <c r="D28">
         <v>182</v>
       </c>
-      <c r="E28" t="s">
-        <v>94</v>
+      <c r="E28">
+        <v>2074</v>
       </c>
       <c r="F28">
         <v>6</v>
@@ -2114,7 +2139,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
@@ -2145,14 +2170,17 @@
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="B30" t="s">
+        <v>109</v>
+      </c>
       <c r="C30" t="s">
-        <v>1</v>
+        <v>110</v>
       </c>
       <c r="D30">
         <v>300</v>
       </c>
-      <c r="E30" t="s">
-        <v>94</v>
+      <c r="E30">
+        <v>3481</v>
       </c>
       <c r="F30">
         <v>26</v>
@@ -2174,14 +2202,17 @@
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="B31" t="s">
+        <v>106</v>
+      </c>
       <c r="C31" t="s">
         <v>1</v>
       </c>
       <c r="D31">
         <v>307</v>
       </c>
-      <c r="E31" t="s">
-        <v>94</v>
+      <c r="E31">
+        <v>3022</v>
       </c>
       <c r="F31">
         <v>11</v>
@@ -2203,14 +2234,17 @@
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="B32" t="s">
+        <v>106</v>
+      </c>
       <c r="C32" t="s">
         <v>1</v>
       </c>
       <c r="D32">
         <v>312</v>
       </c>
-      <c r="E32" t="s">
-        <v>94</v>
+      <c r="E32">
+        <v>3485</v>
       </c>
       <c r="F32">
         <v>2</v>
@@ -2233,13 +2267,13 @@
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="D33">
         <v>333</v>
       </c>
-      <c r="E33" t="s">
-        <v>94</v>
+      <c r="E33">
+        <v>146064</v>
       </c>
       <c r="F33">
         <v>2</v>
@@ -2262,13 +2296,13 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="D34">
         <v>334</v>
       </c>
-      <c r="E34" t="s">
-        <v>94</v>
+      <c r="E34">
+        <v>146065</v>
       </c>
       <c r="F34">
         <v>2</v>
@@ -2291,13 +2325,13 @@
         <v>34</v>
       </c>
       <c r="C35" t="s">
-        <v>1</v>
+        <v>107</v>
       </c>
       <c r="D35">
         <v>335</v>
       </c>
-      <c r="E35" t="s">
-        <v>94</v>
+      <c r="E35">
+        <v>3494</v>
       </c>
       <c r="F35">
         <v>2</v>
@@ -2320,7 +2354,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
@@ -2351,14 +2385,17 @@
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="B37" t="s">
+        <v>106</v>
+      </c>
       <c r="C37" t="s">
         <v>1</v>
       </c>
       <c r="D37">
         <v>377</v>
       </c>
-      <c r="E37" t="s">
-        <v>94</v>
+      <c r="E37">
+        <v>3512</v>
       </c>
       <c r="F37">
         <v>6</v>
@@ -2380,14 +2417,17 @@
       <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
+      <c r="B38" t="s">
+        <v>106</v>
+      </c>
       <c r="C38" t="s">
         <v>1</v>
       </c>
       <c r="D38">
         <v>451</v>
       </c>
-      <c r="E38" t="s">
-        <v>94</v>
+      <c r="E38">
+        <v>3543</v>
       </c>
       <c r="F38">
         <v>2</v>
@@ -2409,14 +2449,17 @@
       <c r="A39" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="B39" t="s">
+        <v>106</v>
+      </c>
       <c r="C39" t="s">
         <v>1</v>
       </c>
       <c r="D39">
         <v>458</v>
       </c>
-      <c r="E39" t="s">
-        <v>94</v>
+      <c r="E39">
+        <v>3549</v>
       </c>
       <c r="F39">
         <v>4</v>
@@ -2438,14 +2481,17 @@
       <c r="A40" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="B40" t="s">
+        <v>106</v>
+      </c>
       <c r="C40" t="s">
         <v>1</v>
       </c>
       <c r="D40">
         <v>469</v>
       </c>
-      <c r="E40" t="s">
-        <v>94</v>
+      <c r="E40">
+        <v>3560</v>
       </c>
       <c r="F40">
         <v>6</v>
@@ -2467,14 +2513,17 @@
       <c r="A41" s="3" t="s">
         <v>40</v>
       </c>
+      <c r="B41" t="s">
+        <v>106</v>
+      </c>
       <c r="C41" t="s">
         <v>1</v>
       </c>
       <c r="D41">
         <v>470</v>
       </c>
-      <c r="E41" t="s">
-        <v>94</v>
+      <c r="E41">
+        <v>3561</v>
       </c>
       <c r="F41">
         <v>2</v>
@@ -2496,14 +2545,17 @@
       <c r="A42" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="B42" t="s">
+        <v>109</v>
+      </c>
       <c r="C42" t="s">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="D42">
         <v>554</v>
       </c>
-      <c r="E42" t="s">
-        <v>94</v>
+      <c r="E42">
+        <v>3573</v>
       </c>
       <c r="F42">
         <v>10</v>
@@ -2525,14 +2577,17 @@
       <c r="A43" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="B43" t="s">
+        <v>109</v>
+      </c>
       <c r="C43" t="s">
-        <v>1</v>
+        <v>112</v>
       </c>
       <c r="D43">
         <v>1038</v>
       </c>
-      <c r="E43" t="s">
-        <v>94</v>
+      <c r="E43">
+        <v>3891</v>
       </c>
       <c r="F43">
         <v>2</v>
@@ -2587,7 +2642,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C45" t="s">
         <v>1</v>
@@ -2618,14 +2673,17 @@
       <c r="A46" s="3" t="s">
         <v>45</v>
       </c>
+      <c r="B46" t="s">
+        <v>106</v>
+      </c>
       <c r="C46" t="s">
         <v>1</v>
       </c>
       <c r="D46">
         <v>1050</v>
       </c>
-      <c r="E46" t="s">
-        <v>94</v>
+      <c r="E46">
+        <v>3903</v>
       </c>
       <c r="F46">
         <v>2</v>
@@ -2967,7 +3025,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C58" t="s">
         <v>1</v>
@@ -3176,10 +3234,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C65" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D65">
         <v>1479</v>
@@ -3613,14 +3671,17 @@
       <c r="A80" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="B80" t="s">
+        <v>104</v>
+      </c>
       <c r="C80" t="s">
         <v>1</v>
       </c>
       <c r="D80">
         <v>1590</v>
       </c>
-      <c r="E80" t="s">
-        <v>94</v>
+      <c r="E80">
+        <v>7592</v>
       </c>
       <c r="F80">
         <v>2</v>
@@ -3642,14 +3703,17 @@
       <c r="A81" s="3" t="s">
         <v>80</v>
       </c>
+      <c r="B81" t="s">
+        <v>102</v>
+      </c>
       <c r="C81" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D81">
         <v>4134</v>
       </c>
-      <c r="E81" t="s">
-        <v>94</v>
+      <c r="E81">
+        <v>14966</v>
       </c>
       <c r="F81">
         <v>2</v>
@@ -3668,8 +3732,11 @@
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="5" t="s">
         <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>104</v>
       </c>
       <c r="C82" t="s">
         <v>1</v>
@@ -3677,8 +3744,8 @@
       <c r="D82">
         <v>4135</v>
       </c>
-      <c r="E82" t="s">
-        <v>94</v>
+      <c r="E82">
+        <v>34539</v>
       </c>
       <c r="F82">
         <v>2</v>
@@ -3732,14 +3799,17 @@
       <c r="A84" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="B84" t="s">
+        <v>104</v>
+      </c>
       <c r="C84" t="s">
         <v>1</v>
       </c>
       <c r="D84">
         <v>4538</v>
       </c>
-      <c r="E84" t="s">
-        <v>94</v>
+      <c r="E84">
+        <v>14969</v>
       </c>
       <c r="F84">
         <v>5</v>
@@ -3761,14 +3831,17 @@
       <c r="A85" s="3" t="s">
         <v>84</v>
       </c>
+      <c r="B85" t="s">
+        <v>104</v>
+      </c>
       <c r="C85" t="s">
         <v>1</v>
       </c>
       <c r="D85">
         <v>6332</v>
       </c>
-      <c r="E85" t="s">
-        <v>94</v>
+      <c r="E85">
+        <v>14968</v>
       </c>
       <c r="F85">
         <v>2</v>
@@ -3790,14 +3863,17 @@
       <c r="A86" s="3" t="s">
         <v>85</v>
       </c>
+      <c r="B86" t="s">
+        <v>104</v>
+      </c>
       <c r="C86" t="s">
         <v>1</v>
       </c>
       <c r="D86">
         <v>23380</v>
       </c>
-      <c r="E86" t="s">
-        <v>94</v>
+      <c r="E86">
+        <v>14967</v>
       </c>
       <c r="F86">
         <v>6</v>
@@ -3819,14 +3895,17 @@
       <c r="A87" s="3" t="s">
         <v>86</v>
       </c>
+      <c r="B87" t="s">
+        <v>104</v>
+      </c>
       <c r="C87" t="s">
         <v>1</v>
       </c>
       <c r="D87">
         <v>23381</v>
       </c>
-      <c r="E87" t="s">
-        <v>94</v>
+      <c r="E87">
+        <v>125920</v>
       </c>
       <c r="F87">
         <v>2</v>
@@ -3848,14 +3927,17 @@
       <c r="A88" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="B88" t="s">
+        <v>104</v>
+      </c>
       <c r="C88" t="s">
         <v>1</v>
       </c>
       <c r="D88">
         <v>23512</v>
       </c>
-      <c r="E88" t="s">
-        <v>94</v>
+      <c r="E88">
+        <v>146606</v>
       </c>
       <c r="F88">
         <v>2</v>
@@ -3877,14 +3959,17 @@
       <c r="A89" s="3" t="s">
         <v>88</v>
       </c>
+      <c r="B89" t="s">
+        <v>104</v>
+      </c>
       <c r="C89" t="s">
         <v>1</v>
       </c>
       <c r="D89">
         <v>40496</v>
       </c>
-      <c r="E89" t="s">
-        <v>94</v>
+      <c r="E89">
+        <v>125921</v>
       </c>
       <c r="F89">
         <v>10</v>
@@ -3906,14 +3991,17 @@
       <c r="A90" s="3" t="s">
         <v>89</v>
       </c>
+      <c r="B90" t="s">
+        <v>104</v>
+      </c>
       <c r="C90" t="s">
         <v>1</v>
       </c>
       <c r="D90">
         <v>40499</v>
       </c>
-      <c r="E90" t="s">
-        <v>94</v>
+      <c r="E90">
+        <v>125922</v>
       </c>
       <c r="F90">
         <v>11</v>
@@ -3935,14 +4023,17 @@
       <c r="A91" s="3" t="s">
         <v>90</v>
       </c>
+      <c r="B91" t="s">
+        <v>104</v>
+      </c>
       <c r="C91" t="s">
         <v>1</v>
       </c>
       <c r="D91">
         <v>40536</v>
       </c>
-      <c r="E91" t="s">
-        <v>94</v>
+      <c r="E91">
+        <v>146607</v>
       </c>
       <c r="F91">
         <v>2</v>
@@ -3964,14 +4055,17 @@
       <c r="A92" s="3" t="s">
         <v>91</v>
       </c>
+      <c r="B92" t="s">
+        <v>102</v>
+      </c>
       <c r="C92" t="s">
-        <v>1</v>
+        <v>108</v>
       </c>
       <c r="D92">
         <v>40668</v>
       </c>
-      <c r="E92" t="s">
-        <v>94</v>
+      <c r="E92">
+        <v>146195</v>
       </c>
       <c r="F92">
         <v>3</v>
@@ -3993,14 +4087,17 @@
       <c r="A93" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="B93" t="s">
+        <v>104</v>
+      </c>
       <c r="C93" t="s">
         <v>1</v>
       </c>
       <c r="D93">
         <v>40981</v>
       </c>
-      <c r="E93" t="s">
-        <v>94</v>
+      <c r="E93">
+        <v>125923</v>
       </c>
       <c r="F93">
         <v>2</v>

</xml_diff>

<commit_message>
Fix, clean up preformance work documention
</commit_message>
<xml_diff>
--- a/benchmark/Configuration.xlsx
+++ b/benchmark/Configuration.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\autem\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46596795-FA5F-40FB-A05C-1679AA855A8F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580DAA2F-99C2-42C1-BC82-7BD1D96D15F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openml_100" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,14 +29,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="117">
   <si>
     <t>kr-vs-kp</t>
   </si>
   <si>
-    <t xml:space="preserve"> None</t>
-  </si>
-  <si>
     <t>letter</t>
   </si>
   <si>
@@ -309,9 +307,6 @@
     <t>Australian</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -342,34 +337,49 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Run</t>
-  </si>
-  <si>
     <t>Select</t>
   </si>
   <si>
     <t>Complete</t>
   </si>
   <si>
-    <t>Wrong config</t>
-  </si>
-  <si>
-    <t>Baseline missing</t>
-  </si>
-  <si>
-    <t>Problem</t>
-  </si>
-  <si>
-    <t>Long runtime</t>
-  </si>
-  <si>
-    <t>Wide</t>
-  </si>
-  <si>
-    <t>Very wide</t>
-  </si>
-  <si>
-    <t>Wide, Long</t>
+    <t>Benchmark Summary</t>
+  </si>
+  <si>
+    <t>Jobs Complete</t>
+  </si>
+  <si>
+    <t>Jobs left to run</t>
+  </si>
+  <si>
+    <t>Total Jobs</t>
+  </si>
+  <si>
+    <t>Jobs with issues</t>
+  </si>
+  <si>
+    <t>Suspend</t>
+  </si>
+  <si>
+    <t>Overly high rating. However simulation accuracy is on par with bench mark accuracies. Possibly lucked out in validation set selection.</t>
+  </si>
+  <si>
+    <t>Jobs suspended</t>
+  </si>
+  <si>
+    <t>Too wide right now.</t>
+  </si>
+  <si>
+    <t>Suspect long runtime. Run when being monitoried</t>
+  </si>
+  <si>
+    <t>Too long right now.</t>
+  </si>
+  <si>
+    <t>Taking a little time. We want this done!</t>
+  </si>
+  <si>
+    <t>Too wide right now</t>
   </si>
 </sst>
 </file>
@@ -1218,17 +1228,17 @@
   <dimension ref="A1:J93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomRight" activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -1240,45 +1250,42 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D2">
         <v>37</v>
@@ -1304,13 +1311,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D3">
         <v>54</v>
@@ -1336,13 +1340,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D4">
         <v>50</v>
@@ -1368,13 +1369,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D5">
         <v>18</v>
@@ -1400,13 +1398,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D6">
         <v>11</v>
@@ -1432,13 +1427,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D7">
         <v>38</v>
@@ -1464,13 +1456,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D8">
         <v>29</v>
@@ -1496,13 +1485,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D9">
         <v>42</v>
@@ -1528,13 +1514,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D10">
         <v>15</v>
@@ -1560,13 +1543,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D11">
         <v>23</v>
@@ -1592,13 +1572,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
-      </c>
-      <c r="C12" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D12">
         <v>24</v>
@@ -1624,13 +1601,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>106</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D13">
         <v>28</v>
@@ -1656,13 +1630,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D14">
         <v>31</v>
@@ -1688,13 +1659,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D15">
         <v>32</v>
@@ -1723,10 +1691,7 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>106</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D16">
         <v>3</v>
@@ -1752,13 +1717,10 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>106</v>
-      </c>
-      <c r="C17" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D17">
         <v>6</v>
@@ -1784,13 +1746,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>106</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D18">
         <v>12</v>
@@ -1816,13 +1775,10 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D19">
         <v>14</v>
@@ -1848,13 +1804,10 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D20">
         <v>16</v>
@@ -1880,13 +1833,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>106</v>
-      </c>
-      <c r="C21" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D21">
         <v>20</v>
@@ -1912,13 +1862,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
-      </c>
-      <c r="C22" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D22">
         <v>22</v>
@@ -1944,13 +1891,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>106</v>
-      </c>
-      <c r="C23" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D23">
         <v>36</v>
@@ -1976,13 +1920,10 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D24">
         <v>44</v>
@@ -2008,13 +1949,10 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D25">
         <v>46</v>
@@ -2040,13 +1978,10 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
-      </c>
-      <c r="C26" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D26">
         <v>60</v>
@@ -2072,13 +2007,10 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D27">
         <v>151</v>
@@ -2104,13 +2036,10 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>106</v>
-      </c>
-      <c r="C28" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D28">
         <v>182</v>
@@ -2136,13 +2065,10 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D29">
         <v>188</v>
@@ -2168,13 +2094,13 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>109</v>
       </c>
       <c r="C30" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D30">
         <v>300</v>
@@ -2200,13 +2126,10 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>106</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D31">
         <v>307</v>
@@ -2232,13 +2155,10 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
-      </c>
-      <c r="C32" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D32">
         <v>312</v>
@@ -2264,16 +2184,16 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" t="s">
-        <v>107</v>
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>103</v>
       </c>
       <c r="D33">
         <v>333</v>
       </c>
-      <c r="E33">
-        <v>146064</v>
+      <c r="E33" s="3">
+        <v>3492</v>
       </c>
       <c r="F33">
         <v>2</v>
@@ -2293,16 +2213,16 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" t="s">
-        <v>107</v>
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>103</v>
       </c>
       <c r="D34">
         <v>334</v>
       </c>
       <c r="E34">
-        <v>146065</v>
+        <v>3493</v>
       </c>
       <c r="F34">
         <v>2</v>
@@ -2322,10 +2242,10 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" t="s">
-        <v>107</v>
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>103</v>
       </c>
       <c r="D35">
         <v>335</v>
@@ -2351,13 +2271,10 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>106</v>
-      </c>
-      <c r="C36" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D36">
         <v>375</v>
@@ -2383,13 +2300,10 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D37">
         <v>377</v>
@@ -2415,13 +2329,10 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>106</v>
-      </c>
-      <c r="C38" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D38">
         <v>451</v>
@@ -2447,13 +2358,10 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>106</v>
-      </c>
-      <c r="C39" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D39">
         <v>458</v>
@@ -2479,13 +2387,13 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C40" t="s">
-        <v>1</v>
+        <v>110</v>
       </c>
       <c r="D40">
         <v>469</v>
@@ -2511,13 +2419,10 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>106</v>
-      </c>
-      <c r="C41" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D41">
         <v>470</v>
@@ -2543,13 +2448,13 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
         <v>109</v>
       </c>
       <c r="C42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D42">
         <v>554</v>
@@ -2575,7 +2480,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
         <v>109</v>
@@ -2607,13 +2512,10 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>104</v>
-      </c>
-      <c r="C44" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D44">
         <v>1046</v>
@@ -2639,13 +2541,10 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>106</v>
-      </c>
-      <c r="C45" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D45">
         <v>1049</v>
@@ -2671,13 +2570,10 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>106</v>
-      </c>
-      <c r="C46" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D46">
         <v>1050</v>
@@ -2703,16 +2599,13 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C47" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="D47">
         <v>1053</v>
       </c>
       <c r="E47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F47">
         <v>2</v>
@@ -2732,16 +2625,13 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C48" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="D48">
         <v>1063</v>
       </c>
       <c r="E48" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F48">
         <v>2</v>
@@ -2761,16 +2651,13 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="D49">
         <v>1067</v>
       </c>
       <c r="E49" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F49">
         <v>2</v>
@@ -2790,16 +2677,13 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="D50">
         <v>1068</v>
       </c>
       <c r="E50" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F50">
         <v>2</v>
@@ -2819,16 +2703,13 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C51" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="D51">
         <v>1112</v>
       </c>
       <c r="E51" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F51">
         <v>2</v>
@@ -2848,16 +2729,13 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C52" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="D52">
         <v>1114</v>
       </c>
       <c r="E52" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F52">
         <v>2</v>
@@ -2877,16 +2755,13 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C53" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="D53">
         <v>1120</v>
       </c>
       <c r="E53" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F53">
         <v>2</v>
@@ -2906,16 +2781,13 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C54" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="D54">
         <v>1459</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F54">
         <v>10</v>
@@ -2935,16 +2807,13 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C55" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="D55">
         <v>1461</v>
       </c>
       <c r="E55" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F55">
         <v>2</v>
@@ -2964,16 +2833,13 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C56" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="D56">
         <v>1462</v>
       </c>
       <c r="E56" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F56">
         <v>2</v>
@@ -2993,16 +2859,13 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C57" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="D57">
         <v>1464</v>
       </c>
       <c r="E57" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F57">
         <v>2</v>
@@ -3022,13 +2885,10 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>106</v>
-      </c>
-      <c r="C58" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D58">
         <v>1466</v>
@@ -3054,16 +2914,13 @@
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C59" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="D59">
         <v>1467</v>
       </c>
       <c r="E59" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F59">
         <v>2</v>
@@ -3083,16 +2940,13 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C60" t="s">
-        <v>1</v>
+        <v>58</v>
       </c>
       <c r="D60">
         <v>1468</v>
       </c>
       <c r="E60" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F60">
         <v>9</v>
@@ -3112,13 +2966,10 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>104</v>
-      </c>
-      <c r="C61" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D61">
         <v>1471</v>
@@ -3144,16 +2995,13 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C62" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="D62">
         <v>1475</v>
       </c>
       <c r="E62" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F62">
         <v>6</v>
@@ -3173,16 +3021,13 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C63" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="D63">
         <v>1476</v>
       </c>
       <c r="E63" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F63">
         <v>6</v>
@@ -3202,16 +3047,13 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C64" t="s">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="D64">
         <v>1478</v>
       </c>
       <c r="E64" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F64">
         <v>6</v>
@@ -3231,13 +3073,13 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C65" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D65">
         <v>1479</v>
@@ -3263,16 +3105,13 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C66" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="D66">
         <v>1480</v>
       </c>
       <c r="E66" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F66">
         <v>2</v>
@@ -3292,16 +3131,13 @@
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C67" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="D67">
         <v>1485</v>
       </c>
       <c r="E67" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F67">
         <v>2</v>
@@ -3321,16 +3157,13 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C68" t="s">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="D68">
         <v>1486</v>
       </c>
       <c r="E68" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F68">
         <v>2</v>
@@ -3350,16 +3183,13 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C69" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="D69">
         <v>1487</v>
       </c>
       <c r="E69" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F69">
         <v>2</v>
@@ -3379,16 +3209,13 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C70" t="s">
-        <v>1</v>
+        <v>68</v>
       </c>
       <c r="D70">
         <v>1489</v>
       </c>
       <c r="E70" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F70">
         <v>2</v>
@@ -3408,16 +3235,13 @@
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C71" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="D71">
         <v>1491</v>
       </c>
       <c r="E71" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F71">
         <v>100</v>
@@ -3437,16 +3261,13 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C72" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="D72">
         <v>1492</v>
       </c>
       <c r="E72" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F72">
         <v>100</v>
@@ -3466,16 +3287,13 @@
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C73" t="s">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="D73">
         <v>1493</v>
       </c>
       <c r="E73" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F73">
         <v>100</v>
@@ -3495,16 +3313,13 @@
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C74" t="s">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="D74">
         <v>1494</v>
       </c>
       <c r="E74" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F74">
         <v>2</v>
@@ -3524,16 +3339,13 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C75" t="s">
-        <v>1</v>
+        <v>73</v>
       </c>
       <c r="D75">
         <v>1497</v>
       </c>
       <c r="E75" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F75">
         <v>4</v>
@@ -3553,16 +3365,13 @@
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C76" t="s">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="D76">
         <v>1501</v>
       </c>
       <c r="E76" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F76">
         <v>10</v>
@@ -3582,16 +3391,13 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C77" t="s">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="D77">
         <v>1504</v>
       </c>
       <c r="E77" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F77">
         <v>2</v>
@@ -3611,16 +3417,13 @@
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C78" t="s">
-        <v>1</v>
+        <v>76</v>
       </c>
       <c r="D78">
         <v>1510</v>
       </c>
       <c r="E78" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F78">
         <v>2</v>
@@ -3640,16 +3443,13 @@
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C79" t="s">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="D79">
         <v>1515</v>
       </c>
       <c r="E79" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F79">
         <v>20</v>
@@ -3669,13 +3469,10 @@
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>104</v>
-      </c>
-      <c r="C80" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D80">
         <v>1590</v>
@@ -3701,13 +3498,13 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C81" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D81">
         <v>4134</v>
@@ -3733,13 +3530,10 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>104</v>
-      </c>
-      <c r="C82" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D82">
         <v>4135</v>
@@ -3765,13 +3559,10 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>104</v>
-      </c>
-      <c r="C83" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D83">
         <v>4534</v>
@@ -3797,13 +3588,10 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>104</v>
-      </c>
-      <c r="C84" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D84">
         <v>4538</v>
@@ -3829,13 +3617,10 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>104</v>
-      </c>
-      <c r="C85" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D85">
         <v>6332</v>
@@ -3861,13 +3646,10 @@
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>104</v>
-      </c>
-      <c r="C86" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D86">
         <v>23380</v>
@@ -3893,13 +3675,10 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>104</v>
-      </c>
-      <c r="C87" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D87">
         <v>23381</v>
@@ -3925,13 +3704,13 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C88" t="s">
-        <v>1</v>
+        <v>114</v>
       </c>
       <c r="D88">
         <v>23512</v>
@@ -3957,13 +3736,10 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>104</v>
-      </c>
-      <c r="C89" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D89">
         <v>40496</v>
@@ -3989,13 +3765,10 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>104</v>
-      </c>
-      <c r="C90" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D90">
         <v>40499</v>
@@ -4021,13 +3794,13 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C91" t="s">
-        <v>1</v>
+        <v>113</v>
       </c>
       <c r="D91">
         <v>40536</v>
@@ -4053,13 +3826,13 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C92" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="D92">
         <v>40668</v>
@@ -4085,13 +3858,10 @@
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>104</v>
-      </c>
-      <c r="C93" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="D93">
         <v>40981</v>
@@ -4119,4 +3889,72 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB9340E-482C-4D65-A19A-95DA974A01A0}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3">
+        <f>COUNTIF(openml_100!B2:B93, "=Run")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4">
+        <f>COUNTIF(openml_100!B2:B93, "=Complete")</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5">
+        <f>COUNTIF(openml_100!B3:B94, "=Suspend")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6">
+        <f>COUNTIF(openml_100!B2:B93, "=Issue")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7">
+        <f>B3+B4+B5+B6</f>
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Use inter model accuracy to ensure diverse models
</commit_message>
<xml_diff>
--- a/benchmark/Configuration.xlsx
+++ b/benchmark/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\autem\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9C6617-6C86-497F-BA06-9AA77A050BED}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F03F9EA-6566-4119-AFB7-039728B84F0B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="113">
   <si>
     <t>kr-vs-kp</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t>Converge warning</t>
+  </si>
+  <si>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1218,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B44" sqref="B44"/>
+      <selection pane="bottomRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,7 +1276,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E2">
         <v>37</v>
@@ -1302,7 +1305,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E3">
         <v>54</v>
@@ -1331,7 +1334,7 @@
         <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D4" t="s">
         <v>111</v>
@@ -1363,7 +1366,7 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E5">
         <v>50</v>
@@ -1392,7 +1395,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E6">
         <v>18</v>
@@ -1421,7 +1424,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E7">
         <v>11</v>
@@ -1450,7 +1453,7 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E8">
         <v>38</v>
@@ -1479,7 +1482,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E9">
         <v>29</v>
@@ -1508,7 +1511,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E10">
         <v>42</v>
@@ -1537,7 +1540,7 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E11">
         <v>15</v>
@@ -1566,7 +1569,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E12">
         <v>23</v>
@@ -1595,7 +1598,7 @@
         <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E13">
         <v>470</v>
@@ -1624,7 +1627,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E14">
         <v>24</v>
@@ -1653,7 +1656,7 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E15">
         <v>28</v>
@@ -1682,7 +1685,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E16">
         <v>31</v>
@@ -1711,7 +1714,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E17">
         <v>32</v>
@@ -1740,7 +1743,7 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E18">
         <v>3</v>
@@ -1769,7 +1772,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E19">
         <v>6</v>
@@ -1798,7 +1801,7 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E20">
         <v>12</v>
@@ -1827,7 +1830,7 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E21">
         <v>14</v>
@@ -1856,7 +1859,7 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E22">
         <v>16</v>
@@ -4002,7 +4005,7 @@
       </c>
       <c r="B3">
         <f>COUNTIF(openml_100!B2:B100, "=Run")</f>
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4011,7 +4014,7 @@
       </c>
       <c r="B4">
         <f>COUNTIF(openml_100!B2:B100, "=Complete")</f>
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
STC - Study targeted datasets
</commit_message>
<xml_diff>
--- a/benchmark/Configuration.xlsx
+++ b/benchmark/Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\autem\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7CAC1C-727A-4867-82B6-19222A0ADFD9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F83F8F-A2D3-4567-9250-605C5260E5BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-75" yWindow="960" windowWidth="14640" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openml_100" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="113">
   <si>
     <t>kr-vs-kp</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t>PP1</t>
+  </si>
+  <si>
+    <t>STC</t>
   </si>
 </sst>
 </file>
@@ -1209,29 +1212,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K93"/>
+  <dimension ref="A1:L93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
+      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>99</v>
       </c>
@@ -1244,29 +1247,32 @@
       <c r="D1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1279,29 +1285,32 @@
       <c r="D2" t="s">
         <v>107</v>
       </c>
-      <c r="E2">
-        <v>37</v>
+      <c r="E2" t="s">
+        <v>106</v>
       </c>
       <c r="F2">
         <v>37</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
         <v>9</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>768</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
       <c r="K2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -1314,29 +1323,32 @@
       <c r="D3" t="s">
         <v>107</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3">
         <v>54</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>53</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>4</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>19</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>846</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
       <c r="K3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>91</v>
       </c>
@@ -1349,29 +1361,32 @@
       <c r="D4" t="s">
         <v>107</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4">
         <v>40981</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>125923</v>
       </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
       <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
         <v>15</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>690</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
       <c r="K4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1384,29 +1399,32 @@
       <c r="D5" t="s">
         <v>107</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5">
         <v>50</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>145804</v>
       </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
       <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
         <v>10</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>958</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
       <c r="K5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1419,29 +1437,32 @@
       <c r="D6" t="s">
         <v>107</v>
       </c>
-      <c r="E6">
-        <v>18</v>
+      <c r="E6" t="s">
+        <v>110</v>
       </c>
       <c r="F6">
         <v>18</v>
       </c>
       <c r="G6">
+        <v>18</v>
+      </c>
+      <c r="H6">
         <v>10</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>7</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>2000</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
       <c r="K6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1454,29 +1475,32 @@
       <c r="D7" t="s">
         <v>107</v>
       </c>
-      <c r="E7">
-        <v>11</v>
+      <c r="E7" t="s">
+        <v>110</v>
       </c>
       <c r="F7">
         <v>11</v>
       </c>
       <c r="G7">
+        <v>11</v>
+      </c>
+      <c r="H7">
         <v>3</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>5</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>625</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
       <c r="K7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1489,29 +1513,32 @@
       <c r="D8" t="s">
         <v>107</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8">
         <v>38</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>3021</v>
       </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
       <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
         <v>30</v>
-      </c>
-      <c r="I8">
-        <v>3772</v>
       </c>
       <c r="J8">
         <v>3772</v>
       </c>
       <c r="K8">
+        <v>3772</v>
+      </c>
+      <c r="L8">
         <v>6064</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1524,29 +1551,32 @@
       <c r="D9" t="s">
         <v>110</v>
       </c>
-      <c r="E9">
-        <v>29</v>
+      <c r="E9" t="s">
+        <v>110</v>
       </c>
       <c r="F9">
         <v>29</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
         <v>16</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>690</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>37</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1559,29 +1589,32 @@
       <c r="D10" t="s">
         <v>110</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10">
         <v>42</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>41</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>19</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>36</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>683</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>121</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>2337</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -1594,29 +1627,32 @@
       <c r="D11" t="s">
         <v>110</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11">
         <v>15</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>1779</v>
       </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
       <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
         <v>10</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>699</v>
-      </c>
-      <c r="J11">
-        <v>16</v>
       </c>
       <c r="K11">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1629,29 +1665,32 @@
       <c r="D12" t="s">
         <v>110</v>
       </c>
-      <c r="E12">
-        <v>23</v>
+      <c r="E12" t="s">
+        <v>110</v>
       </c>
       <c r="F12">
         <v>23</v>
       </c>
       <c r="G12">
+        <v>23</v>
+      </c>
+      <c r="H12">
         <v>3</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>10</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>1473</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
       <c r="K12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -1664,29 +1703,32 @@
       <c r="D13" t="s">
         <v>107</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13">
         <v>470</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>3561</v>
       </c>
-      <c r="G13">
-        <v>2</v>
-      </c>
       <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
         <v>10</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>672</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>666</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>1200</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1699,29 +1741,32 @@
       <c r="D14" t="s">
         <v>110</v>
       </c>
-      <c r="E14">
+      <c r="E14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14">
         <v>24</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>1788</v>
       </c>
-      <c r="G14">
-        <v>2</v>
-      </c>
       <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
         <v>23</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>8124</v>
-      </c>
-      <c r="J14">
-        <v>2480</v>
       </c>
       <c r="K14">
         <v>2480</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1734,29 +1779,32 @@
       <c r="D15" t="s">
         <v>110</v>
       </c>
-      <c r="E15">
-        <v>28</v>
+      <c r="E15" t="s">
+        <v>110</v>
       </c>
       <c r="F15">
         <v>28</v>
       </c>
       <c r="G15">
+        <v>28</v>
+      </c>
+      <c r="H15">
         <v>10</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>65</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>5620</v>
       </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
       <c r="K15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1769,29 +1817,32 @@
       <c r="D16" t="s">
         <v>107</v>
       </c>
-      <c r="E16">
-        <v>31</v>
+      <c r="E16" t="s">
+        <v>110</v>
       </c>
       <c r="F16">
         <v>31</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
         <v>21</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>1000</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
       <c r="K16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1804,29 +1855,32 @@
       <c r="D17" t="s">
         <v>110</v>
       </c>
-      <c r="E17">
-        <v>32</v>
+      <c r="E17" t="s">
+        <v>110</v>
       </c>
       <c r="F17">
         <v>32</v>
       </c>
       <c r="G17">
+        <v>32</v>
+      </c>
+      <c r="H17">
         <v>10</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>17</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>10992</v>
       </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
       <c r="K17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -1839,29 +1893,32 @@
       <c r="D18" t="s">
         <v>110</v>
       </c>
-      <c r="E18">
-        <v>3</v>
+      <c r="E18" t="s">
+        <v>110</v>
       </c>
       <c r="F18">
         <v>3</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
         <v>37</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>3196</v>
       </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
       <c r="K18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -1874,29 +1931,32 @@
       <c r="D19" t="s">
         <v>106</v>
       </c>
-      <c r="E19">
-        <v>6</v>
+      <c r="E19" t="s">
+        <v>110</v>
       </c>
       <c r="F19">
         <v>6</v>
       </c>
       <c r="G19">
+        <v>6</v>
+      </c>
+      <c r="H19">
         <v>26</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>17</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>20000</v>
       </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
       <c r="K19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
@@ -1909,29 +1969,32 @@
       <c r="D20" t="s">
         <v>110</v>
       </c>
-      <c r="E20">
-        <v>12</v>
+      <c r="E20" t="s">
+        <v>110</v>
       </c>
       <c r="F20">
         <v>12</v>
       </c>
       <c r="G20">
+        <v>12</v>
+      </c>
+      <c r="H20">
         <v>10</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>217</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>2000</v>
       </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
       <c r="K20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
@@ -1944,29 +2007,32 @@
       <c r="D21" t="s">
         <v>110</v>
       </c>
-      <c r="E21">
+      <c r="E21" t="s">
+        <v>110</v>
+      </c>
+      <c r="F21">
         <v>14</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>1778</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>10</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>77</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>2000</v>
       </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
       <c r="K21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
@@ -1979,29 +2045,32 @@
       <c r="D22" t="s">
         <v>110</v>
       </c>
-      <c r="E22">
-        <v>16</v>
+      <c r="E22" t="s">
+        <v>110</v>
       </c>
       <c r="F22">
         <v>16</v>
       </c>
       <c r="G22">
+        <v>16</v>
+      </c>
+      <c r="H22">
         <v>10</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>65</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>2000</v>
       </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
       <c r="K22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -2014,29 +2083,32 @@
       <c r="D23" t="s">
         <v>106</v>
       </c>
-      <c r="E23">
-        <v>22</v>
+      <c r="E23" t="s">
+        <v>110</v>
       </c>
       <c r="F23">
         <v>22</v>
       </c>
       <c r="G23">
+        <v>22</v>
+      </c>
+      <c r="H23">
         <v>10</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>48</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>2000</v>
       </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
       <c r="K23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
@@ -2049,29 +2121,32 @@
       <c r="D24" t="s">
         <v>110</v>
       </c>
-      <c r="E24">
-        <v>36</v>
+      <c r="E24" t="s">
+        <v>110</v>
       </c>
       <c r="F24">
         <v>36</v>
       </c>
       <c r="G24">
+        <v>36</v>
+      </c>
+      <c r="H24">
         <v>7</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>20</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>2310</v>
       </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
       <c r="K24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
@@ -2084,29 +2159,32 @@
       <c r="D25" t="s">
         <v>110</v>
       </c>
-      <c r="E25">
+      <c r="E25" t="s">
+        <v>110</v>
+      </c>
+      <c r="F25">
         <v>44</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>43</v>
       </c>
-      <c r="G25">
-        <v>2</v>
-      </c>
       <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25">
         <v>58</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>4601</v>
       </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
       <c r="K25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
@@ -2119,29 +2197,32 @@
       <c r="D26" t="s">
         <v>106</v>
       </c>
-      <c r="E26">
+      <c r="E26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F26">
         <v>46</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>45</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>3</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>62</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>3190</v>
       </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
       <c r="K26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
@@ -2154,29 +2235,32 @@
       <c r="D27" t="s">
         <v>110</v>
       </c>
-      <c r="E27">
+      <c r="E27" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27">
         <v>60</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>58</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>3</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>41</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>5000</v>
       </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
       <c r="K27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
@@ -2189,29 +2273,32 @@
       <c r="D28" t="s">
         <v>106</v>
       </c>
-      <c r="E28">
+      <c r="E28" t="s">
+        <v>106</v>
+      </c>
+      <c r="F28">
         <v>151</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>219</v>
       </c>
-      <c r="G28">
-        <v>2</v>
-      </c>
       <c r="H28">
+        <v>2</v>
+      </c>
+      <c r="I28">
         <v>9</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>45312</v>
       </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
       <c r="K28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
@@ -2224,29 +2311,32 @@
       <c r="D29" t="s">
         <v>106</v>
       </c>
-      <c r="E29">
+      <c r="E29" t="s">
+        <v>110</v>
+      </c>
+      <c r="F29">
         <v>182</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>2074</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>6</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>37</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>6430</v>
       </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
       <c r="K29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
@@ -2259,29 +2349,32 @@
       <c r="D30" t="s">
         <v>106</v>
       </c>
-      <c r="E30">
+      <c r="E30" t="s">
+        <v>106</v>
+      </c>
+      <c r="F30">
         <v>188</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>2125</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>5</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>20</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>736</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>95</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>448</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
@@ -2294,29 +2387,32 @@
       <c r="D31" t="s">
         <v>106</v>
       </c>
-      <c r="E31">
+      <c r="E31" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31">
         <v>307</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>3022</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>11</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>13</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>990</v>
       </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
       <c r="K31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -2329,29 +2425,32 @@
       <c r="D32" t="s">
         <v>110</v>
       </c>
-      <c r="E32">
+      <c r="E32" t="s">
+        <v>110</v>
+      </c>
+      <c r="F32">
         <v>312</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>3485</v>
       </c>
-      <c r="G32">
-        <v>2</v>
-      </c>
       <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32">
         <v>300</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>2407</v>
       </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
       <c r="K32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
@@ -2364,29 +2463,32 @@
       <c r="D33" t="s">
         <v>106</v>
       </c>
-      <c r="E33">
+      <c r="E33" t="s">
+        <v>106</v>
+      </c>
+      <c r="F33">
         <v>333</v>
       </c>
-      <c r="F33" s="2">
+      <c r="G33" s="2">
         <v>3492</v>
       </c>
-      <c r="G33">
-        <v>2</v>
-      </c>
       <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33">
         <v>7</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>556</v>
       </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
       <c r="K33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -2399,29 +2501,32 @@
       <c r="D34" t="s">
         <v>106</v>
       </c>
-      <c r="E34">
+      <c r="E34" t="s">
+        <v>106</v>
+      </c>
+      <c r="F34">
         <v>334</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>3493</v>
       </c>
-      <c r="G34">
-        <v>2</v>
-      </c>
       <c r="H34">
+        <v>2</v>
+      </c>
+      <c r="I34">
         <v>7</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>601</v>
       </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
       <c r="K34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -2434,29 +2539,32 @@
       <c r="D35" t="s">
         <v>106</v>
       </c>
-      <c r="E35">
+      <c r="E35" t="s">
+        <v>106</v>
+      </c>
+      <c r="F35">
         <v>335</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>3494</v>
       </c>
-      <c r="G35">
-        <v>2</v>
-      </c>
       <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
         <v>7</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>554</v>
       </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
       <c r="K35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -2469,29 +2577,32 @@
       <c r="D36" t="s">
         <v>110</v>
       </c>
-      <c r="E36">
+      <c r="E36" t="s">
+        <v>110</v>
+      </c>
+      <c r="F36">
         <v>375</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>4544</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>9</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>15</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>9961</v>
       </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
       <c r="K36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -2504,29 +2615,32 @@
       <c r="D37" t="s">
         <v>110</v>
       </c>
-      <c r="E37">
+      <c r="E37" t="s">
+        <v>110</v>
+      </c>
+      <c r="F37">
         <v>377</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>3512</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>6</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>62</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <v>600</v>
       </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
       <c r="K37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
@@ -2539,29 +2653,32 @@
       <c r="D38" t="s">
         <v>110</v>
       </c>
-      <c r="E38">
+      <c r="E38" t="s">
+        <v>110</v>
+      </c>
+      <c r="F38">
         <v>451</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>3543</v>
       </c>
-      <c r="G38">
-        <v>2</v>
-      </c>
       <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
         <v>6</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <v>500</v>
-      </c>
-      <c r="J38">
-        <v>32</v>
       </c>
       <c r="K38">
         <v>32</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
@@ -2574,29 +2691,32 @@
       <c r="D39" t="s">
         <v>106</v>
       </c>
-      <c r="E39">
+      <c r="E39" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39">
         <v>458</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>3549</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>4</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>71</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>841</v>
       </c>
-      <c r="J39">
-        <v>0</v>
-      </c>
       <c r="K39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
@@ -2609,29 +2729,32 @@
       <c r="D40" t="s">
         <v>106</v>
       </c>
-      <c r="E40">
+      <c r="E40" t="s">
+        <v>110</v>
+      </c>
+      <c r="F40">
         <v>469</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>3560</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>6</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>5</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <v>797</v>
       </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
       <c r="K40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>42</v>
       </c>
@@ -2644,29 +2767,32 @@
       <c r="D41" t="s">
         <v>110</v>
       </c>
-      <c r="E41">
+      <c r="E41" t="s">
+        <v>110</v>
+      </c>
+      <c r="F41">
         <v>1046</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>3899</v>
       </c>
-      <c r="G41">
-        <v>2</v>
-      </c>
       <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
         <v>6</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <v>15545</v>
       </c>
-      <c r="J41">
-        <v>0</v>
-      </c>
       <c r="K41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>43</v>
       </c>
@@ -2679,29 +2805,32 @@
       <c r="D42" t="s">
         <v>110</v>
       </c>
-      <c r="E42">
+      <c r="E42" t="s">
+        <v>110</v>
+      </c>
+      <c r="F42">
         <v>1049</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>3902</v>
       </c>
-      <c r="G42">
-        <v>2</v>
-      </c>
       <c r="H42">
+        <v>2</v>
+      </c>
+      <c r="I42">
         <v>38</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <v>1458</v>
       </c>
-      <c r="J42">
-        <v>0</v>
-      </c>
       <c r="K42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>44</v>
       </c>
@@ -2714,29 +2843,32 @@
       <c r="D43" t="s">
         <v>106</v>
       </c>
-      <c r="E43">
+      <c r="E43" t="s">
+        <v>110</v>
+      </c>
+      <c r="F43">
         <v>1050</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>3903</v>
       </c>
-      <c r="G43">
-        <v>2</v>
-      </c>
       <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43">
         <v>38</v>
       </c>
-      <c r="I43">
+      <c r="J43">
         <v>1563</v>
       </c>
-      <c r="J43">
-        <v>0</v>
-      </c>
       <c r="K43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>45</v>
       </c>
@@ -2749,29 +2881,32 @@
       <c r="D44" t="s">
         <v>110</v>
       </c>
-      <c r="E44">
+      <c r="E44" t="s">
+        <v>110</v>
+      </c>
+      <c r="F44">
         <v>1053</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>3904</v>
       </c>
-      <c r="G44">
-        <v>2</v>
-      </c>
       <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44">
         <v>22</v>
       </c>
-      <c r="I44">
+      <c r="J44">
         <v>10885</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <v>5</v>
       </c>
-      <c r="K44">
+      <c r="L44">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>46</v>
       </c>
@@ -2784,29 +2919,32 @@
       <c r="D45" t="s">
         <v>110</v>
       </c>
-      <c r="E45">
+      <c r="E45" t="s">
+        <v>110</v>
+      </c>
+      <c r="F45">
         <v>1063</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>3913</v>
       </c>
-      <c r="G45">
-        <v>2</v>
-      </c>
       <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
         <v>22</v>
       </c>
-      <c r="I45">
+      <c r="J45">
         <v>522</v>
       </c>
-      <c r="J45">
-        <v>0</v>
-      </c>
       <c r="K45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>47</v>
       </c>
@@ -2819,29 +2957,32 @@
       <c r="D46" t="s">
         <v>110</v>
       </c>
-      <c r="E46">
+      <c r="E46" t="s">
+        <v>110</v>
+      </c>
+      <c r="F46">
         <v>1067</v>
       </c>
-      <c r="F46">
+      <c r="G46">
         <v>3917</v>
       </c>
-      <c r="G46">
-        <v>2</v>
-      </c>
       <c r="H46">
+        <v>2</v>
+      </c>
+      <c r="I46">
         <v>22</v>
       </c>
-      <c r="I46">
+      <c r="J46">
         <v>2109</v>
       </c>
-      <c r="J46">
-        <v>0</v>
-      </c>
       <c r="K46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>48</v>
       </c>
@@ -2854,29 +2995,32 @@
       <c r="D47" t="s">
         <v>110</v>
       </c>
-      <c r="E47">
+      <c r="E47" t="s">
+        <v>110</v>
+      </c>
+      <c r="F47">
         <v>1068</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>3918</v>
       </c>
-      <c r="G47">
-        <v>2</v>
-      </c>
       <c r="H47">
+        <v>2</v>
+      </c>
+      <c r="I47">
         <v>22</v>
       </c>
-      <c r="I47">
+      <c r="J47">
         <v>1109</v>
       </c>
-      <c r="J47">
-        <v>0</v>
-      </c>
       <c r="K47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>51</v>
       </c>
@@ -2889,29 +3033,32 @@
       <c r="D48" t="s">
         <v>110</v>
       </c>
-      <c r="E48">
+      <c r="E48" t="s">
+        <v>110</v>
+      </c>
+      <c r="F48">
         <v>1120</v>
       </c>
-      <c r="F48">
+      <c r="G48">
         <v>3954</v>
       </c>
-      <c r="G48">
-        <v>2</v>
-      </c>
       <c r="H48">
+        <v>2</v>
+      </c>
+      <c r="I48">
         <v>12</v>
       </c>
-      <c r="I48">
+      <c r="J48">
         <v>19020</v>
       </c>
-      <c r="J48">
-        <v>0</v>
-      </c>
       <c r="K48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>52</v>
       </c>
@@ -2924,29 +3071,32 @@
       <c r="D49" t="s">
         <v>106</v>
       </c>
-      <c r="E49">
+      <c r="E49" t="s">
+        <v>110</v>
+      </c>
+      <c r="F49">
         <v>1459</v>
       </c>
-      <c r="F49">
+      <c r="G49">
         <v>14964</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>10</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <v>8</v>
       </c>
-      <c r="I49">
+      <c r="J49">
         <v>10218</v>
       </c>
-      <c r="J49">
-        <v>0</v>
-      </c>
       <c r="K49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>54</v>
       </c>
@@ -2959,29 +3109,32 @@
       <c r="D50" t="s">
         <v>110</v>
       </c>
-      <c r="E50">
+      <c r="E50" t="s">
+        <v>110</v>
+      </c>
+      <c r="F50">
         <v>1462</v>
       </c>
-      <c r="F50" s="2">
+      <c r="G50" s="2">
         <v>10093</v>
       </c>
-      <c r="G50">
-        <v>2</v>
-      </c>
       <c r="H50">
+        <v>2</v>
+      </c>
+      <c r="I50">
         <v>5</v>
       </c>
-      <c r="I50">
+      <c r="J50">
         <v>1372</v>
       </c>
-      <c r="J50">
-        <v>0</v>
-      </c>
       <c r="K50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
@@ -2994,29 +3147,32 @@
       <c r="D51" t="s">
         <v>110</v>
       </c>
-      <c r="E51">
+      <c r="E51" t="s">
+        <v>110</v>
+      </c>
+      <c r="F51">
         <v>1464</v>
       </c>
-      <c r="F51">
+      <c r="G51">
         <v>10101</v>
       </c>
-      <c r="G51">
-        <v>2</v>
-      </c>
       <c r="H51">
+        <v>2</v>
+      </c>
+      <c r="I51">
         <v>5</v>
       </c>
-      <c r="I51">
+      <c r="J51">
         <v>748</v>
       </c>
-      <c r="J51">
-        <v>0</v>
-      </c>
       <c r="K51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>56</v>
       </c>
@@ -3029,29 +3185,32 @@
       <c r="D52" t="s">
         <v>110</v>
       </c>
-      <c r="E52">
+      <c r="E52" t="s">
+        <v>110</v>
+      </c>
+      <c r="F52">
         <v>1466</v>
       </c>
-      <c r="F52">
+      <c r="G52">
         <v>9979</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>10</v>
       </c>
-      <c r="H52">
+      <c r="I52">
         <v>36</v>
       </c>
-      <c r="I52">
+      <c r="J52">
         <v>2126</v>
       </c>
-      <c r="J52">
-        <v>0</v>
-      </c>
       <c r="K52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>57</v>
       </c>
@@ -3064,29 +3223,32 @@
       <c r="D53" t="s">
         <v>106</v>
       </c>
-      <c r="E53">
+      <c r="E53" t="s">
+        <v>110</v>
+      </c>
+      <c r="F53">
         <v>1467</v>
       </c>
-      <c r="F53">
+      <c r="G53">
         <v>9980</v>
       </c>
-      <c r="G53">
-        <v>2</v>
-      </c>
       <c r="H53">
+        <v>2</v>
+      </c>
+      <c r="I53">
         <v>21</v>
       </c>
-      <c r="I53">
+      <c r="J53">
         <v>540</v>
       </c>
-      <c r="J53">
-        <v>0</v>
-      </c>
       <c r="K53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
@@ -3099,29 +3261,32 @@
       <c r="D54" t="s">
         <v>110</v>
       </c>
-      <c r="E54">
+      <c r="E54" t="s">
+        <v>110</v>
+      </c>
+      <c r="F54">
         <v>1471</v>
       </c>
-      <c r="F54">
+      <c r="G54">
         <v>9983</v>
       </c>
-      <c r="G54">
-        <v>2</v>
-      </c>
       <c r="H54">
+        <v>2</v>
+      </c>
+      <c r="I54">
         <v>15</v>
       </c>
-      <c r="I54">
+      <c r="J54">
         <v>14980</v>
       </c>
-      <c r="J54">
-        <v>0</v>
-      </c>
       <c r="K54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>60</v>
       </c>
@@ -3134,29 +3299,32 @@
       <c r="D55" t="s">
         <v>106</v>
       </c>
-      <c r="E55">
+      <c r="E55" t="s">
+        <v>110</v>
+      </c>
+      <c r="F55">
         <v>1475</v>
       </c>
-      <c r="F55">
+      <c r="G55">
         <v>9985</v>
       </c>
-      <c r="G55">
+      <c r="H55">
         <v>6</v>
       </c>
-      <c r="H55">
+      <c r="I55">
         <v>52</v>
       </c>
-      <c r="I55">
+      <c r="J55">
         <v>6118</v>
       </c>
-      <c r="J55">
-        <v>0</v>
-      </c>
       <c r="K55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>63</v>
       </c>
@@ -3169,29 +3337,32 @@
       <c r="D56" t="s">
         <v>110</v>
       </c>
-      <c r="E56">
+      <c r="E56" t="s">
+        <v>110</v>
+      </c>
+      <c r="F56">
         <v>1479</v>
       </c>
-      <c r="F56">
+      <c r="G56">
         <v>9970</v>
       </c>
-      <c r="G56">
-        <v>2</v>
-      </c>
       <c r="H56">
+        <v>2</v>
+      </c>
+      <c r="I56">
         <v>101</v>
       </c>
-      <c r="I56">
+      <c r="J56">
         <v>1212</v>
       </c>
-      <c r="J56">
-        <v>0</v>
-      </c>
       <c r="K56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>64</v>
       </c>
@@ -3204,29 +3375,32 @@
       <c r="D57" t="s">
         <v>110</v>
       </c>
-      <c r="E57">
+      <c r="E57" t="s">
+        <v>110</v>
+      </c>
+      <c r="F57">
         <v>1480</v>
       </c>
-      <c r="F57">
+      <c r="G57">
         <v>9971</v>
       </c>
-      <c r="G57">
-        <v>2</v>
-      </c>
       <c r="H57">
+        <v>2</v>
+      </c>
+      <c r="I57">
         <v>11</v>
       </c>
-      <c r="I57">
+      <c r="J57">
         <v>583</v>
       </c>
-      <c r="J57">
-        <v>0</v>
-      </c>
       <c r="K57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>66</v>
       </c>
@@ -3239,29 +3413,32 @@
       <c r="D58" t="s">
         <v>110</v>
       </c>
-      <c r="E58">
+      <c r="E58" t="s">
+        <v>110</v>
+      </c>
+      <c r="F58">
         <v>1486</v>
       </c>
-      <c r="F58">
+      <c r="G58">
         <v>9977</v>
       </c>
-      <c r="G58">
-        <v>2</v>
-      </c>
       <c r="H58">
+        <v>2</v>
+      </c>
+      <c r="I58">
         <v>119</v>
       </c>
-      <c r="I58">
+      <c r="J58">
         <v>34465</v>
       </c>
-      <c r="J58">
-        <v>0</v>
-      </c>
       <c r="K58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>67</v>
       </c>
@@ -3274,29 +3451,32 @@
       <c r="D59" t="s">
         <v>110</v>
       </c>
-      <c r="E59">
+      <c r="E59" t="s">
+        <v>110</v>
+      </c>
+      <c r="F59">
         <v>1487</v>
       </c>
-      <c r="F59">
+      <c r="G59">
         <v>9978</v>
       </c>
-      <c r="G59">
-        <v>2</v>
-      </c>
       <c r="H59">
+        <v>2</v>
+      </c>
+      <c r="I59">
         <v>73</v>
       </c>
-      <c r="I59">
+      <c r="J59">
         <v>2534</v>
       </c>
-      <c r="J59">
-        <v>0</v>
-      </c>
       <c r="K59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>68</v>
       </c>
@@ -3309,29 +3489,32 @@
       <c r="D60" t="s">
         <v>110</v>
       </c>
-      <c r="E60">
+      <c r="E60" t="s">
+        <v>110</v>
+      </c>
+      <c r="F60">
         <v>1489</v>
       </c>
-      <c r="F60">
+      <c r="G60">
         <v>9952</v>
       </c>
-      <c r="G60">
-        <v>2</v>
-      </c>
       <c r="H60">
+        <v>2</v>
+      </c>
+      <c r="I60">
         <v>6</v>
       </c>
-      <c r="I60">
+      <c r="J60">
         <v>5404</v>
       </c>
-      <c r="J60">
-        <v>0</v>
-      </c>
       <c r="K60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>69</v>
       </c>
@@ -3344,29 +3527,32 @@
       <c r="D61" t="s">
         <v>110</v>
       </c>
-      <c r="E61">
+      <c r="E61" t="s">
+        <v>110</v>
+      </c>
+      <c r="F61">
         <v>1491</v>
       </c>
-      <c r="F61">
+      <c r="G61">
         <v>9954</v>
       </c>
-      <c r="G61">
+      <c r="H61">
         <v>100</v>
       </c>
-      <c r="H61">
+      <c r="I61">
         <v>65</v>
       </c>
-      <c r="I61">
+      <c r="J61">
         <v>1600</v>
       </c>
-      <c r="J61">
-        <v>0</v>
-      </c>
       <c r="K61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>70</v>
       </c>
@@ -3379,29 +3565,32 @@
       <c r="D62" t="s">
         <v>110</v>
       </c>
-      <c r="E62">
+      <c r="E62" t="s">
+        <v>110</v>
+      </c>
+      <c r="F62">
         <v>1492</v>
       </c>
-      <c r="F62">
+      <c r="G62">
         <v>9955</v>
       </c>
-      <c r="G62">
+      <c r="H62">
         <v>100</v>
       </c>
-      <c r="H62">
+      <c r="I62">
         <v>65</v>
       </c>
-      <c r="I62">
+      <c r="J62">
         <v>1600</v>
       </c>
-      <c r="J62">
-        <v>0</v>
-      </c>
       <c r="K62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>72</v>
       </c>
@@ -3414,29 +3603,32 @@
       <c r="D63" t="s">
         <v>110</v>
       </c>
-      <c r="E63">
+      <c r="E63" t="s">
+        <v>110</v>
+      </c>
+      <c r="F63">
         <v>1494</v>
       </c>
-      <c r="F63">
+      <c r="G63">
         <v>9957</v>
       </c>
-      <c r="G63">
-        <v>2</v>
-      </c>
       <c r="H63">
+        <v>2</v>
+      </c>
+      <c r="I63">
         <v>42</v>
       </c>
-      <c r="I63">
+      <c r="J63">
         <v>1055</v>
       </c>
-      <c r="J63">
-        <v>0</v>
-      </c>
       <c r="K63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>73</v>
       </c>
@@ -3449,29 +3641,32 @@
       <c r="D64" t="s">
         <v>110</v>
       </c>
-      <c r="E64">
+      <c r="E64" t="s">
+        <v>110</v>
+      </c>
+      <c r="F64">
         <v>1497</v>
       </c>
-      <c r="F64">
+      <c r="G64">
         <v>9960</v>
       </c>
-      <c r="G64">
+      <c r="H64">
         <v>4</v>
       </c>
-      <c r="H64">
+      <c r="I64">
         <v>25</v>
       </c>
-      <c r="I64">
+      <c r="J64">
         <v>5456</v>
       </c>
-      <c r="J64">
-        <v>0</v>
-      </c>
       <c r="K64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>75</v>
       </c>
@@ -3484,29 +3679,32 @@
       <c r="D65" t="s">
         <v>110</v>
       </c>
-      <c r="E65">
+      <c r="E65" t="s">
+        <v>110</v>
+      </c>
+      <c r="F65">
         <v>1504</v>
       </c>
-      <c r="F65">
+      <c r="G65">
         <v>9967</v>
       </c>
-      <c r="G65">
-        <v>2</v>
-      </c>
       <c r="H65">
+        <v>2</v>
+      </c>
+      <c r="I65">
         <v>34</v>
       </c>
-      <c r="I65">
+      <c r="J65">
         <v>1941</v>
       </c>
-      <c r="J65">
-        <v>0</v>
-      </c>
       <c r="K65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>76</v>
       </c>
@@ -3519,29 +3717,32 @@
       <c r="D66" t="s">
         <v>110</v>
       </c>
-      <c r="E66">
+      <c r="E66" t="s">
+        <v>110</v>
+      </c>
+      <c r="F66">
         <v>1510</v>
       </c>
-      <c r="F66">
+      <c r="G66">
         <v>9946</v>
       </c>
-      <c r="G66">
-        <v>2</v>
-      </c>
       <c r="H66">
+        <v>2</v>
+      </c>
+      <c r="I66">
         <v>31</v>
       </c>
-      <c r="I66">
+      <c r="J66">
         <v>569</v>
       </c>
-      <c r="J66">
-        <v>0</v>
-      </c>
       <c r="K66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>78</v>
       </c>
@@ -3554,29 +3755,32 @@
       <c r="D67" t="s">
         <v>110</v>
       </c>
-      <c r="E67">
+      <c r="E67" t="s">
+        <v>110</v>
+      </c>
+      <c r="F67">
         <v>1590</v>
       </c>
-      <c r="F67">
+      <c r="G67">
         <v>7592</v>
       </c>
-      <c r="G67">
-        <v>2</v>
-      </c>
       <c r="H67">
+        <v>2</v>
+      </c>
+      <c r="I67">
         <v>15</v>
       </c>
-      <c r="I67">
+      <c r="J67">
         <v>48842</v>
       </c>
-      <c r="J67">
+      <c r="K67">
         <v>3620</v>
       </c>
-      <c r="K67">
+      <c r="L67">
         <v>6465</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>82</v>
       </c>
@@ -3589,29 +3793,32 @@
       <c r="D68" t="s">
         <v>106</v>
       </c>
-      <c r="E68">
+      <c r="E68" t="s">
+        <v>110</v>
+      </c>
+      <c r="F68">
         <v>4538</v>
       </c>
-      <c r="F68">
+      <c r="G68">
         <v>14969</v>
       </c>
-      <c r="G68">
+      <c r="H68">
         <v>5</v>
       </c>
-      <c r="H68">
+      <c r="I68">
         <v>33</v>
       </c>
-      <c r="I68">
+      <c r="J68">
         <v>9873</v>
       </c>
-      <c r="J68">
-        <v>0</v>
-      </c>
       <c r="K68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>83</v>
       </c>
@@ -3624,29 +3831,32 @@
       <c r="D69" t="s">
         <v>106</v>
       </c>
-      <c r="E69">
+      <c r="E69" t="s">
+        <v>110</v>
+      </c>
+      <c r="F69">
         <v>6332</v>
       </c>
-      <c r="F69">
+      <c r="G69">
         <v>14968</v>
       </c>
-      <c r="G69">
-        <v>2</v>
-      </c>
       <c r="H69">
+        <v>2</v>
+      </c>
+      <c r="I69">
         <v>40</v>
       </c>
-      <c r="I69">
+      <c r="J69">
         <v>540</v>
       </c>
-      <c r="J69">
+      <c r="K69">
         <v>263</v>
       </c>
-      <c r="K69">
+      <c r="L69">
         <v>999</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>84</v>
       </c>
@@ -3659,29 +3869,32 @@
       <c r="D70" t="s">
         <v>110</v>
       </c>
-      <c r="E70">
+      <c r="E70" t="s">
+        <v>110</v>
+      </c>
+      <c r="F70">
         <v>23380</v>
       </c>
-      <c r="F70">
+      <c r="G70">
         <v>14967</v>
       </c>
-      <c r="G70">
+      <c r="H70">
         <v>6</v>
       </c>
-      <c r="H70">
+      <c r="I70">
         <v>35</v>
       </c>
-      <c r="I70">
+      <c r="J70">
         <v>2796</v>
       </c>
-      <c r="J70">
+      <c r="K70">
         <v>2795</v>
       </c>
-      <c r="K70">
+      <c r="L70">
         <v>68100</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>85</v>
       </c>
@@ -3694,29 +3907,32 @@
       <c r="D71" t="s">
         <v>106</v>
       </c>
-      <c r="E71">
+      <c r="E71" t="s">
+        <v>110</v>
+      </c>
+      <c r="F71">
         <v>23381</v>
       </c>
-      <c r="F71">
+      <c r="G71">
         <v>125920</v>
       </c>
-      <c r="G71">
-        <v>2</v>
-      </c>
       <c r="H71">
+        <v>2</v>
+      </c>
+      <c r="I71">
         <v>13</v>
       </c>
-      <c r="I71">
+      <c r="J71">
         <v>500</v>
       </c>
-      <c r="J71">
+      <c r="K71">
         <v>401</v>
       </c>
-      <c r="K71">
+      <c r="L71">
         <v>835</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>87</v>
       </c>
@@ -3729,29 +3945,32 @@
       <c r="D72" t="s">
         <v>110</v>
       </c>
-      <c r="E72">
+      <c r="E72" t="s">
+        <v>110</v>
+      </c>
+      <c r="F72">
         <v>40496</v>
       </c>
-      <c r="F72">
+      <c r="G72">
         <v>125921</v>
       </c>
-      <c r="G72">
+      <c r="H72">
         <v>10</v>
       </c>
-      <c r="H72">
+      <c r="I72">
         <v>8</v>
       </c>
-      <c r="I72">
+      <c r="J72">
         <v>500</v>
       </c>
-      <c r="J72">
-        <v>0</v>
-      </c>
       <c r="K72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>88</v>
       </c>
@@ -3764,29 +3983,32 @@
       <c r="D73" t="s">
         <v>110</v>
       </c>
-      <c r="E73">
+      <c r="E73" t="s">
+        <v>110</v>
+      </c>
+      <c r="F73">
         <v>40499</v>
       </c>
-      <c r="F73">
+      <c r="G73">
         <v>125922</v>
       </c>
-      <c r="G73">
+      <c r="H73">
         <v>11</v>
       </c>
-      <c r="H73">
+      <c r="I73">
         <v>41</v>
       </c>
-      <c r="I73">
+      <c r="J73">
         <v>5500</v>
       </c>
-      <c r="J73">
-        <v>0</v>
-      </c>
       <c r="K73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>89</v>
       </c>
@@ -3799,29 +4021,32 @@
       <c r="D74" t="s">
         <v>110</v>
       </c>
-      <c r="E74">
+      <c r="E74" t="s">
+        <v>110</v>
+      </c>
+      <c r="F74">
         <v>40536</v>
       </c>
-      <c r="F74">
+      <c r="G74">
         <v>146607</v>
       </c>
-      <c r="G74">
-        <v>2</v>
-      </c>
       <c r="H74">
+        <v>2</v>
+      </c>
+      <c r="I74">
         <v>123</v>
       </c>
-      <c r="I74">
+      <c r="J74">
         <v>8378</v>
       </c>
-      <c r="J74">
+      <c r="K74">
         <v>7330</v>
       </c>
-      <c r="K74">
+      <c r="L74">
         <v>18372</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>61</v>
       </c>
@@ -3834,29 +4059,32 @@
       <c r="D75" t="s">
         <v>110</v>
       </c>
-      <c r="E75">
+      <c r="E75" t="s">
+        <v>110</v>
+      </c>
+      <c r="F75">
         <v>1476</v>
       </c>
-      <c r="F75">
+      <c r="G75">
         <v>9986</v>
       </c>
-      <c r="G75">
+      <c r="H75">
         <v>6</v>
       </c>
-      <c r="H75">
+      <c r="I75">
         <v>129</v>
       </c>
-      <c r="I75">
+      <c r="J75">
         <v>13910</v>
       </c>
-      <c r="J75">
-        <v>0</v>
-      </c>
       <c r="K75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>53</v>
       </c>
@@ -3869,29 +4097,32 @@
       <c r="D76" t="s">
         <v>110</v>
       </c>
-      <c r="E76">
+      <c r="E76" t="s">
+        <v>110</v>
+      </c>
+      <c r="F76">
         <v>1461</v>
       </c>
-      <c r="F76">
+      <c r="G76">
         <v>14965</v>
       </c>
-      <c r="G76">
-        <v>2</v>
-      </c>
       <c r="H76">
+        <v>2</v>
+      </c>
+      <c r="I76">
         <v>17</v>
       </c>
-      <c r="I76">
+      <c r="J76">
         <v>45211</v>
       </c>
-      <c r="J76">
-        <v>0</v>
-      </c>
       <c r="K76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>71</v>
       </c>
@@ -3904,29 +4135,32 @@
       <c r="D77" t="s">
         <v>110</v>
       </c>
-      <c r="E77">
+      <c r="E77" t="s">
+        <v>110</v>
+      </c>
+      <c r="F77">
         <v>1493</v>
       </c>
-      <c r="F77">
+      <c r="G77">
         <v>9956</v>
       </c>
-      <c r="G77">
+      <c r="H77">
         <v>100</v>
       </c>
-      <c r="H77">
+      <c r="I77">
         <v>65</v>
       </c>
-      <c r="I77">
+      <c r="J77">
         <v>1599</v>
       </c>
-      <c r="J77">
-        <v>0</v>
-      </c>
       <c r="K77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>81</v>
       </c>
@@ -3939,29 +4173,32 @@
       <c r="D78" t="s">
         <v>110</v>
       </c>
-      <c r="E78">
+      <c r="E78" t="s">
+        <v>110</v>
+      </c>
+      <c r="F78">
         <v>4534</v>
       </c>
-      <c r="F78">
+      <c r="G78">
         <v>34537</v>
       </c>
-      <c r="G78">
-        <v>2</v>
-      </c>
       <c r="H78">
+        <v>2</v>
+      </c>
+      <c r="I78">
         <v>31</v>
       </c>
-      <c r="I78">
+      <c r="J78">
         <v>11055</v>
       </c>
-      <c r="J78">
-        <v>0</v>
-      </c>
       <c r="K78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>90</v>
       </c>
@@ -3974,29 +4211,32 @@
       <c r="D79" t="s">
         <v>106</v>
       </c>
-      <c r="E79">
+      <c r="E79" t="s">
+        <v>110</v>
+      </c>
+      <c r="F79">
         <v>40668</v>
       </c>
-      <c r="F79">
+      <c r="G79">
         <v>146195</v>
       </c>
-      <c r="G79">
+      <c r="H79">
         <v>3</v>
       </c>
-      <c r="H79">
+      <c r="I79">
         <v>43</v>
       </c>
-      <c r="I79">
+      <c r="J79">
         <v>67557</v>
       </c>
-      <c r="J79">
-        <v>0</v>
-      </c>
       <c r="K79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>80</v>
       </c>
@@ -4009,29 +4249,32 @@
       <c r="D80" t="s">
         <v>106</v>
       </c>
-      <c r="E80">
+      <c r="E80" t="s">
+        <v>110</v>
+      </c>
+      <c r="F80">
         <v>4135</v>
       </c>
-      <c r="F80">
+      <c r="G80">
         <v>34539</v>
       </c>
-      <c r="G80">
-        <v>2</v>
-      </c>
       <c r="H80">
+        <v>2</v>
+      </c>
+      <c r="I80">
         <v>10</v>
       </c>
-      <c r="I80">
+      <c r="J80">
         <v>32769</v>
       </c>
-      <c r="J80">
-        <v>0</v>
-      </c>
       <c r="K80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>62</v>
       </c>
@@ -4044,29 +4287,32 @@
       <c r="D81" t="s">
         <v>106</v>
       </c>
-      <c r="E81">
+      <c r="E81" t="s">
+        <v>110</v>
+      </c>
+      <c r="F81">
         <v>1478</v>
       </c>
-      <c r="F81">
+      <c r="G81">
         <v>14970</v>
       </c>
-      <c r="G81">
+      <c r="H81">
         <v>6</v>
       </c>
-      <c r="H81">
+      <c r="I81">
         <v>562</v>
       </c>
-      <c r="I81">
+      <c r="J81">
         <v>10299</v>
       </c>
-      <c r="J81">
-        <v>0</v>
-      </c>
       <c r="K81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>79</v>
       </c>
@@ -4079,29 +4325,32 @@
       <c r="D82" t="s">
         <v>106</v>
       </c>
-      <c r="E82">
+      <c r="E82" t="s">
+        <v>110</v>
+      </c>
+      <c r="F82">
         <v>4134</v>
       </c>
-      <c r="F82">
+      <c r="G82">
         <v>14966</v>
       </c>
-      <c r="G82">
-        <v>2</v>
-      </c>
       <c r="H82">
+        <v>2</v>
+      </c>
+      <c r="I82">
         <v>1777</v>
       </c>
-      <c r="I82">
+      <c r="J82">
         <v>3751</v>
       </c>
-      <c r="J82">
-        <v>0</v>
-      </c>
       <c r="K82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>86</v>
       </c>
@@ -4114,29 +4363,32 @@
       <c r="D83" t="s">
         <v>106</v>
       </c>
-      <c r="E83">
+      <c r="E83" t="s">
+        <v>110</v>
+      </c>
+      <c r="F83">
         <v>23512</v>
       </c>
-      <c r="F83">
+      <c r="G83">
         <v>146606</v>
       </c>
-      <c r="G83">
-        <v>2</v>
-      </c>
       <c r="H83">
+        <v>2</v>
+      </c>
+      <c r="I83">
         <v>29</v>
       </c>
-      <c r="I83">
+      <c r="J83">
         <v>98050</v>
       </c>
-      <c r="J83">
+      <c r="K83">
         <v>1</v>
       </c>
-      <c r="K83">
+      <c r="L83">
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>40</v>
       </c>
@@ -4149,29 +4401,32 @@
       <c r="D84" t="s">
         <v>106</v>
       </c>
-      <c r="E84">
+      <c r="E84" t="s">
+        <v>110</v>
+      </c>
+      <c r="F84">
         <v>554</v>
       </c>
-      <c r="F84">
+      <c r="G84">
         <v>3573</v>
       </c>
-      <c r="G84">
+      <c r="H84">
         <v>10</v>
       </c>
-      <c r="H84">
+      <c r="I84">
         <v>785</v>
       </c>
-      <c r="I84">
+      <c r="J84">
         <v>70000</v>
       </c>
-      <c r="J84">
-        <v>0</v>
-      </c>
       <c r="K84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>41</v>
       </c>
@@ -4184,29 +4439,32 @@
       <c r="D85" t="s">
         <v>106</v>
       </c>
-      <c r="E85">
+      <c r="E85" t="s">
+        <v>110</v>
+      </c>
+      <c r="F85">
         <v>1038</v>
       </c>
-      <c r="F85">
+      <c r="G85">
         <v>3891</v>
       </c>
-      <c r="G85">
-        <v>2</v>
-      </c>
       <c r="H85">
+        <v>2</v>
+      </c>
+      <c r="I85">
         <v>971</v>
       </c>
-      <c r="I85">
+      <c r="J85">
         <v>3468</v>
       </c>
-      <c r="J85">
-        <v>0</v>
-      </c>
       <c r="K85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -4219,29 +4477,32 @@
       <c r="D86" t="s">
         <v>106</v>
       </c>
-      <c r="E86">
+      <c r="E86" t="s">
+        <v>110</v>
+      </c>
+      <c r="F86">
         <v>300</v>
       </c>
-      <c r="F86">
+      <c r="G86">
         <v>3481</v>
       </c>
-      <c r="G86">
+      <c r="H86">
         <v>26</v>
       </c>
-      <c r="H86">
+      <c r="I86">
         <v>618</v>
       </c>
-      <c r="I86">
+      <c r="J86">
         <v>7797</v>
       </c>
-      <c r="J86">
-        <v>0</v>
-      </c>
       <c r="K86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>58</v>
       </c>
@@ -4254,29 +4515,32 @@
       <c r="D87" t="s">
         <v>106</v>
       </c>
-      <c r="E87">
+      <c r="E87" t="s">
+        <v>110</v>
+      </c>
+      <c r="F87">
         <v>1468</v>
       </c>
-      <c r="F87">
+      <c r="G87">
         <v>9981</v>
       </c>
-      <c r="G87">
+      <c r="H87">
         <v>9</v>
       </c>
-      <c r="H87">
+      <c r="I87">
         <v>857</v>
       </c>
-      <c r="I87">
+      <c r="J87">
         <v>1080</v>
       </c>
-      <c r="J87">
-        <v>0</v>
-      </c>
       <c r="K87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>74</v>
       </c>
@@ -4289,29 +4553,32 @@
       <c r="D88" t="s">
         <v>106</v>
       </c>
-      <c r="E88">
+      <c r="E88" t="s">
+        <v>110</v>
+      </c>
+      <c r="F88">
         <v>1501</v>
       </c>
-      <c r="F88">
+      <c r="G88">
         <v>9964</v>
       </c>
-      <c r="G88">
+      <c r="H88">
         <v>10</v>
       </c>
-      <c r="H88">
+      <c r="I88">
         <v>257</v>
       </c>
-      <c r="I88">
+      <c r="J88">
         <v>1593</v>
       </c>
-      <c r="J88">
-        <v>0</v>
-      </c>
       <c r="K88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>77</v>
       </c>
@@ -4324,29 +4591,32 @@
       <c r="D89" t="s">
         <v>106</v>
       </c>
-      <c r="E89">
+      <c r="E89" t="s">
+        <v>110</v>
+      </c>
+      <c r="F89">
         <v>1515</v>
       </c>
-      <c r="F89">
+      <c r="G89">
         <v>9950</v>
       </c>
-      <c r="G89">
+      <c r="H89">
         <v>20</v>
       </c>
-      <c r="H89">
+      <c r="I89">
         <v>1301</v>
       </c>
-      <c r="I89">
+      <c r="J89">
         <v>571</v>
       </c>
-      <c r="J89">
-        <v>0</v>
-      </c>
       <c r="K89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>65</v>
       </c>
@@ -4359,29 +4629,32 @@
       <c r="D90" t="s">
         <v>106</v>
       </c>
-      <c r="E90">
+      <c r="E90" t="s">
+        <v>110</v>
+      </c>
+      <c r="F90">
         <v>1485</v>
       </c>
-      <c r="F90">
+      <c r="G90">
         <v>9976</v>
       </c>
-      <c r="G90">
-        <v>2</v>
-      </c>
       <c r="H90">
+        <v>2</v>
+      </c>
+      <c r="I90">
         <v>501</v>
       </c>
-      <c r="I90">
+      <c r="J90">
         <v>2600</v>
       </c>
-      <c r="J90">
-        <v>0</v>
-      </c>
       <c r="K90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>8</v>
       </c>
@@ -4394,29 +4667,32 @@
       <c r="D91" t="s">
         <v>106</v>
       </c>
-      <c r="E91">
-        <v>20</v>
+      <c r="E91" t="s">
+        <v>110</v>
       </c>
       <c r="F91">
         <v>20</v>
       </c>
       <c r="G91">
+        <v>20</v>
+      </c>
+      <c r="H91">
         <v>10</v>
       </c>
-      <c r="H91">
+      <c r="I91">
         <v>241</v>
       </c>
-      <c r="I91">
+      <c r="J91">
         <v>2000</v>
       </c>
-      <c r="J91">
-        <v>0</v>
-      </c>
       <c r="K91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>49</v>
       </c>
@@ -4429,29 +4705,32 @@
       <c r="D92" t="s">
         <v>106</v>
       </c>
-      <c r="E92">
+      <c r="E92" t="s">
+        <v>110</v>
+      </c>
+      <c r="F92">
         <v>1112</v>
       </c>
-      <c r="F92">
+      <c r="G92">
         <v>3946</v>
       </c>
-      <c r="G92">
-        <v>2</v>
-      </c>
       <c r="H92">
+        <v>2</v>
+      </c>
+      <c r="I92">
         <v>231</v>
-      </c>
-      <c r="I92">
-        <v>50000</v>
       </c>
       <c r="J92">
         <v>50000</v>
       </c>
       <c r="K92">
+        <v>50000</v>
+      </c>
+      <c r="L92">
         <v>8024152</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>50</v>
       </c>
@@ -4464,25 +4743,28 @@
       <c r="D93" t="s">
         <v>106</v>
       </c>
-      <c r="E93">
+      <c r="E93" t="s">
+        <v>110</v>
+      </c>
+      <c r="F93">
         <v>1114</v>
       </c>
-      <c r="F93" s="2">
+      <c r="G93" s="2">
         <v>3948</v>
       </c>
-      <c r="G93">
-        <v>2</v>
-      </c>
       <c r="H93">
+        <v>2</v>
+      </c>
+      <c r="I93">
         <v>231</v>
-      </c>
-      <c r="I93">
-        <v>50000</v>
       </c>
       <c r="J93">
         <v>50000</v>
       </c>
       <c r="K93">
+        <v>50000</v>
+      </c>
+      <c r="L93">
         <v>8024152</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SS-Rank members at end of epoch
</commit_message>
<xml_diff>
--- a/benchmark/Configuration.xlsx
+++ b/benchmark/Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\autem\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F83F8F-A2D3-4567-9250-605C5260E5BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B863584D-2AE3-4F17-8A1D-DB99EAF85BB6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="960" windowWidth="14640" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openml_100" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="113">
   <si>
     <t>kr-vs-kp</t>
   </si>
@@ -307,9 +307,6 @@
     <t>Australian</t>
   </si>
   <si>
-    <t>did</t>
-  </si>
-  <si>
     <t>task_id</t>
   </si>
   <si>
@@ -368,6 +365,9 @@
   </si>
   <si>
     <t>STC</t>
+  </si>
+  <si>
+    <t>SS</t>
   </si>
 </sst>
 </file>
@@ -1215,17 +1215,16 @@
   <dimension ref="A1:L93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="17.7109375" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -1236,40 +1235,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>109</v>
-      </c>
       <c r="D1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1277,19 +1276,19 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
-        <v>106</v>
-      </c>
-      <c r="F2">
-        <v>37</v>
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
       </c>
       <c r="G2">
         <v>37</v>
@@ -1315,19 +1314,19 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F3">
-        <v>54</v>
+        <v>105</v>
+      </c>
+      <c r="F3" t="s">
+        <v>105</v>
       </c>
       <c r="G3">
         <v>53</v>
@@ -1353,19 +1352,19 @@
         <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F4">
-        <v>40981</v>
+        <v>109</v>
+      </c>
+      <c r="F4" t="s">
+        <v>105</v>
       </c>
       <c r="G4">
         <v>125923</v>
@@ -1391,19 +1390,19 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F5">
-        <v>50</v>
+        <v>109</v>
+      </c>
+      <c r="F5" t="s">
+        <v>105</v>
       </c>
       <c r="G5">
         <v>145804</v>
@@ -1429,19 +1428,19 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F6">
-        <v>18</v>
+        <v>109</v>
+      </c>
+      <c r="F6" t="s">
+        <v>105</v>
       </c>
       <c r="G6">
         <v>18</v>
@@ -1467,19 +1466,19 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F7">
-        <v>11</v>
+        <v>109</v>
+      </c>
+      <c r="F7" t="s">
+        <v>105</v>
       </c>
       <c r="G7">
         <v>11</v>
@@ -1505,19 +1504,19 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E8" t="s">
-        <v>110</v>
-      </c>
-      <c r="F8">
-        <v>38</v>
+        <v>109</v>
+      </c>
+      <c r="F8" t="s">
+        <v>109</v>
       </c>
       <c r="G8">
         <v>3021</v>
@@ -1543,19 +1542,19 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E9" t="s">
-        <v>110</v>
-      </c>
-      <c r="F9">
-        <v>29</v>
+        <v>109</v>
+      </c>
+      <c r="F9" t="s">
+        <v>109</v>
       </c>
       <c r="G9">
         <v>29</v>
@@ -1581,19 +1580,19 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E10" t="s">
-        <v>110</v>
-      </c>
-      <c r="F10">
-        <v>42</v>
+        <v>109</v>
+      </c>
+      <c r="F10" t="s">
+        <v>109</v>
       </c>
       <c r="G10">
         <v>41</v>
@@ -1619,19 +1618,19 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E11" t="s">
-        <v>110</v>
-      </c>
-      <c r="F11">
-        <v>15</v>
+        <v>109</v>
+      </c>
+      <c r="F11" t="s">
+        <v>109</v>
       </c>
       <c r="G11">
         <v>1779</v>
@@ -1657,19 +1656,19 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E12" t="s">
-        <v>110</v>
-      </c>
-      <c r="F12">
-        <v>23</v>
+        <v>109</v>
+      </c>
+      <c r="F12" t="s">
+        <v>109</v>
       </c>
       <c r="G12">
         <v>23</v>
@@ -1695,19 +1694,19 @@
         <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E13" t="s">
-        <v>106</v>
-      </c>
-      <c r="F13">
-        <v>470</v>
+        <v>105</v>
+      </c>
+      <c r="F13" t="s">
+        <v>109</v>
       </c>
       <c r="G13">
         <v>3561</v>
@@ -1733,19 +1732,19 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E14" t="s">
-        <v>110</v>
-      </c>
-      <c r="F14">
-        <v>24</v>
+        <v>109</v>
+      </c>
+      <c r="F14" t="s">
+        <v>109</v>
       </c>
       <c r="G14">
         <v>1788</v>
@@ -1771,19 +1770,19 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E15" t="s">
-        <v>110</v>
-      </c>
-      <c r="F15">
-        <v>28</v>
+        <v>109</v>
+      </c>
+      <c r="F15" t="s">
+        <v>109</v>
       </c>
       <c r="G15">
         <v>28</v>
@@ -1809,19 +1808,19 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E16" t="s">
-        <v>110</v>
-      </c>
-      <c r="F16">
-        <v>31</v>
+        <v>109</v>
+      </c>
+      <c r="F16" t="s">
+        <v>109</v>
       </c>
       <c r="G16">
         <v>31</v>
@@ -1847,19 +1846,19 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E17" t="s">
-        <v>110</v>
-      </c>
-      <c r="F17">
-        <v>32</v>
+        <v>109</v>
+      </c>
+      <c r="F17" t="s">
+        <v>109</v>
       </c>
       <c r="G17">
         <v>32</v>
@@ -1885,19 +1884,19 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E18" t="s">
-        <v>110</v>
-      </c>
-      <c r="F18">
-        <v>3</v>
+        <v>109</v>
+      </c>
+      <c r="F18" t="s">
+        <v>109</v>
       </c>
       <c r="G18">
         <v>3</v>
@@ -1923,19 +1922,19 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E19" t="s">
-        <v>110</v>
-      </c>
-      <c r="F19">
-        <v>6</v>
+        <v>109</v>
+      </c>
+      <c r="F19" t="s">
+        <v>109</v>
       </c>
       <c r="G19">
         <v>6</v>
@@ -1961,19 +1960,19 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E20" t="s">
-        <v>110</v>
-      </c>
-      <c r="F20">
-        <v>12</v>
+        <v>109</v>
+      </c>
+      <c r="F20" t="s">
+        <v>109</v>
       </c>
       <c r="G20">
         <v>12</v>
@@ -1999,19 +1998,19 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E21" t="s">
-        <v>110</v>
-      </c>
-      <c r="F21">
-        <v>14</v>
+        <v>109</v>
+      </c>
+      <c r="F21" t="s">
+        <v>109</v>
       </c>
       <c r="G21">
         <v>1778</v>
@@ -2037,19 +2036,19 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E22" t="s">
-        <v>110</v>
-      </c>
-      <c r="F22">
-        <v>16</v>
+        <v>109</v>
+      </c>
+      <c r="F22" t="s">
+        <v>109</v>
       </c>
       <c r="G22">
         <v>16</v>
@@ -2075,19 +2074,19 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E23" t="s">
-        <v>110</v>
-      </c>
-      <c r="F23">
-        <v>22</v>
+        <v>109</v>
+      </c>
+      <c r="F23" t="s">
+        <v>109</v>
       </c>
       <c r="G23">
         <v>22</v>
@@ -2113,19 +2112,19 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E24" t="s">
-        <v>110</v>
-      </c>
-      <c r="F24">
-        <v>36</v>
+        <v>109</v>
+      </c>
+      <c r="F24" t="s">
+        <v>109</v>
       </c>
       <c r="G24">
         <v>36</v>
@@ -2151,19 +2150,19 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E25" t="s">
-        <v>110</v>
-      </c>
-      <c r="F25">
-        <v>44</v>
+        <v>109</v>
+      </c>
+      <c r="F25" t="s">
+        <v>109</v>
       </c>
       <c r="G25">
         <v>43</v>
@@ -2189,19 +2188,19 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E26" t="s">
-        <v>110</v>
-      </c>
-      <c r="F26">
-        <v>46</v>
+        <v>109</v>
+      </c>
+      <c r="F26" t="s">
+        <v>109</v>
       </c>
       <c r="G26">
         <v>45</v>
@@ -2227,19 +2226,19 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E27" t="s">
-        <v>110</v>
-      </c>
-      <c r="F27">
-        <v>60</v>
+        <v>109</v>
+      </c>
+      <c r="F27" t="s">
+        <v>109</v>
       </c>
       <c r="G27">
         <v>58</v>
@@ -2265,19 +2264,19 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E28" t="s">
-        <v>106</v>
-      </c>
-      <c r="F28">
-        <v>151</v>
+        <v>105</v>
+      </c>
+      <c r="F28" t="s">
+        <v>109</v>
       </c>
       <c r="G28">
         <v>219</v>
@@ -2303,19 +2302,19 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E29" t="s">
-        <v>110</v>
-      </c>
-      <c r="F29">
-        <v>182</v>
+        <v>109</v>
+      </c>
+      <c r="F29" t="s">
+        <v>109</v>
       </c>
       <c r="G29">
         <v>2074</v>
@@ -2341,19 +2340,19 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E30" t="s">
-        <v>106</v>
-      </c>
-      <c r="F30">
-        <v>188</v>
+        <v>105</v>
+      </c>
+      <c r="F30" t="s">
+        <v>109</v>
       </c>
       <c r="G30">
         <v>2125</v>
@@ -2379,19 +2378,19 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E31" t="s">
-        <v>106</v>
-      </c>
-      <c r="F31">
-        <v>307</v>
+        <v>105</v>
+      </c>
+      <c r="F31" t="s">
+        <v>109</v>
       </c>
       <c r="G31">
         <v>3022</v>
@@ -2417,19 +2416,19 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E32" t="s">
-        <v>110</v>
-      </c>
-      <c r="F32">
-        <v>312</v>
+        <v>109</v>
+      </c>
+      <c r="F32" t="s">
+        <v>109</v>
       </c>
       <c r="G32">
         <v>3485</v>
@@ -2455,19 +2454,19 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E33" t="s">
-        <v>106</v>
-      </c>
-      <c r="F33">
-        <v>333</v>
+        <v>105</v>
+      </c>
+      <c r="F33" t="s">
+        <v>109</v>
       </c>
       <c r="G33" s="2">
         <v>3492</v>
@@ -2493,19 +2492,19 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E34" t="s">
-        <v>106</v>
-      </c>
-      <c r="F34">
-        <v>334</v>
+        <v>105</v>
+      </c>
+      <c r="F34" t="s">
+        <v>109</v>
       </c>
       <c r="G34">
         <v>3493</v>
@@ -2531,19 +2530,19 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E35" t="s">
-        <v>106</v>
-      </c>
-      <c r="F35">
-        <v>335</v>
+        <v>105</v>
+      </c>
+      <c r="F35" t="s">
+        <v>109</v>
       </c>
       <c r="G35">
         <v>3494</v>
@@ -2569,19 +2568,19 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E36" t="s">
-        <v>110</v>
-      </c>
-      <c r="F36">
-        <v>375</v>
+        <v>109</v>
+      </c>
+      <c r="F36" t="s">
+        <v>109</v>
       </c>
       <c r="G36">
         <v>4544</v>
@@ -2607,19 +2606,19 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E37" t="s">
-        <v>110</v>
-      </c>
-      <c r="F37">
-        <v>377</v>
+        <v>109</v>
+      </c>
+      <c r="F37" t="s">
+        <v>109</v>
       </c>
       <c r="G37">
         <v>3512</v>
@@ -2645,19 +2644,19 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E38" t="s">
-        <v>110</v>
-      </c>
-      <c r="F38">
-        <v>451</v>
+        <v>109</v>
+      </c>
+      <c r="F38" t="s">
+        <v>109</v>
       </c>
       <c r="G38">
         <v>3543</v>
@@ -2683,19 +2682,19 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E39" t="s">
-        <v>106</v>
-      </c>
-      <c r="F39">
-        <v>458</v>
+        <v>105</v>
+      </c>
+      <c r="F39" t="s">
+        <v>109</v>
       </c>
       <c r="G39">
         <v>3549</v>
@@ -2721,19 +2720,19 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E40" t="s">
-        <v>110</v>
-      </c>
-      <c r="F40">
-        <v>469</v>
+        <v>109</v>
+      </c>
+      <c r="F40" t="s">
+        <v>109</v>
       </c>
       <c r="G40">
         <v>3560</v>
@@ -2759,19 +2758,19 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E41" t="s">
-        <v>110</v>
-      </c>
-      <c r="F41">
-        <v>1046</v>
+        <v>109</v>
+      </c>
+      <c r="F41" t="s">
+        <v>109</v>
       </c>
       <c r="G41">
         <v>3899</v>
@@ -2797,19 +2796,19 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C42" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E42" t="s">
-        <v>110</v>
-      </c>
-      <c r="F42">
-        <v>1049</v>
+        <v>109</v>
+      </c>
+      <c r="F42" t="s">
+        <v>109</v>
       </c>
       <c r="G42">
         <v>3902</v>
@@ -2835,19 +2834,19 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E43" t="s">
-        <v>110</v>
-      </c>
-      <c r="F43">
-        <v>1050</v>
+        <v>109</v>
+      </c>
+      <c r="F43" t="s">
+        <v>109</v>
       </c>
       <c r="G43">
         <v>3903</v>
@@ -2873,19 +2872,19 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C44" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E44" t="s">
-        <v>110</v>
-      </c>
-      <c r="F44">
-        <v>1053</v>
+        <v>109</v>
+      </c>
+      <c r="F44" t="s">
+        <v>109</v>
       </c>
       <c r="G44">
         <v>3904</v>
@@ -2911,19 +2910,19 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E45" t="s">
-        <v>110</v>
-      </c>
-      <c r="F45">
-        <v>1063</v>
+        <v>109</v>
+      </c>
+      <c r="F45" t="s">
+        <v>109</v>
       </c>
       <c r="G45">
         <v>3913</v>
@@ -2949,19 +2948,19 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E46" t="s">
-        <v>110</v>
-      </c>
-      <c r="F46">
-        <v>1067</v>
+        <v>109</v>
+      </c>
+      <c r="F46" t="s">
+        <v>109</v>
       </c>
       <c r="G46">
         <v>3917</v>
@@ -2987,19 +2986,19 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D47" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E47" t="s">
-        <v>110</v>
-      </c>
-      <c r="F47">
-        <v>1068</v>
+        <v>109</v>
+      </c>
+      <c r="F47" t="s">
+        <v>109</v>
       </c>
       <c r="G47">
         <v>3918</v>
@@ -3025,19 +3024,19 @@
         <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C48" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E48" t="s">
-        <v>110</v>
-      </c>
-      <c r="F48">
-        <v>1120</v>
+        <v>109</v>
+      </c>
+      <c r="F48" t="s">
+        <v>109</v>
       </c>
       <c r="G48">
         <v>3954</v>
@@ -3063,19 +3062,19 @@
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E49" t="s">
-        <v>110</v>
-      </c>
-      <c r="F49">
-        <v>1459</v>
+        <v>109</v>
+      </c>
+      <c r="F49" t="s">
+        <v>109</v>
       </c>
       <c r="G49">
         <v>14964</v>
@@ -3101,19 +3100,19 @@
         <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D50" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E50" t="s">
-        <v>110</v>
-      </c>
-      <c r="F50">
-        <v>1462</v>
+        <v>109</v>
+      </c>
+      <c r="F50" t="s">
+        <v>109</v>
       </c>
       <c r="G50" s="2">
         <v>10093</v>
@@ -3139,19 +3138,19 @@
         <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E51" t="s">
-        <v>110</v>
-      </c>
-      <c r="F51">
-        <v>1464</v>
+        <v>109</v>
+      </c>
+      <c r="F51" t="s">
+        <v>109</v>
       </c>
       <c r="G51">
         <v>10101</v>
@@ -3177,19 +3176,19 @@
         <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C52" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E52" t="s">
-        <v>110</v>
-      </c>
-      <c r="F52">
-        <v>1466</v>
+        <v>109</v>
+      </c>
+      <c r="F52" t="s">
+        <v>109</v>
       </c>
       <c r="G52">
         <v>9979</v>
@@ -3215,19 +3214,19 @@
         <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E53" t="s">
-        <v>110</v>
-      </c>
-      <c r="F53">
-        <v>1467</v>
+        <v>109</v>
+      </c>
+      <c r="F53" t="s">
+        <v>109</v>
       </c>
       <c r="G53">
         <v>9980</v>
@@ -3253,19 +3252,19 @@
         <v>59</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C54" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D54" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E54" t="s">
-        <v>110</v>
-      </c>
-      <c r="F54">
-        <v>1471</v>
+        <v>109</v>
+      </c>
+      <c r="F54" t="s">
+        <v>109</v>
       </c>
       <c r="G54">
         <v>9983</v>
@@ -3291,19 +3290,19 @@
         <v>60</v>
       </c>
       <c r="B55" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E55" t="s">
-        <v>110</v>
-      </c>
-      <c r="F55">
-        <v>1475</v>
+        <v>109</v>
+      </c>
+      <c r="F55" t="s">
+        <v>109</v>
       </c>
       <c r="G55">
         <v>9985</v>
@@ -3329,19 +3328,19 @@
         <v>63</v>
       </c>
       <c r="B56" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C56" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D56" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E56" t="s">
-        <v>110</v>
-      </c>
-      <c r="F56">
-        <v>1479</v>
+        <v>109</v>
+      </c>
+      <c r="F56" t="s">
+        <v>109</v>
       </c>
       <c r="G56">
         <v>9970</v>
@@ -3367,19 +3366,19 @@
         <v>64</v>
       </c>
       <c r="B57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E57" t="s">
-        <v>110</v>
-      </c>
-      <c r="F57">
-        <v>1480</v>
+        <v>109</v>
+      </c>
+      <c r="F57" t="s">
+        <v>109</v>
       </c>
       <c r="G57">
         <v>9971</v>
@@ -3405,19 +3404,19 @@
         <v>66</v>
       </c>
       <c r="B58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D58" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E58" t="s">
-        <v>110</v>
-      </c>
-      <c r="F58">
-        <v>1486</v>
+        <v>109</v>
+      </c>
+      <c r="F58" t="s">
+        <v>109</v>
       </c>
       <c r="G58">
         <v>9977</v>
@@ -3443,19 +3442,19 @@
         <v>67</v>
       </c>
       <c r="B59" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C59" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D59" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E59" t="s">
-        <v>110</v>
-      </c>
-      <c r="F59">
-        <v>1487</v>
+        <v>109</v>
+      </c>
+      <c r="F59" t="s">
+        <v>109</v>
       </c>
       <c r="G59">
         <v>9978</v>
@@ -3481,19 +3480,19 @@
         <v>68</v>
       </c>
       <c r="B60" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D60" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E60" t="s">
-        <v>110</v>
-      </c>
-      <c r="F60">
-        <v>1489</v>
+        <v>109</v>
+      </c>
+      <c r="F60" t="s">
+        <v>109</v>
       </c>
       <c r="G60">
         <v>9952</v>
@@ -3519,19 +3518,19 @@
         <v>69</v>
       </c>
       <c r="B61" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C61" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D61" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E61" t="s">
-        <v>110</v>
-      </c>
-      <c r="F61">
-        <v>1491</v>
+        <v>109</v>
+      </c>
+      <c r="F61" t="s">
+        <v>109</v>
       </c>
       <c r="G61">
         <v>9954</v>
@@ -3557,19 +3556,19 @@
         <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D62" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E62" t="s">
-        <v>110</v>
-      </c>
-      <c r="F62">
-        <v>1492</v>
+        <v>109</v>
+      </c>
+      <c r="F62" t="s">
+        <v>109</v>
       </c>
       <c r="G62">
         <v>9955</v>
@@ -3595,19 +3594,19 @@
         <v>72</v>
       </c>
       <c r="B63" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C63" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D63" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E63" t="s">
-        <v>110</v>
-      </c>
-      <c r="F63">
-        <v>1494</v>
+        <v>109</v>
+      </c>
+      <c r="F63" t="s">
+        <v>109</v>
       </c>
       <c r="G63">
         <v>9957</v>
@@ -3633,19 +3632,19 @@
         <v>73</v>
       </c>
       <c r="B64" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C64" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D64" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E64" t="s">
-        <v>110</v>
-      </c>
-      <c r="F64">
-        <v>1497</v>
+        <v>109</v>
+      </c>
+      <c r="F64" t="s">
+        <v>109</v>
       </c>
       <c r="G64">
         <v>9960</v>
@@ -3671,19 +3670,19 @@
         <v>75</v>
       </c>
       <c r="B65" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C65" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D65" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E65" t="s">
-        <v>110</v>
-      </c>
-      <c r="F65">
-        <v>1504</v>
+        <v>109</v>
+      </c>
+      <c r="F65" t="s">
+        <v>109</v>
       </c>
       <c r="G65">
         <v>9967</v>
@@ -3709,19 +3708,19 @@
         <v>76</v>
       </c>
       <c r="B66" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C66" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D66" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E66" t="s">
-        <v>110</v>
-      </c>
-      <c r="F66">
-        <v>1510</v>
+        <v>109</v>
+      </c>
+      <c r="F66" t="s">
+        <v>109</v>
       </c>
       <c r="G66">
         <v>9946</v>
@@ -3747,19 +3746,19 @@
         <v>78</v>
       </c>
       <c r="B67" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C67" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D67" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E67" t="s">
-        <v>110</v>
-      </c>
-      <c r="F67">
-        <v>1590</v>
+        <v>109</v>
+      </c>
+      <c r="F67" t="s">
+        <v>109</v>
       </c>
       <c r="G67">
         <v>7592</v>
@@ -3785,19 +3784,19 @@
         <v>82</v>
       </c>
       <c r="B68" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C68" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D68" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E68" t="s">
-        <v>110</v>
-      </c>
-      <c r="F68">
-        <v>4538</v>
+        <v>109</v>
+      </c>
+      <c r="F68" t="s">
+        <v>109</v>
       </c>
       <c r="G68">
         <v>14969</v>
@@ -3823,19 +3822,19 @@
         <v>83</v>
       </c>
       <c r="B69" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C69" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D69" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E69" t="s">
-        <v>110</v>
-      </c>
-      <c r="F69">
-        <v>6332</v>
+        <v>109</v>
+      </c>
+      <c r="F69" t="s">
+        <v>109</v>
       </c>
       <c r="G69">
         <v>14968</v>
@@ -3861,19 +3860,19 @@
         <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C70" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D70" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E70" t="s">
-        <v>110</v>
-      </c>
-      <c r="F70">
-        <v>23380</v>
+        <v>109</v>
+      </c>
+      <c r="F70" t="s">
+        <v>109</v>
       </c>
       <c r="G70">
         <v>14967</v>
@@ -3899,19 +3898,19 @@
         <v>85</v>
       </c>
       <c r="B71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C71" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D71" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E71" t="s">
-        <v>110</v>
-      </c>
-      <c r="F71">
-        <v>23381</v>
+        <v>109</v>
+      </c>
+      <c r="F71" t="s">
+        <v>109</v>
       </c>
       <c r="G71">
         <v>125920</v>
@@ -3937,19 +3936,19 @@
         <v>87</v>
       </c>
       <c r="B72" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C72" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D72" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E72" t="s">
-        <v>110</v>
-      </c>
-      <c r="F72">
-        <v>40496</v>
+        <v>109</v>
+      </c>
+      <c r="F72" t="s">
+        <v>109</v>
       </c>
       <c r="G72">
         <v>125921</v>
@@ -3975,19 +3974,19 @@
         <v>88</v>
       </c>
       <c r="B73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C73" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D73" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E73" t="s">
-        <v>110</v>
-      </c>
-      <c r="F73">
-        <v>40499</v>
+        <v>109</v>
+      </c>
+      <c r="F73" t="s">
+        <v>109</v>
       </c>
       <c r="G73">
         <v>125922</v>
@@ -4013,19 +4012,19 @@
         <v>89</v>
       </c>
       <c r="B74" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C74" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D74" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E74" t="s">
-        <v>110</v>
-      </c>
-      <c r="F74">
-        <v>40536</v>
+        <v>109</v>
+      </c>
+      <c r="F74" t="s">
+        <v>109</v>
       </c>
       <c r="G74">
         <v>146607</v>
@@ -4051,19 +4050,19 @@
         <v>61</v>
       </c>
       <c r="B75" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C75" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D75" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E75" t="s">
-        <v>110</v>
-      </c>
-      <c r="F75">
-        <v>1476</v>
+        <v>109</v>
+      </c>
+      <c r="F75" t="s">
+        <v>109</v>
       </c>
       <c r="G75">
         <v>9986</v>
@@ -4089,19 +4088,19 @@
         <v>53</v>
       </c>
       <c r="B76" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C76" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E76" t="s">
-        <v>110</v>
-      </c>
-      <c r="F76">
-        <v>1461</v>
+        <v>109</v>
+      </c>
+      <c r="F76" t="s">
+        <v>109</v>
       </c>
       <c r="G76">
         <v>14965</v>
@@ -4127,19 +4126,19 @@
         <v>71</v>
       </c>
       <c r="B77" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C77" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D77" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E77" t="s">
-        <v>110</v>
-      </c>
-      <c r="F77">
-        <v>1493</v>
+        <v>109</v>
+      </c>
+      <c r="F77" t="s">
+        <v>109</v>
       </c>
       <c r="G77">
         <v>9956</v>
@@ -4165,19 +4164,19 @@
         <v>81</v>
       </c>
       <c r="B78" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C78" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D78" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E78" t="s">
-        <v>110</v>
-      </c>
-      <c r="F78">
-        <v>4534</v>
+        <v>109</v>
+      </c>
+      <c r="F78" t="s">
+        <v>109</v>
       </c>
       <c r="G78">
         <v>34537</v>
@@ -4203,19 +4202,19 @@
         <v>90</v>
       </c>
       <c r="B79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D79" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E79" t="s">
-        <v>110</v>
-      </c>
-      <c r="F79">
-        <v>40668</v>
+        <v>109</v>
+      </c>
+      <c r="F79" t="s">
+        <v>109</v>
       </c>
       <c r="G79">
         <v>146195</v>
@@ -4241,19 +4240,19 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C80" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D80" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E80" t="s">
-        <v>110</v>
-      </c>
-      <c r="F80">
-        <v>4135</v>
+        <v>109</v>
+      </c>
+      <c r="F80" t="s">
+        <v>109</v>
       </c>
       <c r="G80">
         <v>34539</v>
@@ -4279,19 +4278,19 @@
         <v>62</v>
       </c>
       <c r="B81" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C81" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D81" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E81" t="s">
-        <v>110</v>
-      </c>
-      <c r="F81">
-        <v>1478</v>
+        <v>109</v>
+      </c>
+      <c r="F81" t="s">
+        <v>109</v>
       </c>
       <c r="G81">
         <v>14970</v>
@@ -4317,19 +4316,19 @@
         <v>79</v>
       </c>
       <c r="B82" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C82" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D82" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E82" t="s">
-        <v>110</v>
-      </c>
-      <c r="F82">
-        <v>4134</v>
+        <v>109</v>
+      </c>
+      <c r="F82" t="s">
+        <v>109</v>
       </c>
       <c r="G82">
         <v>14966</v>
@@ -4355,19 +4354,19 @@
         <v>86</v>
       </c>
       <c r="B83" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C83" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D83" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E83" t="s">
-        <v>110</v>
-      </c>
-      <c r="F83">
-        <v>23512</v>
+        <v>109</v>
+      </c>
+      <c r="F83" t="s">
+        <v>109</v>
       </c>
       <c r="G83">
         <v>146606</v>
@@ -4393,19 +4392,19 @@
         <v>40</v>
       </c>
       <c r="B84" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C84" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D84" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E84" t="s">
-        <v>110</v>
-      </c>
-      <c r="F84">
-        <v>554</v>
+        <v>109</v>
+      </c>
+      <c r="F84" t="s">
+        <v>109</v>
       </c>
       <c r="G84">
         <v>3573</v>
@@ -4431,19 +4430,19 @@
         <v>41</v>
       </c>
       <c r="B85" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C85" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D85" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E85" t="s">
-        <v>110</v>
-      </c>
-      <c r="F85">
-        <v>1038</v>
+        <v>109</v>
+      </c>
+      <c r="F85" t="s">
+        <v>109</v>
       </c>
       <c r="G85">
         <v>3891</v>
@@ -4469,19 +4468,19 @@
         <v>28</v>
       </c>
       <c r="B86" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C86" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D86" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E86" t="s">
-        <v>110</v>
-      </c>
-      <c r="F86">
-        <v>300</v>
+        <v>109</v>
+      </c>
+      <c r="F86" t="s">
+        <v>109</v>
       </c>
       <c r="G86">
         <v>3481</v>
@@ -4507,19 +4506,19 @@
         <v>58</v>
       </c>
       <c r="B87" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C87" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D87" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E87" t="s">
-        <v>110</v>
-      </c>
-      <c r="F87">
-        <v>1468</v>
+        <v>109</v>
+      </c>
+      <c r="F87" t="s">
+        <v>109</v>
       </c>
       <c r="G87">
         <v>9981</v>
@@ -4545,19 +4544,19 @@
         <v>74</v>
       </c>
       <c r="B88" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C88" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D88" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E88" t="s">
-        <v>110</v>
-      </c>
-      <c r="F88">
-        <v>1501</v>
+        <v>109</v>
+      </c>
+      <c r="F88" t="s">
+        <v>109</v>
       </c>
       <c r="G88">
         <v>9964</v>
@@ -4583,19 +4582,19 @@
         <v>77</v>
       </c>
       <c r="B89" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C89" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D89" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E89" t="s">
-        <v>110</v>
-      </c>
-      <c r="F89">
-        <v>1515</v>
+        <v>109</v>
+      </c>
+      <c r="F89" t="s">
+        <v>109</v>
       </c>
       <c r="G89">
         <v>9950</v>
@@ -4621,19 +4620,19 @@
         <v>65</v>
       </c>
       <c r="B90" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C90" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D90" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E90" t="s">
-        <v>110</v>
-      </c>
-      <c r="F90">
-        <v>1485</v>
+        <v>109</v>
+      </c>
+      <c r="F90" t="s">
+        <v>109</v>
       </c>
       <c r="G90">
         <v>9976</v>
@@ -4659,19 +4658,19 @@
         <v>8</v>
       </c>
       <c r="B91" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C91" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D91" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E91" t="s">
-        <v>110</v>
-      </c>
-      <c r="F91">
-        <v>20</v>
+        <v>109</v>
+      </c>
+      <c r="F91" t="s">
+        <v>109</v>
       </c>
       <c r="G91">
         <v>20</v>
@@ -4697,19 +4696,19 @@
         <v>49</v>
       </c>
       <c r="B92" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C92" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D92" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E92" t="s">
-        <v>110</v>
-      </c>
-      <c r="F92">
-        <v>1112</v>
+        <v>109</v>
+      </c>
+      <c r="F92" t="s">
+        <v>109</v>
       </c>
       <c r="G92">
         <v>3946</v>
@@ -4735,19 +4734,19 @@
         <v>50</v>
       </c>
       <c r="B93" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C93" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D93" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E93" t="s">
-        <v>110</v>
-      </c>
-      <c r="F93">
-        <v>1114</v>
+        <v>109</v>
+      </c>
+      <c r="F93" t="s">
+        <v>109</v>
       </c>
       <c r="G93" s="2">
         <v>3948</v>
@@ -4789,12 +4788,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="e">
         <f>COUNTIF(openml_100!#REF!, "=Run")</f>
@@ -4803,7 +4802,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" t="e">
         <f>COUNTIF(openml_100!#REF!, "=Complete")</f>
@@ -4812,7 +4811,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" t="e">
         <f>COUNTIF(openml_100!#REF!, "=Suspend")</f>
@@ -4821,7 +4820,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B6" t="e">
         <f>COUNTIF(openml_100!#REF!, "=Issue")</f>
@@ -4830,7 +4829,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" t="e">
         <f>B3+B4+B5+B6</f>

</xml_diff>

<commit_message>
SS-Compare against PP1 study
</commit_message>
<xml_diff>
--- a/benchmark/Configuration.xlsx
+++ b/benchmark/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\autem\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B863584D-2AE3-4F17-8A1D-DB99EAF85BB6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA20676-77DA-490C-9347-61174D2B739A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="112">
   <si>
     <t>kr-vs-kp</t>
   </si>
@@ -362,9 +362,6 @@
   </si>
   <si>
     <t>PP1</t>
-  </si>
-  <si>
-    <t>STC</t>
   </si>
   <si>
     <t>SS</t>
@@ -1212,28 +1209,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L93"/>
+  <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>98</v>
       </c>
@@ -1249,29 +1246,26 @@
       <c r="E1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>112</v>
+      <c r="F1" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1287,29 +1281,26 @@
       <c r="E2" t="s">
         <v>105</v>
       </c>
-      <c r="F2" t="s">
-        <v>105</v>
+      <c r="F2">
+        <v>37</v>
       </c>
       <c r="G2">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="I2">
-        <v>9</v>
+        <v>768</v>
       </c>
       <c r="J2">
-        <v>768</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -1325,29 +1316,26 @@
       <c r="E3" t="s">
         <v>105</v>
       </c>
-      <c r="F3" t="s">
-        <v>105</v>
+      <c r="F3">
+        <v>53</v>
       </c>
       <c r="G3">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="I3">
-        <v>19</v>
+        <v>846</v>
       </c>
       <c r="J3">
-        <v>846</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>91</v>
       </c>
@@ -1361,31 +1349,28 @@
         <v>106</v>
       </c>
       <c r="E4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F4" t="s">
-        <v>105</v>
+        <v>105</v>
+      </c>
+      <c r="F4">
+        <v>125923</v>
       </c>
       <c r="G4">
-        <v>125923</v>
+        <v>2</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I4">
-        <v>15</v>
+        <v>690</v>
       </c>
       <c r="J4">
-        <v>690</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1399,31 +1384,28 @@
         <v>106</v>
       </c>
       <c r="E5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F5" t="s">
-        <v>105</v>
+        <v>105</v>
+      </c>
+      <c r="F5">
+        <v>145804</v>
       </c>
       <c r="G5">
-        <v>145804</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I5">
-        <v>10</v>
+        <v>958</v>
       </c>
       <c r="J5">
-        <v>958</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1437,31 +1419,28 @@
         <v>106</v>
       </c>
       <c r="E6" t="s">
-        <v>109</v>
-      </c>
-      <c r="F6" t="s">
-        <v>105</v>
+        <v>105</v>
+      </c>
+      <c r="F6">
+        <v>18</v>
       </c>
       <c r="G6">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="H6">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I6">
-        <v>7</v>
+        <v>2000</v>
       </c>
       <c r="J6">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1475,31 +1454,28 @@
         <v>106</v>
       </c>
       <c r="E7" t="s">
-        <v>109</v>
-      </c>
-      <c r="F7" t="s">
-        <v>105</v>
+        <v>105</v>
+      </c>
+      <c r="F7">
+        <v>11</v>
       </c>
       <c r="G7">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I7">
-        <v>5</v>
+        <v>625</v>
       </c>
       <c r="J7">
-        <v>625</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <v>0</v>
       </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1513,31 +1489,28 @@
         <v>106</v>
       </c>
       <c r="E8" t="s">
-        <v>109</v>
-      </c>
-      <c r="F8" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F8">
+        <v>3021</v>
       </c>
       <c r="G8">
-        <v>3021</v>
+        <v>2</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="I8">
-        <v>30</v>
+        <v>3772</v>
       </c>
       <c r="J8">
         <v>3772</v>
       </c>
       <c r="K8">
-        <v>3772</v>
-      </c>
-      <c r="L8">
         <v>6064</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1553,29 +1526,26 @@
       <c r="E9" t="s">
         <v>109</v>
       </c>
-      <c r="F9" t="s">
-        <v>109</v>
+      <c r="F9">
+        <v>29</v>
       </c>
       <c r="G9">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="I9">
-        <v>16</v>
+        <v>690</v>
       </c>
       <c r="J9">
-        <v>690</v>
+        <v>37</v>
       </c>
       <c r="K9">
-        <v>37</v>
-      </c>
-      <c r="L9">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1591,29 +1561,26 @@
       <c r="E10" t="s">
         <v>109</v>
       </c>
-      <c r="F10" t="s">
-        <v>109</v>
+      <c r="F10">
+        <v>41</v>
       </c>
       <c r="G10">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="H10">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="I10">
-        <v>36</v>
+        <v>683</v>
       </c>
       <c r="J10">
-        <v>683</v>
+        <v>121</v>
       </c>
       <c r="K10">
-        <v>121</v>
-      </c>
-      <c r="L10">
         <v>2337</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -1629,29 +1596,26 @@
       <c r="E11" t="s">
         <v>109</v>
       </c>
-      <c r="F11" t="s">
-        <v>109</v>
+      <c r="F11">
+        <v>1779</v>
       </c>
       <c r="G11">
-        <v>1779</v>
+        <v>2</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I11">
-        <v>10</v>
+        <v>699</v>
       </c>
       <c r="J11">
-        <v>699</v>
+        <v>16</v>
       </c>
       <c r="K11">
         <v>16</v>
       </c>
-      <c r="L11">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1667,29 +1631,26 @@
       <c r="E12" t="s">
         <v>109</v>
       </c>
-      <c r="F12" t="s">
-        <v>109</v>
+      <c r="F12">
+        <v>23</v>
       </c>
       <c r="G12">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="H12">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I12">
-        <v>10</v>
+        <v>1473</v>
       </c>
       <c r="J12">
-        <v>1473</v>
+        <v>0</v>
       </c>
       <c r="K12">
         <v>0</v>
       </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -1705,29 +1666,26 @@
       <c r="E13" t="s">
         <v>105</v>
       </c>
-      <c r="F13" t="s">
-        <v>109</v>
+      <c r="F13">
+        <v>3561</v>
       </c>
       <c r="G13">
-        <v>3561</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I13">
-        <v>10</v>
+        <v>672</v>
       </c>
       <c r="J13">
-        <v>672</v>
+        <v>666</v>
       </c>
       <c r="K13">
-        <v>666</v>
-      </c>
-      <c r="L13">
         <v>1200</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1743,29 +1701,26 @@
       <c r="E14" t="s">
         <v>109</v>
       </c>
-      <c r="F14" t="s">
-        <v>109</v>
+      <c r="F14">
+        <v>1788</v>
       </c>
       <c r="G14">
-        <v>1788</v>
+        <v>2</v>
       </c>
       <c r="H14">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="I14">
-        <v>23</v>
+        <v>8124</v>
       </c>
       <c r="J14">
-        <v>8124</v>
+        <v>2480</v>
       </c>
       <c r="K14">
         <v>2480</v>
       </c>
-      <c r="L14">
-        <v>2480</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1781,29 +1736,26 @@
       <c r="E15" t="s">
         <v>109</v>
       </c>
-      <c r="F15" t="s">
-        <v>109</v>
+      <c r="F15">
+        <v>28</v>
       </c>
       <c r="G15">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="H15">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="I15">
-        <v>65</v>
+        <v>5620</v>
       </c>
       <c r="J15">
-        <v>5620</v>
+        <v>0</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1817,31 +1769,28 @@
         <v>106</v>
       </c>
       <c r="E16" t="s">
-        <v>109</v>
-      </c>
-      <c r="F16" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F16">
+        <v>31</v>
       </c>
       <c r="G16">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="H16">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I16">
-        <v>21</v>
+        <v>1000</v>
       </c>
       <c r="J16">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1857,29 +1806,26 @@
       <c r="E17" t="s">
         <v>109</v>
       </c>
-      <c r="F17" t="s">
-        <v>109</v>
+      <c r="F17">
+        <v>32</v>
       </c>
       <c r="G17">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="H17">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="I17">
-        <v>17</v>
+        <v>10992</v>
       </c>
       <c r="J17">
-        <v>10992</v>
+        <v>0</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -1895,29 +1841,26 @@
       <c r="E18" t="s">
         <v>109</v>
       </c>
-      <c r="F18" t="s">
-        <v>109</v>
+      <c r="F18">
+        <v>3</v>
       </c>
       <c r="G18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H18">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="I18">
-        <v>37</v>
+        <v>3196</v>
       </c>
       <c r="J18">
-        <v>3196</v>
+        <v>0</v>
       </c>
       <c r="K18">
         <v>0</v>
       </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -1931,31 +1874,28 @@
         <v>105</v>
       </c>
       <c r="E19" t="s">
-        <v>109</v>
-      </c>
-      <c r="F19" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F19">
+        <v>6</v>
       </c>
       <c r="G19">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="H19">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="I19">
-        <v>17</v>
+        <v>20000</v>
       </c>
       <c r="J19">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="K19">
         <v>0</v>
       </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
@@ -1971,29 +1911,26 @@
       <c r="E20" t="s">
         <v>109</v>
       </c>
-      <c r="F20" t="s">
-        <v>109</v>
+      <c r="F20">
+        <v>12</v>
       </c>
       <c r="G20">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H20">
-        <v>10</v>
+        <v>217</v>
       </c>
       <c r="I20">
-        <v>217</v>
+        <v>2000</v>
       </c>
       <c r="J20">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
@@ -2009,29 +1946,26 @@
       <c r="E21" t="s">
         <v>109</v>
       </c>
-      <c r="F21" t="s">
-        <v>109</v>
+      <c r="F21">
+        <v>1778</v>
       </c>
       <c r="G21">
-        <v>1778</v>
+        <v>10</v>
       </c>
       <c r="H21">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="I21">
-        <v>77</v>
+        <v>2000</v>
       </c>
       <c r="J21">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
@@ -2047,29 +1981,26 @@
       <c r="E22" t="s">
         <v>109</v>
       </c>
-      <c r="F22" t="s">
-        <v>109</v>
+      <c r="F22">
+        <v>16</v>
       </c>
       <c r="G22">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="H22">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="I22">
-        <v>65</v>
+        <v>2000</v>
       </c>
       <c r="J22">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -2083,31 +2014,28 @@
         <v>105</v>
       </c>
       <c r="E23" t="s">
-        <v>109</v>
-      </c>
-      <c r="F23" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F23">
+        <v>22</v>
       </c>
       <c r="G23">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H23">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="I23">
-        <v>48</v>
+        <v>2000</v>
       </c>
       <c r="J23">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
@@ -2123,29 +2051,26 @@
       <c r="E24" t="s">
         <v>109</v>
       </c>
-      <c r="F24" t="s">
-        <v>109</v>
+      <c r="F24">
+        <v>36</v>
       </c>
       <c r="G24">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="H24">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I24">
-        <v>20</v>
+        <v>2310</v>
       </c>
       <c r="J24">
-        <v>2310</v>
+        <v>0</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
@@ -2161,29 +2086,26 @@
       <c r="E25" t="s">
         <v>109</v>
       </c>
-      <c r="F25" t="s">
-        <v>109</v>
+      <c r="F25">
+        <v>43</v>
       </c>
       <c r="G25">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="H25">
-        <v>2</v>
+        <v>58</v>
       </c>
       <c r="I25">
-        <v>58</v>
+        <v>4601</v>
       </c>
       <c r="J25">
-        <v>4601</v>
+        <v>0</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
@@ -2197,31 +2119,28 @@
         <v>105</v>
       </c>
       <c r="E26" t="s">
-        <v>109</v>
-      </c>
-      <c r="F26" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F26">
+        <v>45</v>
       </c>
       <c r="G26">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="H26">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="I26">
-        <v>62</v>
+        <v>3190</v>
       </c>
       <c r="J26">
-        <v>3190</v>
+        <v>0</v>
       </c>
       <c r="K26">
         <v>0</v>
       </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
@@ -2237,29 +2156,26 @@
       <c r="E27" t="s">
         <v>109</v>
       </c>
-      <c r="F27" t="s">
-        <v>109</v>
+      <c r="F27">
+        <v>58</v>
       </c>
       <c r="G27">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="H27">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="I27">
-        <v>41</v>
+        <v>5000</v>
       </c>
       <c r="J27">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="K27">
         <v>0</v>
       </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
@@ -2275,29 +2191,26 @@
       <c r="E28" t="s">
         <v>105</v>
       </c>
-      <c r="F28" t="s">
-        <v>109</v>
+      <c r="F28">
+        <v>219</v>
       </c>
       <c r="G28">
-        <v>219</v>
+        <v>2</v>
       </c>
       <c r="H28">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="I28">
-        <v>9</v>
+        <v>45312</v>
       </c>
       <c r="J28">
-        <v>45312</v>
+        <v>0</v>
       </c>
       <c r="K28">
         <v>0</v>
       </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
@@ -2311,31 +2224,28 @@
         <v>105</v>
       </c>
       <c r="E29" t="s">
-        <v>109</v>
-      </c>
-      <c r="F29" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F29">
+        <v>2074</v>
       </c>
       <c r="G29">
-        <v>2074</v>
+        <v>6</v>
       </c>
       <c r="H29">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="I29">
-        <v>37</v>
+        <v>6430</v>
       </c>
       <c r="J29">
-        <v>6430</v>
+        <v>0</v>
       </c>
       <c r="K29">
         <v>0</v>
       </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
@@ -2351,29 +2261,26 @@
       <c r="E30" t="s">
         <v>105</v>
       </c>
-      <c r="F30" t="s">
-        <v>109</v>
+      <c r="F30">
+        <v>2125</v>
       </c>
       <c r="G30">
-        <v>2125</v>
+        <v>5</v>
       </c>
       <c r="H30">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="I30">
-        <v>20</v>
+        <v>736</v>
       </c>
       <c r="J30">
-        <v>736</v>
+        <v>95</v>
       </c>
       <c r="K30">
-        <v>95</v>
-      </c>
-      <c r="L30">
         <v>448</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
@@ -2389,29 +2296,26 @@
       <c r="E31" t="s">
         <v>105</v>
       </c>
-      <c r="F31" t="s">
-        <v>109</v>
+      <c r="F31">
+        <v>3022</v>
       </c>
       <c r="G31">
-        <v>3022</v>
+        <v>11</v>
       </c>
       <c r="H31">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I31">
-        <v>13</v>
+        <v>990</v>
       </c>
       <c r="J31">
-        <v>990</v>
+        <v>0</v>
       </c>
       <c r="K31">
         <v>0</v>
       </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -2427,29 +2331,26 @@
       <c r="E32" t="s">
         <v>109</v>
       </c>
-      <c r="F32" t="s">
-        <v>109</v>
+      <c r="F32">
+        <v>3485</v>
       </c>
       <c r="G32">
-        <v>3485</v>
+        <v>2</v>
       </c>
       <c r="H32">
-        <v>2</v>
+        <v>300</v>
       </c>
       <c r="I32">
-        <v>300</v>
+        <v>2407</v>
       </c>
       <c r="J32">
-        <v>2407</v>
+        <v>0</v>
       </c>
       <c r="K32">
         <v>0</v>
       </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
@@ -2465,29 +2366,26 @@
       <c r="E33" t="s">
         <v>105</v>
       </c>
-      <c r="F33" t="s">
-        <v>109</v>
-      </c>
-      <c r="G33" s="2">
+      <c r="F33" s="2">
         <v>3492</v>
       </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
       <c r="H33">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I33">
-        <v>7</v>
+        <v>556</v>
       </c>
       <c r="J33">
-        <v>556</v>
+        <v>0</v>
       </c>
       <c r="K33">
         <v>0</v>
       </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -2503,29 +2401,26 @@
       <c r="E34" t="s">
         <v>105</v>
       </c>
-      <c r="F34" t="s">
-        <v>109</v>
+      <c r="F34">
+        <v>3493</v>
       </c>
       <c r="G34">
-        <v>3493</v>
+        <v>2</v>
       </c>
       <c r="H34">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I34">
-        <v>7</v>
+        <v>601</v>
       </c>
       <c r="J34">
-        <v>601</v>
+        <v>0</v>
       </c>
       <c r="K34">
         <v>0</v>
       </c>
-      <c r="L34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -2541,29 +2436,26 @@
       <c r="E35" t="s">
         <v>105</v>
       </c>
-      <c r="F35" t="s">
-        <v>109</v>
+      <c r="F35">
+        <v>3494</v>
       </c>
       <c r="G35">
-        <v>3494</v>
+        <v>2</v>
       </c>
       <c r="H35">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I35">
-        <v>7</v>
+        <v>554</v>
       </c>
       <c r="J35">
-        <v>554</v>
+        <v>0</v>
       </c>
       <c r="K35">
         <v>0</v>
       </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -2579,29 +2471,26 @@
       <c r="E36" t="s">
         <v>109</v>
       </c>
-      <c r="F36" t="s">
-        <v>109</v>
+      <c r="F36">
+        <v>4544</v>
       </c>
       <c r="G36">
-        <v>4544</v>
+        <v>9</v>
       </c>
       <c r="H36">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I36">
-        <v>15</v>
+        <v>9961</v>
       </c>
       <c r="J36">
-        <v>9961</v>
+        <v>0</v>
       </c>
       <c r="K36">
         <v>0</v>
       </c>
-      <c r="L36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -2617,29 +2506,26 @@
       <c r="E37" t="s">
         <v>109</v>
       </c>
-      <c r="F37" t="s">
-        <v>109</v>
+      <c r="F37">
+        <v>3512</v>
       </c>
       <c r="G37">
-        <v>3512</v>
+        <v>6</v>
       </c>
       <c r="H37">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="I37">
-        <v>62</v>
+        <v>600</v>
       </c>
       <c r="J37">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="K37">
         <v>0</v>
       </c>
-      <c r="L37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
@@ -2655,29 +2541,26 @@
       <c r="E38" t="s">
         <v>109</v>
       </c>
-      <c r="F38" t="s">
-        <v>109</v>
+      <c r="F38">
+        <v>3543</v>
       </c>
       <c r="G38">
-        <v>3543</v>
+        <v>2</v>
       </c>
       <c r="H38">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I38">
-        <v>6</v>
+        <v>500</v>
       </c>
       <c r="J38">
-        <v>500</v>
+        <v>32</v>
       </c>
       <c r="K38">
         <v>32</v>
       </c>
-      <c r="L38">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
@@ -2693,29 +2576,26 @@
       <c r="E39" t="s">
         <v>105</v>
       </c>
-      <c r="F39" t="s">
-        <v>109</v>
+      <c r="F39">
+        <v>3549</v>
       </c>
       <c r="G39">
-        <v>3549</v>
+        <v>4</v>
       </c>
       <c r="H39">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="I39">
-        <v>71</v>
+        <v>841</v>
       </c>
       <c r="J39">
-        <v>841</v>
+        <v>0</v>
       </c>
       <c r="K39">
         <v>0</v>
       </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
@@ -2729,31 +2609,28 @@
         <v>105</v>
       </c>
       <c r="E40" t="s">
-        <v>109</v>
-      </c>
-      <c r="F40" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F40">
+        <v>3560</v>
       </c>
       <c r="G40">
-        <v>3560</v>
+        <v>6</v>
       </c>
       <c r="H40">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I40">
-        <v>5</v>
+        <v>797</v>
       </c>
       <c r="J40">
-        <v>797</v>
+        <v>0</v>
       </c>
       <c r="K40">
         <v>0</v>
       </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>42</v>
       </c>
@@ -2769,29 +2646,26 @@
       <c r="E41" t="s">
         <v>109</v>
       </c>
-      <c r="F41" t="s">
-        <v>109</v>
+      <c r="F41">
+        <v>3899</v>
       </c>
       <c r="G41">
-        <v>3899</v>
+        <v>2</v>
       </c>
       <c r="H41">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I41">
-        <v>6</v>
+        <v>15545</v>
       </c>
       <c r="J41">
-        <v>15545</v>
+        <v>0</v>
       </c>
       <c r="K41">
         <v>0</v>
       </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>43</v>
       </c>
@@ -2807,29 +2681,26 @@
       <c r="E42" t="s">
         <v>109</v>
       </c>
-      <c r="F42" t="s">
-        <v>109</v>
+      <c r="F42">
+        <v>3902</v>
       </c>
       <c r="G42">
-        <v>3902</v>
+        <v>2</v>
       </c>
       <c r="H42">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="I42">
-        <v>38</v>
+        <v>1458</v>
       </c>
       <c r="J42">
-        <v>1458</v>
+        <v>0</v>
       </c>
       <c r="K42">
         <v>0</v>
       </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>44</v>
       </c>
@@ -2843,31 +2714,28 @@
         <v>105</v>
       </c>
       <c r="E43" t="s">
-        <v>109</v>
-      </c>
-      <c r="F43" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F43">
+        <v>3903</v>
       </c>
       <c r="G43">
-        <v>3903</v>
+        <v>2</v>
       </c>
       <c r="H43">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="I43">
-        <v>38</v>
+        <v>1563</v>
       </c>
       <c r="J43">
-        <v>1563</v>
+        <v>0</v>
       </c>
       <c r="K43">
         <v>0</v>
       </c>
-      <c r="L43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>45</v>
       </c>
@@ -2883,29 +2751,26 @@
       <c r="E44" t="s">
         <v>109</v>
       </c>
-      <c r="F44" t="s">
-        <v>109</v>
+      <c r="F44">
+        <v>3904</v>
       </c>
       <c r="G44">
-        <v>3904</v>
+        <v>2</v>
       </c>
       <c r="H44">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="I44">
-        <v>22</v>
+        <v>10885</v>
       </c>
       <c r="J44">
-        <v>10885</v>
+        <v>5</v>
       </c>
       <c r="K44">
-        <v>5</v>
-      </c>
-      <c r="L44">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>46</v>
       </c>
@@ -2921,29 +2786,26 @@
       <c r="E45" t="s">
         <v>109</v>
       </c>
-      <c r="F45" t="s">
-        <v>109</v>
+      <c r="F45">
+        <v>3913</v>
       </c>
       <c r="G45">
-        <v>3913</v>
+        <v>2</v>
       </c>
       <c r="H45">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="I45">
-        <v>22</v>
+        <v>522</v>
       </c>
       <c r="J45">
-        <v>522</v>
+        <v>0</v>
       </c>
       <c r="K45">
         <v>0</v>
       </c>
-      <c r="L45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>47</v>
       </c>
@@ -2959,29 +2821,26 @@
       <c r="E46" t="s">
         <v>109</v>
       </c>
-      <c r="F46" t="s">
-        <v>109</v>
+      <c r="F46">
+        <v>3917</v>
       </c>
       <c r="G46">
-        <v>3917</v>
+        <v>2</v>
       </c>
       <c r="H46">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="I46">
-        <v>22</v>
+        <v>2109</v>
       </c>
       <c r="J46">
-        <v>2109</v>
+        <v>0</v>
       </c>
       <c r="K46">
         <v>0</v>
       </c>
-      <c r="L46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>48</v>
       </c>
@@ -2997,29 +2856,26 @@
       <c r="E47" t="s">
         <v>109</v>
       </c>
-      <c r="F47" t="s">
-        <v>109</v>
+      <c r="F47">
+        <v>3918</v>
       </c>
       <c r="G47">
-        <v>3918</v>
+        <v>2</v>
       </c>
       <c r="H47">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="I47">
-        <v>22</v>
+        <v>1109</v>
       </c>
       <c r="J47">
-        <v>1109</v>
+        <v>0</v>
       </c>
       <c r="K47">
         <v>0</v>
       </c>
-      <c r="L47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>51</v>
       </c>
@@ -3035,29 +2891,26 @@
       <c r="E48" t="s">
         <v>109</v>
       </c>
-      <c r="F48" t="s">
-        <v>109</v>
+      <c r="F48">
+        <v>3954</v>
       </c>
       <c r="G48">
-        <v>3954</v>
+        <v>2</v>
       </c>
       <c r="H48">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="I48">
-        <v>12</v>
+        <v>19020</v>
       </c>
       <c r="J48">
-        <v>19020</v>
+        <v>0</v>
       </c>
       <c r="K48">
         <v>0</v>
       </c>
-      <c r="L48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>52</v>
       </c>
@@ -3071,31 +2924,28 @@
         <v>105</v>
       </c>
       <c r="E49" t="s">
-        <v>109</v>
-      </c>
-      <c r="F49" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F49">
+        <v>14964</v>
       </c>
       <c r="G49">
-        <v>14964</v>
+        <v>10</v>
       </c>
       <c r="H49">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I49">
-        <v>8</v>
+        <v>10218</v>
       </c>
       <c r="J49">
-        <v>10218</v>
+        <v>0</v>
       </c>
       <c r="K49">
         <v>0</v>
       </c>
-      <c r="L49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>54</v>
       </c>
@@ -3111,29 +2961,26 @@
       <c r="E50" t="s">
         <v>109</v>
       </c>
-      <c r="F50" t="s">
-        <v>109</v>
-      </c>
-      <c r="G50" s="2">
+      <c r="F50" s="2">
         <v>10093</v>
       </c>
+      <c r="G50">
+        <v>2</v>
+      </c>
       <c r="H50">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I50">
-        <v>5</v>
+        <v>1372</v>
       </c>
       <c r="J50">
-        <v>1372</v>
+        <v>0</v>
       </c>
       <c r="K50">
         <v>0</v>
       </c>
-      <c r="L50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
@@ -3149,29 +2996,26 @@
       <c r="E51" t="s">
         <v>109</v>
       </c>
-      <c r="F51" t="s">
-        <v>109</v>
+      <c r="F51">
+        <v>10101</v>
       </c>
       <c r="G51">
-        <v>10101</v>
+        <v>2</v>
       </c>
       <c r="H51">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I51">
-        <v>5</v>
+        <v>748</v>
       </c>
       <c r="J51">
-        <v>748</v>
+        <v>0</v>
       </c>
       <c r="K51">
         <v>0</v>
       </c>
-      <c r="L51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>56</v>
       </c>
@@ -3187,29 +3031,26 @@
       <c r="E52" t="s">
         <v>109</v>
       </c>
-      <c r="F52" t="s">
-        <v>109</v>
+      <c r="F52">
+        <v>9979</v>
       </c>
       <c r="G52">
-        <v>9979</v>
+        <v>10</v>
       </c>
       <c r="H52">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="I52">
-        <v>36</v>
+        <v>2126</v>
       </c>
       <c r="J52">
-        <v>2126</v>
+        <v>0</v>
       </c>
       <c r="K52">
         <v>0</v>
       </c>
-      <c r="L52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>57</v>
       </c>
@@ -3223,31 +3064,28 @@
         <v>105</v>
       </c>
       <c r="E53" t="s">
-        <v>109</v>
-      </c>
-      <c r="F53" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F53">
+        <v>9980</v>
       </c>
       <c r="G53">
-        <v>9980</v>
+        <v>2</v>
       </c>
       <c r="H53">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="I53">
-        <v>21</v>
+        <v>540</v>
       </c>
       <c r="J53">
-        <v>540</v>
+        <v>0</v>
       </c>
       <c r="K53">
         <v>0</v>
       </c>
-      <c r="L53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
@@ -3263,29 +3101,26 @@
       <c r="E54" t="s">
         <v>109</v>
       </c>
-      <c r="F54" t="s">
-        <v>109</v>
+      <c r="F54">
+        <v>9983</v>
       </c>
       <c r="G54">
-        <v>9983</v>
+        <v>2</v>
       </c>
       <c r="H54">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I54">
-        <v>15</v>
+        <v>14980</v>
       </c>
       <c r="J54">
-        <v>14980</v>
+        <v>0</v>
       </c>
       <c r="K54">
         <v>0</v>
       </c>
-      <c r="L54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>60</v>
       </c>
@@ -3299,31 +3134,28 @@
         <v>105</v>
       </c>
       <c r="E55" t="s">
-        <v>109</v>
-      </c>
-      <c r="F55" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F55">
+        <v>9985</v>
       </c>
       <c r="G55">
-        <v>9985</v>
+        <v>6</v>
       </c>
       <c r="H55">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="I55">
-        <v>52</v>
+        <v>6118</v>
       </c>
       <c r="J55">
-        <v>6118</v>
+        <v>0</v>
       </c>
       <c r="K55">
         <v>0</v>
       </c>
-      <c r="L55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>63</v>
       </c>
@@ -3339,29 +3171,26 @@
       <c r="E56" t="s">
         <v>109</v>
       </c>
-      <c r="F56" t="s">
-        <v>109</v>
+      <c r="F56">
+        <v>9970</v>
       </c>
       <c r="G56">
-        <v>9970</v>
+        <v>2</v>
       </c>
       <c r="H56">
-        <v>2</v>
+        <v>101</v>
       </c>
       <c r="I56">
-        <v>101</v>
+        <v>1212</v>
       </c>
       <c r="J56">
-        <v>1212</v>
+        <v>0</v>
       </c>
       <c r="K56">
         <v>0</v>
       </c>
-      <c r="L56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>64</v>
       </c>
@@ -3377,29 +3206,26 @@
       <c r="E57" t="s">
         <v>109</v>
       </c>
-      <c r="F57" t="s">
-        <v>109</v>
+      <c r="F57">
+        <v>9971</v>
       </c>
       <c r="G57">
-        <v>9971</v>
+        <v>2</v>
       </c>
       <c r="H57">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="I57">
-        <v>11</v>
+        <v>583</v>
       </c>
       <c r="J57">
-        <v>583</v>
+        <v>0</v>
       </c>
       <c r="K57">
         <v>0</v>
       </c>
-      <c r="L57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>66</v>
       </c>
@@ -3415,29 +3241,26 @@
       <c r="E58" t="s">
         <v>109</v>
       </c>
-      <c r="F58" t="s">
-        <v>109</v>
+      <c r="F58">
+        <v>9977</v>
       </c>
       <c r="G58">
-        <v>9977</v>
+        <v>2</v>
       </c>
       <c r="H58">
-        <v>2</v>
+        <v>119</v>
       </c>
       <c r="I58">
-        <v>119</v>
+        <v>34465</v>
       </c>
       <c r="J58">
-        <v>34465</v>
+        <v>0</v>
       </c>
       <c r="K58">
         <v>0</v>
       </c>
-      <c r="L58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>67</v>
       </c>
@@ -3453,29 +3276,26 @@
       <c r="E59" t="s">
         <v>109</v>
       </c>
-      <c r="F59" t="s">
-        <v>109</v>
+      <c r="F59">
+        <v>9978</v>
       </c>
       <c r="G59">
-        <v>9978</v>
+        <v>2</v>
       </c>
       <c r="H59">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="I59">
-        <v>73</v>
+        <v>2534</v>
       </c>
       <c r="J59">
-        <v>2534</v>
+        <v>0</v>
       </c>
       <c r="K59">
         <v>0</v>
       </c>
-      <c r="L59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>68</v>
       </c>
@@ -3491,29 +3311,26 @@
       <c r="E60" t="s">
         <v>109</v>
       </c>
-      <c r="F60" t="s">
-        <v>109</v>
+      <c r="F60">
+        <v>9952</v>
       </c>
       <c r="G60">
-        <v>9952</v>
+        <v>2</v>
       </c>
       <c r="H60">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I60">
-        <v>6</v>
+        <v>5404</v>
       </c>
       <c r="J60">
-        <v>5404</v>
+        <v>0</v>
       </c>
       <c r="K60">
         <v>0</v>
       </c>
-      <c r="L60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>69</v>
       </c>
@@ -3529,29 +3346,26 @@
       <c r="E61" t="s">
         <v>109</v>
       </c>
-      <c r="F61" t="s">
-        <v>109</v>
+      <c r="F61">
+        <v>9954</v>
       </c>
       <c r="G61">
-        <v>9954</v>
+        <v>100</v>
       </c>
       <c r="H61">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="I61">
-        <v>65</v>
+        <v>1600</v>
       </c>
       <c r="J61">
-        <v>1600</v>
+        <v>0</v>
       </c>
       <c r="K61">
         <v>0</v>
       </c>
-      <c r="L61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>70</v>
       </c>
@@ -3567,29 +3381,26 @@
       <c r="E62" t="s">
         <v>109</v>
       </c>
-      <c r="F62" t="s">
-        <v>109</v>
+      <c r="F62">
+        <v>9955</v>
       </c>
       <c r="G62">
-        <v>9955</v>
+        <v>100</v>
       </c>
       <c r="H62">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="I62">
-        <v>65</v>
+        <v>1600</v>
       </c>
       <c r="J62">
-        <v>1600</v>
+        <v>0</v>
       </c>
       <c r="K62">
         <v>0</v>
       </c>
-      <c r="L62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>72</v>
       </c>
@@ -3605,29 +3416,26 @@
       <c r="E63" t="s">
         <v>109</v>
       </c>
-      <c r="F63" t="s">
-        <v>109</v>
+      <c r="F63">
+        <v>9957</v>
       </c>
       <c r="G63">
-        <v>9957</v>
+        <v>2</v>
       </c>
       <c r="H63">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="I63">
-        <v>42</v>
+        <v>1055</v>
       </c>
       <c r="J63">
-        <v>1055</v>
+        <v>0</v>
       </c>
       <c r="K63">
         <v>0</v>
       </c>
-      <c r="L63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>73</v>
       </c>
@@ -3643,29 +3451,26 @@
       <c r="E64" t="s">
         <v>109</v>
       </c>
-      <c r="F64" t="s">
-        <v>109</v>
+      <c r="F64">
+        <v>9960</v>
       </c>
       <c r="G64">
-        <v>9960</v>
+        <v>4</v>
       </c>
       <c r="H64">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="I64">
-        <v>25</v>
+        <v>5456</v>
       </c>
       <c r="J64">
-        <v>5456</v>
+        <v>0</v>
       </c>
       <c r="K64">
         <v>0</v>
       </c>
-      <c r="L64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>75</v>
       </c>
@@ -3681,29 +3486,26 @@
       <c r="E65" t="s">
         <v>109</v>
       </c>
-      <c r="F65" t="s">
-        <v>109</v>
+      <c r="F65">
+        <v>9967</v>
       </c>
       <c r="G65">
-        <v>9967</v>
+        <v>2</v>
       </c>
       <c r="H65">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="I65">
-        <v>34</v>
+        <v>1941</v>
       </c>
       <c r="J65">
-        <v>1941</v>
+        <v>0</v>
       </c>
       <c r="K65">
         <v>0</v>
       </c>
-      <c r="L65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>76</v>
       </c>
@@ -3719,29 +3521,26 @@
       <c r="E66" t="s">
         <v>109</v>
       </c>
-      <c r="F66" t="s">
-        <v>109</v>
+      <c r="F66">
+        <v>9946</v>
       </c>
       <c r="G66">
-        <v>9946</v>
+        <v>2</v>
       </c>
       <c r="H66">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="I66">
-        <v>31</v>
+        <v>569</v>
       </c>
       <c r="J66">
-        <v>569</v>
+        <v>0</v>
       </c>
       <c r="K66">
         <v>0</v>
       </c>
-      <c r="L66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>78</v>
       </c>
@@ -3757,29 +3556,26 @@
       <c r="E67" t="s">
         <v>109</v>
       </c>
-      <c r="F67" t="s">
-        <v>109</v>
+      <c r="F67">
+        <v>7592</v>
       </c>
       <c r="G67">
-        <v>7592</v>
+        <v>2</v>
       </c>
       <c r="H67">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I67">
-        <v>15</v>
+        <v>48842</v>
       </c>
       <c r="J67">
-        <v>48842</v>
+        <v>3620</v>
       </c>
       <c r="K67">
-        <v>3620</v>
-      </c>
-      <c r="L67">
         <v>6465</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>82</v>
       </c>
@@ -3793,31 +3589,28 @@
         <v>105</v>
       </c>
       <c r="E68" t="s">
-        <v>109</v>
-      </c>
-      <c r="F68" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F68">
+        <v>14969</v>
       </c>
       <c r="G68">
-        <v>14969</v>
+        <v>5</v>
       </c>
       <c r="H68">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="I68">
-        <v>33</v>
+        <v>9873</v>
       </c>
       <c r="J68">
-        <v>9873</v>
+        <v>0</v>
       </c>
       <c r="K68">
         <v>0</v>
       </c>
-      <c r="L68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>83</v>
       </c>
@@ -3831,31 +3624,28 @@
         <v>105</v>
       </c>
       <c r="E69" t="s">
-        <v>109</v>
-      </c>
-      <c r="F69" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F69">
+        <v>14968</v>
       </c>
       <c r="G69">
-        <v>14968</v>
+        <v>2</v>
       </c>
       <c r="H69">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="I69">
-        <v>40</v>
+        <v>540</v>
       </c>
       <c r="J69">
-        <v>540</v>
+        <v>263</v>
       </c>
       <c r="K69">
-        <v>263</v>
-      </c>
-      <c r="L69">
         <v>999</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>84</v>
       </c>
@@ -3871,29 +3661,26 @@
       <c r="E70" t="s">
         <v>109</v>
       </c>
-      <c r="F70" t="s">
-        <v>109</v>
+      <c r="F70">
+        <v>14967</v>
       </c>
       <c r="G70">
-        <v>14967</v>
+        <v>6</v>
       </c>
       <c r="H70">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="I70">
-        <v>35</v>
+        <v>2796</v>
       </c>
       <c r="J70">
-        <v>2796</v>
+        <v>2795</v>
       </c>
       <c r="K70">
-        <v>2795</v>
-      </c>
-      <c r="L70">
         <v>68100</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>85</v>
       </c>
@@ -3907,31 +3694,28 @@
         <v>105</v>
       </c>
       <c r="E71" t="s">
-        <v>109</v>
-      </c>
-      <c r="F71" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F71">
+        <v>125920</v>
       </c>
       <c r="G71">
-        <v>125920</v>
+        <v>2</v>
       </c>
       <c r="H71">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="I71">
-        <v>13</v>
+        <v>500</v>
       </c>
       <c r="J71">
-        <v>500</v>
+        <v>401</v>
       </c>
       <c r="K71">
-        <v>401</v>
-      </c>
-      <c r="L71">
         <v>835</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>87</v>
       </c>
@@ -3947,29 +3731,26 @@
       <c r="E72" t="s">
         <v>109</v>
       </c>
-      <c r="F72" t="s">
-        <v>109</v>
+      <c r="F72">
+        <v>125921</v>
       </c>
       <c r="G72">
-        <v>125921</v>
+        <v>10</v>
       </c>
       <c r="H72">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I72">
-        <v>8</v>
+        <v>500</v>
       </c>
       <c r="J72">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="K72">
         <v>0</v>
       </c>
-      <c r="L72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>88</v>
       </c>
@@ -3985,29 +3766,26 @@
       <c r="E73" t="s">
         <v>109</v>
       </c>
-      <c r="F73" t="s">
-        <v>109</v>
+      <c r="F73">
+        <v>125922</v>
       </c>
       <c r="G73">
-        <v>125922</v>
+        <v>11</v>
       </c>
       <c r="H73">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="I73">
-        <v>41</v>
+        <v>5500</v>
       </c>
       <c r="J73">
-        <v>5500</v>
+        <v>0</v>
       </c>
       <c r="K73">
         <v>0</v>
       </c>
-      <c r="L73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>89</v>
       </c>
@@ -4023,29 +3801,26 @@
       <c r="E74" t="s">
         <v>109</v>
       </c>
-      <c r="F74" t="s">
-        <v>109</v>
+      <c r="F74">
+        <v>146607</v>
       </c>
       <c r="G74">
-        <v>146607</v>
+        <v>2</v>
       </c>
       <c r="H74">
-        <v>2</v>
+        <v>123</v>
       </c>
       <c r="I74">
-        <v>123</v>
+        <v>8378</v>
       </c>
       <c r="J74">
-        <v>8378</v>
+        <v>7330</v>
       </c>
       <c r="K74">
-        <v>7330</v>
-      </c>
-      <c r="L74">
         <v>18372</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>61</v>
       </c>
@@ -4061,29 +3836,26 @@
       <c r="E75" t="s">
         <v>109</v>
       </c>
-      <c r="F75" t="s">
-        <v>109</v>
+      <c r="F75">
+        <v>9986</v>
       </c>
       <c r="G75">
-        <v>9986</v>
+        <v>6</v>
       </c>
       <c r="H75">
-        <v>6</v>
+        <v>129</v>
       </c>
       <c r="I75">
-        <v>129</v>
+        <v>13910</v>
       </c>
       <c r="J75">
-        <v>13910</v>
+        <v>0</v>
       </c>
       <c r="K75">
         <v>0</v>
       </c>
-      <c r="L75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>53</v>
       </c>
@@ -4099,29 +3871,26 @@
       <c r="E76" t="s">
         <v>109</v>
       </c>
-      <c r="F76" t="s">
-        <v>109</v>
+      <c r="F76">
+        <v>14965</v>
       </c>
       <c r="G76">
-        <v>14965</v>
+        <v>2</v>
       </c>
       <c r="H76">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="I76">
-        <v>17</v>
+        <v>45211</v>
       </c>
       <c r="J76">
-        <v>45211</v>
+        <v>0</v>
       </c>
       <c r="K76">
         <v>0</v>
       </c>
-      <c r="L76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>71</v>
       </c>
@@ -4137,29 +3906,26 @@
       <c r="E77" t="s">
         <v>109</v>
       </c>
-      <c r="F77" t="s">
-        <v>109</v>
+      <c r="F77">
+        <v>9956</v>
       </c>
       <c r="G77">
-        <v>9956</v>
+        <v>100</v>
       </c>
       <c r="H77">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="I77">
-        <v>65</v>
+        <v>1599</v>
       </c>
       <c r="J77">
-        <v>1599</v>
+        <v>0</v>
       </c>
       <c r="K77">
         <v>0</v>
       </c>
-      <c r="L77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>81</v>
       </c>
@@ -4175,29 +3941,26 @@
       <c r="E78" t="s">
         <v>109</v>
       </c>
-      <c r="F78" t="s">
-        <v>109</v>
+      <c r="F78">
+        <v>34537</v>
       </c>
       <c r="G78">
-        <v>34537</v>
+        <v>2</v>
       </c>
       <c r="H78">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="I78">
-        <v>31</v>
+        <v>11055</v>
       </c>
       <c r="J78">
-        <v>11055</v>
+        <v>0</v>
       </c>
       <c r="K78">
         <v>0</v>
       </c>
-      <c r="L78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>90</v>
       </c>
@@ -4211,31 +3974,28 @@
         <v>105</v>
       </c>
       <c r="E79" t="s">
-        <v>109</v>
-      </c>
-      <c r="F79" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F79">
+        <v>146195</v>
       </c>
       <c r="G79">
-        <v>146195</v>
+        <v>3</v>
       </c>
       <c r="H79">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="I79">
-        <v>43</v>
+        <v>67557</v>
       </c>
       <c r="J79">
-        <v>67557</v>
+        <v>0</v>
       </c>
       <c r="K79">
         <v>0</v>
       </c>
-      <c r="L79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>80</v>
       </c>
@@ -4249,31 +4009,28 @@
         <v>105</v>
       </c>
       <c r="E80" t="s">
-        <v>109</v>
-      </c>
-      <c r="F80" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F80">
+        <v>34539</v>
       </c>
       <c r="G80">
-        <v>34539</v>
+        <v>2</v>
       </c>
       <c r="H80">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I80">
-        <v>10</v>
+        <v>32769</v>
       </c>
       <c r="J80">
-        <v>32769</v>
+        <v>0</v>
       </c>
       <c r="K80">
         <v>0</v>
       </c>
-      <c r="L80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>62</v>
       </c>
@@ -4287,31 +4044,28 @@
         <v>105</v>
       </c>
       <c r="E81" t="s">
-        <v>109</v>
-      </c>
-      <c r="F81" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F81">
+        <v>14970</v>
       </c>
       <c r="G81">
-        <v>14970</v>
+        <v>6</v>
       </c>
       <c r="H81">
-        <v>6</v>
+        <v>562</v>
       </c>
       <c r="I81">
-        <v>562</v>
+        <v>10299</v>
       </c>
       <c r="J81">
-        <v>10299</v>
+        <v>0</v>
       </c>
       <c r="K81">
         <v>0</v>
       </c>
-      <c r="L81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>79</v>
       </c>
@@ -4325,31 +4079,28 @@
         <v>105</v>
       </c>
       <c r="E82" t="s">
-        <v>109</v>
-      </c>
-      <c r="F82" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F82">
+        <v>14966</v>
       </c>
       <c r="G82">
-        <v>14966</v>
+        <v>2</v>
       </c>
       <c r="H82">
-        <v>2</v>
+        <v>1777</v>
       </c>
       <c r="I82">
-        <v>1777</v>
+        <v>3751</v>
       </c>
       <c r="J82">
-        <v>3751</v>
+        <v>0</v>
       </c>
       <c r="K82">
         <v>0</v>
       </c>
-      <c r="L82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>86</v>
       </c>
@@ -4363,31 +4114,28 @@
         <v>105</v>
       </c>
       <c r="E83" t="s">
-        <v>109</v>
-      </c>
-      <c r="F83" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F83">
+        <v>146606</v>
       </c>
       <c r="G83">
-        <v>146606</v>
+        <v>2</v>
       </c>
       <c r="H83">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="I83">
-        <v>29</v>
+        <v>98050</v>
       </c>
       <c r="J83">
-        <v>98050</v>
+        <v>1</v>
       </c>
       <c r="K83">
-        <v>1</v>
-      </c>
-      <c r="L83">
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>40</v>
       </c>
@@ -4401,31 +4149,28 @@
         <v>105</v>
       </c>
       <c r="E84" t="s">
-        <v>109</v>
-      </c>
-      <c r="F84" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F84">
+        <v>3573</v>
       </c>
       <c r="G84">
-        <v>3573</v>
+        <v>10</v>
       </c>
       <c r="H84">
-        <v>10</v>
+        <v>785</v>
       </c>
       <c r="I84">
-        <v>785</v>
+        <v>70000</v>
       </c>
       <c r="J84">
-        <v>70000</v>
+        <v>0</v>
       </c>
       <c r="K84">
         <v>0</v>
       </c>
-      <c r="L84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>41</v>
       </c>
@@ -4439,31 +4184,28 @@
         <v>105</v>
       </c>
       <c r="E85" t="s">
-        <v>109</v>
-      </c>
-      <c r="F85" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F85">
+        <v>3891</v>
       </c>
       <c r="G85">
-        <v>3891</v>
+        <v>2</v>
       </c>
       <c r="H85">
-        <v>2</v>
+        <v>971</v>
       </c>
       <c r="I85">
-        <v>971</v>
+        <v>3468</v>
       </c>
       <c r="J85">
-        <v>3468</v>
+        <v>0</v>
       </c>
       <c r="K85">
         <v>0</v>
       </c>
-      <c r="L85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -4477,31 +4219,28 @@
         <v>105</v>
       </c>
       <c r="E86" t="s">
-        <v>109</v>
-      </c>
-      <c r="F86" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F86">
+        <v>3481</v>
       </c>
       <c r="G86">
-        <v>3481</v>
+        <v>26</v>
       </c>
       <c r="H86">
-        <v>26</v>
+        <v>618</v>
       </c>
       <c r="I86">
-        <v>618</v>
+        <v>7797</v>
       </c>
       <c r="J86">
-        <v>7797</v>
+        <v>0</v>
       </c>
       <c r="K86">
         <v>0</v>
       </c>
-      <c r="L86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>58</v>
       </c>
@@ -4515,31 +4254,28 @@
         <v>105</v>
       </c>
       <c r="E87" t="s">
-        <v>109</v>
-      </c>
-      <c r="F87" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F87">
+        <v>9981</v>
       </c>
       <c r="G87">
-        <v>9981</v>
+        <v>9</v>
       </c>
       <c r="H87">
-        <v>9</v>
+        <v>857</v>
       </c>
       <c r="I87">
-        <v>857</v>
+        <v>1080</v>
       </c>
       <c r="J87">
-        <v>1080</v>
+        <v>0</v>
       </c>
       <c r="K87">
         <v>0</v>
       </c>
-      <c r="L87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>74</v>
       </c>
@@ -4553,31 +4289,28 @@
         <v>105</v>
       </c>
       <c r="E88" t="s">
-        <v>109</v>
-      </c>
-      <c r="F88" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F88">
+        <v>9964</v>
       </c>
       <c r="G88">
-        <v>9964</v>
+        <v>10</v>
       </c>
       <c r="H88">
-        <v>10</v>
+        <v>257</v>
       </c>
       <c r="I88">
-        <v>257</v>
+        <v>1593</v>
       </c>
       <c r="J88">
-        <v>1593</v>
+        <v>0</v>
       </c>
       <c r="K88">
         <v>0</v>
       </c>
-      <c r="L88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>77</v>
       </c>
@@ -4591,31 +4324,28 @@
         <v>105</v>
       </c>
       <c r="E89" t="s">
-        <v>109</v>
-      </c>
-      <c r="F89" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F89">
+        <v>9950</v>
       </c>
       <c r="G89">
-        <v>9950</v>
+        <v>20</v>
       </c>
       <c r="H89">
-        <v>20</v>
+        <v>1301</v>
       </c>
       <c r="I89">
-        <v>1301</v>
+        <v>571</v>
       </c>
       <c r="J89">
-        <v>571</v>
+        <v>0</v>
       </c>
       <c r="K89">
         <v>0</v>
       </c>
-      <c r="L89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>65</v>
       </c>
@@ -4629,31 +4359,28 @@
         <v>105</v>
       </c>
       <c r="E90" t="s">
-        <v>109</v>
-      </c>
-      <c r="F90" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F90">
+        <v>9976</v>
       </c>
       <c r="G90">
-        <v>9976</v>
+        <v>2</v>
       </c>
       <c r="H90">
-        <v>2</v>
+        <v>501</v>
       </c>
       <c r="I90">
-        <v>501</v>
+        <v>2600</v>
       </c>
       <c r="J90">
-        <v>2600</v>
+        <v>0</v>
       </c>
       <c r="K90">
         <v>0</v>
       </c>
-      <c r="L90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>8</v>
       </c>
@@ -4667,31 +4394,28 @@
         <v>105</v>
       </c>
       <c r="E91" t="s">
-        <v>109</v>
-      </c>
-      <c r="F91" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F91">
+        <v>20</v>
       </c>
       <c r="G91">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H91">
-        <v>10</v>
+        <v>241</v>
       </c>
       <c r="I91">
-        <v>241</v>
+        <v>2000</v>
       </c>
       <c r="J91">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="K91">
         <v>0</v>
       </c>
-      <c r="L91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>49</v>
       </c>
@@ -4705,31 +4429,28 @@
         <v>105</v>
       </c>
       <c r="E92" t="s">
-        <v>109</v>
-      </c>
-      <c r="F92" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="F92">
+        <v>3946</v>
       </c>
       <c r="G92">
-        <v>3946</v>
+        <v>2</v>
       </c>
       <c r="H92">
-        <v>2</v>
+        <v>231</v>
       </c>
       <c r="I92">
-        <v>231</v>
+        <v>50000</v>
       </c>
       <c r="J92">
         <v>50000</v>
       </c>
       <c r="K92">
-        <v>50000</v>
-      </c>
-      <c r="L92">
         <v>8024152</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>50</v>
       </c>
@@ -4743,27 +4464,24 @@
         <v>105</v>
       </c>
       <c r="E93" t="s">
-        <v>109</v>
-      </c>
-      <c r="F93" t="s">
-        <v>109</v>
-      </c>
-      <c r="G93" s="2">
+        <v>105</v>
+      </c>
+      <c r="F93" s="2">
         <v>3948</v>
       </c>
+      <c r="G93">
+        <v>2</v>
+      </c>
       <c r="H93">
-        <v>2</v>
+        <v>231</v>
       </c>
       <c r="I93">
-        <v>231</v>
+        <v>50000</v>
       </c>
       <c r="J93">
         <v>50000</v>
       </c>
       <c r="K93">
-        <v>50000</v>
-      </c>
-      <c r="L93">
         <v>8024152</v>
       </c>
     </row>

</xml_diff>

<commit_message>
SS-Voting contest uses best ranked member of prior species
</commit_message>
<xml_diff>
--- a/benchmark/Configuration.xlsx
+++ b/benchmark/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\autem\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA20676-77DA-490C-9347-61174D2B739A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAE231D-917C-42B8-96A7-E4C2483CEC35}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="113">
   <si>
     <t>kr-vs-kp</t>
   </si>
@@ -365,6 +365,9 @@
   </si>
   <si>
     <t>SS</t>
+  </si>
+  <si>
+    <t>SS2</t>
   </si>
 </sst>
 </file>
@@ -1209,28 +1212,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K93"/>
+  <dimension ref="A1:L93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>98</v>
       </c>
@@ -1246,26 +1249,29 @@
       <c r="E1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1281,26 +1287,29 @@
       <c r="E2" t="s">
         <v>105</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2">
         <v>37</v>
       </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
       <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
         <v>9</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>768</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
       <c r="K2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -1316,26 +1325,29 @@
       <c r="E3" t="s">
         <v>105</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3">
         <v>53</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>4</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>19</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>846</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
       <c r="K3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>91</v>
       </c>
@@ -1351,26 +1363,29 @@
       <c r="E4" t="s">
         <v>105</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4">
         <v>125923</v>
       </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
       <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
         <v>15</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>690</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
       <c r="K4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1386,26 +1401,29 @@
       <c r="E5" t="s">
         <v>105</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5">
         <v>145804</v>
       </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
       <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
         <v>10</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>958</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
       <c r="K5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1421,26 +1439,29 @@
       <c r="E6" t="s">
         <v>105</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6">
         <v>18</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>10</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>7</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>2000</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
       <c r="K6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1456,26 +1477,29 @@
       <c r="E7" t="s">
         <v>105</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7">
         <v>11</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>3</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>5</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>625</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
       <c r="K7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1491,26 +1515,29 @@
       <c r="E8" t="s">
         <v>105</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8">
         <v>3021</v>
       </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
       <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
         <v>30</v>
-      </c>
-      <c r="I8">
-        <v>3772</v>
       </c>
       <c r="J8">
         <v>3772</v>
       </c>
       <c r="K8">
+        <v>3772</v>
+      </c>
+      <c r="L8">
         <v>6064</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1526,26 +1553,29 @@
       <c r="E9" t="s">
         <v>109</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G9">
         <v>29</v>
       </c>
-      <c r="G9">
-        <v>2</v>
-      </c>
       <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
         <v>16</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>690</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>37</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1561,26 +1591,29 @@
       <c r="E10" t="s">
         <v>109</v>
       </c>
-      <c r="F10">
+      <c r="F10" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10">
         <v>41</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>19</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>36</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>683</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>121</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>2337</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -1596,26 +1629,29 @@
       <c r="E11" t="s">
         <v>109</v>
       </c>
-      <c r="F11">
+      <c r="F11" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11">
         <v>1779</v>
       </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
       <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11">
         <v>10</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>699</v>
-      </c>
-      <c r="J11">
-        <v>16</v>
       </c>
       <c r="K11">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1631,26 +1667,29 @@
       <c r="E12" t="s">
         <v>109</v>
       </c>
-      <c r="F12">
+      <c r="F12" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12">
         <v>23</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>3</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>10</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>1473</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
       <c r="K12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -1666,26 +1705,29 @@
       <c r="E13" t="s">
         <v>105</v>
       </c>
-      <c r="F13">
+      <c r="F13" t="s">
+        <v>105</v>
+      </c>
+      <c r="G13">
         <v>3561</v>
       </c>
-      <c r="G13">
-        <v>2</v>
-      </c>
       <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
         <v>10</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>672</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>666</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>1200</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1701,26 +1743,29 @@
       <c r="E14" t="s">
         <v>109</v>
       </c>
-      <c r="F14">
+      <c r="F14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14">
         <v>1788</v>
       </c>
-      <c r="G14">
-        <v>2</v>
-      </c>
       <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
         <v>23</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>8124</v>
-      </c>
-      <c r="J14">
-        <v>2480</v>
       </c>
       <c r="K14">
         <v>2480</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1736,26 +1781,29 @@
       <c r="E15" t="s">
         <v>109</v>
       </c>
-      <c r="F15">
+      <c r="F15" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15">
         <v>28</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>10</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>65</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>5620</v>
       </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
       <c r="K15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1771,26 +1819,29 @@
       <c r="E16" t="s">
         <v>105</v>
       </c>
-      <c r="F16">
+      <c r="F16" t="s">
+        <v>105</v>
+      </c>
+      <c r="G16">
         <v>31</v>
       </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
       <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16">
         <v>21</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>1000</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
       <c r="K16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1806,26 +1857,29 @@
       <c r="E17" t="s">
         <v>109</v>
       </c>
-      <c r="F17">
+      <c r="F17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17">
         <v>32</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>10</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>17</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>10992</v>
       </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
       <c r="K17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -1841,26 +1895,29 @@
       <c r="E18" t="s">
         <v>109</v>
       </c>
-      <c r="F18">
+      <c r="F18" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18">
         <v>3</v>
       </c>
-      <c r="G18">
-        <v>2</v>
-      </c>
       <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
         <v>37</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>3196</v>
       </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
       <c r="K18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -1876,26 +1933,29 @@
       <c r="E19" t="s">
         <v>105</v>
       </c>
-      <c r="F19">
+      <c r="F19" t="s">
+        <v>105</v>
+      </c>
+      <c r="G19">
         <v>6</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>26</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>17</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>20000</v>
       </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
       <c r="K19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
@@ -1911,26 +1971,29 @@
       <c r="E20" t="s">
         <v>109</v>
       </c>
-      <c r="F20">
+      <c r="F20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G20">
         <v>12</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>10</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>217</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>2000</v>
       </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
       <c r="K20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
@@ -1946,26 +2009,29 @@
       <c r="E21" t="s">
         <v>109</v>
       </c>
-      <c r="F21">
+      <c r="F21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21">
         <v>1778</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>10</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>77</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>2000</v>
       </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
       <c r="K21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
@@ -1981,26 +2047,29 @@
       <c r="E22" t="s">
         <v>109</v>
       </c>
-      <c r="F22">
+      <c r="F22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G22">
         <v>16</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>10</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>65</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>2000</v>
       </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
       <c r="K22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -2016,26 +2085,29 @@
       <c r="E23" t="s">
         <v>105</v>
       </c>
-      <c r="F23">
+      <c r="F23" t="s">
+        <v>105</v>
+      </c>
+      <c r="G23">
         <v>22</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>10</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>48</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>2000</v>
       </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
       <c r="K23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
@@ -2051,26 +2123,29 @@
       <c r="E24" t="s">
         <v>109</v>
       </c>
-      <c r="F24">
+      <c r="F24" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24">
         <v>36</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>7</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>20</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>2310</v>
       </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
       <c r="K24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
@@ -2086,26 +2161,29 @@
       <c r="E25" t="s">
         <v>109</v>
       </c>
-      <c r="F25">
+      <c r="F25" t="s">
+        <v>109</v>
+      </c>
+      <c r="G25">
         <v>43</v>
       </c>
-      <c r="G25">
-        <v>2</v>
-      </c>
       <c r="H25">
+        <v>2</v>
+      </c>
+      <c r="I25">
         <v>58</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>4601</v>
       </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
       <c r="K25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
@@ -2121,26 +2199,29 @@
       <c r="E26" t="s">
         <v>105</v>
       </c>
-      <c r="F26">
+      <c r="F26" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26">
         <v>45</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>3</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>62</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>3190</v>
       </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
       <c r="K26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
@@ -2156,26 +2237,29 @@
       <c r="E27" t="s">
         <v>109</v>
       </c>
-      <c r="F27">
+      <c r="F27" t="s">
+        <v>109</v>
+      </c>
+      <c r="G27">
         <v>58</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>3</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>41</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>5000</v>
       </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
       <c r="K27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
@@ -2191,26 +2275,29 @@
       <c r="E28" t="s">
         <v>105</v>
       </c>
-      <c r="F28">
+      <c r="F28" t="s">
+        <v>105</v>
+      </c>
+      <c r="G28">
         <v>219</v>
       </c>
-      <c r="G28">
-        <v>2</v>
-      </c>
       <c r="H28">
+        <v>2</v>
+      </c>
+      <c r="I28">
         <v>9</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>45312</v>
       </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
       <c r="K28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
@@ -2226,26 +2313,29 @@
       <c r="E29" t="s">
         <v>105</v>
       </c>
-      <c r="F29">
+      <c r="F29" t="s">
+        <v>105</v>
+      </c>
+      <c r="G29">
         <v>2074</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>6</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>37</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>6430</v>
       </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
       <c r="K29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
@@ -2261,26 +2351,29 @@
       <c r="E30" t="s">
         <v>105</v>
       </c>
-      <c r="F30">
+      <c r="F30" t="s">
+        <v>105</v>
+      </c>
+      <c r="G30">
         <v>2125</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>5</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>20</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>736</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>95</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>448</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
@@ -2296,26 +2389,29 @@
       <c r="E31" t="s">
         <v>105</v>
       </c>
-      <c r="F31">
+      <c r="F31" t="s">
+        <v>105</v>
+      </c>
+      <c r="G31">
         <v>3022</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>11</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>13</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>990</v>
       </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
       <c r="K31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -2331,26 +2427,29 @@
       <c r="E32" t="s">
         <v>109</v>
       </c>
-      <c r="F32">
+      <c r="F32" t="s">
+        <v>109</v>
+      </c>
+      <c r="G32">
         <v>3485</v>
       </c>
-      <c r="G32">
-        <v>2</v>
-      </c>
       <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32">
         <v>300</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>2407</v>
       </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
       <c r="K32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
@@ -2366,26 +2465,29 @@
       <c r="E33" t="s">
         <v>105</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" t="s">
+        <v>105</v>
+      </c>
+      <c r="G33" s="2">
         <v>3492</v>
       </c>
-      <c r="G33">
-        <v>2</v>
-      </c>
       <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33">
         <v>7</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>556</v>
       </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
       <c r="K33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -2401,26 +2503,29 @@
       <c r="E34" t="s">
         <v>105</v>
       </c>
-      <c r="F34">
+      <c r="F34" t="s">
+        <v>105</v>
+      </c>
+      <c r="G34">
         <v>3493</v>
       </c>
-      <c r="G34">
-        <v>2</v>
-      </c>
       <c r="H34">
+        <v>2</v>
+      </c>
+      <c r="I34">
         <v>7</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>601</v>
       </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
       <c r="K34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -2436,26 +2541,29 @@
       <c r="E35" t="s">
         <v>105</v>
       </c>
-      <c r="F35">
+      <c r="F35" t="s">
+        <v>105</v>
+      </c>
+      <c r="G35">
         <v>3494</v>
       </c>
-      <c r="G35">
-        <v>2</v>
-      </c>
       <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
         <v>7</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>554</v>
       </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
       <c r="K35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -2471,26 +2579,29 @@
       <c r="E36" t="s">
         <v>109</v>
       </c>
-      <c r="F36">
+      <c r="F36" t="s">
+        <v>109</v>
+      </c>
+      <c r="G36">
         <v>4544</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>9</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>15</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>9961</v>
       </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
       <c r="K36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -2506,26 +2617,29 @@
       <c r="E37" t="s">
         <v>109</v>
       </c>
-      <c r="F37">
+      <c r="F37" t="s">
+        <v>109</v>
+      </c>
+      <c r="G37">
         <v>3512</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>6</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>62</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <v>600</v>
       </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
       <c r="K37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
@@ -2541,26 +2655,29 @@
       <c r="E38" t="s">
         <v>109</v>
       </c>
-      <c r="F38">
+      <c r="F38" t="s">
+        <v>109</v>
+      </c>
+      <c r="G38">
         <v>3543</v>
       </c>
-      <c r="G38">
-        <v>2</v>
-      </c>
       <c r="H38">
+        <v>2</v>
+      </c>
+      <c r="I38">
         <v>6</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <v>500</v>
-      </c>
-      <c r="J38">
-        <v>32</v>
       </c>
       <c r="K38">
         <v>32</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
@@ -2576,26 +2693,29 @@
       <c r="E39" t="s">
         <v>105</v>
       </c>
-      <c r="F39">
+      <c r="F39" t="s">
+        <v>105</v>
+      </c>
+      <c r="G39">
         <v>3549</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>4</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>71</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>841</v>
       </c>
-      <c r="J39">
-        <v>0</v>
-      </c>
       <c r="K39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
@@ -2611,26 +2731,29 @@
       <c r="E40" t="s">
         <v>105</v>
       </c>
-      <c r="F40">
+      <c r="F40" t="s">
+        <v>105</v>
+      </c>
+      <c r="G40">
         <v>3560</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>6</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>5</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <v>797</v>
       </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
       <c r="K40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>42</v>
       </c>
@@ -2646,26 +2769,29 @@
       <c r="E41" t="s">
         <v>109</v>
       </c>
-      <c r="F41">
+      <c r="F41" t="s">
+        <v>109</v>
+      </c>
+      <c r="G41">
         <v>3899</v>
       </c>
-      <c r="G41">
-        <v>2</v>
-      </c>
       <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
         <v>6</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <v>15545</v>
       </c>
-      <c r="J41">
-        <v>0</v>
-      </c>
       <c r="K41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>43</v>
       </c>
@@ -2681,26 +2807,29 @@
       <c r="E42" t="s">
         <v>109</v>
       </c>
-      <c r="F42">
+      <c r="F42" t="s">
+        <v>109</v>
+      </c>
+      <c r="G42">
         <v>3902</v>
       </c>
-      <c r="G42">
-        <v>2</v>
-      </c>
       <c r="H42">
+        <v>2</v>
+      </c>
+      <c r="I42">
         <v>38</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <v>1458</v>
       </c>
-      <c r="J42">
-        <v>0</v>
-      </c>
       <c r="K42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>44</v>
       </c>
@@ -2716,26 +2845,29 @@
       <c r="E43" t="s">
         <v>105</v>
       </c>
-      <c r="F43">
+      <c r="F43" t="s">
+        <v>105</v>
+      </c>
+      <c r="G43">
         <v>3903</v>
       </c>
-      <c r="G43">
-        <v>2</v>
-      </c>
       <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43">
         <v>38</v>
       </c>
-      <c r="I43">
+      <c r="J43">
         <v>1563</v>
       </c>
-      <c r="J43">
-        <v>0</v>
-      </c>
       <c r="K43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>45</v>
       </c>
@@ -2751,26 +2883,29 @@
       <c r="E44" t="s">
         <v>109</v>
       </c>
-      <c r="F44">
+      <c r="F44" t="s">
+        <v>109</v>
+      </c>
+      <c r="G44">
         <v>3904</v>
       </c>
-      <c r="G44">
-        <v>2</v>
-      </c>
       <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="I44">
         <v>22</v>
       </c>
-      <c r="I44">
+      <c r="J44">
         <v>10885</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <v>5</v>
       </c>
-      <c r="K44">
+      <c r="L44">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>46</v>
       </c>
@@ -2786,26 +2921,29 @@
       <c r="E45" t="s">
         <v>109</v>
       </c>
-      <c r="F45">
+      <c r="F45" t="s">
+        <v>109</v>
+      </c>
+      <c r="G45">
         <v>3913</v>
       </c>
-      <c r="G45">
-        <v>2</v>
-      </c>
       <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
         <v>22</v>
       </c>
-      <c r="I45">
+      <c r="J45">
         <v>522</v>
       </c>
-      <c r="J45">
-        <v>0</v>
-      </c>
       <c r="K45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>47</v>
       </c>
@@ -2821,26 +2959,29 @@
       <c r="E46" t="s">
         <v>109</v>
       </c>
-      <c r="F46">
+      <c r="F46" t="s">
+        <v>109</v>
+      </c>
+      <c r="G46">
         <v>3917</v>
       </c>
-      <c r="G46">
-        <v>2</v>
-      </c>
       <c r="H46">
+        <v>2</v>
+      </c>
+      <c r="I46">
         <v>22</v>
       </c>
-      <c r="I46">
+      <c r="J46">
         <v>2109</v>
       </c>
-      <c r="J46">
-        <v>0</v>
-      </c>
       <c r="K46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>48</v>
       </c>
@@ -2856,26 +2997,29 @@
       <c r="E47" t="s">
         <v>109</v>
       </c>
-      <c r="F47">
+      <c r="F47" t="s">
+        <v>109</v>
+      </c>
+      <c r="G47">
         <v>3918</v>
       </c>
-      <c r="G47">
-        <v>2</v>
-      </c>
       <c r="H47">
+        <v>2</v>
+      </c>
+      <c r="I47">
         <v>22</v>
       </c>
-      <c r="I47">
+      <c r="J47">
         <v>1109</v>
       </c>
-      <c r="J47">
-        <v>0</v>
-      </c>
       <c r="K47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>51</v>
       </c>
@@ -2891,26 +3035,29 @@
       <c r="E48" t="s">
         <v>109</v>
       </c>
-      <c r="F48">
+      <c r="F48" t="s">
+        <v>109</v>
+      </c>
+      <c r="G48">
         <v>3954</v>
       </c>
-      <c r="G48">
-        <v>2</v>
-      </c>
       <c r="H48">
+        <v>2</v>
+      </c>
+      <c r="I48">
         <v>12</v>
       </c>
-      <c r="I48">
+      <c r="J48">
         <v>19020</v>
       </c>
-      <c r="J48">
-        <v>0</v>
-      </c>
       <c r="K48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>52</v>
       </c>
@@ -2926,26 +3073,29 @@
       <c r="E49" t="s">
         <v>105</v>
       </c>
-      <c r="F49">
+      <c r="F49" t="s">
+        <v>105</v>
+      </c>
+      <c r="G49">
         <v>14964</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>10</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <v>8</v>
       </c>
-      <c r="I49">
+      <c r="J49">
         <v>10218</v>
       </c>
-      <c r="J49">
-        <v>0</v>
-      </c>
       <c r="K49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>54</v>
       </c>
@@ -2961,26 +3111,29 @@
       <c r="E50" t="s">
         <v>109</v>
       </c>
-      <c r="F50" s="2">
+      <c r="F50" t="s">
+        <v>109</v>
+      </c>
+      <c r="G50" s="2">
         <v>10093</v>
       </c>
-      <c r="G50">
-        <v>2</v>
-      </c>
       <c r="H50">
+        <v>2</v>
+      </c>
+      <c r="I50">
         <v>5</v>
       </c>
-      <c r="I50">
+      <c r="J50">
         <v>1372</v>
       </c>
-      <c r="J50">
-        <v>0</v>
-      </c>
       <c r="K50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
@@ -2996,26 +3149,29 @@
       <c r="E51" t="s">
         <v>109</v>
       </c>
-      <c r="F51">
+      <c r="F51" t="s">
+        <v>109</v>
+      </c>
+      <c r="G51">
         <v>10101</v>
       </c>
-      <c r="G51">
-        <v>2</v>
-      </c>
       <c r="H51">
+        <v>2</v>
+      </c>
+      <c r="I51">
         <v>5</v>
       </c>
-      <c r="I51">
+      <c r="J51">
         <v>748</v>
       </c>
-      <c r="J51">
-        <v>0</v>
-      </c>
       <c r="K51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>56</v>
       </c>
@@ -3031,26 +3187,29 @@
       <c r="E52" t="s">
         <v>109</v>
       </c>
-      <c r="F52">
+      <c r="F52" t="s">
+        <v>109</v>
+      </c>
+      <c r="G52">
         <v>9979</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>10</v>
       </c>
-      <c r="H52">
+      <c r="I52">
         <v>36</v>
       </c>
-      <c r="I52">
+      <c r="J52">
         <v>2126</v>
       </c>
-      <c r="J52">
-        <v>0</v>
-      </c>
       <c r="K52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>57</v>
       </c>
@@ -3066,26 +3225,29 @@
       <c r="E53" t="s">
         <v>105</v>
       </c>
-      <c r="F53">
+      <c r="F53" t="s">
+        <v>105</v>
+      </c>
+      <c r="G53">
         <v>9980</v>
       </c>
-      <c r="G53">
-        <v>2</v>
-      </c>
       <c r="H53">
+        <v>2</v>
+      </c>
+      <c r="I53">
         <v>21</v>
       </c>
-      <c r="I53">
+      <c r="J53">
         <v>540</v>
       </c>
-      <c r="J53">
-        <v>0</v>
-      </c>
       <c r="K53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
@@ -3101,26 +3263,29 @@
       <c r="E54" t="s">
         <v>109</v>
       </c>
-      <c r="F54">
+      <c r="F54" t="s">
+        <v>109</v>
+      </c>
+      <c r="G54">
         <v>9983</v>
       </c>
-      <c r="G54">
-        <v>2</v>
-      </c>
       <c r="H54">
+        <v>2</v>
+      </c>
+      <c r="I54">
         <v>15</v>
       </c>
-      <c r="I54">
+      <c r="J54">
         <v>14980</v>
       </c>
-      <c r="J54">
-        <v>0</v>
-      </c>
       <c r="K54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>60</v>
       </c>
@@ -3136,26 +3301,29 @@
       <c r="E55" t="s">
         <v>105</v>
       </c>
-      <c r="F55">
+      <c r="F55" t="s">
+        <v>105</v>
+      </c>
+      <c r="G55">
         <v>9985</v>
       </c>
-      <c r="G55">
+      <c r="H55">
         <v>6</v>
       </c>
-      <c r="H55">
+      <c r="I55">
         <v>52</v>
       </c>
-      <c r="I55">
+      <c r="J55">
         <v>6118</v>
       </c>
-      <c r="J55">
-        <v>0</v>
-      </c>
       <c r="K55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>63</v>
       </c>
@@ -3171,26 +3339,29 @@
       <c r="E56" t="s">
         <v>109</v>
       </c>
-      <c r="F56">
+      <c r="F56" t="s">
+        <v>109</v>
+      </c>
+      <c r="G56">
         <v>9970</v>
       </c>
-      <c r="G56">
-        <v>2</v>
-      </c>
       <c r="H56">
+        <v>2</v>
+      </c>
+      <c r="I56">
         <v>101</v>
       </c>
-      <c r="I56">
+      <c r="J56">
         <v>1212</v>
       </c>
-      <c r="J56">
-        <v>0</v>
-      </c>
       <c r="K56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>64</v>
       </c>
@@ -3206,26 +3377,29 @@
       <c r="E57" t="s">
         <v>109</v>
       </c>
-      <c r="F57">
+      <c r="F57" t="s">
+        <v>109</v>
+      </c>
+      <c r="G57">
         <v>9971</v>
       </c>
-      <c r="G57">
-        <v>2</v>
-      </c>
       <c r="H57">
+        <v>2</v>
+      </c>
+      <c r="I57">
         <v>11</v>
       </c>
-      <c r="I57">
+      <c r="J57">
         <v>583</v>
       </c>
-      <c r="J57">
-        <v>0</v>
-      </c>
       <c r="K57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>66</v>
       </c>
@@ -3241,26 +3415,29 @@
       <c r="E58" t="s">
         <v>109</v>
       </c>
-      <c r="F58">
+      <c r="F58" t="s">
+        <v>109</v>
+      </c>
+      <c r="G58">
         <v>9977</v>
       </c>
-      <c r="G58">
-        <v>2</v>
-      </c>
       <c r="H58">
+        <v>2</v>
+      </c>
+      <c r="I58">
         <v>119</v>
       </c>
-      <c r="I58">
+      <c r="J58">
         <v>34465</v>
       </c>
-      <c r="J58">
-        <v>0</v>
-      </c>
       <c r="K58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>67</v>
       </c>
@@ -3276,26 +3453,29 @@
       <c r="E59" t="s">
         <v>109</v>
       </c>
-      <c r="F59">
+      <c r="F59" t="s">
+        <v>109</v>
+      </c>
+      <c r="G59">
         <v>9978</v>
       </c>
-      <c r="G59">
-        <v>2</v>
-      </c>
       <c r="H59">
+        <v>2</v>
+      </c>
+      <c r="I59">
         <v>73</v>
       </c>
-      <c r="I59">
+      <c r="J59">
         <v>2534</v>
       </c>
-      <c r="J59">
-        <v>0</v>
-      </c>
       <c r="K59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>68</v>
       </c>
@@ -3311,26 +3491,29 @@
       <c r="E60" t="s">
         <v>109</v>
       </c>
-      <c r="F60">
+      <c r="F60" t="s">
+        <v>109</v>
+      </c>
+      <c r="G60">
         <v>9952</v>
       </c>
-      <c r="G60">
-        <v>2</v>
-      </c>
       <c r="H60">
+        <v>2</v>
+      </c>
+      <c r="I60">
         <v>6</v>
       </c>
-      <c r="I60">
+      <c r="J60">
         <v>5404</v>
       </c>
-      <c r="J60">
-        <v>0</v>
-      </c>
       <c r="K60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>69</v>
       </c>
@@ -3346,26 +3529,29 @@
       <c r="E61" t="s">
         <v>109</v>
       </c>
-      <c r="F61">
+      <c r="F61" t="s">
+        <v>109</v>
+      </c>
+      <c r="G61">
         <v>9954</v>
       </c>
-      <c r="G61">
+      <c r="H61">
         <v>100</v>
       </c>
-      <c r="H61">
+      <c r="I61">
         <v>65</v>
       </c>
-      <c r="I61">
+      <c r="J61">
         <v>1600</v>
       </c>
-      <c r="J61">
-        <v>0</v>
-      </c>
       <c r="K61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>70</v>
       </c>
@@ -3381,26 +3567,29 @@
       <c r="E62" t="s">
         <v>109</v>
       </c>
-      <c r="F62">
+      <c r="F62" t="s">
+        <v>109</v>
+      </c>
+      <c r="G62">
         <v>9955</v>
       </c>
-      <c r="G62">
+      <c r="H62">
         <v>100</v>
       </c>
-      <c r="H62">
+      <c r="I62">
         <v>65</v>
       </c>
-      <c r="I62">
+      <c r="J62">
         <v>1600</v>
       </c>
-      <c r="J62">
-        <v>0</v>
-      </c>
       <c r="K62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>72</v>
       </c>
@@ -3416,26 +3605,29 @@
       <c r="E63" t="s">
         <v>109</v>
       </c>
-      <c r="F63">
+      <c r="F63" t="s">
+        <v>109</v>
+      </c>
+      <c r="G63">
         <v>9957</v>
       </c>
-      <c r="G63">
-        <v>2</v>
-      </c>
       <c r="H63">
+        <v>2</v>
+      </c>
+      <c r="I63">
         <v>42</v>
       </c>
-      <c r="I63">
+      <c r="J63">
         <v>1055</v>
       </c>
-      <c r="J63">
-        <v>0</v>
-      </c>
       <c r="K63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>73</v>
       </c>
@@ -3451,26 +3643,29 @@
       <c r="E64" t="s">
         <v>109</v>
       </c>
-      <c r="F64">
+      <c r="F64" t="s">
+        <v>109</v>
+      </c>
+      <c r="G64">
         <v>9960</v>
       </c>
-      <c r="G64">
+      <c r="H64">
         <v>4</v>
       </c>
-      <c r="H64">
+      <c r="I64">
         <v>25</v>
       </c>
-      <c r="I64">
+      <c r="J64">
         <v>5456</v>
       </c>
-      <c r="J64">
-        <v>0</v>
-      </c>
       <c r="K64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>75</v>
       </c>
@@ -3486,26 +3681,29 @@
       <c r="E65" t="s">
         <v>109</v>
       </c>
-      <c r="F65">
+      <c r="F65" t="s">
+        <v>109</v>
+      </c>
+      <c r="G65">
         <v>9967</v>
       </c>
-      <c r="G65">
-        <v>2</v>
-      </c>
       <c r="H65">
+        <v>2</v>
+      </c>
+      <c r="I65">
         <v>34</v>
       </c>
-      <c r="I65">
+      <c r="J65">
         <v>1941</v>
       </c>
-      <c r="J65">
-        <v>0</v>
-      </c>
       <c r="K65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>76</v>
       </c>
@@ -3521,26 +3719,29 @@
       <c r="E66" t="s">
         <v>109</v>
       </c>
-      <c r="F66">
+      <c r="F66" t="s">
+        <v>109</v>
+      </c>
+      <c r="G66">
         <v>9946</v>
       </c>
-      <c r="G66">
-        <v>2</v>
-      </c>
       <c r="H66">
+        <v>2</v>
+      </c>
+      <c r="I66">
         <v>31</v>
       </c>
-      <c r="I66">
+      <c r="J66">
         <v>569</v>
       </c>
-      <c r="J66">
-        <v>0</v>
-      </c>
       <c r="K66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>78</v>
       </c>
@@ -3556,26 +3757,29 @@
       <c r="E67" t="s">
         <v>109</v>
       </c>
-      <c r="F67">
+      <c r="F67" t="s">
+        <v>109</v>
+      </c>
+      <c r="G67">
         <v>7592</v>
       </c>
-      <c r="G67">
-        <v>2</v>
-      </c>
       <c r="H67">
+        <v>2</v>
+      </c>
+      <c r="I67">
         <v>15</v>
       </c>
-      <c r="I67">
+      <c r="J67">
         <v>48842</v>
       </c>
-      <c r="J67">
+      <c r="K67">
         <v>3620</v>
       </c>
-      <c r="K67">
+      <c r="L67">
         <v>6465</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>82</v>
       </c>
@@ -3591,26 +3795,29 @@
       <c r="E68" t="s">
         <v>105</v>
       </c>
-      <c r="F68">
+      <c r="F68" t="s">
+        <v>105</v>
+      </c>
+      <c r="G68">
         <v>14969</v>
       </c>
-      <c r="G68">
+      <c r="H68">
         <v>5</v>
       </c>
-      <c r="H68">
+      <c r="I68">
         <v>33</v>
       </c>
-      <c r="I68">
+      <c r="J68">
         <v>9873</v>
       </c>
-      <c r="J68">
-        <v>0</v>
-      </c>
       <c r="K68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>83</v>
       </c>
@@ -3626,26 +3833,29 @@
       <c r="E69" t="s">
         <v>105</v>
       </c>
-      <c r="F69">
+      <c r="F69" t="s">
+        <v>105</v>
+      </c>
+      <c r="G69">
         <v>14968</v>
       </c>
-      <c r="G69">
-        <v>2</v>
-      </c>
       <c r="H69">
+        <v>2</v>
+      </c>
+      <c r="I69">
         <v>40</v>
       </c>
-      <c r="I69">
+      <c r="J69">
         <v>540</v>
       </c>
-      <c r="J69">
+      <c r="K69">
         <v>263</v>
       </c>
-      <c r="K69">
+      <c r="L69">
         <v>999</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>84</v>
       </c>
@@ -3661,26 +3871,29 @@
       <c r="E70" t="s">
         <v>109</v>
       </c>
-      <c r="F70">
+      <c r="F70" t="s">
+        <v>109</v>
+      </c>
+      <c r="G70">
         <v>14967</v>
       </c>
-      <c r="G70">
+      <c r="H70">
         <v>6</v>
       </c>
-      <c r="H70">
+      <c r="I70">
         <v>35</v>
       </c>
-      <c r="I70">
+      <c r="J70">
         <v>2796</v>
       </c>
-      <c r="J70">
+      <c r="K70">
         <v>2795</v>
       </c>
-      <c r="K70">
+      <c r="L70">
         <v>68100</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>85</v>
       </c>
@@ -3696,26 +3909,29 @@
       <c r="E71" t="s">
         <v>105</v>
       </c>
-      <c r="F71">
+      <c r="F71" t="s">
+        <v>105</v>
+      </c>
+      <c r="G71">
         <v>125920</v>
       </c>
-      <c r="G71">
-        <v>2</v>
-      </c>
       <c r="H71">
+        <v>2</v>
+      </c>
+      <c r="I71">
         <v>13</v>
       </c>
-      <c r="I71">
+      <c r="J71">
         <v>500</v>
       </c>
-      <c r="J71">
+      <c r="K71">
         <v>401</v>
       </c>
-      <c r="K71">
+      <c r="L71">
         <v>835</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>87</v>
       </c>
@@ -3731,26 +3947,29 @@
       <c r="E72" t="s">
         <v>109</v>
       </c>
-      <c r="F72">
+      <c r="F72" t="s">
+        <v>109</v>
+      </c>
+      <c r="G72">
         <v>125921</v>
       </c>
-      <c r="G72">
+      <c r="H72">
         <v>10</v>
       </c>
-      <c r="H72">
+      <c r="I72">
         <v>8</v>
       </c>
-      <c r="I72">
+      <c r="J72">
         <v>500</v>
       </c>
-      <c r="J72">
-        <v>0</v>
-      </c>
       <c r="K72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>88</v>
       </c>
@@ -3766,26 +3985,29 @@
       <c r="E73" t="s">
         <v>109</v>
       </c>
-      <c r="F73">
+      <c r="F73" t="s">
+        <v>109</v>
+      </c>
+      <c r="G73">
         <v>125922</v>
       </c>
-      <c r="G73">
+      <c r="H73">
         <v>11</v>
       </c>
-      <c r="H73">
+      <c r="I73">
         <v>41</v>
       </c>
-      <c r="I73">
+      <c r="J73">
         <v>5500</v>
       </c>
-      <c r="J73">
-        <v>0</v>
-      </c>
       <c r="K73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>89</v>
       </c>
@@ -3801,26 +4023,29 @@
       <c r="E74" t="s">
         <v>109</v>
       </c>
-      <c r="F74">
+      <c r="F74" t="s">
+        <v>109</v>
+      </c>
+      <c r="G74">
         <v>146607</v>
       </c>
-      <c r="G74">
-        <v>2</v>
-      </c>
       <c r="H74">
+        <v>2</v>
+      </c>
+      <c r="I74">
         <v>123</v>
       </c>
-      <c r="I74">
+      <c r="J74">
         <v>8378</v>
       </c>
-      <c r="J74">
+      <c r="K74">
         <v>7330</v>
       </c>
-      <c r="K74">
+      <c r="L74">
         <v>18372</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>61</v>
       </c>
@@ -3836,26 +4061,29 @@
       <c r="E75" t="s">
         <v>109</v>
       </c>
-      <c r="F75">
+      <c r="F75" t="s">
+        <v>109</v>
+      </c>
+      <c r="G75">
         <v>9986</v>
       </c>
-      <c r="G75">
+      <c r="H75">
         <v>6</v>
       </c>
-      <c r="H75">
+      <c r="I75">
         <v>129</v>
       </c>
-      <c r="I75">
+      <c r="J75">
         <v>13910</v>
       </c>
-      <c r="J75">
-        <v>0</v>
-      </c>
       <c r="K75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>53</v>
       </c>
@@ -3871,26 +4099,29 @@
       <c r="E76" t="s">
         <v>109</v>
       </c>
-      <c r="F76">
+      <c r="F76" t="s">
+        <v>109</v>
+      </c>
+      <c r="G76">
         <v>14965</v>
       </c>
-      <c r="G76">
-        <v>2</v>
-      </c>
       <c r="H76">
+        <v>2</v>
+      </c>
+      <c r="I76">
         <v>17</v>
       </c>
-      <c r="I76">
+      <c r="J76">
         <v>45211</v>
       </c>
-      <c r="J76">
-        <v>0</v>
-      </c>
       <c r="K76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>71</v>
       </c>
@@ -3906,26 +4137,29 @@
       <c r="E77" t="s">
         <v>109</v>
       </c>
-      <c r="F77">
+      <c r="F77" t="s">
+        <v>109</v>
+      </c>
+      <c r="G77">
         <v>9956</v>
       </c>
-      <c r="G77">
+      <c r="H77">
         <v>100</v>
       </c>
-      <c r="H77">
+      <c r="I77">
         <v>65</v>
       </c>
-      <c r="I77">
+      <c r="J77">
         <v>1599</v>
       </c>
-      <c r="J77">
-        <v>0</v>
-      </c>
       <c r="K77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>81</v>
       </c>
@@ -3941,26 +4175,29 @@
       <c r="E78" t="s">
         <v>109</v>
       </c>
-      <c r="F78">
+      <c r="F78" t="s">
+        <v>109</v>
+      </c>
+      <c r="G78">
         <v>34537</v>
       </c>
-      <c r="G78">
-        <v>2</v>
-      </c>
       <c r="H78">
+        <v>2</v>
+      </c>
+      <c r="I78">
         <v>31</v>
       </c>
-      <c r="I78">
+      <c r="J78">
         <v>11055</v>
       </c>
-      <c r="J78">
-        <v>0</v>
-      </c>
       <c r="K78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>90</v>
       </c>
@@ -3976,26 +4213,29 @@
       <c r="E79" t="s">
         <v>105</v>
       </c>
-      <c r="F79">
+      <c r="F79" t="s">
+        <v>105</v>
+      </c>
+      <c r="G79">
         <v>146195</v>
       </c>
-      <c r="G79">
+      <c r="H79">
         <v>3</v>
       </c>
-      <c r="H79">
+      <c r="I79">
         <v>43</v>
       </c>
-      <c r="I79">
+      <c r="J79">
         <v>67557</v>
       </c>
-      <c r="J79">
-        <v>0</v>
-      </c>
       <c r="K79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>80</v>
       </c>
@@ -4011,26 +4251,29 @@
       <c r="E80" t="s">
         <v>105</v>
       </c>
-      <c r="F80">
+      <c r="F80" t="s">
+        <v>105</v>
+      </c>
+      <c r="G80">
         <v>34539</v>
       </c>
-      <c r="G80">
-        <v>2</v>
-      </c>
       <c r="H80">
+        <v>2</v>
+      </c>
+      <c r="I80">
         <v>10</v>
       </c>
-      <c r="I80">
+      <c r="J80">
         <v>32769</v>
       </c>
-      <c r="J80">
-        <v>0</v>
-      </c>
       <c r="K80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>62</v>
       </c>
@@ -4046,26 +4289,29 @@
       <c r="E81" t="s">
         <v>105</v>
       </c>
-      <c r="F81">
+      <c r="F81" t="s">
+        <v>105</v>
+      </c>
+      <c r="G81">
         <v>14970</v>
       </c>
-      <c r="G81">
+      <c r="H81">
         <v>6</v>
       </c>
-      <c r="H81">
+      <c r="I81">
         <v>562</v>
       </c>
-      <c r="I81">
+      <c r="J81">
         <v>10299</v>
       </c>
-      <c r="J81">
-        <v>0</v>
-      </c>
       <c r="K81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>79</v>
       </c>
@@ -4081,26 +4327,29 @@
       <c r="E82" t="s">
         <v>105</v>
       </c>
-      <c r="F82">
+      <c r="F82" t="s">
+        <v>105</v>
+      </c>
+      <c r="G82">
         <v>14966</v>
       </c>
-      <c r="G82">
-        <v>2</v>
-      </c>
       <c r="H82">
+        <v>2</v>
+      </c>
+      <c r="I82">
         <v>1777</v>
       </c>
-      <c r="I82">
+      <c r="J82">
         <v>3751</v>
       </c>
-      <c r="J82">
-        <v>0</v>
-      </c>
       <c r="K82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>86</v>
       </c>
@@ -4116,26 +4365,29 @@
       <c r="E83" t="s">
         <v>105</v>
       </c>
-      <c r="F83">
+      <c r="F83" t="s">
+        <v>105</v>
+      </c>
+      <c r="G83">
         <v>146606</v>
       </c>
-      <c r="G83">
-        <v>2</v>
-      </c>
       <c r="H83">
+        <v>2</v>
+      </c>
+      <c r="I83">
         <v>29</v>
       </c>
-      <c r="I83">
+      <c r="J83">
         <v>98050</v>
       </c>
-      <c r="J83">
+      <c r="K83">
         <v>1</v>
       </c>
-      <c r="K83">
+      <c r="L83">
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>40</v>
       </c>
@@ -4151,26 +4403,29 @@
       <c r="E84" t="s">
         <v>105</v>
       </c>
-      <c r="F84">
+      <c r="F84" t="s">
+        <v>105</v>
+      </c>
+      <c r="G84">
         <v>3573</v>
       </c>
-      <c r="G84">
+      <c r="H84">
         <v>10</v>
       </c>
-      <c r="H84">
+      <c r="I84">
         <v>785</v>
       </c>
-      <c r="I84">
+      <c r="J84">
         <v>70000</v>
       </c>
-      <c r="J84">
-        <v>0</v>
-      </c>
       <c r="K84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>41</v>
       </c>
@@ -4186,26 +4441,29 @@
       <c r="E85" t="s">
         <v>105</v>
       </c>
-      <c r="F85">
+      <c r="F85" t="s">
+        <v>105</v>
+      </c>
+      <c r="G85">
         <v>3891</v>
       </c>
-      <c r="G85">
-        <v>2</v>
-      </c>
       <c r="H85">
+        <v>2</v>
+      </c>
+      <c r="I85">
         <v>971</v>
       </c>
-      <c r="I85">
+      <c r="J85">
         <v>3468</v>
       </c>
-      <c r="J85">
-        <v>0</v>
-      </c>
       <c r="K85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -4221,26 +4479,29 @@
       <c r="E86" t="s">
         <v>105</v>
       </c>
-      <c r="F86">
+      <c r="F86" t="s">
+        <v>105</v>
+      </c>
+      <c r="G86">
         <v>3481</v>
       </c>
-      <c r="G86">
+      <c r="H86">
         <v>26</v>
       </c>
-      <c r="H86">
+      <c r="I86">
         <v>618</v>
       </c>
-      <c r="I86">
+      <c r="J86">
         <v>7797</v>
       </c>
-      <c r="J86">
-        <v>0</v>
-      </c>
       <c r="K86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>58</v>
       </c>
@@ -4256,26 +4517,29 @@
       <c r="E87" t="s">
         <v>105</v>
       </c>
-      <c r="F87">
+      <c r="F87" t="s">
+        <v>105</v>
+      </c>
+      <c r="G87">
         <v>9981</v>
       </c>
-      <c r="G87">
+      <c r="H87">
         <v>9</v>
       </c>
-      <c r="H87">
+      <c r="I87">
         <v>857</v>
       </c>
-      <c r="I87">
+      <c r="J87">
         <v>1080</v>
       </c>
-      <c r="J87">
-        <v>0</v>
-      </c>
       <c r="K87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>74</v>
       </c>
@@ -4291,26 +4555,29 @@
       <c r="E88" t="s">
         <v>105</v>
       </c>
-      <c r="F88">
+      <c r="F88" t="s">
+        <v>105</v>
+      </c>
+      <c r="G88">
         <v>9964</v>
       </c>
-      <c r="G88">
+      <c r="H88">
         <v>10</v>
       </c>
-      <c r="H88">
+      <c r="I88">
         <v>257</v>
       </c>
-      <c r="I88">
+      <c r="J88">
         <v>1593</v>
       </c>
-      <c r="J88">
-        <v>0</v>
-      </c>
       <c r="K88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>77</v>
       </c>
@@ -4326,26 +4593,29 @@
       <c r="E89" t="s">
         <v>105</v>
       </c>
-      <c r="F89">
+      <c r="F89" t="s">
+        <v>105</v>
+      </c>
+      <c r="G89">
         <v>9950</v>
       </c>
-      <c r="G89">
+      <c r="H89">
         <v>20</v>
       </c>
-      <c r="H89">
+      <c r="I89">
         <v>1301</v>
       </c>
-      <c r="I89">
+      <c r="J89">
         <v>571</v>
       </c>
-      <c r="J89">
-        <v>0</v>
-      </c>
       <c r="K89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>65</v>
       </c>
@@ -4361,26 +4631,29 @@
       <c r="E90" t="s">
         <v>105</v>
       </c>
-      <c r="F90">
+      <c r="F90" t="s">
+        <v>105</v>
+      </c>
+      <c r="G90">
         <v>9976</v>
       </c>
-      <c r="G90">
-        <v>2</v>
-      </c>
       <c r="H90">
+        <v>2</v>
+      </c>
+      <c r="I90">
         <v>501</v>
       </c>
-      <c r="I90">
+      <c r="J90">
         <v>2600</v>
       </c>
-      <c r="J90">
-        <v>0</v>
-      </c>
       <c r="K90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>8</v>
       </c>
@@ -4396,26 +4669,29 @@
       <c r="E91" t="s">
         <v>105</v>
       </c>
-      <c r="F91">
+      <c r="F91" t="s">
+        <v>105</v>
+      </c>
+      <c r="G91">
         <v>20</v>
       </c>
-      <c r="G91">
+      <c r="H91">
         <v>10</v>
       </c>
-      <c r="H91">
+      <c r="I91">
         <v>241</v>
       </c>
-      <c r="I91">
+      <c r="J91">
         <v>2000</v>
       </c>
-      <c r="J91">
-        <v>0</v>
-      </c>
       <c r="K91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>49</v>
       </c>
@@ -4431,26 +4707,29 @@
       <c r="E92" t="s">
         <v>105</v>
       </c>
-      <c r="F92">
+      <c r="F92" t="s">
+        <v>105</v>
+      </c>
+      <c r="G92">
         <v>3946</v>
       </c>
-      <c r="G92">
-        <v>2</v>
-      </c>
       <c r="H92">
+        <v>2</v>
+      </c>
+      <c r="I92">
         <v>231</v>
-      </c>
-      <c r="I92">
-        <v>50000</v>
       </c>
       <c r="J92">
         <v>50000</v>
       </c>
       <c r="K92">
+        <v>50000</v>
+      </c>
+      <c r="L92">
         <v>8024152</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>50</v>
       </c>
@@ -4466,22 +4745,25 @@
       <c r="E93" t="s">
         <v>105</v>
       </c>
-      <c r="F93" s="2">
+      <c r="F93" t="s">
+        <v>105</v>
+      </c>
+      <c r="G93" s="2">
         <v>3948</v>
       </c>
-      <c r="G93">
-        <v>2</v>
-      </c>
       <c r="H93">
+        <v>2</v>
+      </c>
+      <c r="I93">
         <v>231</v>
-      </c>
-      <c r="I93">
-        <v>50000</v>
       </c>
       <c r="J93">
         <v>50000</v>
       </c>
       <c r="K93">
+        <v>50000</v>
+      </c>
+      <c r="L93">
         <v>8024152</v>
       </c>
     </row>

</xml_diff>

<commit_message>
LC1 - Run List Configuration
</commit_message>
<xml_diff>
--- a/benchmark/Configuration.xlsx
+++ b/benchmark/Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\autem\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAE231D-917C-42B8-96A7-E4C2483CEC35}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71818FC0-CA0F-40E9-8889-885FDD64C3B7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10860" yWindow="1890" windowWidth="14640" windowHeight="11655" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openml_100" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="111">
   <si>
     <t>kr-vs-kp</t>
   </si>
@@ -352,22 +352,16 @@
     <t>Complete</t>
   </si>
   <si>
-    <t>gp_comp</t>
-  </si>
-  <si>
-    <t>quick_verifier</t>
-  </si>
-  <si>
     <t>Wait</t>
   </si>
   <si>
     <t>PP1</t>
   </si>
   <si>
-    <t>SS</t>
-  </si>
-  <si>
     <t>SS2</t>
+  </si>
+  <si>
+    <t>LC1</t>
   </si>
 </sst>
 </file>
@@ -1212,66 +1206,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L93"/>
+  <dimension ref="A1:J93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1279,37 +1267,31 @@
         <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F2" t="s">
-        <v>105</v>
+        <v>105</v>
+      </c>
+      <c r="E2">
+        <v>37</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>768</v>
       </c>
       <c r="I2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>768</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -1317,37 +1299,31 @@
         <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F3" t="s">
-        <v>105</v>
+        <v>105</v>
+      </c>
+      <c r="E3">
+        <v>53</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>846</v>
       </c>
       <c r="I3">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>846</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>91</v>
       </c>
@@ -1355,37 +1331,31 @@
         <v>106</v>
       </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F4" t="s">
-        <v>105</v>
+        <v>105</v>
+      </c>
+      <c r="E4">
+        <v>125923</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>125923</v>
+        <v>15</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>690</v>
       </c>
       <c r="I4">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>690</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1393,37 +1363,31 @@
         <v>106</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E5" t="s">
-        <v>105</v>
-      </c>
-      <c r="F5" t="s">
-        <v>105</v>
+        <v>105</v>
+      </c>
+      <c r="E5">
+        <v>145804</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>145804</v>
+        <v>10</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>958</v>
       </c>
       <c r="I5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>958</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1431,37 +1395,31 @@
         <v>106</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
-      </c>
-      <c r="E6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F6" t="s">
-        <v>105</v>
+        <v>105</v>
+      </c>
+      <c r="E6">
+        <v>18</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
       </c>
       <c r="G6">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="H6">
-        <v>10</v>
+        <v>2000</v>
       </c>
       <c r="I6">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>2000</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1469,37 +1427,31 @@
         <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E7" t="s">
-        <v>105</v>
-      </c>
-      <c r="F7" t="s">
-        <v>105</v>
+        <v>105</v>
+      </c>
+      <c r="E7">
+        <v>11</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>625</v>
       </c>
       <c r="I7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>625</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1507,189 +1459,159 @@
         <v>106</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
-      </c>
-      <c r="E8" t="s">
-        <v>105</v>
-      </c>
-      <c r="F8" t="s">
-        <v>105</v>
+        <v>105</v>
+      </c>
+      <c r="E8">
+        <v>3021</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
       </c>
       <c r="G8">
-        <v>3021</v>
+        <v>30</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>3772</v>
       </c>
       <c r="I8">
-        <v>30</v>
+        <v>3772</v>
       </c>
       <c r="J8">
-        <v>3772</v>
-      </c>
-      <c r="K8">
-        <v>3772</v>
-      </c>
-      <c r="L8">
         <v>6064</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s">
-        <v>109</v>
-      </c>
-      <c r="E9" t="s">
-        <v>109</v>
-      </c>
-      <c r="F9" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E9">
+        <v>29</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
       </c>
       <c r="G9">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>690</v>
       </c>
       <c r="I9">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="J9">
-        <v>690</v>
-      </c>
-      <c r="K9">
-        <v>37</v>
-      </c>
-      <c r="L9">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E10" t="s">
-        <v>109</v>
-      </c>
-      <c r="F10" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E10">
+        <v>41</v>
+      </c>
+      <c r="F10">
+        <v>19</v>
       </c>
       <c r="G10">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H10">
-        <v>19</v>
+        <v>683</v>
       </c>
       <c r="I10">
-        <v>36</v>
+        <v>121</v>
       </c>
       <c r="J10">
-        <v>683</v>
-      </c>
-      <c r="K10">
-        <v>121</v>
-      </c>
-      <c r="L10">
         <v>2337</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D11" t="s">
-        <v>109</v>
-      </c>
-      <c r="E11" t="s">
-        <v>109</v>
-      </c>
-      <c r="F11" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E11">
+        <v>1779</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
       </c>
       <c r="G11">
-        <v>1779</v>
+        <v>10</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>699</v>
       </c>
       <c r="I11">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J11">
-        <v>699</v>
-      </c>
-      <c r="K11">
         <v>16</v>
       </c>
-      <c r="L11">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E12" t="s">
-        <v>109</v>
-      </c>
-      <c r="F12" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E12">
+        <v>23</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
       </c>
       <c r="G12">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="H12">
-        <v>3</v>
+        <v>1473</v>
       </c>
       <c r="I12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>1473</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -1697,113 +1619,95 @@
         <v>106</v>
       </c>
       <c r="C13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D13" t="s">
-        <v>106</v>
-      </c>
-      <c r="E13" t="s">
-        <v>105</v>
-      </c>
-      <c r="F13" t="s">
-        <v>105</v>
+        <v>105</v>
+      </c>
+      <c r="E13">
+        <v>3561</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
       </c>
       <c r="G13">
-        <v>3561</v>
+        <v>10</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>672</v>
       </c>
       <c r="I13">
-        <v>10</v>
+        <v>666</v>
       </c>
       <c r="J13">
-        <v>672</v>
-      </c>
-      <c r="K13">
-        <v>666</v>
-      </c>
-      <c r="L13">
         <v>1200</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
-      </c>
-      <c r="E14" t="s">
-        <v>109</v>
-      </c>
-      <c r="F14" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E14">
+        <v>1788</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
       </c>
       <c r="G14">
-        <v>1788</v>
+        <v>23</v>
       </c>
       <c r="H14">
-        <v>2</v>
+        <v>8124</v>
       </c>
       <c r="I14">
-        <v>23</v>
+        <v>2480</v>
       </c>
       <c r="J14">
-        <v>8124</v>
-      </c>
-      <c r="K14">
         <v>2480</v>
       </c>
-      <c r="L14">
-        <v>2480</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D15" t="s">
-        <v>109</v>
-      </c>
-      <c r="E15" t="s">
-        <v>109</v>
-      </c>
-      <c r="F15" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E15">
+        <v>28</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
       </c>
       <c r="G15">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="H15">
-        <v>10</v>
+        <v>5620</v>
       </c>
       <c r="I15">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="J15">
-        <v>5620</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1811,1258 +1715,1060 @@
         <v>106</v>
       </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D16" t="s">
-        <v>106</v>
-      </c>
-      <c r="E16" t="s">
-        <v>105</v>
-      </c>
-      <c r="F16" t="s">
-        <v>105</v>
+        <v>105</v>
+      </c>
+      <c r="E16">
+        <v>31</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
       </c>
       <c r="G16">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="H16">
-        <v>2</v>
+        <v>1000</v>
       </c>
       <c r="I16">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="J16">
-        <v>1000</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E17" t="s">
-        <v>109</v>
-      </c>
-      <c r="F17" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E17">
+        <v>32</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
       </c>
       <c r="G17">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="H17">
-        <v>10</v>
+        <v>10992</v>
       </c>
       <c r="I17">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>10992</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D18" t="s">
-        <v>109</v>
-      </c>
-      <c r="E18" t="s">
-        <v>109</v>
-      </c>
-      <c r="F18" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
       </c>
       <c r="G18">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="H18">
-        <v>2</v>
+        <v>3196</v>
       </c>
       <c r="I18">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="J18">
-        <v>3196</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D19" t="s">
         <v>105</v>
       </c>
-      <c r="E19" t="s">
-        <v>105</v>
-      </c>
-      <c r="F19" t="s">
-        <v>105</v>
+      <c r="E19">
+        <v>6</v>
+      </c>
+      <c r="F19">
+        <v>26</v>
       </c>
       <c r="G19">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="H19">
-        <v>26</v>
+        <v>20000</v>
       </c>
       <c r="I19">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="J19">
-        <v>20000</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D20" t="s">
-        <v>109</v>
-      </c>
-      <c r="E20" t="s">
-        <v>109</v>
-      </c>
-      <c r="F20" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20">
+        <v>10</v>
       </c>
       <c r="G20">
-        <v>12</v>
+        <v>217</v>
       </c>
       <c r="H20">
-        <v>10</v>
+        <v>2000</v>
       </c>
       <c r="I20">
-        <v>217</v>
+        <v>0</v>
       </c>
       <c r="J20">
-        <v>2000</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D21" t="s">
-        <v>109</v>
-      </c>
-      <c r="E21" t="s">
-        <v>109</v>
-      </c>
-      <c r="F21" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E21">
+        <v>1778</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
       </c>
       <c r="G21">
-        <v>1778</v>
+        <v>77</v>
       </c>
       <c r="H21">
-        <v>10</v>
+        <v>2000</v>
       </c>
       <c r="I21">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="J21">
-        <v>2000</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D22" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" t="s">
-        <v>109</v>
-      </c>
-      <c r="F22" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E22">
+        <v>16</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
       </c>
       <c r="G22">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="H22">
-        <v>10</v>
+        <v>2000</v>
       </c>
       <c r="I22">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="J22">
-        <v>2000</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D23" t="s">
         <v>105</v>
       </c>
-      <c r="E23" t="s">
-        <v>105</v>
-      </c>
-      <c r="F23" t="s">
-        <v>105</v>
+      <c r="E23">
+        <v>22</v>
+      </c>
+      <c r="F23">
+        <v>10</v>
       </c>
       <c r="G23">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="H23">
-        <v>10</v>
+        <v>2000</v>
       </c>
       <c r="I23">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="J23">
-        <v>2000</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C24" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D24" t="s">
-        <v>109</v>
-      </c>
-      <c r="E24" t="s">
-        <v>109</v>
-      </c>
-      <c r="F24" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E24">
+        <v>36</v>
+      </c>
+      <c r="F24">
+        <v>7</v>
       </c>
       <c r="G24">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="H24">
-        <v>7</v>
+        <v>2310</v>
       </c>
       <c r="I24">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J24">
-        <v>2310</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D25" t="s">
-        <v>109</v>
-      </c>
-      <c r="E25" t="s">
-        <v>109</v>
-      </c>
-      <c r="F25" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E25">
+        <v>43</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
       </c>
       <c r="G25">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="H25">
-        <v>2</v>
+        <v>4601</v>
       </c>
       <c r="I25">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="J25">
-        <v>4601</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D26" t="s">
         <v>105</v>
       </c>
-      <c r="E26" t="s">
-        <v>105</v>
-      </c>
-      <c r="F26" t="s">
-        <v>105</v>
+      <c r="E26">
+        <v>45</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
       </c>
       <c r="G26">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="H26">
-        <v>3</v>
+        <v>3190</v>
       </c>
       <c r="I26">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="J26">
-        <v>3190</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D27" t="s">
-        <v>109</v>
-      </c>
-      <c r="E27" t="s">
-        <v>109</v>
-      </c>
-      <c r="F27" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E27">
+        <v>58</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
       </c>
       <c r="G27">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="H27">
-        <v>3</v>
+        <v>5000</v>
       </c>
       <c r="I27">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="J27">
-        <v>5000</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D28" t="s">
         <v>105</v>
       </c>
-      <c r="E28" t="s">
-        <v>105</v>
-      </c>
-      <c r="F28" t="s">
-        <v>105</v>
+      <c r="E28">
+        <v>219</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
       </c>
       <c r="G28">
-        <v>219</v>
+        <v>9</v>
       </c>
       <c r="H28">
-        <v>2</v>
+        <v>45312</v>
       </c>
       <c r="I28">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J28">
-        <v>45312</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D29" t="s">
         <v>105</v>
       </c>
-      <c r="E29" t="s">
-        <v>105</v>
-      </c>
-      <c r="F29" t="s">
-        <v>105</v>
+      <c r="E29">
+        <v>2074</v>
+      </c>
+      <c r="F29">
+        <v>6</v>
       </c>
       <c r="G29">
-        <v>2074</v>
+        <v>37</v>
       </c>
       <c r="H29">
-        <v>6</v>
+        <v>6430</v>
       </c>
       <c r="I29">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="J29">
-        <v>6430</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D30" t="s">
         <v>105</v>
       </c>
-      <c r="E30" t="s">
-        <v>105</v>
-      </c>
-      <c r="F30" t="s">
-        <v>105</v>
+      <c r="E30">
+        <v>2125</v>
+      </c>
+      <c r="F30">
+        <v>5</v>
       </c>
       <c r="G30">
-        <v>2125</v>
+        <v>20</v>
       </c>
       <c r="H30">
-        <v>5</v>
+        <v>736</v>
       </c>
       <c r="I30">
-        <v>20</v>
+        <v>95</v>
       </c>
       <c r="J30">
-        <v>736</v>
-      </c>
-      <c r="K30">
-        <v>95</v>
-      </c>
-      <c r="L30">
         <v>448</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D31" t="s">
         <v>105</v>
       </c>
-      <c r="E31" t="s">
-        <v>105</v>
-      </c>
-      <c r="F31" t="s">
-        <v>105</v>
+      <c r="E31">
+        <v>3022</v>
+      </c>
+      <c r="F31">
+        <v>11</v>
       </c>
       <c r="G31">
-        <v>3022</v>
+        <v>13</v>
       </c>
       <c r="H31">
-        <v>11</v>
+        <v>990</v>
       </c>
       <c r="I31">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="J31">
-        <v>990</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D32" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" t="s">
-        <v>109</v>
-      </c>
-      <c r="F32" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E32">
+        <v>3485</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
       </c>
       <c r="G32">
-        <v>3485</v>
+        <v>300</v>
       </c>
       <c r="H32">
-        <v>2</v>
+        <v>2407</v>
       </c>
       <c r="I32">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="J32">
-        <v>2407</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D33" t="s">
         <v>105</v>
       </c>
-      <c r="E33" t="s">
-        <v>105</v>
-      </c>
-      <c r="F33" t="s">
-        <v>105</v>
-      </c>
-      <c r="G33" s="2">
+      <c r="E33" s="2">
         <v>3492</v>
       </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <v>7</v>
+      </c>
       <c r="H33">
-        <v>2</v>
+        <v>556</v>
       </c>
       <c r="I33">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J33">
-        <v>556</v>
-      </c>
-      <c r="K33">
-        <v>0</v>
-      </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D34" t="s">
         <v>105</v>
       </c>
-      <c r="E34" t="s">
-        <v>105</v>
-      </c>
-      <c r="F34" t="s">
-        <v>105</v>
+      <c r="E34">
+        <v>3493</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
       </c>
       <c r="G34">
-        <v>3493</v>
+        <v>7</v>
       </c>
       <c r="H34">
-        <v>2</v>
+        <v>601</v>
       </c>
       <c r="I34">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J34">
-        <v>601</v>
-      </c>
-      <c r="K34">
-        <v>0</v>
-      </c>
-      <c r="L34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D35" t="s">
         <v>105</v>
       </c>
-      <c r="E35" t="s">
-        <v>105</v>
-      </c>
-      <c r="F35" t="s">
-        <v>105</v>
+      <c r="E35">
+        <v>3494</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
       </c>
       <c r="G35">
-        <v>3494</v>
+        <v>7</v>
       </c>
       <c r="H35">
-        <v>2</v>
+        <v>554</v>
       </c>
       <c r="I35">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J35">
-        <v>554</v>
-      </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D36" t="s">
-        <v>109</v>
-      </c>
-      <c r="E36" t="s">
-        <v>109</v>
-      </c>
-      <c r="F36" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E36">
+        <v>4544</v>
+      </c>
+      <c r="F36">
+        <v>9</v>
       </c>
       <c r="G36">
-        <v>4544</v>
+        <v>15</v>
       </c>
       <c r="H36">
-        <v>9</v>
+        <v>9961</v>
       </c>
       <c r="I36">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J36">
-        <v>9961</v>
-      </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
-      <c r="L36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D37" t="s">
-        <v>109</v>
-      </c>
-      <c r="E37" t="s">
-        <v>109</v>
-      </c>
-      <c r="F37" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E37">
+        <v>3512</v>
+      </c>
+      <c r="F37">
+        <v>6</v>
       </c>
       <c r="G37">
-        <v>3512</v>
+        <v>62</v>
       </c>
       <c r="H37">
-        <v>6</v>
+        <v>600</v>
       </c>
       <c r="I37">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="J37">
-        <v>600</v>
-      </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
-      <c r="L37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D38" t="s">
-        <v>109</v>
-      </c>
-      <c r="E38" t="s">
-        <v>109</v>
-      </c>
-      <c r="F38" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E38">
+        <v>3543</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
       </c>
       <c r="G38">
-        <v>3543</v>
+        <v>6</v>
       </c>
       <c r="H38">
-        <v>2</v>
+        <v>500</v>
       </c>
       <c r="I38">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="J38">
-        <v>500</v>
-      </c>
-      <c r="K38">
         <v>32</v>
       </c>
-      <c r="L38">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D39" t="s">
         <v>105</v>
       </c>
-      <c r="E39" t="s">
-        <v>105</v>
-      </c>
-      <c r="F39" t="s">
-        <v>105</v>
+      <c r="E39">
+        <v>3549</v>
+      </c>
+      <c r="F39">
+        <v>4</v>
       </c>
       <c r="G39">
-        <v>3549</v>
+        <v>71</v>
       </c>
       <c r="H39">
-        <v>4</v>
+        <v>841</v>
       </c>
       <c r="I39">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="J39">
-        <v>841</v>
-      </c>
-      <c r="K39">
-        <v>0</v>
-      </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D40" t="s">
         <v>105</v>
       </c>
-      <c r="E40" t="s">
-        <v>105</v>
-      </c>
-      <c r="F40" t="s">
-        <v>105</v>
+      <c r="E40">
+        <v>3560</v>
+      </c>
+      <c r="F40">
+        <v>6</v>
       </c>
       <c r="G40">
-        <v>3560</v>
+        <v>5</v>
       </c>
       <c r="H40">
-        <v>6</v>
+        <v>797</v>
       </c>
       <c r="I40">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J40">
-        <v>797</v>
-      </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D41" t="s">
-        <v>109</v>
-      </c>
-      <c r="E41" t="s">
-        <v>109</v>
-      </c>
-      <c r="F41" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E41">
+        <v>3899</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
       </c>
       <c r="G41">
-        <v>3899</v>
+        <v>6</v>
       </c>
       <c r="H41">
-        <v>2</v>
+        <v>15545</v>
       </c>
       <c r="I41">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J41">
-        <v>15545</v>
-      </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D42" t="s">
-        <v>109</v>
-      </c>
-      <c r="E42" t="s">
-        <v>109</v>
-      </c>
-      <c r="F42" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E42">
+        <v>3902</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
       </c>
       <c r="G42">
-        <v>3902</v>
+        <v>38</v>
       </c>
       <c r="H42">
-        <v>2</v>
+        <v>1458</v>
       </c>
       <c r="I42">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="J42">
-        <v>1458</v>
-      </c>
-      <c r="K42">
-        <v>0</v>
-      </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C43" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D43" t="s">
         <v>105</v>
       </c>
-      <c r="E43" t="s">
-        <v>105</v>
-      </c>
-      <c r="F43" t="s">
-        <v>105</v>
+      <c r="E43">
+        <v>3903</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
       </c>
       <c r="G43">
-        <v>3903</v>
+        <v>38</v>
       </c>
       <c r="H43">
-        <v>2</v>
+        <v>1563</v>
       </c>
       <c r="I43">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="J43">
-        <v>1563</v>
-      </c>
-      <c r="K43">
-        <v>0</v>
-      </c>
-      <c r="L43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C44" t="s">
         <v>105</v>
       </c>
       <c r="D44" t="s">
-        <v>109</v>
-      </c>
-      <c r="E44" t="s">
-        <v>109</v>
-      </c>
-      <c r="F44" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E44">
+        <v>3904</v>
+      </c>
+      <c r="F44">
+        <v>2</v>
       </c>
       <c r="G44">
-        <v>3904</v>
+        <v>22</v>
       </c>
       <c r="H44">
-        <v>2</v>
+        <v>10885</v>
       </c>
       <c r="I44">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="J44">
-        <v>10885</v>
-      </c>
-      <c r="K44">
-        <v>5</v>
-      </c>
-      <c r="L44">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C45" t="s">
         <v>105</v>
       </c>
       <c r="D45" t="s">
-        <v>109</v>
-      </c>
-      <c r="E45" t="s">
-        <v>109</v>
-      </c>
-      <c r="F45" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E45">
+        <v>3913</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
       </c>
       <c r="G45">
-        <v>3913</v>
+        <v>22</v>
       </c>
       <c r="H45">
-        <v>2</v>
+        <v>522</v>
       </c>
       <c r="I45">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="J45">
-        <v>522</v>
-      </c>
-      <c r="K45">
-        <v>0</v>
-      </c>
-      <c r="L45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C46" t="s">
         <v>105</v>
       </c>
       <c r="D46" t="s">
-        <v>109</v>
-      </c>
-      <c r="E46" t="s">
-        <v>109</v>
-      </c>
-      <c r="F46" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E46">
+        <v>3917</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
       </c>
       <c r="G46">
-        <v>3917</v>
+        <v>22</v>
       </c>
       <c r="H46">
-        <v>2</v>
+        <v>2109</v>
       </c>
       <c r="I46">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="J46">
-        <v>2109</v>
-      </c>
-      <c r="K46">
-        <v>0</v>
-      </c>
-      <c r="L46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C47" t="s">
         <v>105</v>
       </c>
       <c r="D47" t="s">
-        <v>109</v>
-      </c>
-      <c r="E47" t="s">
-        <v>109</v>
-      </c>
-      <c r="F47" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E47">
+        <v>3918</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
       </c>
       <c r="G47">
-        <v>3918</v>
+        <v>22</v>
       </c>
       <c r="H47">
-        <v>2</v>
+        <v>1109</v>
       </c>
       <c r="I47">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="J47">
-        <v>1109</v>
-      </c>
-      <c r="K47">
-        <v>0</v>
-      </c>
-      <c r="L47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C48" t="s">
         <v>105</v>
       </c>
       <c r="D48" t="s">
-        <v>109</v>
-      </c>
-      <c r="E48" t="s">
-        <v>109</v>
-      </c>
-      <c r="F48" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E48">
+        <v>3954</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
       </c>
       <c r="G48">
-        <v>3954</v>
+        <v>12</v>
       </c>
       <c r="H48">
-        <v>2</v>
+        <v>19020</v>
       </c>
       <c r="I48">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J48">
-        <v>19020</v>
-      </c>
-      <c r="K48">
-        <v>0</v>
-      </c>
-      <c r="L48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C49" t="s">
         <v>105</v>
@@ -3070,151 +2776,127 @@
       <c r="D49" t="s">
         <v>105</v>
       </c>
-      <c r="E49" t="s">
-        <v>105</v>
-      </c>
-      <c r="F49" t="s">
-        <v>105</v>
+      <c r="E49">
+        <v>14964</v>
+      </c>
+      <c r="F49">
+        <v>10</v>
       </c>
       <c r="G49">
-        <v>14964</v>
+        <v>8</v>
       </c>
       <c r="H49">
-        <v>10</v>
+        <v>10218</v>
       </c>
       <c r="I49">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J49">
-        <v>10218</v>
-      </c>
-      <c r="K49">
-        <v>0</v>
-      </c>
-      <c r="L49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C50" t="s">
         <v>105</v>
       </c>
       <c r="D50" t="s">
-        <v>109</v>
-      </c>
-      <c r="E50" t="s">
-        <v>109</v>
-      </c>
-      <c r="F50" t="s">
-        <v>109</v>
-      </c>
-      <c r="G50" s="2">
+        <v>107</v>
+      </c>
+      <c r="E50" s="2">
         <v>10093</v>
       </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <v>5</v>
+      </c>
       <c r="H50">
-        <v>2</v>
+        <v>1372</v>
       </c>
       <c r="I50">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J50">
-        <v>1372</v>
-      </c>
-      <c r="K50">
-        <v>0</v>
-      </c>
-      <c r="L50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C51" t="s">
         <v>105</v>
       </c>
       <c r="D51" t="s">
-        <v>109</v>
-      </c>
-      <c r="E51" t="s">
-        <v>109</v>
-      </c>
-      <c r="F51" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E51">
+        <v>10101</v>
+      </c>
+      <c r="F51">
+        <v>2</v>
       </c>
       <c r="G51">
-        <v>10101</v>
+        <v>5</v>
       </c>
       <c r="H51">
-        <v>2</v>
+        <v>748</v>
       </c>
       <c r="I51">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J51">
-        <v>748</v>
-      </c>
-      <c r="K51">
-        <v>0</v>
-      </c>
-      <c r="L51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C52" t="s">
         <v>105</v>
       </c>
       <c r="D52" t="s">
-        <v>109</v>
-      </c>
-      <c r="E52" t="s">
-        <v>109</v>
-      </c>
-      <c r="F52" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E52">
+        <v>9979</v>
+      </c>
+      <c r="F52">
+        <v>10</v>
       </c>
       <c r="G52">
-        <v>9979</v>
+        <v>36</v>
       </c>
       <c r="H52">
-        <v>10</v>
+        <v>2126</v>
       </c>
       <c r="I52">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="J52">
-        <v>2126</v>
-      </c>
-      <c r="K52">
-        <v>0</v>
-      </c>
-      <c r="L52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C53" t="s">
         <v>105</v>
@@ -3222,75 +2904,63 @@
       <c r="D53" t="s">
         <v>105</v>
       </c>
-      <c r="E53" t="s">
-        <v>105</v>
-      </c>
-      <c r="F53" t="s">
-        <v>105</v>
+      <c r="E53">
+        <v>9980</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
       </c>
       <c r="G53">
-        <v>9980</v>
+        <v>21</v>
       </c>
       <c r="H53">
-        <v>2</v>
+        <v>540</v>
       </c>
       <c r="I53">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="J53">
-        <v>540</v>
-      </c>
-      <c r="K53">
-        <v>0</v>
-      </c>
-      <c r="L53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B54" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C54" t="s">
         <v>105</v>
       </c>
       <c r="D54" t="s">
-        <v>109</v>
-      </c>
-      <c r="E54" t="s">
-        <v>109</v>
-      </c>
-      <c r="F54" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E54">
+        <v>9983</v>
+      </c>
+      <c r="F54">
+        <v>2</v>
       </c>
       <c r="G54">
-        <v>9983</v>
+        <v>15</v>
       </c>
       <c r="H54">
-        <v>2</v>
+        <v>14980</v>
       </c>
       <c r="I54">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="J54">
-        <v>14980</v>
-      </c>
-      <c r="K54">
-        <v>0</v>
-      </c>
-      <c r="L54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C55" t="s">
         <v>105</v>
@@ -3298,493 +2968,415 @@
       <c r="D55" t="s">
         <v>105</v>
       </c>
-      <c r="E55" t="s">
-        <v>105</v>
-      </c>
-      <c r="F55" t="s">
-        <v>105</v>
+      <c r="E55">
+        <v>9985</v>
+      </c>
+      <c r="F55">
+        <v>6</v>
       </c>
       <c r="G55">
-        <v>9985</v>
+        <v>52</v>
       </c>
       <c r="H55">
-        <v>6</v>
+        <v>6118</v>
       </c>
       <c r="I55">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="J55">
-        <v>6118</v>
-      </c>
-      <c r="K55">
-        <v>0</v>
-      </c>
-      <c r="L55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B56" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C56" t="s">
         <v>105</v>
       </c>
       <c r="D56" t="s">
-        <v>109</v>
-      </c>
-      <c r="E56" t="s">
-        <v>109</v>
-      </c>
-      <c r="F56" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E56">
+        <v>9970</v>
+      </c>
+      <c r="F56">
+        <v>2</v>
       </c>
       <c r="G56">
-        <v>9970</v>
+        <v>101</v>
       </c>
       <c r="H56">
-        <v>2</v>
+        <v>1212</v>
       </c>
       <c r="I56">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="J56">
-        <v>1212</v>
-      </c>
-      <c r="K56">
-        <v>0</v>
-      </c>
-      <c r="L56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B57" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C57" t="s">
         <v>105</v>
       </c>
       <c r="D57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E57" t="s">
-        <v>109</v>
-      </c>
-      <c r="F57" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E57">
+        <v>9971</v>
+      </c>
+      <c r="F57">
+        <v>2</v>
       </c>
       <c r="G57">
-        <v>9971</v>
+        <v>11</v>
       </c>
       <c r="H57">
-        <v>2</v>
+        <v>583</v>
       </c>
       <c r="I57">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="J57">
-        <v>583</v>
-      </c>
-      <c r="K57">
-        <v>0</v>
-      </c>
-      <c r="L57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B58" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C58" t="s">
         <v>105</v>
       </c>
       <c r="D58" t="s">
-        <v>109</v>
-      </c>
-      <c r="E58" t="s">
-        <v>109</v>
-      </c>
-      <c r="F58" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E58">
+        <v>9977</v>
+      </c>
+      <c r="F58">
+        <v>2</v>
       </c>
       <c r="G58">
-        <v>9977</v>
+        <v>119</v>
       </c>
       <c r="H58">
-        <v>2</v>
+        <v>34465</v>
       </c>
       <c r="I58">
-        <v>119</v>
+        <v>0</v>
       </c>
       <c r="J58">
-        <v>34465</v>
-      </c>
-      <c r="K58">
-        <v>0</v>
-      </c>
-      <c r="L58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B59" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C59" t="s">
         <v>105</v>
       </c>
       <c r="D59" t="s">
-        <v>109</v>
-      </c>
-      <c r="E59" t="s">
-        <v>109</v>
-      </c>
-      <c r="F59" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E59">
+        <v>9978</v>
+      </c>
+      <c r="F59">
+        <v>2</v>
       </c>
       <c r="G59">
-        <v>9978</v>
+        <v>73</v>
       </c>
       <c r="H59">
-        <v>2</v>
+        <v>2534</v>
       </c>
       <c r="I59">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="J59">
-        <v>2534</v>
-      </c>
-      <c r="K59">
-        <v>0</v>
-      </c>
-      <c r="L59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B60" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C60" t="s">
         <v>105</v>
       </c>
       <c r="D60" t="s">
-        <v>109</v>
-      </c>
-      <c r="E60" t="s">
-        <v>109</v>
-      </c>
-      <c r="F60" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E60">
+        <v>9952</v>
+      </c>
+      <c r="F60">
+        <v>2</v>
       </c>
       <c r="G60">
-        <v>9952</v>
+        <v>6</v>
       </c>
       <c r="H60">
-        <v>2</v>
+        <v>5404</v>
       </c>
       <c r="I60">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J60">
-        <v>5404</v>
-      </c>
-      <c r="K60">
-        <v>0</v>
-      </c>
-      <c r="L60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B61" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C61" t="s">
         <v>105</v>
       </c>
       <c r="D61" t="s">
-        <v>109</v>
-      </c>
-      <c r="E61" t="s">
-        <v>109</v>
-      </c>
-      <c r="F61" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E61">
+        <v>9954</v>
+      </c>
+      <c r="F61">
+        <v>100</v>
       </c>
       <c r="G61">
-        <v>9954</v>
+        <v>65</v>
       </c>
       <c r="H61">
-        <v>100</v>
+        <v>1600</v>
       </c>
       <c r="I61">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="J61">
-        <v>1600</v>
-      </c>
-      <c r="K61">
-        <v>0</v>
-      </c>
-      <c r="L61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C62" t="s">
         <v>105</v>
       </c>
       <c r="D62" t="s">
-        <v>109</v>
-      </c>
-      <c r="E62" t="s">
-        <v>109</v>
-      </c>
-      <c r="F62" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E62">
+        <v>9955</v>
+      </c>
+      <c r="F62">
+        <v>100</v>
       </c>
       <c r="G62">
-        <v>9955</v>
+        <v>65</v>
       </c>
       <c r="H62">
-        <v>100</v>
+        <v>1600</v>
       </c>
       <c r="I62">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="J62">
-        <v>1600</v>
-      </c>
-      <c r="K62">
-        <v>0</v>
-      </c>
-      <c r="L62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B63" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C63" t="s">
         <v>105</v>
       </c>
       <c r="D63" t="s">
-        <v>109</v>
-      </c>
-      <c r="E63" t="s">
-        <v>109</v>
-      </c>
-      <c r="F63" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E63">
+        <v>9957</v>
+      </c>
+      <c r="F63">
+        <v>2</v>
       </c>
       <c r="G63">
-        <v>9957</v>
+        <v>42</v>
       </c>
       <c r="H63">
-        <v>2</v>
+        <v>1055</v>
       </c>
       <c r="I63">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="J63">
-        <v>1055</v>
-      </c>
-      <c r="K63">
-        <v>0</v>
-      </c>
-      <c r="L63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B64" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C64" t="s">
         <v>105</v>
       </c>
       <c r="D64" t="s">
-        <v>109</v>
-      </c>
-      <c r="E64" t="s">
-        <v>109</v>
-      </c>
-      <c r="F64" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E64">
+        <v>9960</v>
+      </c>
+      <c r="F64">
+        <v>4</v>
       </c>
       <c r="G64">
-        <v>9960</v>
+        <v>25</v>
       </c>
       <c r="H64">
-        <v>4</v>
+        <v>5456</v>
       </c>
       <c r="I64">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="J64">
-        <v>5456</v>
-      </c>
-      <c r="K64">
-        <v>0</v>
-      </c>
-      <c r="L64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B65" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C65" t="s">
         <v>105</v>
       </c>
       <c r="D65" t="s">
-        <v>109</v>
-      </c>
-      <c r="E65" t="s">
-        <v>109</v>
-      </c>
-      <c r="F65" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E65">
+        <v>9967</v>
+      </c>
+      <c r="F65">
+        <v>2</v>
       </c>
       <c r="G65">
-        <v>9967</v>
+        <v>34</v>
       </c>
       <c r="H65">
-        <v>2</v>
+        <v>1941</v>
       </c>
       <c r="I65">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="J65">
-        <v>1941</v>
-      </c>
-      <c r="K65">
-        <v>0</v>
-      </c>
-      <c r="L65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B66" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C66" t="s">
         <v>105</v>
       </c>
       <c r="D66" t="s">
-        <v>109</v>
-      </c>
-      <c r="E66" t="s">
-        <v>109</v>
-      </c>
-      <c r="F66" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E66">
+        <v>9946</v>
+      </c>
+      <c r="F66">
+        <v>2</v>
       </c>
       <c r="G66">
-        <v>9946</v>
+        <v>31</v>
       </c>
       <c r="H66">
-        <v>2</v>
+        <v>569</v>
       </c>
       <c r="I66">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="J66">
-        <v>569</v>
-      </c>
-      <c r="K66">
-        <v>0</v>
-      </c>
-      <c r="L66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B67" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C67" t="s">
         <v>105</v>
       </c>
       <c r="D67" t="s">
-        <v>109</v>
-      </c>
-      <c r="E67" t="s">
-        <v>109</v>
-      </c>
-      <c r="F67" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E67">
+        <v>7592</v>
+      </c>
+      <c r="F67">
+        <v>2</v>
       </c>
       <c r="G67">
-        <v>7592</v>
+        <v>15</v>
       </c>
       <c r="H67">
-        <v>2</v>
+        <v>48842</v>
       </c>
       <c r="I67">
-        <v>15</v>
+        <v>3620</v>
       </c>
       <c r="J67">
-        <v>48842</v>
-      </c>
-      <c r="K67">
-        <v>3620</v>
-      </c>
-      <c r="L67">
         <v>6465</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B68" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C68" t="s">
         <v>105</v>
@@ -3792,37 +3384,31 @@
       <c r="D68" t="s">
         <v>105</v>
       </c>
-      <c r="E68" t="s">
-        <v>105</v>
-      </c>
-      <c r="F68" t="s">
-        <v>105</v>
+      <c r="E68">
+        <v>14969</v>
+      </c>
+      <c r="F68">
+        <v>5</v>
       </c>
       <c r="G68">
-        <v>14969</v>
+        <v>33</v>
       </c>
       <c r="H68">
-        <v>5</v>
+        <v>9873</v>
       </c>
       <c r="I68">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="J68">
-        <v>9873</v>
-      </c>
-      <c r="K68">
-        <v>0</v>
-      </c>
-      <c r="L68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B69" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C69" t="s">
         <v>105</v>
@@ -3830,75 +3416,63 @@
       <c r="D69" t="s">
         <v>105</v>
       </c>
-      <c r="E69" t="s">
-        <v>105</v>
-      </c>
-      <c r="F69" t="s">
-        <v>105</v>
+      <c r="E69">
+        <v>14968</v>
+      </c>
+      <c r="F69">
+        <v>2</v>
       </c>
       <c r="G69">
-        <v>14968</v>
+        <v>40</v>
       </c>
       <c r="H69">
-        <v>2</v>
+        <v>540</v>
       </c>
       <c r="I69">
-        <v>40</v>
+        <v>263</v>
       </c>
       <c r="J69">
-        <v>540</v>
-      </c>
-      <c r="K69">
-        <v>263</v>
-      </c>
-      <c r="L69">
         <v>999</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C70" t="s">
         <v>105</v>
       </c>
       <c r="D70" t="s">
-        <v>109</v>
-      </c>
-      <c r="E70" t="s">
-        <v>109</v>
-      </c>
-      <c r="F70" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E70">
+        <v>14967</v>
+      </c>
+      <c r="F70">
+        <v>6</v>
       </c>
       <c r="G70">
-        <v>14967</v>
+        <v>35</v>
       </c>
       <c r="H70">
-        <v>6</v>
+        <v>2796</v>
       </c>
       <c r="I70">
-        <v>35</v>
+        <v>2795</v>
       </c>
       <c r="J70">
-        <v>2796</v>
-      </c>
-      <c r="K70">
-        <v>2795</v>
-      </c>
-      <c r="L70">
         <v>68100</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B71" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C71" t="s">
         <v>105</v>
@@ -3906,298 +3480,250 @@
       <c r="D71" t="s">
         <v>105</v>
       </c>
-      <c r="E71" t="s">
-        <v>105</v>
-      </c>
-      <c r="F71" t="s">
-        <v>105</v>
+      <c r="E71">
+        <v>125920</v>
+      </c>
+      <c r="F71">
+        <v>2</v>
       </c>
       <c r="G71">
-        <v>125920</v>
+        <v>13</v>
       </c>
       <c r="H71">
-        <v>2</v>
+        <v>500</v>
       </c>
       <c r="I71">
-        <v>13</v>
+        <v>401</v>
       </c>
       <c r="J71">
-        <v>500</v>
-      </c>
-      <c r="K71">
-        <v>401</v>
-      </c>
-      <c r="L71">
         <v>835</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B72" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C72" t="s">
         <v>105</v>
       </c>
       <c r="D72" t="s">
-        <v>109</v>
-      </c>
-      <c r="E72" t="s">
-        <v>109</v>
-      </c>
-      <c r="F72" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E72">
+        <v>125921</v>
+      </c>
+      <c r="F72">
+        <v>10</v>
       </c>
       <c r="G72">
-        <v>125921</v>
+        <v>8</v>
       </c>
       <c r="H72">
-        <v>10</v>
+        <v>500</v>
       </c>
       <c r="I72">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="J72">
-        <v>500</v>
-      </c>
-      <c r="K72">
-        <v>0</v>
-      </c>
-      <c r="L72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B73" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C73" t="s">
         <v>105</v>
       </c>
       <c r="D73" t="s">
-        <v>109</v>
-      </c>
-      <c r="E73" t="s">
-        <v>109</v>
-      </c>
-      <c r="F73" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E73">
+        <v>125922</v>
+      </c>
+      <c r="F73">
+        <v>11</v>
       </c>
       <c r="G73">
-        <v>125922</v>
+        <v>41</v>
       </c>
       <c r="H73">
-        <v>11</v>
+        <v>5500</v>
       </c>
       <c r="I73">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="J73">
-        <v>5500</v>
-      </c>
-      <c r="K73">
-        <v>0</v>
-      </c>
-      <c r="L73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B74" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C74" t="s">
         <v>105</v>
       </c>
       <c r="D74" t="s">
-        <v>109</v>
-      </c>
-      <c r="E74" t="s">
-        <v>109</v>
-      </c>
-      <c r="F74" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E74">
+        <v>146607</v>
+      </c>
+      <c r="F74">
+        <v>2</v>
       </c>
       <c r="G74">
-        <v>146607</v>
+        <v>123</v>
       </c>
       <c r="H74">
-        <v>2</v>
+        <v>8378</v>
       </c>
       <c r="I74">
-        <v>123</v>
+        <v>7330</v>
       </c>
       <c r="J74">
-        <v>8378</v>
-      </c>
-      <c r="K74">
-        <v>7330</v>
-      </c>
-      <c r="L74">
         <v>18372</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B75" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C75" t="s">
         <v>105</v>
       </c>
       <c r="D75" t="s">
-        <v>109</v>
-      </c>
-      <c r="E75" t="s">
-        <v>109</v>
-      </c>
-      <c r="F75" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E75">
+        <v>9986</v>
+      </c>
+      <c r="F75">
+        <v>6</v>
       </c>
       <c r="G75">
-        <v>9986</v>
+        <v>129</v>
       </c>
       <c r="H75">
-        <v>6</v>
+        <v>13910</v>
       </c>
       <c r="I75">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="J75">
-        <v>13910</v>
-      </c>
-      <c r="K75">
-        <v>0</v>
-      </c>
-      <c r="L75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B76" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C76" t="s">
         <v>105</v>
       </c>
       <c r="D76" t="s">
-        <v>109</v>
-      </c>
-      <c r="E76" t="s">
-        <v>109</v>
-      </c>
-      <c r="F76" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E76">
+        <v>14965</v>
+      </c>
+      <c r="F76">
+        <v>2</v>
       </c>
       <c r="G76">
-        <v>14965</v>
+        <v>17</v>
       </c>
       <c r="H76">
-        <v>2</v>
+        <v>45211</v>
       </c>
       <c r="I76">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="J76">
-        <v>45211</v>
-      </c>
-      <c r="K76">
-        <v>0</v>
-      </c>
-      <c r="L76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B77" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C77" t="s">
         <v>105</v>
       </c>
       <c r="D77" t="s">
-        <v>109</v>
-      </c>
-      <c r="E77" t="s">
-        <v>109</v>
-      </c>
-      <c r="F77" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E77">
+        <v>9956</v>
+      </c>
+      <c r="F77">
+        <v>100</v>
       </c>
       <c r="G77">
-        <v>9956</v>
+        <v>65</v>
       </c>
       <c r="H77">
-        <v>100</v>
+        <v>1599</v>
       </c>
       <c r="I77">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="J77">
-        <v>1599</v>
-      </c>
-      <c r="K77">
-        <v>0</v>
-      </c>
-      <c r="L77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B78" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C78" t="s">
         <v>105</v>
       </c>
       <c r="D78" t="s">
-        <v>109</v>
-      </c>
-      <c r="E78" t="s">
-        <v>109</v>
-      </c>
-      <c r="F78" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E78">
+        <v>34537</v>
+      </c>
+      <c r="F78">
+        <v>2</v>
       </c>
       <c r="G78">
-        <v>34537</v>
+        <v>31</v>
       </c>
       <c r="H78">
-        <v>2</v>
+        <v>11055</v>
       </c>
       <c r="I78">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="J78">
-        <v>11055</v>
-      </c>
-      <c r="K78">
-        <v>0</v>
-      </c>
-      <c r="L78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>90</v>
       </c>
@@ -4210,32 +3736,26 @@
       <c r="D79" t="s">
         <v>105</v>
       </c>
-      <c r="E79" t="s">
-        <v>105</v>
-      </c>
-      <c r="F79" t="s">
-        <v>105</v>
+      <c r="E79">
+        <v>146195</v>
+      </c>
+      <c r="F79">
+        <v>3</v>
       </c>
       <c r="G79">
-        <v>146195</v>
+        <v>43</v>
       </c>
       <c r="H79">
-        <v>3</v>
+        <v>67557</v>
       </c>
       <c r="I79">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="J79">
-        <v>67557</v>
-      </c>
-      <c r="K79">
-        <v>0</v>
-      </c>
-      <c r="L79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>80</v>
       </c>
@@ -4248,32 +3768,26 @@
       <c r="D80" t="s">
         <v>105</v>
       </c>
-      <c r="E80" t="s">
-        <v>105</v>
-      </c>
-      <c r="F80" t="s">
-        <v>105</v>
+      <c r="E80">
+        <v>34539</v>
+      </c>
+      <c r="F80">
+        <v>2</v>
       </c>
       <c r="G80">
-        <v>34539</v>
+        <v>10</v>
       </c>
       <c r="H80">
-        <v>2</v>
+        <v>32769</v>
       </c>
       <c r="I80">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J80">
-        <v>32769</v>
-      </c>
-      <c r="K80">
-        <v>0</v>
-      </c>
-      <c r="L80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>62</v>
       </c>
@@ -4286,32 +3800,26 @@
       <c r="D81" t="s">
         <v>105</v>
       </c>
-      <c r="E81" t="s">
-        <v>105</v>
-      </c>
-      <c r="F81" t="s">
-        <v>105</v>
+      <c r="E81">
+        <v>14970</v>
+      </c>
+      <c r="F81">
+        <v>6</v>
       </c>
       <c r="G81">
-        <v>14970</v>
+        <v>562</v>
       </c>
       <c r="H81">
-        <v>6</v>
+        <v>10299</v>
       </c>
       <c r="I81">
-        <v>562</v>
+        <v>0</v>
       </c>
       <c r="J81">
-        <v>10299</v>
-      </c>
-      <c r="K81">
-        <v>0</v>
-      </c>
-      <c r="L81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>79</v>
       </c>
@@ -4324,32 +3832,26 @@
       <c r="D82" t="s">
         <v>105</v>
       </c>
-      <c r="E82" t="s">
-        <v>105</v>
-      </c>
-      <c r="F82" t="s">
-        <v>105</v>
+      <c r="E82">
+        <v>14966</v>
+      </c>
+      <c r="F82">
+        <v>2</v>
       </c>
       <c r="G82">
-        <v>14966</v>
+        <v>1777</v>
       </c>
       <c r="H82">
-        <v>2</v>
+        <v>3751</v>
       </c>
       <c r="I82">
-        <v>1777</v>
+        <v>0</v>
       </c>
       <c r="J82">
-        <v>3751</v>
-      </c>
-      <c r="K82">
-        <v>0</v>
-      </c>
-      <c r="L82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>86</v>
       </c>
@@ -4362,32 +3864,26 @@
       <c r="D83" t="s">
         <v>105</v>
       </c>
-      <c r="E83" t="s">
-        <v>105</v>
-      </c>
-      <c r="F83" t="s">
-        <v>105</v>
+      <c r="E83">
+        <v>146606</v>
+      </c>
+      <c r="F83">
+        <v>2</v>
       </c>
       <c r="G83">
-        <v>146606</v>
+        <v>29</v>
       </c>
       <c r="H83">
-        <v>2</v>
+        <v>98050</v>
       </c>
       <c r="I83">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="J83">
-        <v>98050</v>
-      </c>
-      <c r="K83">
-        <v>1</v>
-      </c>
-      <c r="L83">
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>40</v>
       </c>
@@ -4400,32 +3896,26 @@
       <c r="D84" t="s">
         <v>105</v>
       </c>
-      <c r="E84" t="s">
-        <v>105</v>
-      </c>
-      <c r="F84" t="s">
-        <v>105</v>
+      <c r="E84">
+        <v>3573</v>
+      </c>
+      <c r="F84">
+        <v>10</v>
       </c>
       <c r="G84">
-        <v>3573</v>
+        <v>785</v>
       </c>
       <c r="H84">
-        <v>10</v>
+        <v>70000</v>
       </c>
       <c r="I84">
-        <v>785</v>
+        <v>0</v>
       </c>
       <c r="J84">
-        <v>70000</v>
-      </c>
-      <c r="K84">
-        <v>0</v>
-      </c>
-      <c r="L84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>41</v>
       </c>
@@ -4438,32 +3928,26 @@
       <c r="D85" t="s">
         <v>105</v>
       </c>
-      <c r="E85" t="s">
-        <v>105</v>
-      </c>
-      <c r="F85" t="s">
-        <v>105</v>
+      <c r="E85">
+        <v>3891</v>
+      </c>
+      <c r="F85">
+        <v>2</v>
       </c>
       <c r="G85">
-        <v>3891</v>
+        <v>971</v>
       </c>
       <c r="H85">
-        <v>2</v>
+        <v>3468</v>
       </c>
       <c r="I85">
-        <v>971</v>
+        <v>0</v>
       </c>
       <c r="J85">
-        <v>3468</v>
-      </c>
-      <c r="K85">
-        <v>0</v>
-      </c>
-      <c r="L85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -4476,32 +3960,26 @@
       <c r="D86" t="s">
         <v>105</v>
       </c>
-      <c r="E86" t="s">
-        <v>105</v>
-      </c>
-      <c r="F86" t="s">
-        <v>105</v>
+      <c r="E86">
+        <v>3481</v>
+      </c>
+      <c r="F86">
+        <v>26</v>
       </c>
       <c r="G86">
-        <v>3481</v>
+        <v>618</v>
       </c>
       <c r="H86">
-        <v>26</v>
+        <v>7797</v>
       </c>
       <c r="I86">
-        <v>618</v>
+        <v>0</v>
       </c>
       <c r="J86">
-        <v>7797</v>
-      </c>
-      <c r="K86">
-        <v>0</v>
-      </c>
-      <c r="L86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>58</v>
       </c>
@@ -4514,32 +3992,26 @@
       <c r="D87" t="s">
         <v>105</v>
       </c>
-      <c r="E87" t="s">
-        <v>105</v>
-      </c>
-      <c r="F87" t="s">
-        <v>105</v>
+      <c r="E87">
+        <v>9981</v>
+      </c>
+      <c r="F87">
+        <v>9</v>
       </c>
       <c r="G87">
-        <v>9981</v>
+        <v>857</v>
       </c>
       <c r="H87">
-        <v>9</v>
+        <v>1080</v>
       </c>
       <c r="I87">
-        <v>857</v>
+        <v>0</v>
       </c>
       <c r="J87">
-        <v>1080</v>
-      </c>
-      <c r="K87">
-        <v>0</v>
-      </c>
-      <c r="L87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>74</v>
       </c>
@@ -4552,32 +4024,26 @@
       <c r="D88" t="s">
         <v>105</v>
       </c>
-      <c r="E88" t="s">
-        <v>105</v>
-      </c>
-      <c r="F88" t="s">
-        <v>105</v>
+      <c r="E88">
+        <v>9964</v>
+      </c>
+      <c r="F88">
+        <v>10</v>
       </c>
       <c r="G88">
-        <v>9964</v>
+        <v>257</v>
       </c>
       <c r="H88">
-        <v>10</v>
+        <v>1593</v>
       </c>
       <c r="I88">
-        <v>257</v>
+        <v>0</v>
       </c>
       <c r="J88">
-        <v>1593</v>
-      </c>
-      <c r="K88">
-        <v>0</v>
-      </c>
-      <c r="L88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>77</v>
       </c>
@@ -4590,32 +4056,26 @@
       <c r="D89" t="s">
         <v>105</v>
       </c>
-      <c r="E89" t="s">
-        <v>105</v>
-      </c>
-      <c r="F89" t="s">
-        <v>105</v>
+      <c r="E89">
+        <v>9950</v>
+      </c>
+      <c r="F89">
+        <v>20</v>
       </c>
       <c r="G89">
-        <v>9950</v>
+        <v>1301</v>
       </c>
       <c r="H89">
-        <v>20</v>
+        <v>571</v>
       </c>
       <c r="I89">
-        <v>1301</v>
+        <v>0</v>
       </c>
       <c r="J89">
-        <v>571</v>
-      </c>
-      <c r="K89">
-        <v>0</v>
-      </c>
-      <c r="L89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>65</v>
       </c>
@@ -4628,32 +4088,26 @@
       <c r="D90" t="s">
         <v>105</v>
       </c>
-      <c r="E90" t="s">
-        <v>105</v>
-      </c>
-      <c r="F90" t="s">
-        <v>105</v>
+      <c r="E90">
+        <v>9976</v>
+      </c>
+      <c r="F90">
+        <v>2</v>
       </c>
       <c r="G90">
-        <v>9976</v>
+        <v>501</v>
       </c>
       <c r="H90">
-        <v>2</v>
+        <v>2600</v>
       </c>
       <c r="I90">
-        <v>501</v>
+        <v>0</v>
       </c>
       <c r="J90">
-        <v>2600</v>
-      </c>
-      <c r="K90">
-        <v>0</v>
-      </c>
-      <c r="L90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>8</v>
       </c>
@@ -4666,32 +4120,26 @@
       <c r="D91" t="s">
         <v>105</v>
       </c>
-      <c r="E91" t="s">
-        <v>105</v>
-      </c>
-      <c r="F91" t="s">
-        <v>105</v>
+      <c r="E91">
+        <v>20</v>
+      </c>
+      <c r="F91">
+        <v>10</v>
       </c>
       <c r="G91">
-        <v>20</v>
+        <v>241</v>
       </c>
       <c r="H91">
-        <v>10</v>
+        <v>2000</v>
       </c>
       <c r="I91">
-        <v>241</v>
+        <v>0</v>
       </c>
       <c r="J91">
-        <v>2000</v>
-      </c>
-      <c r="K91">
-        <v>0</v>
-      </c>
-      <c r="L91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>49</v>
       </c>
@@ -4704,32 +4152,26 @@
       <c r="D92" t="s">
         <v>105</v>
       </c>
-      <c r="E92" t="s">
-        <v>105</v>
-      </c>
-      <c r="F92" t="s">
-        <v>105</v>
+      <c r="E92">
+        <v>3946</v>
+      </c>
+      <c r="F92">
+        <v>2</v>
       </c>
       <c r="G92">
-        <v>3946</v>
+        <v>231</v>
       </c>
       <c r="H92">
-        <v>2</v>
+        <v>50000</v>
       </c>
       <c r="I92">
-        <v>231</v>
+        <v>50000</v>
       </c>
       <c r="J92">
-        <v>50000</v>
-      </c>
-      <c r="K92">
-        <v>50000</v>
-      </c>
-      <c r="L92">
         <v>8024152</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>50</v>
       </c>
@@ -4742,28 +4184,22 @@
       <c r="D93" t="s">
         <v>105</v>
       </c>
-      <c r="E93" t="s">
-        <v>105</v>
-      </c>
-      <c r="F93" t="s">
-        <v>105</v>
-      </c>
-      <c r="G93" s="2">
+      <c r="E93" s="2">
         <v>3948</v>
       </c>
+      <c r="F93">
+        <v>2</v>
+      </c>
+      <c r="G93">
+        <v>231</v>
+      </c>
       <c r="H93">
-        <v>2</v>
+        <v>50000</v>
       </c>
       <c r="I93">
-        <v>231</v>
+        <v>50000</v>
       </c>
       <c r="J93">
-        <v>50000</v>
-      </c>
-      <c r="K93">
-        <v>50000</v>
-      </c>
-      <c r="L93">
         <v>8024152</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PP2 - Introduce Classification Ensemble hyper learner
</commit_message>
<xml_diff>
--- a/benchmark/Configuration.xlsx
+++ b/benchmark/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\autem\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6A1FEF-6DD4-4FF4-9060-7C1101E7EC16}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A28650-F7B7-45FF-834D-2136EB568607}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="117">
   <si>
     <t>kr-vs-kp</t>
   </si>
@@ -358,7 +358,28 @@
     <t>wide</t>
   </si>
   <si>
-    <t>SN1</t>
+    <t>boom</t>
+  </si>
+  <si>
+    <t>PP2</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>progressing</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>unattempted</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>ensemble_snapshot</t>
   </si>
 </sst>
 </file>
@@ -1203,28 +1224,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I93"/>
+  <dimension ref="A1:J93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="37" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>98</v>
       </c>
@@ -1232,28 +1254,31 @@
         <v>106</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1261,28 +1286,28 @@
         <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2">
+        <v>115</v>
+      </c>
+      <c r="E2">
         <v>37</v>
       </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
       <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
         <v>9</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>768</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
       <c r="I2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -1290,28 +1315,28 @@
         <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3">
+        <v>115</v>
+      </c>
+      <c r="E3">
         <v>53</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>4</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>19</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>846</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
       <c r="I3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>91</v>
       </c>
@@ -1319,28 +1344,28 @@
         <v>107</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4">
+        <v>112</v>
+      </c>
+      <c r="E4">
         <v>125923</v>
       </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
       <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
         <v>15</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>690</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
       <c r="I4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1348,28 +1373,28 @@
         <v>107</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5">
+        <v>115</v>
+      </c>
+      <c r="E5">
         <v>145804</v>
       </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
       <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
         <v>10</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>958</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
       <c r="I5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1377,28 +1402,28 @@
         <v>107</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D6">
+        <v>115</v>
+      </c>
+      <c r="E6">
         <v>18</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>10</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>7</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>2000</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
       <c r="I6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1406,28 +1431,28 @@
         <v>107</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D7">
+        <v>112</v>
+      </c>
+      <c r="E7">
         <v>11</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>3</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>5</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>625</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
       <c r="I7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1435,28 +1460,28 @@
         <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D8">
+        <v>115</v>
+      </c>
+      <c r="E8">
         <v>3021</v>
       </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
       <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
         <v>30</v>
-      </c>
-      <c r="G8">
-        <v>3772</v>
       </c>
       <c r="H8">
         <v>3772</v>
       </c>
       <c r="I8">
+        <v>3772</v>
+      </c>
+      <c r="J8">
         <v>6064</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1464,28 +1489,28 @@
         <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
-      </c>
-      <c r="D9">
+        <v>112</v>
+      </c>
+      <c r="E9">
         <v>29</v>
       </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
       <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
         <v>16</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>690</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>37</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1493,28 +1518,28 @@
         <v>107</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
-      </c>
-      <c r="D10">
+        <v>115</v>
+      </c>
+      <c r="E10">
         <v>41</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>19</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>36</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>683</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>121</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>2337</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -1522,28 +1547,28 @@
         <v>107</v>
       </c>
       <c r="C11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D11">
+        <v>115</v>
+      </c>
+      <c r="E11">
         <v>1779</v>
       </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
       <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
         <v>10</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>699</v>
-      </c>
-      <c r="H11">
-        <v>16</v>
       </c>
       <c r="I11">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1551,28 +1576,28 @@
         <v>107</v>
       </c>
       <c r="C12" t="s">
-        <v>105</v>
-      </c>
-      <c r="D12">
+        <v>115</v>
+      </c>
+      <c r="E12">
         <v>23</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>3</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>10</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>1473</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
       <c r="I12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -1580,28 +1605,28 @@
         <v>107</v>
       </c>
       <c r="C13" t="s">
-        <v>105</v>
-      </c>
-      <c r="D13">
+        <v>115</v>
+      </c>
+      <c r="E13">
         <v>3561</v>
       </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
       <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
         <v>10</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>672</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>666</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>1200</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1609,28 +1634,28 @@
         <v>107</v>
       </c>
       <c r="C14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D14">
+        <v>115</v>
+      </c>
+      <c r="E14">
         <v>1788</v>
       </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
       <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
         <v>23</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>8124</v>
-      </c>
-      <c r="H14">
-        <v>2480</v>
       </c>
       <c r="I14">
         <v>2480</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1638,28 +1663,28 @@
         <v>107</v>
       </c>
       <c r="C15" t="s">
-        <v>105</v>
-      </c>
-      <c r="D15">
+        <v>115</v>
+      </c>
+      <c r="E15">
         <v>28</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>10</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>65</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>5620</v>
       </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
       <c r="I15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1667,28 +1692,28 @@
         <v>107</v>
       </c>
       <c r="C16" t="s">
-        <v>105</v>
-      </c>
-      <c r="D16">
+        <v>112</v>
+      </c>
+      <c r="E16">
         <v>31</v>
       </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
       <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
         <v>21</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>1000</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
       <c r="I16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1696,28 +1721,28 @@
         <v>107</v>
       </c>
       <c r="C17" t="s">
-        <v>105</v>
-      </c>
-      <c r="D17">
+        <v>115</v>
+      </c>
+      <c r="E17">
         <v>32</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>10</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>17</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>10992</v>
       </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
       <c r="I17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -1725,28 +1750,28 @@
         <v>107</v>
       </c>
       <c r="C18" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18">
+        <v>115</v>
+      </c>
+      <c r="E18">
         <v>3</v>
       </c>
-      <c r="E18">
-        <v>2</v>
-      </c>
       <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
         <v>37</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>3196</v>
       </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
       <c r="I18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -1754,28 +1779,28 @@
         <v>107</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
-      </c>
-      <c r="D19">
+        <v>115</v>
+      </c>
+      <c r="E19">
         <v>6</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>26</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>17</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>20000</v>
       </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
       <c r="I19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
@@ -1783,28 +1808,28 @@
         <v>107</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
-      </c>
-      <c r="D20">
+        <v>112</v>
+      </c>
+      <c r="E20">
         <v>12</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>10</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>217</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>2000</v>
       </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
       <c r="I20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
@@ -1812,28 +1837,28 @@
         <v>107</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21">
+        <v>115</v>
+      </c>
+      <c r="E21">
         <v>1778</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>10</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>77</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>2000</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
       <c r="I21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
@@ -1841,28 +1866,28 @@
         <v>107</v>
       </c>
       <c r="C22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D22">
+        <v>115</v>
+      </c>
+      <c r="E22">
         <v>16</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>10</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>65</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>2000</v>
       </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
       <c r="I22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -1870,28 +1895,28 @@
         <v>107</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
-      </c>
-      <c r="D23">
+        <v>115</v>
+      </c>
+      <c r="E23">
         <v>22</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>10</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>48</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>2000</v>
       </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
       <c r="I23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
@@ -1899,28 +1924,28 @@
         <v>107</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
-      </c>
-      <c r="D24">
+        <v>115</v>
+      </c>
+      <c r="E24">
         <v>36</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>7</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>20</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>2310</v>
       </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
       <c r="I24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
@@ -1928,28 +1953,28 @@
         <v>107</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
-      </c>
-      <c r="D25">
+        <v>115</v>
+      </c>
+      <c r="E25">
         <v>43</v>
       </c>
-      <c r="E25">
-        <v>2</v>
-      </c>
       <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
         <v>58</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>4601</v>
       </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
       <c r="I25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
@@ -1957,28 +1982,28 @@
         <v>107</v>
       </c>
       <c r="C26" t="s">
-        <v>105</v>
-      </c>
-      <c r="D26">
+        <v>115</v>
+      </c>
+      <c r="E26">
         <v>45</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>3</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>62</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>3190</v>
       </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
       <c r="I26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
@@ -1986,28 +2011,28 @@
         <v>107</v>
       </c>
       <c r="C27" t="s">
-        <v>105</v>
-      </c>
-      <c r="D27">
+        <v>115</v>
+      </c>
+      <c r="E27">
         <v>58</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>3</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>41</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>5000</v>
       </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
       <c r="I27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
@@ -2015,28 +2040,28 @@
         <v>107</v>
       </c>
       <c r="C28" t="s">
-        <v>105</v>
-      </c>
-      <c r="D28">
+        <v>112</v>
+      </c>
+      <c r="E28">
         <v>219</v>
       </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
       <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28">
         <v>9</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>45312</v>
       </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
       <c r="I28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
@@ -2044,28 +2069,28 @@
         <v>107</v>
       </c>
       <c r="C29" t="s">
-        <v>105</v>
-      </c>
-      <c r="D29">
+        <v>115</v>
+      </c>
+      <c r="E29">
         <v>2074</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>6</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>37</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>6430</v>
       </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
       <c r="I29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>27</v>
       </c>
@@ -2073,28 +2098,28 @@
         <v>107</v>
       </c>
       <c r="C30" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30">
+        <v>112</v>
+      </c>
+      <c r="E30">
         <v>2125</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>5</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>20</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>736</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>95</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>448</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
@@ -2102,28 +2127,28 @@
         <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>105</v>
-      </c>
-      <c r="D31">
+        <v>112</v>
+      </c>
+      <c r="E31">
         <v>3022</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>11</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>13</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>990</v>
       </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
       <c r="I31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -2131,28 +2156,28 @@
         <v>107</v>
       </c>
       <c r="C32" t="s">
-        <v>105</v>
-      </c>
-      <c r="D32">
+        <v>115</v>
+      </c>
+      <c r="E32">
         <v>3485</v>
       </c>
-      <c r="E32">
-        <v>2</v>
-      </c>
       <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
         <v>300</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>2407</v>
       </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
       <c r="I32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
@@ -2160,57 +2185,60 @@
         <v>107</v>
       </c>
       <c r="C33" t="s">
+        <v>112</v>
+      </c>
+      <c r="E33" s="2">
+        <v>3492</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <v>7</v>
+      </c>
+      <c r="H33">
+        <v>556</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" t="s">
         <v>105</v>
       </c>
-      <c r="D33" s="2">
-        <v>3492</v>
-      </c>
-      <c r="E33">
-        <v>2</v>
-      </c>
-      <c r="F33">
+      <c r="E34">
+        <v>3493</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34">
         <v>7</v>
       </c>
-      <c r="G33">
-        <v>556</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
-        <v>107</v>
-      </c>
-      <c r="C34" t="s">
-        <v>105</v>
-      </c>
-      <c r="D34">
-        <v>3493</v>
-      </c>
-      <c r="E34">
-        <v>2</v>
-      </c>
-      <c r="F34">
-        <v>7</v>
-      </c>
-      <c r="G34">
+      <c r="H34">
         <v>601</v>
       </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
       <c r="I34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -2218,28 +2246,28 @@
         <v>107</v>
       </c>
       <c r="C35" t="s">
-        <v>105</v>
-      </c>
-      <c r="D35">
+        <v>115</v>
+      </c>
+      <c r="E35">
         <v>3494</v>
       </c>
-      <c r="E35">
-        <v>2</v>
-      </c>
       <c r="F35">
+        <v>2</v>
+      </c>
+      <c r="G35">
         <v>7</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>554</v>
       </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
       <c r="I35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -2247,28 +2275,28 @@
         <v>107</v>
       </c>
       <c r="C36" t="s">
-        <v>105</v>
-      </c>
-      <c r="D36">
+        <v>115</v>
+      </c>
+      <c r="E36">
         <v>4544</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>9</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>15</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>9961</v>
       </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
       <c r="I36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -2276,28 +2304,28 @@
         <v>107</v>
       </c>
       <c r="C37" t="s">
-        <v>105</v>
-      </c>
-      <c r="D37">
+        <v>115</v>
+      </c>
+      <c r="E37">
         <v>3512</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>6</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>62</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>600</v>
       </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
       <c r="I37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
@@ -2305,28 +2333,28 @@
         <v>107</v>
       </c>
       <c r="C38" t="s">
-        <v>105</v>
-      </c>
-      <c r="D38">
+        <v>115</v>
+      </c>
+      <c r="E38">
         <v>3543</v>
       </c>
-      <c r="E38">
-        <v>2</v>
-      </c>
       <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38">
         <v>6</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>500</v>
-      </c>
-      <c r="H38">
-        <v>32</v>
       </c>
       <c r="I38">
         <v>32</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
@@ -2334,28 +2362,28 @@
         <v>107</v>
       </c>
       <c r="C39" t="s">
-        <v>105</v>
-      </c>
-      <c r="D39">
+        <v>115</v>
+      </c>
+      <c r="E39">
         <v>3549</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>4</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>71</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>841</v>
       </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
       <c r="I39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
@@ -2363,28 +2391,28 @@
         <v>107</v>
       </c>
       <c r="C40" t="s">
-        <v>105</v>
-      </c>
-      <c r="D40">
+        <v>115</v>
+      </c>
+      <c r="E40">
         <v>3560</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>6</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>5</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>797</v>
       </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
       <c r="I40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>42</v>
       </c>
@@ -2392,28 +2420,28 @@
         <v>107</v>
       </c>
       <c r="C41" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41">
+        <v>115</v>
+      </c>
+      <c r="E41">
         <v>3899</v>
       </c>
-      <c r="E41">
-        <v>2</v>
-      </c>
       <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41">
         <v>6</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>15545</v>
       </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
       <c r="I41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>43</v>
       </c>
@@ -2421,28 +2449,28 @@
         <v>107</v>
       </c>
       <c r="C42" t="s">
-        <v>105</v>
-      </c>
-      <c r="D42">
+        <v>115</v>
+      </c>
+      <c r="E42">
         <v>3902</v>
       </c>
-      <c r="E42">
-        <v>2</v>
-      </c>
       <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
         <v>38</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>1458</v>
       </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
       <c r="I42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>44</v>
       </c>
@@ -2450,28 +2478,28 @@
         <v>107</v>
       </c>
       <c r="C43" t="s">
-        <v>105</v>
-      </c>
-      <c r="D43">
+        <v>115</v>
+      </c>
+      <c r="E43">
         <v>3903</v>
       </c>
-      <c r="E43">
-        <v>2</v>
-      </c>
       <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43">
         <v>38</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>1563</v>
       </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
       <c r="I43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>45</v>
       </c>
@@ -2479,28 +2507,28 @@
         <v>107</v>
       </c>
       <c r="C44" t="s">
-        <v>105</v>
-      </c>
-      <c r="D44">
+        <v>115</v>
+      </c>
+      <c r="E44">
         <v>3904</v>
       </c>
-      <c r="E44">
-        <v>2</v>
-      </c>
       <c r="F44">
+        <v>2</v>
+      </c>
+      <c r="G44">
         <v>22</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>10885</v>
       </c>
-      <c r="H44">
+      <c r="I44">
         <v>5</v>
       </c>
-      <c r="I44">
+      <c r="J44">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>46</v>
       </c>
@@ -2508,28 +2536,28 @@
         <v>107</v>
       </c>
       <c r="C45" t="s">
-        <v>105</v>
-      </c>
-      <c r="D45">
+        <v>115</v>
+      </c>
+      <c r="E45">
         <v>3913</v>
       </c>
-      <c r="E45">
-        <v>2</v>
-      </c>
       <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45">
         <v>22</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>522</v>
       </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
       <c r="I45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>47</v>
       </c>
@@ -2537,28 +2565,28 @@
         <v>107</v>
       </c>
       <c r="C46" t="s">
-        <v>105</v>
-      </c>
-      <c r="D46">
+        <v>115</v>
+      </c>
+      <c r="E46">
         <v>3917</v>
       </c>
-      <c r="E46">
-        <v>2</v>
-      </c>
       <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="G46">
         <v>22</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>2109</v>
       </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
       <c r="I46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>48</v>
       </c>
@@ -2566,28 +2594,28 @@
         <v>107</v>
       </c>
       <c r="C47" t="s">
-        <v>105</v>
-      </c>
-      <c r="D47">
+        <v>115</v>
+      </c>
+      <c r="E47">
         <v>3918</v>
       </c>
-      <c r="E47">
-        <v>2</v>
-      </c>
       <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="G47">
         <v>22</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>1109</v>
       </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
       <c r="I47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>51</v>
       </c>
@@ -2595,28 +2623,28 @@
         <v>107</v>
       </c>
       <c r="C48" t="s">
-        <v>105</v>
-      </c>
-      <c r="D48">
+        <v>112</v>
+      </c>
+      <c r="E48">
         <v>3954</v>
       </c>
-      <c r="E48">
-        <v>2</v>
-      </c>
       <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48">
         <v>12</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>19020</v>
       </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
       <c r="I48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>52</v>
       </c>
@@ -2624,28 +2652,28 @@
         <v>107</v>
       </c>
       <c r="C49" t="s">
-        <v>105</v>
-      </c>
-      <c r="D49">
+        <v>112</v>
+      </c>
+      <c r="E49">
         <v>14964</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>10</v>
       </c>
-      <c r="F49">
+      <c r="G49">
         <v>8</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>10218</v>
       </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
       <c r="I49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>54</v>
       </c>
@@ -2653,28 +2681,28 @@
         <v>107</v>
       </c>
       <c r="C50" t="s">
-        <v>105</v>
-      </c>
-      <c r="D50" s="2">
+        <v>115</v>
+      </c>
+      <c r="E50" s="2">
         <v>10093</v>
       </c>
-      <c r="E50">
-        <v>2</v>
-      </c>
       <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50">
         <v>5</v>
       </c>
-      <c r="G50">
+      <c r="H50">
         <v>1372</v>
       </c>
-      <c r="H50">
-        <v>0</v>
-      </c>
       <c r="I50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
@@ -2682,28 +2710,28 @@
         <v>107</v>
       </c>
       <c r="C51" t="s">
-        <v>105</v>
-      </c>
-      <c r="D51">
+        <v>115</v>
+      </c>
+      <c r="E51">
         <v>10101</v>
       </c>
-      <c r="E51">
-        <v>2</v>
-      </c>
       <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="G51">
         <v>5</v>
       </c>
-      <c r="G51">
+      <c r="H51">
         <v>748</v>
       </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
       <c r="I51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>56</v>
       </c>
@@ -2711,28 +2739,28 @@
         <v>107</v>
       </c>
       <c r="C52" t="s">
-        <v>105</v>
-      </c>
-      <c r="D52">
+        <v>115</v>
+      </c>
+      <c r="E52">
         <v>9979</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>10</v>
       </c>
-      <c r="F52">
+      <c r="G52">
         <v>36</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>2126</v>
       </c>
-      <c r="H52">
-        <v>0</v>
-      </c>
       <c r="I52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>57</v>
       </c>
@@ -2740,28 +2768,28 @@
         <v>107</v>
       </c>
       <c r="C53" t="s">
-        <v>105</v>
-      </c>
-      <c r="D53">
+        <v>112</v>
+      </c>
+      <c r="E53">
         <v>9980</v>
       </c>
-      <c r="E53">
-        <v>2</v>
-      </c>
       <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="G53">
         <v>21</v>
       </c>
-      <c r="G53">
+      <c r="H53">
         <v>540</v>
       </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
       <c r="I53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
@@ -2769,28 +2797,28 @@
         <v>107</v>
       </c>
       <c r="C54" t="s">
-        <v>105</v>
-      </c>
-      <c r="D54">
+        <v>115</v>
+      </c>
+      <c r="E54">
         <v>9983</v>
       </c>
-      <c r="E54">
-        <v>2</v>
-      </c>
       <c r="F54">
+        <v>2</v>
+      </c>
+      <c r="G54">
         <v>15</v>
       </c>
-      <c r="G54">
+      <c r="H54">
         <v>14980</v>
       </c>
-      <c r="H54">
-        <v>0</v>
-      </c>
       <c r="I54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>60</v>
       </c>
@@ -2798,28 +2826,28 @@
         <v>107</v>
       </c>
       <c r="C55" t="s">
-        <v>105</v>
-      </c>
-      <c r="D55">
+        <v>112</v>
+      </c>
+      <c r="E55">
         <v>9985</v>
       </c>
-      <c r="E55">
+      <c r="F55">
         <v>6</v>
       </c>
-      <c r="F55">
+      <c r="G55">
         <v>52</v>
       </c>
-      <c r="G55">
+      <c r="H55">
         <v>6118</v>
       </c>
-      <c r="H55">
-        <v>0</v>
-      </c>
       <c r="I55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>63</v>
       </c>
@@ -2827,28 +2855,28 @@
         <v>107</v>
       </c>
       <c r="C56" t="s">
-        <v>105</v>
-      </c>
-      <c r="D56">
+        <v>115</v>
+      </c>
+      <c r="E56">
         <v>9970</v>
       </c>
-      <c r="E56">
-        <v>2</v>
-      </c>
       <c r="F56">
+        <v>2</v>
+      </c>
+      <c r="G56">
         <v>101</v>
       </c>
-      <c r="G56">
+      <c r="H56">
         <v>1212</v>
       </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
       <c r="I56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>64</v>
       </c>
@@ -2856,28 +2884,28 @@
         <v>107</v>
       </c>
       <c r="C57" t="s">
-        <v>105</v>
-      </c>
-      <c r="D57">
+        <v>115</v>
+      </c>
+      <c r="E57">
         <v>9971</v>
       </c>
-      <c r="E57">
-        <v>2</v>
-      </c>
       <c r="F57">
+        <v>2</v>
+      </c>
+      <c r="G57">
         <v>11</v>
       </c>
-      <c r="G57">
+      <c r="H57">
         <v>583</v>
       </c>
-      <c r="H57">
-        <v>0</v>
-      </c>
       <c r="I57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>66</v>
       </c>
@@ -2885,28 +2913,28 @@
         <v>108</v>
       </c>
       <c r="C58" t="s">
-        <v>105</v>
-      </c>
-      <c r="D58">
+        <v>115</v>
+      </c>
+      <c r="E58">
         <v>9977</v>
       </c>
-      <c r="E58">
-        <v>2</v>
-      </c>
       <c r="F58">
+        <v>2</v>
+      </c>
+      <c r="G58">
         <v>119</v>
       </c>
-      <c r="G58">
+      <c r="H58">
         <v>34465</v>
       </c>
-      <c r="H58">
-        <v>0</v>
-      </c>
       <c r="I58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>67</v>
       </c>
@@ -2914,28 +2942,28 @@
         <v>107</v>
       </c>
       <c r="C59" t="s">
-        <v>105</v>
-      </c>
-      <c r="D59">
+        <v>115</v>
+      </c>
+      <c r="E59">
         <v>9978</v>
       </c>
-      <c r="E59">
-        <v>2</v>
-      </c>
       <c r="F59">
+        <v>2</v>
+      </c>
+      <c r="G59">
         <v>73</v>
       </c>
-      <c r="G59">
+      <c r="H59">
         <v>2534</v>
       </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
       <c r="I59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>68</v>
       </c>
@@ -2943,28 +2971,28 @@
         <v>107</v>
       </c>
       <c r="C60" t="s">
-        <v>105</v>
-      </c>
-      <c r="D60">
+        <v>115</v>
+      </c>
+      <c r="E60">
         <v>9952</v>
       </c>
-      <c r="E60">
-        <v>2</v>
-      </c>
       <c r="F60">
+        <v>2</v>
+      </c>
+      <c r="G60">
         <v>6</v>
       </c>
-      <c r="G60">
+      <c r="H60">
         <v>5404</v>
       </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
       <c r="I60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>69</v>
       </c>
@@ -2972,28 +3000,28 @@
         <v>107</v>
       </c>
       <c r="C61" t="s">
-        <v>105</v>
-      </c>
-      <c r="D61">
+        <v>112</v>
+      </c>
+      <c r="E61">
         <v>9954</v>
       </c>
-      <c r="E61">
+      <c r="F61">
         <v>100</v>
       </c>
-      <c r="F61">
+      <c r="G61">
         <v>65</v>
       </c>
-      <c r="G61">
+      <c r="H61">
         <v>1600</v>
       </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
       <c r="I61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>70</v>
       </c>
@@ -3001,28 +3029,28 @@
         <v>107</v>
       </c>
       <c r="C62" t="s">
-        <v>105</v>
-      </c>
-      <c r="D62">
+        <v>112</v>
+      </c>
+      <c r="E62">
         <v>9955</v>
       </c>
-      <c r="E62">
+      <c r="F62">
         <v>100</v>
       </c>
-      <c r="F62">
+      <c r="G62">
         <v>65</v>
       </c>
-      <c r="G62">
+      <c r="H62">
         <v>1600</v>
       </c>
-      <c r="H62">
-        <v>0</v>
-      </c>
       <c r="I62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>72</v>
       </c>
@@ -3030,28 +3058,28 @@
         <v>107</v>
       </c>
       <c r="C63" t="s">
-        <v>105</v>
-      </c>
-      <c r="D63">
+        <v>115</v>
+      </c>
+      <c r="E63">
         <v>9957</v>
       </c>
-      <c r="E63">
-        <v>2</v>
-      </c>
       <c r="F63">
+        <v>2</v>
+      </c>
+      <c r="G63">
         <v>42</v>
       </c>
-      <c r="G63">
+      <c r="H63">
         <v>1055</v>
       </c>
-      <c r="H63">
-        <v>0</v>
-      </c>
       <c r="I63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>73</v>
       </c>
@@ -3059,28 +3087,28 @@
         <v>107</v>
       </c>
       <c r="C64" t="s">
-        <v>105</v>
-      </c>
-      <c r="D64">
+        <v>115</v>
+      </c>
+      <c r="E64">
         <v>9960</v>
       </c>
-      <c r="E64">
+      <c r="F64">
         <v>4</v>
       </c>
-      <c r="F64">
+      <c r="G64">
         <v>25</v>
       </c>
-      <c r="G64">
+      <c r="H64">
         <v>5456</v>
       </c>
-      <c r="H64">
-        <v>0</v>
-      </c>
       <c r="I64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>75</v>
       </c>
@@ -3088,28 +3116,28 @@
         <v>107</v>
       </c>
       <c r="C65" t="s">
-        <v>105</v>
-      </c>
-      <c r="D65">
+        <v>115</v>
+      </c>
+      <c r="E65">
         <v>9967</v>
       </c>
-      <c r="E65">
-        <v>2</v>
-      </c>
       <c r="F65">
+        <v>2</v>
+      </c>
+      <c r="G65">
         <v>34</v>
       </c>
-      <c r="G65">
+      <c r="H65">
         <v>1941</v>
       </c>
-      <c r="H65">
-        <v>0</v>
-      </c>
       <c r="I65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>76</v>
       </c>
@@ -3117,28 +3145,28 @@
         <v>107</v>
       </c>
       <c r="C66" t="s">
-        <v>105</v>
-      </c>
-      <c r="D66">
+        <v>115</v>
+      </c>
+      <c r="E66">
         <v>9946</v>
       </c>
-      <c r="E66">
-        <v>2</v>
-      </c>
       <c r="F66">
+        <v>2</v>
+      </c>
+      <c r="G66">
         <v>31</v>
       </c>
-      <c r="G66">
+      <c r="H66">
         <v>569</v>
       </c>
-      <c r="H66">
-        <v>0</v>
-      </c>
       <c r="I66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>78</v>
       </c>
@@ -3146,28 +3174,28 @@
         <v>107</v>
       </c>
       <c r="C67" t="s">
-        <v>105</v>
-      </c>
-      <c r="D67">
+        <v>115</v>
+      </c>
+      <c r="E67">
         <v>7592</v>
       </c>
-      <c r="E67">
-        <v>2</v>
-      </c>
       <c r="F67">
+        <v>2</v>
+      </c>
+      <c r="G67">
         <v>15</v>
       </c>
-      <c r="G67">
+      <c r="H67">
         <v>48842</v>
       </c>
-      <c r="H67">
+      <c r="I67">
         <v>3620</v>
       </c>
-      <c r="I67">
+      <c r="J67">
         <v>6465</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>82</v>
       </c>
@@ -3175,28 +3203,28 @@
         <v>107</v>
       </c>
       <c r="C68" t="s">
-        <v>105</v>
-      </c>
-      <c r="D68">
+        <v>112</v>
+      </c>
+      <c r="E68">
         <v>14969</v>
       </c>
-      <c r="E68">
+      <c r="F68">
         <v>5</v>
       </c>
-      <c r="F68">
+      <c r="G68">
         <v>33</v>
       </c>
-      <c r="G68">
+      <c r="H68">
         <v>9873</v>
       </c>
-      <c r="H68">
-        <v>0</v>
-      </c>
       <c r="I68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>83</v>
       </c>
@@ -3204,28 +3232,28 @@
         <v>107</v>
       </c>
       <c r="C69" t="s">
-        <v>105</v>
-      </c>
-      <c r="D69">
+        <v>112</v>
+      </c>
+      <c r="E69">
         <v>14968</v>
       </c>
-      <c r="E69">
-        <v>2</v>
-      </c>
       <c r="F69">
+        <v>2</v>
+      </c>
+      <c r="G69">
         <v>40</v>
       </c>
-      <c r="G69">
+      <c r="H69">
         <v>540</v>
       </c>
-      <c r="H69">
+      <c r="I69">
         <v>263</v>
       </c>
-      <c r="I69">
+      <c r="J69">
         <v>999</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>84</v>
       </c>
@@ -3233,28 +3261,28 @@
         <v>107</v>
       </c>
       <c r="C70" t="s">
-        <v>105</v>
-      </c>
-      <c r="D70">
+        <v>115</v>
+      </c>
+      <c r="E70">
         <v>14967</v>
       </c>
-      <c r="E70">
+      <c r="F70">
         <v>6</v>
       </c>
-      <c r="F70">
+      <c r="G70">
         <v>35</v>
       </c>
-      <c r="G70">
+      <c r="H70">
         <v>2796</v>
       </c>
-      <c r="H70">
+      <c r="I70">
         <v>2795</v>
       </c>
-      <c r="I70">
+      <c r="J70">
         <v>68100</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>85</v>
       </c>
@@ -3262,28 +3290,28 @@
         <v>107</v>
       </c>
       <c r="C71" t="s">
-        <v>105</v>
-      </c>
-      <c r="D71">
+        <v>112</v>
+      </c>
+      <c r="E71">
         <v>125920</v>
       </c>
-      <c r="E71">
-        <v>2</v>
-      </c>
       <c r="F71">
+        <v>2</v>
+      </c>
+      <c r="G71">
         <v>13</v>
       </c>
-      <c r="G71">
+      <c r="H71">
         <v>500</v>
       </c>
-      <c r="H71">
+      <c r="I71">
         <v>401</v>
       </c>
-      <c r="I71">
+      <c r="J71">
         <v>835</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>87</v>
       </c>
@@ -3291,28 +3319,28 @@
         <v>107</v>
       </c>
       <c r="C72" t="s">
-        <v>105</v>
-      </c>
-      <c r="D72">
+        <v>115</v>
+      </c>
+      <c r="E72">
         <v>125921</v>
       </c>
-      <c r="E72">
+      <c r="F72">
         <v>10</v>
       </c>
-      <c r="F72">
+      <c r="G72">
         <v>8</v>
       </c>
-      <c r="G72">
+      <c r="H72">
         <v>500</v>
       </c>
-      <c r="H72">
-        <v>0</v>
-      </c>
       <c r="I72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>88</v>
       </c>
@@ -3320,28 +3348,28 @@
         <v>107</v>
       </c>
       <c r="C73" t="s">
-        <v>105</v>
-      </c>
-      <c r="D73">
+        <v>115</v>
+      </c>
+      <c r="E73">
         <v>125922</v>
       </c>
-      <c r="E73">
+      <c r="F73">
         <v>11</v>
       </c>
-      <c r="F73">
+      <c r="G73">
         <v>41</v>
       </c>
-      <c r="G73">
+      <c r="H73">
         <v>5500</v>
       </c>
-      <c r="H73">
-        <v>0</v>
-      </c>
       <c r="I73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>89</v>
       </c>
@@ -3349,28 +3377,28 @@
         <v>108</v>
       </c>
       <c r="C74" t="s">
-        <v>105</v>
-      </c>
-      <c r="D74">
+        <v>114</v>
+      </c>
+      <c r="E74">
         <v>146607</v>
       </c>
-      <c r="E74">
-        <v>2</v>
-      </c>
       <c r="F74">
+        <v>2</v>
+      </c>
+      <c r="G74">
         <v>123</v>
       </c>
-      <c r="G74">
+      <c r="H74">
         <v>8378</v>
       </c>
-      <c r="H74">
+      <c r="I74">
         <v>7330</v>
       </c>
-      <c r="I74">
+      <c r="J74">
         <v>18372</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>61</v>
       </c>
@@ -3378,28 +3406,28 @@
         <v>108</v>
       </c>
       <c r="C75" t="s">
-        <v>105</v>
-      </c>
-      <c r="D75">
+        <v>114</v>
+      </c>
+      <c r="E75">
         <v>9986</v>
       </c>
-      <c r="E75">
+      <c r="F75">
         <v>6</v>
       </c>
-      <c r="F75">
+      <c r="G75">
         <v>129</v>
       </c>
-      <c r="G75">
+      <c r="H75">
         <v>13910</v>
       </c>
-      <c r="H75">
-        <v>0</v>
-      </c>
       <c r="I75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>53</v>
       </c>
@@ -3407,28 +3435,28 @@
         <v>107</v>
       </c>
       <c r="C76" t="s">
-        <v>105</v>
-      </c>
-      <c r="D76">
+        <v>112</v>
+      </c>
+      <c r="E76">
         <v>14965</v>
       </c>
-      <c r="E76">
-        <v>2</v>
-      </c>
       <c r="F76">
+        <v>2</v>
+      </c>
+      <c r="G76">
         <v>17</v>
       </c>
-      <c r="G76">
+      <c r="H76">
         <v>45211</v>
       </c>
-      <c r="H76">
-        <v>0</v>
-      </c>
       <c r="I76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>71</v>
       </c>
@@ -3436,28 +3464,28 @@
         <v>107</v>
       </c>
       <c r="C77" t="s">
-        <v>105</v>
-      </c>
-      <c r="D77">
+        <v>112</v>
+      </c>
+      <c r="E77">
         <v>9956</v>
       </c>
-      <c r="E77">
+      <c r="F77">
         <v>100</v>
       </c>
-      <c r="F77">
+      <c r="G77">
         <v>65</v>
       </c>
-      <c r="G77">
+      <c r="H77">
         <v>1599</v>
       </c>
-      <c r="H77">
-        <v>0</v>
-      </c>
       <c r="I77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>81</v>
       </c>
@@ -3465,28 +3493,28 @@
         <v>107</v>
       </c>
       <c r="C78" t="s">
-        <v>105</v>
-      </c>
-      <c r="D78">
+        <v>115</v>
+      </c>
+      <c r="E78">
         <v>34537</v>
       </c>
-      <c r="E78">
-        <v>2</v>
-      </c>
       <c r="F78">
+        <v>2</v>
+      </c>
+      <c r="G78">
         <v>31</v>
       </c>
-      <c r="G78">
+      <c r="H78">
         <v>11055</v>
       </c>
-      <c r="H78">
-        <v>0</v>
-      </c>
       <c r="I78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>90</v>
       </c>
@@ -3494,57 +3522,57 @@
         <v>107</v>
       </c>
       <c r="C79" t="s">
-        <v>105</v>
-      </c>
-      <c r="D79">
+        <v>112</v>
+      </c>
+      <c r="E79">
         <v>146195</v>
       </c>
-      <c r="E79">
+      <c r="F79">
         <v>3</v>
       </c>
-      <c r="F79">
+      <c r="G79">
         <v>43</v>
       </c>
-      <c r="G79">
+      <c r="H79">
         <v>67557</v>
       </c>
-      <c r="H79">
-        <v>0</v>
-      </c>
       <c r="I79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C80" t="s">
-        <v>105</v>
-      </c>
-      <c r="D80">
+        <v>113</v>
+      </c>
+      <c r="E80">
         <v>34539</v>
       </c>
-      <c r="E80">
-        <v>2</v>
-      </c>
       <c r="F80">
+        <v>2</v>
+      </c>
+      <c r="G80">
         <v>10</v>
       </c>
-      <c r="G80">
+      <c r="H80">
         <v>32769</v>
       </c>
-      <c r="H80">
-        <v>0</v>
-      </c>
       <c r="I80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>62</v>
       </c>
@@ -3552,28 +3580,28 @@
         <v>108</v>
       </c>
       <c r="C81" t="s">
-        <v>105</v>
-      </c>
-      <c r="D81">
+        <v>114</v>
+      </c>
+      <c r="E81">
         <v>14970</v>
       </c>
-      <c r="E81">
+      <c r="F81">
         <v>6</v>
       </c>
-      <c r="F81">
+      <c r="G81">
         <v>562</v>
       </c>
-      <c r="G81">
+      <c r="H81">
         <v>10299</v>
       </c>
-      <c r="H81">
-        <v>0</v>
-      </c>
       <c r="I81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>79</v>
       </c>
@@ -3581,28 +3609,28 @@
         <v>108</v>
       </c>
       <c r="C82" t="s">
-        <v>105</v>
-      </c>
-      <c r="D82">
+        <v>114</v>
+      </c>
+      <c r="E82">
         <v>14966</v>
       </c>
-      <c r="E82">
-        <v>2</v>
-      </c>
       <c r="F82">
+        <v>2</v>
+      </c>
+      <c r="G82">
         <v>1777</v>
       </c>
-      <c r="G82">
+      <c r="H82">
         <v>3751</v>
       </c>
-      <c r="H82">
-        <v>0</v>
-      </c>
       <c r="I82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>86</v>
       </c>
@@ -3610,28 +3638,28 @@
         <v>107</v>
       </c>
       <c r="C83" t="s">
-        <v>105</v>
-      </c>
-      <c r="D83">
+        <v>114</v>
+      </c>
+      <c r="E83">
         <v>146606</v>
       </c>
-      <c r="E83">
-        <v>2</v>
-      </c>
       <c r="F83">
+        <v>2</v>
+      </c>
+      <c r="G83">
         <v>29</v>
       </c>
-      <c r="G83">
+      <c r="H83">
         <v>98050</v>
       </c>
-      <c r="H83">
+      <c r="I83">
         <v>1</v>
       </c>
-      <c r="I83">
+      <c r="J83">
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>40</v>
       </c>
@@ -3639,28 +3667,28 @@
         <v>108</v>
       </c>
       <c r="C84" t="s">
-        <v>105</v>
-      </c>
-      <c r="D84">
+        <v>114</v>
+      </c>
+      <c r="E84">
         <v>3573</v>
       </c>
-      <c r="E84">
+      <c r="F84">
         <v>10</v>
       </c>
-      <c r="F84">
+      <c r="G84">
         <v>785</v>
       </c>
-      <c r="G84">
+      <c r="H84">
         <v>70000</v>
       </c>
-      <c r="H84">
-        <v>0</v>
-      </c>
       <c r="I84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>41</v>
       </c>
@@ -3668,28 +3696,28 @@
         <v>108</v>
       </c>
       <c r="C85" t="s">
-        <v>105</v>
-      </c>
-      <c r="D85">
+        <v>114</v>
+      </c>
+      <c r="E85">
         <v>3891</v>
       </c>
-      <c r="E85">
-        <v>2</v>
-      </c>
       <c r="F85">
+        <v>2</v>
+      </c>
+      <c r="G85">
         <v>971</v>
       </c>
-      <c r="G85">
+      <c r="H85">
         <v>3468</v>
       </c>
-      <c r="H85">
-        <v>0</v>
-      </c>
       <c r="I85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -3697,28 +3725,28 @@
         <v>108</v>
       </c>
       <c r="C86" t="s">
-        <v>105</v>
-      </c>
-      <c r="D86">
+        <v>114</v>
+      </c>
+      <c r="E86">
         <v>3481</v>
       </c>
-      <c r="E86">
+      <c r="F86">
         <v>26</v>
       </c>
-      <c r="F86">
+      <c r="G86">
         <v>618</v>
       </c>
-      <c r="G86">
+      <c r="H86">
         <v>7797</v>
       </c>
-      <c r="H86">
-        <v>0</v>
-      </c>
       <c r="I86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>58</v>
       </c>
@@ -3726,28 +3754,28 @@
         <v>108</v>
       </c>
       <c r="C87" t="s">
-        <v>105</v>
-      </c>
-      <c r="D87">
+        <v>114</v>
+      </c>
+      <c r="E87">
         <v>9981</v>
       </c>
-      <c r="E87">
+      <c r="F87">
         <v>9</v>
       </c>
-      <c r="F87">
+      <c r="G87">
         <v>857</v>
       </c>
-      <c r="G87">
+      <c r="H87">
         <v>1080</v>
       </c>
-      <c r="H87">
-        <v>0</v>
-      </c>
       <c r="I87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>74</v>
       </c>
@@ -3755,28 +3783,28 @@
         <v>108</v>
       </c>
       <c r="C88" t="s">
-        <v>105</v>
-      </c>
-      <c r="D88">
+        <v>114</v>
+      </c>
+      <c r="E88">
         <v>9964</v>
       </c>
-      <c r="E88">
+      <c r="F88">
         <v>10</v>
       </c>
-      <c r="F88">
+      <c r="G88">
         <v>257</v>
       </c>
-      <c r="G88">
+      <c r="H88">
         <v>1593</v>
       </c>
-      <c r="H88">
-        <v>0</v>
-      </c>
       <c r="I88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>77</v>
       </c>
@@ -3784,28 +3812,28 @@
         <v>108</v>
       </c>
       <c r="C89" t="s">
-        <v>105</v>
-      </c>
-      <c r="D89">
+        <v>114</v>
+      </c>
+      <c r="E89">
         <v>9950</v>
       </c>
-      <c r="E89">
+      <c r="F89">
         <v>20</v>
       </c>
-      <c r="F89">
+      <c r="G89">
         <v>1301</v>
       </c>
-      <c r="G89">
+      <c r="H89">
         <v>571</v>
       </c>
-      <c r="H89">
-        <v>0</v>
-      </c>
       <c r="I89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>65</v>
       </c>
@@ -3813,28 +3841,28 @@
         <v>108</v>
       </c>
       <c r="C90" t="s">
-        <v>105</v>
-      </c>
-      <c r="D90">
+        <v>114</v>
+      </c>
+      <c r="E90">
         <v>9976</v>
       </c>
-      <c r="E90">
-        <v>2</v>
-      </c>
       <c r="F90">
+        <v>2</v>
+      </c>
+      <c r="G90">
         <v>501</v>
       </c>
-      <c r="G90">
+      <c r="H90">
         <v>2600</v>
       </c>
-      <c r="H90">
-        <v>0</v>
-      </c>
       <c r="I90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>8</v>
       </c>
@@ -3842,28 +3870,28 @@
         <v>108</v>
       </c>
       <c r="C91" t="s">
-        <v>105</v>
-      </c>
-      <c r="D91">
+        <v>114</v>
+      </c>
+      <c r="E91">
         <v>20</v>
       </c>
-      <c r="E91">
+      <c r="F91">
         <v>10</v>
       </c>
-      <c r="F91">
+      <c r="G91">
         <v>241</v>
       </c>
-      <c r="G91">
+      <c r="H91">
         <v>2000</v>
       </c>
-      <c r="H91">
-        <v>0</v>
-      </c>
       <c r="I91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>49</v>
       </c>
@@ -3871,28 +3899,28 @@
         <v>108</v>
       </c>
       <c r="C92" t="s">
-        <v>105</v>
-      </c>
-      <c r="D92">
+        <v>114</v>
+      </c>
+      <c r="E92">
         <v>3946</v>
       </c>
-      <c r="E92">
-        <v>2</v>
-      </c>
       <c r="F92">
+        <v>2</v>
+      </c>
+      <c r="G92">
         <v>231</v>
-      </c>
-      <c r="G92">
-        <v>50000</v>
       </c>
       <c r="H92">
         <v>50000</v>
       </c>
       <c r="I92">
+        <v>50000</v>
+      </c>
+      <c r="J92">
         <v>8024152</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>50</v>
       </c>
@@ -3900,24 +3928,24 @@
         <v>108</v>
       </c>
       <c r="C93" t="s">
-        <v>105</v>
-      </c>
-      <c r="D93" s="2">
+        <v>114</v>
+      </c>
+      <c r="E93" s="2">
         <v>3948</v>
       </c>
-      <c r="E93">
-        <v>2</v>
-      </c>
       <c r="F93">
+        <v>2</v>
+      </c>
+      <c r="G93">
         <v>231</v>
-      </c>
-      <c r="G93">
-        <v>50000</v>
       </c>
       <c r="H93">
         <v>50000</v>
       </c>
       <c r="I93">
+        <v>50000</v>
+      </c>
+      <c r="J93">
         <v>8024152</v>
       </c>
     </row>

</xml_diff>

<commit_message>
PP2 - Convert everything to containers
</commit_message>
<xml_diff>
--- a/benchmark/Configuration.xlsx
+++ b/benchmark/Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\autem\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A28650-F7B7-45FF-834D-2136EB568607}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DF1A74-FD58-48F8-AF25-6A17DEA17E61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19650" yWindow="1440" windowWidth="18240" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openml_100" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="118">
   <si>
     <t>kr-vs-kp</t>
   </si>
@@ -380,6 +380,9 @@
   </si>
   <si>
     <t>ensemble_snapshot</t>
+  </si>
+  <si>
+    <t>standard</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1233,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,7 +1344,7 @@
         <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
         <v>112</v>
@@ -1428,10 +1431,13 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C7" t="s">
         <v>112</v>
+      </c>
+      <c r="D7" t="s">
+        <v>105</v>
       </c>
       <c r="E7">
         <v>11</v>
@@ -1486,7 +1492,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="C9" t="s">
         <v>112</v>
@@ -1689,10 +1695,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C16" t="s">
         <v>112</v>
+      </c>
+      <c r="D16" t="s">
+        <v>105</v>
       </c>
       <c r="E16">
         <v>31</v>
@@ -1805,7 +1814,7 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="C20" t="s">
         <v>112</v>
@@ -2037,10 +2046,13 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C28" t="s">
         <v>112</v>
+      </c>
+      <c r="D28" t="s">
+        <v>105</v>
       </c>
       <c r="E28">
         <v>219</v>
@@ -2095,10 +2107,13 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C30" t="s">
         <v>112</v>
+      </c>
+      <c r="D30" t="s">
+        <v>105</v>
       </c>
       <c r="E30">
         <v>2125</v>
@@ -2124,10 +2139,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="C31" t="s">
         <v>112</v>
+      </c>
+      <c r="D31" t="s">
+        <v>105</v>
       </c>
       <c r="E31">
         <v>3022</v>
@@ -2182,10 +2200,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C33" t="s">
         <v>112</v>
+      </c>
+      <c r="D33" t="s">
+        <v>105</v>
       </c>
       <c r="E33" s="2">
         <v>3492</v>
@@ -2214,10 +2235,7 @@
         <v>116</v>
       </c>
       <c r="C34" t="s">
-        <v>112</v>
-      </c>
-      <c r="D34" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="E34">
         <v>3493</v>
@@ -2620,10 +2638,13 @@
         <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C48" t="s">
         <v>112</v>
+      </c>
+      <c r="D48" t="s">
+        <v>105</v>
       </c>
       <c r="E48">
         <v>3954</v>
@@ -2649,10 +2670,13 @@
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C49" t="s">
         <v>112</v>
+      </c>
+      <c r="D49" t="s">
+        <v>105</v>
       </c>
       <c r="E49">
         <v>14964</v>
@@ -2765,7 +2789,7 @@
         <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="C53" t="s">
         <v>112</v>
@@ -2823,10 +2847,13 @@
         <v>60</v>
       </c>
       <c r="B55" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C55" t="s">
         <v>112</v>
+      </c>
+      <c r="D55" t="s">
+        <v>105</v>
       </c>
       <c r="E55">
         <v>9985</v>
@@ -2997,10 +3024,13 @@
         <v>69</v>
       </c>
       <c r="B61" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C61" t="s">
         <v>112</v>
+      </c>
+      <c r="D61" t="s">
+        <v>105</v>
       </c>
       <c r="E61">
         <v>9954</v>
@@ -3026,10 +3056,13 @@
         <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C62" t="s">
         <v>112</v>
+      </c>
+      <c r="D62" t="s">
+        <v>105</v>
       </c>
       <c r="E62">
         <v>9955</v>
@@ -3200,10 +3233,13 @@
         <v>82</v>
       </c>
       <c r="B68" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C68" t="s">
         <v>112</v>
+      </c>
+      <c r="D68" t="s">
+        <v>105</v>
       </c>
       <c r="E68">
         <v>14969</v>
@@ -3229,10 +3265,13 @@
         <v>83</v>
       </c>
       <c r="B69" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C69" t="s">
         <v>112</v>
+      </c>
+      <c r="D69" t="s">
+        <v>105</v>
       </c>
       <c r="E69">
         <v>14968</v>
@@ -3287,7 +3326,7 @@
         <v>85</v>
       </c>
       <c r="B71" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="C71" t="s">
         <v>112</v>
@@ -3432,7 +3471,7 @@
         <v>53</v>
       </c>
       <c r="B76" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="C76" t="s">
         <v>112</v>
@@ -3461,10 +3500,13 @@
         <v>71</v>
       </c>
       <c r="B77" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C77" t="s">
         <v>112</v>
+      </c>
+      <c r="D77" t="s">
+        <v>105</v>
       </c>
       <c r="E77">
         <v>9956</v>
@@ -3519,7 +3561,7 @@
         <v>90</v>
       </c>
       <c r="B79" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="C79" t="s">
         <v>112</v>

</xml_diff>

<commit_message>
PP2 - Create standard workflows
</commit_message>
<xml_diff>
--- a/benchmark/Configuration.xlsx
+++ b/benchmark/Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\autem\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DF1A74-FD58-48F8-AF25-6A17DEA17E61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DD6A48-9F9B-4363-B231-6BDB5EA8F839}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19650" yWindow="1440" windowWidth="18240" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6105" yWindow="510" windowWidth="18240" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openml_100" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="118">
   <si>
     <t>kr-vs-kp</t>
   </si>
@@ -1233,7 +1233,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,6 +1349,9 @@
       <c r="C4" t="s">
         <v>112</v>
       </c>
+      <c r="D4" t="s">
+        <v>105</v>
+      </c>
       <c r="E4">
         <v>125923</v>
       </c>
@@ -1431,7 +1434,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
         <v>112</v>
@@ -1497,6 +1500,9 @@
       <c r="C9" t="s">
         <v>112</v>
       </c>
+      <c r="D9" t="s">
+        <v>105</v>
+      </c>
       <c r="E9">
         <v>29</v>
       </c>
@@ -1695,7 +1701,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C16" t="s">
         <v>112</v>
@@ -1819,6 +1825,9 @@
       <c r="C20" t="s">
         <v>112</v>
       </c>
+      <c r="D20" t="s">
+        <v>105</v>
+      </c>
       <c r="E20">
         <v>12</v>
       </c>
@@ -2203,10 +2212,7 @@
         <v>116</v>
       </c>
       <c r="C33" t="s">
-        <v>112</v>
-      </c>
-      <c r="D33" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="E33" s="2">
         <v>3492</v>
@@ -2794,6 +2800,9 @@
       <c r="C53" t="s">
         <v>112</v>
       </c>
+      <c r="D53" t="s">
+        <v>105</v>
+      </c>
       <c r="E53">
         <v>9980</v>
       </c>
@@ -3024,7 +3033,7 @@
         <v>69</v>
       </c>
       <c r="B61" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C61" t="s">
         <v>112</v>
@@ -3056,7 +3065,7 @@
         <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C62" t="s">
         <v>112</v>
@@ -3331,6 +3340,9 @@
       <c r="C71" t="s">
         <v>112</v>
       </c>
+      <c r="D71" t="s">
+        <v>105</v>
+      </c>
       <c r="E71">
         <v>125920</v>
       </c>
@@ -3476,6 +3488,9 @@
       <c r="C76" t="s">
         <v>112</v>
       </c>
+      <c r="D76" t="s">
+        <v>105</v>
+      </c>
       <c r="E76">
         <v>14965</v>
       </c>
@@ -3565,6 +3580,9 @@
       </c>
       <c r="C79" t="s">
         <v>112</v>
+      </c>
+      <c r="D79" t="s">
+        <v>105</v>
       </c>
       <c r="E79">
         <v>146195</v>

</xml_diff>

<commit_message>
PP2 - Introduce Trees and Hammer configurations
</commit_message>
<xml_diff>
--- a/benchmark/Configuration.xlsx
+++ b/benchmark/Configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\autem\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DD6A48-9F9B-4363-B231-6BDB5EA8F839}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C5F348-5329-45A4-9F39-AB70E4DFA54F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6105" yWindow="510" windowWidth="18240" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7455" yWindow="435" windowWidth="18240" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openml_100" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="120">
   <si>
     <t>kr-vs-kp</t>
   </si>
@@ -370,19 +370,25 @@
     <t>progressing</t>
   </si>
   <si>
-    <t>fail</t>
-  </si>
-  <si>
     <t>unattempted</t>
   </si>
   <si>
     <t>complete</t>
   </si>
   <si>
-    <t>ensemble_snapshot</t>
-  </si>
-  <si>
-    <t>standard</t>
+    <t>nonlinear</t>
+  </si>
+  <si>
+    <t>investigate</t>
+  </si>
+  <si>
+    <t>long runtime</t>
+  </si>
+  <si>
+    <t>trees</t>
+  </si>
+  <si>
+    <t>hammer</t>
   </si>
 </sst>
 </file>
@@ -1233,14 +1239,15 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C80" sqref="C80"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="4" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -1254,10 +1261,10 @@
         <v>98</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>110</v>
@@ -1286,10 +1293,10 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E2">
         <v>37</v>
@@ -1315,10 +1322,10 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E3">
         <v>53</v>
@@ -1344,10 +1351,10 @@
         <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C4" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="D4" t="s">
         <v>105</v>
@@ -1376,10 +1383,10 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E5">
         <v>145804</v>
@@ -1405,10 +1412,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C6" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E6">
         <v>18</v>
@@ -1434,13 +1441,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="E7">
         <v>11</v>
@@ -1466,10 +1470,10 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C8" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E8">
         <v>3021</v>
@@ -1495,13 +1499,10 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
-      </c>
-      <c r="D9" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="E9">
         <v>29</v>
@@ -1527,10 +1528,10 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C10" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E10">
         <v>41</v>
@@ -1556,10 +1557,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C11" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E11">
         <v>1779</v>
@@ -1585,10 +1586,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E12">
         <v>23</v>
@@ -1614,10 +1615,10 @@
         <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E13">
         <v>3561</v>
@@ -1643,10 +1644,10 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C14" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E14">
         <v>1788</v>
@@ -1672,10 +1673,10 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E15">
         <v>28</v>
@@ -1701,13 +1702,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C16" t="s">
-        <v>112</v>
-      </c>
-      <c r="D16" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="E16">
         <v>31</v>
@@ -1733,10 +1731,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C17" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E17">
         <v>32</v>
@@ -1762,10 +1760,10 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C18" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E18">
         <v>3</v>
@@ -1791,10 +1789,10 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E19">
         <v>6</v>
@@ -1820,13 +1818,10 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C20" t="s">
-        <v>112</v>
-      </c>
-      <c r="D20" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E20">
         <v>12</v>
@@ -1852,10 +1847,10 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C21" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E21">
         <v>1778</v>
@@ -1881,10 +1876,10 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E22">
         <v>16</v>
@@ -1910,10 +1905,10 @@
         <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C23" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E23">
         <v>22</v>
@@ -1939,10 +1934,10 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C24" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E24">
         <v>36</v>
@@ -1968,10 +1963,10 @@
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C25" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E25">
         <v>43</v>
@@ -1997,10 +1992,10 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C26" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E26">
         <v>45</v>
@@ -2026,10 +2021,10 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C27" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E27">
         <v>58</v>
@@ -2058,10 +2053,7 @@
         <v>116</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
-      </c>
-      <c r="D28" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="E28">
         <v>219</v>
@@ -2087,10 +2079,10 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C29" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E29">
         <v>2074</v>
@@ -2116,13 +2108,10 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C30" t="s">
-        <v>112</v>
-      </c>
-      <c r="D30" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="E30">
         <v>2125</v>
@@ -2148,13 +2137,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C31" t="s">
-        <v>112</v>
-      </c>
-      <c r="D31" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="E31">
         <v>3022</v>
@@ -2180,10 +2166,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C32" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E32">
         <v>3485</v>
@@ -2209,10 +2195,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C33" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E33" s="2">
         <v>3492</v>
@@ -2238,10 +2224,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C34" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E34">
         <v>3493</v>
@@ -2267,10 +2253,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C35" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E35">
         <v>3494</v>
@@ -2296,10 +2282,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C36" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E36">
         <v>4544</v>
@@ -2325,10 +2311,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C37" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E37">
         <v>3512</v>
@@ -2354,10 +2340,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C38" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E38">
         <v>3543</v>
@@ -2383,10 +2369,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C39" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E39">
         <v>3549</v>
@@ -2412,10 +2398,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C40" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E40">
         <v>3560</v>
@@ -2441,10 +2427,10 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C41" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E41">
         <v>3899</v>
@@ -2470,10 +2456,10 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C42" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E42">
         <v>3902</v>
@@ -2499,10 +2485,10 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C43" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E43">
         <v>3903</v>
@@ -2528,10 +2514,10 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C44" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E44">
         <v>3904</v>
@@ -2557,10 +2543,10 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C45" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E45">
         <v>3913</v>
@@ -2586,10 +2572,10 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C46" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E46">
         <v>3917</v>
@@ -2615,10 +2601,10 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C47" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E47">
         <v>3918</v>
@@ -2644,13 +2630,10 @@
         <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C48" t="s">
-        <v>112</v>
-      </c>
-      <c r="D48" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="E48">
         <v>3954</v>
@@ -2679,10 +2662,7 @@
         <v>116</v>
       </c>
       <c r="C49" t="s">
-        <v>112</v>
-      </c>
-      <c r="D49" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="E49">
         <v>14964</v>
@@ -2708,10 +2688,10 @@
         <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C50" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E50" s="2">
         <v>10093</v>
@@ -2737,10 +2717,10 @@
         <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C51" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E51">
         <v>10101</v>
@@ -2766,10 +2746,10 @@
         <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C52" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E52">
         <v>9979</v>
@@ -2795,13 +2775,10 @@
         <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C53" t="s">
-        <v>112</v>
-      </c>
-      <c r="D53" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="E53">
         <v>9980</v>
@@ -2827,10 +2804,10 @@
         <v>59</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C54" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E54">
         <v>9983</v>
@@ -2859,10 +2836,7 @@
         <v>116</v>
       </c>
       <c r="C55" t="s">
-        <v>112</v>
-      </c>
-      <c r="D55" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="E55">
         <v>9985</v>
@@ -2888,10 +2862,10 @@
         <v>63</v>
       </c>
       <c r="B56" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C56" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E56">
         <v>9970</v>
@@ -2917,10 +2891,10 @@
         <v>64</v>
       </c>
       <c r="B57" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C57" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E57">
         <v>9971</v>
@@ -2946,10 +2920,10 @@
         <v>66</v>
       </c>
       <c r="B58" t="s">
+        <v>114</v>
+      </c>
+      <c r="C58" t="s">
         <v>108</v>
-      </c>
-      <c r="C58" t="s">
-        <v>115</v>
       </c>
       <c r="E58">
         <v>9977</v>
@@ -2975,10 +2949,10 @@
         <v>67</v>
       </c>
       <c r="B59" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C59" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E59">
         <v>9978</v>
@@ -3004,10 +2978,10 @@
         <v>68</v>
       </c>
       <c r="B60" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C60" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E60">
         <v>9952</v>
@@ -3033,13 +3007,10 @@
         <v>69</v>
       </c>
       <c r="B61" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C61" t="s">
-        <v>112</v>
-      </c>
-      <c r="D61" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="E61">
         <v>9954</v>
@@ -3065,13 +3036,10 @@
         <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C62" t="s">
-        <v>112</v>
-      </c>
-      <c r="D62" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="E62">
         <v>9955</v>
@@ -3097,10 +3065,10 @@
         <v>72</v>
       </c>
       <c r="B63" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C63" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E63">
         <v>9957</v>
@@ -3126,10 +3094,10 @@
         <v>73</v>
       </c>
       <c r="B64" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C64" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E64">
         <v>9960</v>
@@ -3155,10 +3123,10 @@
         <v>75</v>
       </c>
       <c r="B65" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C65" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E65">
         <v>9967</v>
@@ -3184,10 +3152,10 @@
         <v>76</v>
       </c>
       <c r="B66" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C66" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E66">
         <v>9946</v>
@@ -3213,10 +3181,10 @@
         <v>78</v>
       </c>
       <c r="B67" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C67" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E67">
         <v>7592</v>
@@ -3242,13 +3210,10 @@
         <v>82</v>
       </c>
       <c r="B68" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C68" t="s">
-        <v>112</v>
-      </c>
-      <c r="D68" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E68">
         <v>14969</v>
@@ -3274,13 +3239,10 @@
         <v>83</v>
       </c>
       <c r="B69" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C69" t="s">
-        <v>112</v>
-      </c>
-      <c r="D69" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="E69">
         <v>14968</v>
@@ -3306,10 +3268,10 @@
         <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C70" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E70">
         <v>14967</v>
@@ -3335,13 +3297,10 @@
         <v>85</v>
       </c>
       <c r="B71" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C71" t="s">
-        <v>112</v>
-      </c>
-      <c r="D71" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="E71">
         <v>125920</v>
@@ -3367,10 +3326,10 @@
         <v>87</v>
       </c>
       <c r="B72" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C72" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E72">
         <v>125921</v>
@@ -3396,10 +3355,10 @@
         <v>88</v>
       </c>
       <c r="B73" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C73" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E73">
         <v>125922</v>
@@ -3425,10 +3384,10 @@
         <v>89</v>
       </c>
       <c r="B74" t="s">
+        <v>113</v>
+      </c>
+      <c r="C74" t="s">
         <v>108</v>
-      </c>
-      <c r="C74" t="s">
-        <v>114</v>
       </c>
       <c r="E74">
         <v>146607</v>
@@ -3454,10 +3413,10 @@
         <v>61</v>
       </c>
       <c r="B75" t="s">
+        <v>113</v>
+      </c>
+      <c r="C75" t="s">
         <v>108</v>
-      </c>
-      <c r="C75" t="s">
-        <v>114</v>
       </c>
       <c r="E75">
         <v>9986</v>
@@ -3483,13 +3442,10 @@
         <v>53</v>
       </c>
       <c r="B76" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C76" t="s">
-        <v>112</v>
-      </c>
-      <c r="D76" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="E76">
         <v>14965</v>
@@ -3515,13 +3471,10 @@
         <v>71</v>
       </c>
       <c r="B77" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C77" t="s">
-        <v>112</v>
-      </c>
-      <c r="D77" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="E77">
         <v>9956</v>
@@ -3547,10 +3500,10 @@
         <v>81</v>
       </c>
       <c r="B78" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="C78" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E78">
         <v>34537</v>
@@ -3576,13 +3529,10 @@
         <v>90</v>
       </c>
       <c r="B79" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C79" t="s">
-        <v>112</v>
-      </c>
-      <c r="D79" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="E79">
         <v>146195</v>
@@ -3608,10 +3558,10 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
+        <v>117</v>
+      </c>
+      <c r="C80" t="s">
         <v>109</v>
-      </c>
-      <c r="C80" t="s">
-        <v>113</v>
       </c>
       <c r="E80">
         <v>34539</v>
@@ -3637,10 +3587,10 @@
         <v>62</v>
       </c>
       <c r="B81" t="s">
+        <v>113</v>
+      </c>
+      <c r="C81" t="s">
         <v>108</v>
-      </c>
-      <c r="C81" t="s">
-        <v>114</v>
       </c>
       <c r="E81">
         <v>14970</v>
@@ -3666,10 +3616,10 @@
         <v>79</v>
       </c>
       <c r="B82" t="s">
+        <v>113</v>
+      </c>
+      <c r="C82" t="s">
         <v>108</v>
-      </c>
-      <c r="C82" t="s">
-        <v>114</v>
       </c>
       <c r="E82">
         <v>14966</v>
@@ -3695,10 +3645,10 @@
         <v>86</v>
       </c>
       <c r="B83" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C83" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E83">
         <v>146606</v>
@@ -3724,10 +3674,10 @@
         <v>40</v>
       </c>
       <c r="B84" t="s">
+        <v>113</v>
+      </c>
+      <c r="C84" t="s">
         <v>108</v>
-      </c>
-      <c r="C84" t="s">
-        <v>114</v>
       </c>
       <c r="E84">
         <v>3573</v>
@@ -3753,10 +3703,10 @@
         <v>41</v>
       </c>
       <c r="B85" t="s">
+        <v>113</v>
+      </c>
+      <c r="C85" t="s">
         <v>108</v>
-      </c>
-      <c r="C85" t="s">
-        <v>114</v>
       </c>
       <c r="E85">
         <v>3891</v>
@@ -3782,10 +3732,10 @@
         <v>28</v>
       </c>
       <c r="B86" t="s">
+        <v>113</v>
+      </c>
+      <c r="C86" t="s">
         <v>108</v>
-      </c>
-      <c r="C86" t="s">
-        <v>114</v>
       </c>
       <c r="E86">
         <v>3481</v>
@@ -3811,10 +3761,10 @@
         <v>58</v>
       </c>
       <c r="B87" t="s">
+        <v>113</v>
+      </c>
+      <c r="C87" t="s">
         <v>108</v>
-      </c>
-      <c r="C87" t="s">
-        <v>114</v>
       </c>
       <c r="E87">
         <v>9981</v>
@@ -3840,10 +3790,10 @@
         <v>74</v>
       </c>
       <c r="B88" t="s">
+        <v>113</v>
+      </c>
+      <c r="C88" t="s">
         <v>108</v>
-      </c>
-      <c r="C88" t="s">
-        <v>114</v>
       </c>
       <c r="E88">
         <v>9964</v>
@@ -3869,10 +3819,10 @@
         <v>77</v>
       </c>
       <c r="B89" t="s">
+        <v>113</v>
+      </c>
+      <c r="C89" t="s">
         <v>108</v>
-      </c>
-      <c r="C89" t="s">
-        <v>114</v>
       </c>
       <c r="E89">
         <v>9950</v>
@@ -3898,10 +3848,10 @@
         <v>65</v>
       </c>
       <c r="B90" t="s">
+        <v>113</v>
+      </c>
+      <c r="C90" t="s">
         <v>108</v>
-      </c>
-      <c r="C90" t="s">
-        <v>114</v>
       </c>
       <c r="E90">
         <v>9976</v>
@@ -3927,10 +3877,10 @@
         <v>8</v>
       </c>
       <c r="B91" t="s">
+        <v>113</v>
+      </c>
+      <c r="C91" t="s">
         <v>108</v>
-      </c>
-      <c r="C91" t="s">
-        <v>114</v>
       </c>
       <c r="E91">
         <v>20</v>
@@ -3956,10 +3906,10 @@
         <v>49</v>
       </c>
       <c r="B92" t="s">
+        <v>113</v>
+      </c>
+      <c r="C92" t="s">
         <v>108</v>
-      </c>
-      <c r="C92" t="s">
-        <v>114</v>
       </c>
       <c r="E92">
         <v>3946</v>
@@ -3985,10 +3935,10 @@
         <v>50</v>
       </c>
       <c r="B93" t="s">
+        <v>113</v>
+      </c>
+      <c r="C93" t="s">
         <v>108</v>
-      </c>
-      <c r="C93" t="s">
-        <v>114</v>
       </c>
       <c r="E93" s="2">
         <v>3948</v>

</xml_diff>

<commit_message>
SP1 - Complete move to settings
</commit_message>
<xml_diff>
--- a/benchmark/Configuration.xlsx
+++ b/benchmark/Configuration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\autem\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC04F58-B57E-47F4-A434-A36624F47AD9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E513ADA-BE92-4628-B517-D9EC3516C97B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3225" yWindow="1305" windowWidth="18240" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="openml_100" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="134">
   <si>
     <t>kr-vs-kp</t>
   </si>
@@ -416,6 +416,21 @@
   </si>
   <si>
     <t>trees_short</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>svm</t>
+  </si>
+  <si>
+    <t>Learner</t>
+  </si>
+  <si>
+    <t>SP1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1260,31 +1275,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K93"/>
+  <dimension ref="A1:M93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D49" sqref="D49"/>
+      <selection pane="bottomRight" activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="37" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="37" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>98</v>
       </c>
@@ -1298,28 +1314,34 @@
         <v>106</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1329,26 +1351,32 @@
       <c r="D2" t="s">
         <v>107</v>
       </c>
-      <c r="F2">
+      <c r="E2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2">
         <v>37</v>
       </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
         <v>9</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>768</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -1358,26 +1386,32 @@
       <c r="D3" t="s">
         <v>107</v>
       </c>
-      <c r="F3">
+      <c r="E3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3">
         <v>53</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>4</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>19</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>846</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>91</v>
       </c>
@@ -1388,28 +1422,34 @@
         <v>114</v>
       </c>
       <c r="E4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F4">
+        <v>129</v>
+      </c>
+      <c r="F4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" t="s">
+        <v>115</v>
+      </c>
+      <c r="H4">
         <v>125923</v>
       </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
         <v>15</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>690</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1419,26 +1459,32 @@
       <c r="D5" t="s">
         <v>107</v>
       </c>
-      <c r="F5">
+      <c r="E5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H5">
         <v>145804</v>
       </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
         <v>10</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>958</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1448,26 +1494,32 @@
       <c r="D6" t="s">
         <v>107</v>
       </c>
-      <c r="F6">
+      <c r="E6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H6">
         <v>18</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>10</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>7</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>2000</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1478,28 +1530,34 @@
         <v>125</v>
       </c>
       <c r="E7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F7">
+        <v>130</v>
+      </c>
+      <c r="F7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7">
         <v>11</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>3</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>5</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>625</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1509,26 +1567,32 @@
       <c r="D8" t="s">
         <v>107</v>
       </c>
-      <c r="F8">
+      <c r="E8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H8">
         <v>3021</v>
       </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8">
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
         <v>30</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>3772</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>3772</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>6064</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1539,28 +1603,34 @@
         <v>126</v>
       </c>
       <c r="E9" t="s">
-        <v>115</v>
-      </c>
-      <c r="F9">
+        <v>117</v>
+      </c>
+      <c r="F9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G9" t="s">
+        <v>115</v>
+      </c>
+      <c r="H9">
         <v>29</v>
       </c>
-      <c r="G9">
-        <v>2</v>
-      </c>
-      <c r="H9">
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
         <v>16</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>690</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>37</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1570,26 +1640,32 @@
       <c r="D10" t="s">
         <v>107</v>
       </c>
-      <c r="F10">
+      <c r="E10" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" t="s">
+        <v>115</v>
+      </c>
+      <c r="H10">
         <v>41</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>19</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>36</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>683</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>121</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>2337</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -1599,26 +1675,32 @@
       <c r="D11" t="s">
         <v>107</v>
       </c>
-      <c r="F11">
+      <c r="E11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H11">
         <v>1779</v>
       </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
-      <c r="H11">
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
         <v>10</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>699</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>16</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1628,26 +1710,32 @@
       <c r="D12" t="s">
         <v>107</v>
       </c>
-      <c r="F12">
+      <c r="E12" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" t="s">
+        <v>115</v>
+      </c>
+      <c r="H12">
         <v>23</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>3</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>10</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>1473</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -1657,26 +1745,32 @@
       <c r="D13" t="s">
         <v>107</v>
       </c>
-      <c r="F13">
+      <c r="E13" t="s">
+        <v>129</v>
+      </c>
+      <c r="G13" t="s">
+        <v>115</v>
+      </c>
+      <c r="H13">
         <v>3561</v>
       </c>
-      <c r="G13">
-        <v>2</v>
-      </c>
-      <c r="H13">
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
         <v>10</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <v>672</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <v>666</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <v>1200</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1686,26 +1780,32 @@
       <c r="D14" t="s">
         <v>107</v>
       </c>
-      <c r="F14">
+      <c r="E14" t="s">
+        <v>129</v>
+      </c>
+      <c r="G14" t="s">
+        <v>115</v>
+      </c>
+      <c r="H14">
         <v>1788</v>
       </c>
-      <c r="G14">
-        <v>2</v>
-      </c>
-      <c r="H14">
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
         <v>23</v>
       </c>
-      <c r="I14">
+      <c r="K14">
         <v>8124</v>
       </c>
-      <c r="J14">
+      <c r="L14">
         <v>2480</v>
       </c>
-      <c r="K14">
+      <c r="M14">
         <v>2480</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1715,26 +1815,32 @@
       <c r="D15" t="s">
         <v>107</v>
       </c>
-      <c r="F15">
+      <c r="E15" t="s">
+        <v>129</v>
+      </c>
+      <c r="G15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H15">
         <v>28</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <v>10</v>
       </c>
-      <c r="H15">
+      <c r="J15">
         <v>65</v>
       </c>
-      <c r="I15">
+      <c r="K15">
         <v>5620</v>
       </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1745,28 +1851,34 @@
         <v>126</v>
       </c>
       <c r="E16" t="s">
-        <v>115</v>
-      </c>
-      <c r="F16">
+        <v>117</v>
+      </c>
+      <c r="F16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" t="s">
+        <v>115</v>
+      </c>
+      <c r="H16">
         <v>31</v>
       </c>
-      <c r="G16">
-        <v>2</v>
-      </c>
-      <c r="H16">
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
         <v>21</v>
       </c>
-      <c r="I16">
+      <c r="K16">
         <v>1000</v>
       </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1776,26 +1888,32 @@
       <c r="D17" t="s">
         <v>107</v>
       </c>
-      <c r="F17">
+      <c r="E17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G17" t="s">
+        <v>115</v>
+      </c>
+      <c r="H17">
         <v>32</v>
       </c>
-      <c r="G17">
+      <c r="I17">
         <v>10</v>
       </c>
-      <c r="H17">
+      <c r="J17">
         <v>17</v>
       </c>
-      <c r="I17">
+      <c r="K17">
         <v>10992</v>
       </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -1805,26 +1923,32 @@
       <c r="D18" t="s">
         <v>107</v>
       </c>
-      <c r="F18">
+      <c r="E18" t="s">
+        <v>129</v>
+      </c>
+      <c r="G18" t="s">
+        <v>115</v>
+      </c>
+      <c r="H18">
         <v>3</v>
       </c>
-      <c r="G18">
-        <v>2</v>
-      </c>
-      <c r="H18">
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
         <v>37</v>
       </c>
-      <c r="I18">
+      <c r="K18">
         <v>3196</v>
       </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -1834,26 +1958,32 @@
       <c r="D19" t="s">
         <v>107</v>
       </c>
-      <c r="F19">
+      <c r="E19" t="s">
+        <v>129</v>
+      </c>
+      <c r="G19" t="s">
+        <v>115</v>
+      </c>
+      <c r="H19">
         <v>6</v>
       </c>
-      <c r="G19">
+      <c r="I19">
         <v>26</v>
       </c>
-      <c r="H19">
+      <c r="J19">
         <v>17</v>
       </c>
-      <c r="I19">
+      <c r="K19">
         <v>20000</v>
       </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
@@ -1863,26 +1993,32 @@
       <c r="D20" t="s">
         <v>114</v>
       </c>
-      <c r="F20">
+      <c r="E20" t="s">
+        <v>129</v>
+      </c>
+      <c r="G20" t="s">
+        <v>115</v>
+      </c>
+      <c r="H20">
         <v>12</v>
       </c>
-      <c r="G20">
+      <c r="I20">
         <v>10</v>
       </c>
-      <c r="H20">
+      <c r="J20">
         <v>217</v>
       </c>
-      <c r="I20">
+      <c r="K20">
         <v>2000</v>
       </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
@@ -1892,26 +2028,32 @@
       <c r="D21" t="s">
         <v>107</v>
       </c>
-      <c r="F21">
+      <c r="E21" t="s">
+        <v>129</v>
+      </c>
+      <c r="G21" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21">
         <v>1778</v>
       </c>
-      <c r="G21">
+      <c r="I21">
         <v>10</v>
       </c>
-      <c r="H21">
+      <c r="J21">
         <v>77</v>
       </c>
-      <c r="I21">
+      <c r="K21">
         <v>2000</v>
       </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
@@ -1921,26 +2063,32 @@
       <c r="D22" t="s">
         <v>107</v>
       </c>
-      <c r="F22">
+      <c r="E22" t="s">
+        <v>129</v>
+      </c>
+      <c r="G22" t="s">
+        <v>115</v>
+      </c>
+      <c r="H22">
         <v>16</v>
       </c>
-      <c r="G22">
+      <c r="I22">
         <v>10</v>
       </c>
-      <c r="H22">
+      <c r="J22">
         <v>65</v>
       </c>
-      <c r="I22">
+      <c r="K22">
         <v>2000</v>
       </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -1950,26 +2098,32 @@
       <c r="D23" t="s">
         <v>107</v>
       </c>
-      <c r="F23">
+      <c r="E23" t="s">
+        <v>129</v>
+      </c>
+      <c r="G23" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23">
         <v>22</v>
       </c>
-      <c r="G23">
+      <c r="I23">
         <v>10</v>
       </c>
-      <c r="H23">
+      <c r="J23">
         <v>48</v>
       </c>
-      <c r="I23">
+      <c r="K23">
         <v>2000</v>
       </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
@@ -1979,26 +2133,32 @@
       <c r="D24" t="s">
         <v>107</v>
       </c>
-      <c r="F24">
+      <c r="E24" t="s">
+        <v>129</v>
+      </c>
+      <c r="G24" t="s">
+        <v>115</v>
+      </c>
+      <c r="H24">
         <v>36</v>
       </c>
-      <c r="G24">
+      <c r="I24">
         <v>7</v>
       </c>
-      <c r="H24">
+      <c r="J24">
         <v>20</v>
       </c>
-      <c r="I24">
+      <c r="K24">
         <v>2310</v>
       </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
@@ -2011,26 +2171,32 @@
       <c r="D25" t="s">
         <v>107</v>
       </c>
-      <c r="F25">
+      <c r="E25" t="s">
+        <v>129</v>
+      </c>
+      <c r="G25" t="s">
+        <v>115</v>
+      </c>
+      <c r="H25">
         <v>43</v>
       </c>
-      <c r="G25">
-        <v>2</v>
-      </c>
-      <c r="H25">
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25">
         <v>58</v>
       </c>
-      <c r="I25">
+      <c r="K25">
         <v>4601</v>
       </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
@@ -2040,26 +2206,32 @@
       <c r="D26" t="s">
         <v>107</v>
       </c>
-      <c r="F26">
+      <c r="E26" t="s">
+        <v>129</v>
+      </c>
+      <c r="G26" t="s">
+        <v>115</v>
+      </c>
+      <c r="H26">
         <v>45</v>
       </c>
-      <c r="G26">
+      <c r="I26">
         <v>3</v>
       </c>
-      <c r="H26">
+      <c r="J26">
         <v>62</v>
       </c>
-      <c r="I26">
+      <c r="K26">
         <v>3190</v>
       </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
@@ -2069,26 +2241,32 @@
       <c r="D27" t="s">
         <v>107</v>
       </c>
-      <c r="F27">
+      <c r="E27" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" t="s">
+        <v>115</v>
+      </c>
+      <c r="H27">
         <v>58</v>
       </c>
-      <c r="G27">
+      <c r="I27">
         <v>3</v>
       </c>
-      <c r="H27">
+      <c r="J27">
         <v>41</v>
       </c>
-      <c r="I27">
+      <c r="K27">
         <v>5000</v>
       </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -2098,26 +2276,32 @@
       <c r="D28" t="s">
         <v>107</v>
       </c>
-      <c r="F28">
+      <c r="E28" t="s">
+        <v>129</v>
+      </c>
+      <c r="G28" t="s">
+        <v>115</v>
+      </c>
+      <c r="H28">
         <v>2074</v>
       </c>
-      <c r="G28">
+      <c r="I28">
         <v>6</v>
       </c>
-      <c r="H28">
+      <c r="J28">
         <v>37</v>
       </c>
-      <c r="I28">
+      <c r="K28">
         <v>6430</v>
       </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -2131,28 +2315,34 @@
         <v>113</v>
       </c>
       <c r="E29" t="s">
-        <v>115</v>
-      </c>
-      <c r="F29">
+        <v>113</v>
+      </c>
+      <c r="F29" t="s">
+        <v>115</v>
+      </c>
+      <c r="G29" t="s">
+        <v>115</v>
+      </c>
+      <c r="H29">
         <v>2125</v>
       </c>
-      <c r="G29">
+      <c r="I29">
         <v>5</v>
       </c>
-      <c r="H29">
+      <c r="J29">
         <v>20</v>
       </c>
-      <c r="I29">
+      <c r="K29">
         <v>736</v>
       </c>
-      <c r="J29">
+      <c r="L29">
         <v>95</v>
       </c>
-      <c r="K29">
+      <c r="M29">
         <v>448</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -2162,26 +2352,32 @@
       <c r="D30" t="s">
         <v>114</v>
       </c>
-      <c r="F30">
+      <c r="E30" t="s">
+        <v>129</v>
+      </c>
+      <c r="G30" t="s">
+        <v>115</v>
+      </c>
+      <c r="H30">
         <v>3022</v>
       </c>
-      <c r="G30">
+      <c r="I30">
         <v>11</v>
       </c>
-      <c r="H30">
+      <c r="J30">
         <v>13</v>
       </c>
-      <c r="I30">
+      <c r="K30">
         <v>990</v>
       </c>
-      <c r="J30">
-        <v>0</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -2191,26 +2387,32 @@
       <c r="D31" t="s">
         <v>107</v>
       </c>
-      <c r="F31">
+      <c r="E31" t="s">
+        <v>129</v>
+      </c>
+      <c r="G31" t="s">
+        <v>115</v>
+      </c>
+      <c r="H31">
         <v>3485</v>
       </c>
-      <c r="G31">
-        <v>2</v>
-      </c>
-      <c r="H31">
+      <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="J31">
         <v>300</v>
       </c>
-      <c r="I31">
+      <c r="K31">
         <v>2407</v>
       </c>
-      <c r="J31">
-        <v>0</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
@@ -2221,28 +2423,34 @@
         <v>113</v>
       </c>
       <c r="E32" t="s">
-        <v>115</v>
-      </c>
-      <c r="F32" s="2">
+        <v>113</v>
+      </c>
+      <c r="F32" t="s">
+        <v>115</v>
+      </c>
+      <c r="G32" t="s">
+        <v>115</v>
+      </c>
+      <c r="H32" s="2">
         <v>3492</v>
       </c>
-      <c r="G32">
-        <v>2</v>
-      </c>
-      <c r="H32">
+      <c r="I32">
+        <v>2</v>
+      </c>
+      <c r="J32">
         <v>7</v>
       </c>
-      <c r="I32">
+      <c r="K32">
         <v>556</v>
       </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>32</v>
       </c>
@@ -2253,28 +2461,34 @@
         <v>128</v>
       </c>
       <c r="E33" t="s">
-        <v>115</v>
-      </c>
-      <c r="F33">
+        <v>113</v>
+      </c>
+      <c r="F33" t="s">
+        <v>115</v>
+      </c>
+      <c r="G33" t="s">
+        <v>115</v>
+      </c>
+      <c r="H33">
         <v>3493</v>
       </c>
-      <c r="G33">
-        <v>2</v>
-      </c>
-      <c r="H33">
+      <c r="I33">
+        <v>2</v>
+      </c>
+      <c r="J33">
         <v>7</v>
       </c>
-      <c r="I33">
+      <c r="K33">
         <v>601</v>
       </c>
-      <c r="J33">
-        <v>0</v>
-      </c>
-      <c r="K33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
@@ -2285,28 +2499,34 @@
         <v>107</v>
       </c>
       <c r="E34" t="s">
-        <v>115</v>
-      </c>
-      <c r="F34">
+        <v>129</v>
+      </c>
+      <c r="F34" t="s">
+        <v>115</v>
+      </c>
+      <c r="G34" t="s">
+        <v>115</v>
+      </c>
+      <c r="H34">
         <v>3494</v>
       </c>
-      <c r="G34">
-        <v>2</v>
-      </c>
-      <c r="H34">
+      <c r="I34">
+        <v>2</v>
+      </c>
+      <c r="J34">
         <v>7</v>
       </c>
-      <c r="I34">
+      <c r="K34">
         <v>554</v>
       </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
-      <c r="K34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -2316,26 +2536,32 @@
       <c r="D35" t="s">
         <v>107</v>
       </c>
-      <c r="F35">
+      <c r="E35" t="s">
+        <v>129</v>
+      </c>
+      <c r="G35" t="s">
+        <v>115</v>
+      </c>
+      <c r="H35">
         <v>4544</v>
       </c>
-      <c r="G35">
+      <c r="I35">
         <v>9</v>
       </c>
-      <c r="H35">
+      <c r="J35">
         <v>15</v>
       </c>
-      <c r="I35">
+      <c r="K35">
         <v>9961</v>
       </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
@@ -2345,26 +2571,32 @@
       <c r="D36" t="s">
         <v>107</v>
       </c>
-      <c r="F36">
+      <c r="E36" t="s">
+        <v>129</v>
+      </c>
+      <c r="G36" t="s">
+        <v>115</v>
+      </c>
+      <c r="H36">
         <v>3512</v>
       </c>
-      <c r="G36">
+      <c r="I36">
         <v>6</v>
       </c>
-      <c r="H36">
+      <c r="J36">
         <v>62</v>
       </c>
-      <c r="I36">
+      <c r="K36">
         <v>600</v>
       </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
@@ -2374,26 +2606,32 @@
       <c r="D37" t="s">
         <v>107</v>
       </c>
-      <c r="F37">
+      <c r="E37" t="s">
+        <v>129</v>
+      </c>
+      <c r="G37" t="s">
+        <v>115</v>
+      </c>
+      <c r="H37">
         <v>3543</v>
       </c>
-      <c r="G37">
-        <v>2</v>
-      </c>
-      <c r="H37">
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37">
         <v>6</v>
       </c>
-      <c r="I37">
+      <c r="K37">
         <v>500</v>
       </c>
-      <c r="J37">
+      <c r="L37">
         <v>32</v>
       </c>
-      <c r="K37">
+      <c r="M37">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
@@ -2403,26 +2641,32 @@
       <c r="D38" t="s">
         <v>107</v>
       </c>
-      <c r="F38">
+      <c r="E38" t="s">
+        <v>129</v>
+      </c>
+      <c r="G38" t="s">
+        <v>115</v>
+      </c>
+      <c r="H38">
         <v>3549</v>
       </c>
-      <c r="G38">
+      <c r="I38">
         <v>4</v>
       </c>
-      <c r="H38">
+      <c r="J38">
         <v>71</v>
       </c>
-      <c r="I38">
+      <c r="K38">
         <v>841</v>
       </c>
-      <c r="J38">
-        <v>0</v>
-      </c>
-      <c r="K38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
@@ -2432,26 +2676,32 @@
       <c r="D39" t="s">
         <v>107</v>
       </c>
-      <c r="F39">
+      <c r="E39" t="s">
+        <v>129</v>
+      </c>
+      <c r="G39" t="s">
+        <v>115</v>
+      </c>
+      <c r="H39">
         <v>3560</v>
       </c>
-      <c r="G39">
+      <c r="I39">
         <v>6</v>
       </c>
-      <c r="H39">
+      <c r="J39">
         <v>5</v>
       </c>
-      <c r="I39">
+      <c r="K39">
         <v>797</v>
       </c>
-      <c r="J39">
-        <v>0</v>
-      </c>
-      <c r="K39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>42</v>
       </c>
@@ -2461,26 +2711,32 @@
       <c r="D40" t="s">
         <v>107</v>
       </c>
-      <c r="F40">
+      <c r="E40" t="s">
+        <v>129</v>
+      </c>
+      <c r="G40" t="s">
+        <v>115</v>
+      </c>
+      <c r="H40">
         <v>3899</v>
       </c>
-      <c r="G40">
-        <v>2</v>
-      </c>
-      <c r="H40">
+      <c r="I40">
+        <v>2</v>
+      </c>
+      <c r="J40">
         <v>6</v>
       </c>
-      <c r="I40">
+      <c r="K40">
         <v>15545</v>
       </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>43</v>
       </c>
@@ -2490,26 +2746,32 @@
       <c r="D41" t="s">
         <v>107</v>
       </c>
-      <c r="F41">
+      <c r="E41" t="s">
+        <v>129</v>
+      </c>
+      <c r="G41" t="s">
+        <v>115</v>
+      </c>
+      <c r="H41">
         <v>3902</v>
       </c>
-      <c r="G41">
-        <v>2</v>
-      </c>
-      <c r="H41">
+      <c r="I41">
+        <v>2</v>
+      </c>
+      <c r="J41">
         <v>38</v>
       </c>
-      <c r="I41">
+      <c r="K41">
         <v>1458</v>
       </c>
-      <c r="J41">
-        <v>0</v>
-      </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>44</v>
       </c>
@@ -2519,26 +2781,32 @@
       <c r="D42" t="s">
         <v>107</v>
       </c>
-      <c r="F42">
+      <c r="E42" t="s">
+        <v>129</v>
+      </c>
+      <c r="G42" t="s">
+        <v>115</v>
+      </c>
+      <c r="H42">
         <v>3903</v>
       </c>
-      <c r="G42">
-        <v>2</v>
-      </c>
-      <c r="H42">
+      <c r="I42">
+        <v>2</v>
+      </c>
+      <c r="J42">
         <v>38</v>
       </c>
-      <c r="I42">
+      <c r="K42">
         <v>1563</v>
       </c>
-      <c r="J42">
-        <v>0</v>
-      </c>
-      <c r="K42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>45</v>
       </c>
@@ -2548,26 +2816,32 @@
       <c r="D43" t="s">
         <v>107</v>
       </c>
-      <c r="F43">
+      <c r="E43" t="s">
+        <v>129</v>
+      </c>
+      <c r="G43" t="s">
+        <v>115</v>
+      </c>
+      <c r="H43">
         <v>3904</v>
       </c>
-      <c r="G43">
-        <v>2</v>
-      </c>
-      <c r="H43">
+      <c r="I43">
+        <v>2</v>
+      </c>
+      <c r="J43">
         <v>22</v>
       </c>
-      <c r="I43">
+      <c r="K43">
         <v>10885</v>
       </c>
-      <c r="J43">
+      <c r="L43">
         <v>5</v>
       </c>
-      <c r="K43">
+      <c r="M43">
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>46</v>
       </c>
@@ -2577,26 +2851,32 @@
       <c r="D44" t="s">
         <v>107</v>
       </c>
-      <c r="F44">
+      <c r="E44" t="s">
+        <v>129</v>
+      </c>
+      <c r="G44" t="s">
+        <v>115</v>
+      </c>
+      <c r="H44">
         <v>3913</v>
       </c>
-      <c r="G44">
-        <v>2</v>
-      </c>
-      <c r="H44">
+      <c r="I44">
+        <v>2</v>
+      </c>
+      <c r="J44">
         <v>22</v>
       </c>
-      <c r="I44">
+      <c r="K44">
         <v>522</v>
       </c>
-      <c r="J44">
-        <v>0</v>
-      </c>
-      <c r="K44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>47</v>
       </c>
@@ -2606,26 +2886,32 @@
       <c r="D45" t="s">
         <v>107</v>
       </c>
-      <c r="F45">
+      <c r="E45" t="s">
+        <v>129</v>
+      </c>
+      <c r="G45" t="s">
+        <v>115</v>
+      </c>
+      <c r="H45">
         <v>3917</v>
       </c>
-      <c r="G45">
-        <v>2</v>
-      </c>
-      <c r="H45">
+      <c r="I45">
+        <v>2</v>
+      </c>
+      <c r="J45">
         <v>22</v>
       </c>
-      <c r="I45">
+      <c r="K45">
         <v>2109</v>
       </c>
-      <c r="J45">
-        <v>0</v>
-      </c>
-      <c r="K45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>48</v>
       </c>
@@ -2635,26 +2921,32 @@
       <c r="D46" t="s">
         <v>107</v>
       </c>
-      <c r="F46">
+      <c r="E46" t="s">
+        <v>129</v>
+      </c>
+      <c r="G46" t="s">
+        <v>115</v>
+      </c>
+      <c r="H46">
         <v>3918</v>
       </c>
-      <c r="G46">
-        <v>2</v>
-      </c>
-      <c r="H46">
+      <c r="I46">
+        <v>2</v>
+      </c>
+      <c r="J46">
         <v>22</v>
       </c>
-      <c r="I46">
+      <c r="K46">
         <v>1109</v>
       </c>
-      <c r="J46">
-        <v>0</v>
-      </c>
-      <c r="K46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
@@ -2665,28 +2957,34 @@
         <v>119</v>
       </c>
       <c r="E47" t="s">
+        <v>129</v>
+      </c>
+      <c r="F47" t="s">
         <v>105</v>
       </c>
-      <c r="F47">
+      <c r="G47" t="s">
+        <v>115</v>
+      </c>
+      <c r="H47">
         <v>3954</v>
       </c>
-      <c r="G47">
-        <v>2</v>
-      </c>
-      <c r="H47">
+      <c r="I47">
+        <v>2</v>
+      </c>
+      <c r="J47">
         <v>12</v>
       </c>
-      <c r="I47">
+      <c r="K47">
         <v>19020</v>
       </c>
-      <c r="J47">
-        <v>0</v>
-      </c>
-      <c r="K47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L47">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>52</v>
       </c>
@@ -2697,28 +2995,34 @@
         <v>113</v>
       </c>
       <c r="E48" t="s">
+        <v>113</v>
+      </c>
+      <c r="F48" t="s">
         <v>105</v>
       </c>
-      <c r="F48">
+      <c r="G48" t="s">
+        <v>115</v>
+      </c>
+      <c r="H48">
         <v>14964</v>
       </c>
-      <c r="G48">
+      <c r="I48">
         <v>10</v>
       </c>
-      <c r="H48">
+      <c r="J48">
         <v>8</v>
       </c>
-      <c r="I48">
+      <c r="K48">
         <v>10218</v>
       </c>
-      <c r="J48">
-        <v>0</v>
-      </c>
-      <c r="K48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>25</v>
       </c>
@@ -2729,28 +3033,34 @@
         <v>118</v>
       </c>
       <c r="E49" t="s">
+        <v>113</v>
+      </c>
+      <c r="F49" t="s">
         <v>105</v>
       </c>
-      <c r="F49">
+      <c r="G49" t="s">
+        <v>115</v>
+      </c>
+      <c r="H49">
         <v>219</v>
       </c>
-      <c r="G49">
-        <v>2</v>
-      </c>
-      <c r="H49">
+      <c r="I49">
+        <v>2</v>
+      </c>
+      <c r="J49">
         <v>9</v>
       </c>
-      <c r="I49">
+      <c r="K49">
         <v>45312</v>
       </c>
-      <c r="J49">
-        <v>0</v>
-      </c>
-      <c r="K49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>54</v>
       </c>
@@ -2760,26 +3070,32 @@
       <c r="D50" t="s">
         <v>107</v>
       </c>
-      <c r="F50" s="2">
+      <c r="E50" t="s">
+        <v>129</v>
+      </c>
+      <c r="G50" t="s">
+        <v>115</v>
+      </c>
+      <c r="H50" s="2">
         <v>10093</v>
       </c>
-      <c r="G50">
-        <v>2</v>
-      </c>
-      <c r="H50">
+      <c r="I50">
+        <v>2</v>
+      </c>
+      <c r="J50">
         <v>5</v>
       </c>
-      <c r="I50">
+      <c r="K50">
         <v>1372</v>
       </c>
-      <c r="J50">
-        <v>0</v>
-      </c>
-      <c r="K50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
@@ -2789,26 +3105,32 @@
       <c r="D51" t="s">
         <v>107</v>
       </c>
-      <c r="F51">
+      <c r="E51" t="s">
+        <v>129</v>
+      </c>
+      <c r="G51" t="s">
+        <v>115</v>
+      </c>
+      <c r="H51">
         <v>10101</v>
       </c>
-      <c r="G51">
-        <v>2</v>
-      </c>
-      <c r="H51">
+      <c r="I51">
+        <v>2</v>
+      </c>
+      <c r="J51">
         <v>5</v>
       </c>
-      <c r="I51">
+      <c r="K51">
         <v>748</v>
       </c>
-      <c r="J51">
-        <v>0</v>
-      </c>
-      <c r="K51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>56</v>
       </c>
@@ -2818,26 +3140,32 @@
       <c r="D52" t="s">
         <v>107</v>
       </c>
-      <c r="F52">
+      <c r="E52" t="s">
+        <v>129</v>
+      </c>
+      <c r="G52" t="s">
+        <v>115</v>
+      </c>
+      <c r="H52">
         <v>9979</v>
       </c>
-      <c r="G52">
+      <c r="I52">
         <v>10</v>
       </c>
-      <c r="H52">
+      <c r="J52">
         <v>36</v>
       </c>
-      <c r="I52">
+      <c r="K52">
         <v>2126</v>
       </c>
-      <c r="J52">
-        <v>0</v>
-      </c>
-      <c r="K52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>57</v>
       </c>
@@ -2847,26 +3175,32 @@
       <c r="D53" t="s">
         <v>114</v>
       </c>
-      <c r="F53">
+      <c r="E53" t="s">
+        <v>129</v>
+      </c>
+      <c r="G53" t="s">
+        <v>115</v>
+      </c>
+      <c r="H53">
         <v>9980</v>
       </c>
-      <c r="G53">
-        <v>2</v>
-      </c>
-      <c r="H53">
+      <c r="I53">
+        <v>2</v>
+      </c>
+      <c r="J53">
         <v>21</v>
       </c>
-      <c r="I53">
+      <c r="K53">
         <v>540</v>
       </c>
-      <c r="J53">
-        <v>0</v>
-      </c>
-      <c r="K53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
@@ -2876,26 +3210,32 @@
       <c r="D54" t="s">
         <v>107</v>
       </c>
-      <c r="F54">
+      <c r="E54" t="s">
+        <v>129</v>
+      </c>
+      <c r="G54" t="s">
+        <v>115</v>
+      </c>
+      <c r="H54">
         <v>9983</v>
       </c>
-      <c r="G54">
-        <v>2</v>
-      </c>
-      <c r="H54">
+      <c r="I54">
+        <v>2</v>
+      </c>
+      <c r="J54">
         <v>15</v>
       </c>
-      <c r="I54">
+      <c r="K54">
         <v>14980</v>
       </c>
-      <c r="J54">
-        <v>0</v>
-      </c>
-      <c r="K54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>60</v>
       </c>
@@ -2906,28 +3246,34 @@
         <v>119</v>
       </c>
       <c r="E55" t="s">
+        <v>129</v>
+      </c>
+      <c r="F55" t="s">
         <v>105</v>
       </c>
-      <c r="F55">
+      <c r="G55" t="s">
+        <v>115</v>
+      </c>
+      <c r="H55">
         <v>9985</v>
       </c>
-      <c r="G55">
+      <c r="I55">
         <v>6</v>
       </c>
-      <c r="H55">
+      <c r="J55">
         <v>52</v>
       </c>
-      <c r="I55">
+      <c r="K55">
         <v>6118</v>
       </c>
-      <c r="J55">
-        <v>0</v>
-      </c>
-      <c r="K55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>63</v>
       </c>
@@ -2937,26 +3283,32 @@
       <c r="D56" t="s">
         <v>107</v>
       </c>
-      <c r="F56">
+      <c r="E56" t="s">
+        <v>129</v>
+      </c>
+      <c r="G56" t="s">
+        <v>115</v>
+      </c>
+      <c r="H56">
         <v>9970</v>
       </c>
-      <c r="G56">
-        <v>2</v>
-      </c>
-      <c r="H56">
+      <c r="I56">
+        <v>2</v>
+      </c>
+      <c r="J56">
         <v>101</v>
       </c>
-      <c r="I56">
+      <c r="K56">
         <v>1212</v>
       </c>
-      <c r="J56">
-        <v>0</v>
-      </c>
-      <c r="K56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>64</v>
       </c>
@@ -2966,26 +3318,32 @@
       <c r="D57" t="s">
         <v>107</v>
       </c>
-      <c r="F57">
+      <c r="E57" t="s">
+        <v>129</v>
+      </c>
+      <c r="G57" t="s">
+        <v>115</v>
+      </c>
+      <c r="H57">
         <v>9971</v>
       </c>
-      <c r="G57">
-        <v>2</v>
-      </c>
-      <c r="H57">
+      <c r="I57">
+        <v>2</v>
+      </c>
+      <c r="J57">
         <v>11</v>
       </c>
-      <c r="I57">
+      <c r="K57">
         <v>583</v>
       </c>
-      <c r="J57">
-        <v>0</v>
-      </c>
-      <c r="K57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>66</v>
       </c>
@@ -2998,55 +3356,64 @@
       <c r="D58" t="s">
         <v>108</v>
       </c>
-      <c r="F58">
+      <c r="E58" t="s">
+        <v>108</v>
+      </c>
+      <c r="H58">
         <v>9977</v>
       </c>
-      <c r="G58">
-        <v>2</v>
-      </c>
-      <c r="H58">
+      <c r="I58">
+        <v>2</v>
+      </c>
+      <c r="J58">
         <v>119</v>
       </c>
-      <c r="I58">
+      <c r="K58">
         <v>34465</v>
       </c>
-      <c r="J58">
-        <v>0</v>
-      </c>
-      <c r="K58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B59" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="D59" t="s">
         <v>107</v>
       </c>
-      <c r="F59">
+      <c r="E59" t="s">
+        <v>129</v>
+      </c>
+      <c r="G59" t="s">
+        <v>115</v>
+      </c>
+      <c r="H59">
         <v>9978</v>
       </c>
-      <c r="G59">
-        <v>2</v>
-      </c>
-      <c r="H59">
+      <c r="I59">
+        <v>2</v>
+      </c>
+      <c r="J59">
         <v>73</v>
       </c>
-      <c r="I59">
+      <c r="K59">
         <v>2534</v>
       </c>
-      <c r="J59">
-        <v>0</v>
-      </c>
-      <c r="K59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>68</v>
       </c>
@@ -3056,26 +3423,32 @@
       <c r="D60" t="s">
         <v>107</v>
       </c>
-      <c r="F60">
+      <c r="E60" t="s">
+        <v>129</v>
+      </c>
+      <c r="G60" t="s">
+        <v>115</v>
+      </c>
+      <c r="H60">
         <v>9952</v>
       </c>
-      <c r="G60">
-        <v>2</v>
-      </c>
-      <c r="H60">
+      <c r="I60">
+        <v>2</v>
+      </c>
+      <c r="J60">
         <v>6</v>
       </c>
-      <c r="I60">
+      <c r="K60">
         <v>5404</v>
       </c>
-      <c r="J60">
-        <v>0</v>
-      </c>
-      <c r="K60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>69</v>
       </c>
@@ -3086,28 +3459,34 @@
         <v>113</v>
       </c>
       <c r="E61" t="s">
+        <v>113</v>
+      </c>
+      <c r="F61" t="s">
         <v>105</v>
       </c>
-      <c r="F61">
+      <c r="G61" t="s">
+        <v>115</v>
+      </c>
+      <c r="H61">
         <v>9954</v>
       </c>
-      <c r="G61">
+      <c r="I61">
         <v>100</v>
       </c>
-      <c r="H61">
+      <c r="J61">
         <v>65</v>
       </c>
-      <c r="I61">
+      <c r="K61">
         <v>1600</v>
       </c>
-      <c r="J61">
-        <v>0</v>
-      </c>
-      <c r="K61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>70</v>
       </c>
@@ -3118,28 +3497,34 @@
         <v>113</v>
       </c>
       <c r="E62" t="s">
+        <v>113</v>
+      </c>
+      <c r="F62" t="s">
         <v>105</v>
       </c>
-      <c r="F62">
+      <c r="G62" t="s">
+        <v>115</v>
+      </c>
+      <c r="H62">
         <v>9955</v>
       </c>
-      <c r="G62">
+      <c r="I62">
         <v>100</v>
       </c>
-      <c r="H62">
+      <c r="J62">
         <v>65</v>
       </c>
-      <c r="I62">
+      <c r="K62">
         <v>1600</v>
       </c>
-      <c r="J62">
-        <v>0</v>
-      </c>
-      <c r="K62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>72</v>
       </c>
@@ -3149,26 +3534,32 @@
       <c r="D63" t="s">
         <v>107</v>
       </c>
-      <c r="F63">
+      <c r="E63" t="s">
+        <v>129</v>
+      </c>
+      <c r="G63" t="s">
+        <v>115</v>
+      </c>
+      <c r="H63">
         <v>9957</v>
       </c>
-      <c r="G63">
-        <v>2</v>
-      </c>
-      <c r="H63">
+      <c r="I63">
+        <v>2</v>
+      </c>
+      <c r="J63">
         <v>42</v>
       </c>
-      <c r="I63">
+      <c r="K63">
         <v>1055</v>
       </c>
-      <c r="J63">
-        <v>0</v>
-      </c>
-      <c r="K63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L63">
+        <v>0</v>
+      </c>
+      <c r="M63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>73</v>
       </c>
@@ -3178,26 +3569,32 @@
       <c r="D64" t="s">
         <v>107</v>
       </c>
-      <c r="F64">
+      <c r="E64" t="s">
+        <v>129</v>
+      </c>
+      <c r="G64" t="s">
+        <v>115</v>
+      </c>
+      <c r="H64">
         <v>9960</v>
       </c>
-      <c r="G64">
+      <c r="I64">
         <v>4</v>
       </c>
-      <c r="H64">
+      <c r="J64">
         <v>25</v>
       </c>
-      <c r="I64">
+      <c r="K64">
         <v>5456</v>
       </c>
-      <c r="J64">
-        <v>0</v>
-      </c>
-      <c r="K64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L64">
+        <v>0</v>
+      </c>
+      <c r="M64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>75</v>
       </c>
@@ -3207,26 +3604,32 @@
       <c r="D65" t="s">
         <v>107</v>
       </c>
-      <c r="F65">
+      <c r="E65" t="s">
+        <v>129</v>
+      </c>
+      <c r="G65" t="s">
+        <v>115</v>
+      </c>
+      <c r="H65">
         <v>9967</v>
       </c>
-      <c r="G65">
-        <v>2</v>
-      </c>
-      <c r="H65">
+      <c r="I65">
+        <v>2</v>
+      </c>
+      <c r="J65">
         <v>34</v>
       </c>
-      <c r="I65">
+      <c r="K65">
         <v>1941</v>
       </c>
-      <c r="J65">
-        <v>0</v>
-      </c>
-      <c r="K65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>76</v>
       </c>
@@ -3236,26 +3639,32 @@
       <c r="D66" t="s">
         <v>107</v>
       </c>
-      <c r="F66">
+      <c r="E66" t="s">
+        <v>129</v>
+      </c>
+      <c r="G66" t="s">
+        <v>115</v>
+      </c>
+      <c r="H66">
         <v>9946</v>
       </c>
-      <c r="G66">
-        <v>2</v>
-      </c>
-      <c r="H66">
+      <c r="I66">
+        <v>2</v>
+      </c>
+      <c r="J66">
         <v>31</v>
       </c>
-      <c r="I66">
+      <c r="K66">
         <v>569</v>
       </c>
-      <c r="J66">
-        <v>0</v>
-      </c>
-      <c r="K66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>78</v>
       </c>
@@ -3265,26 +3674,32 @@
       <c r="D67" t="s">
         <v>107</v>
       </c>
-      <c r="F67">
+      <c r="E67" t="s">
+        <v>129</v>
+      </c>
+      <c r="G67" t="s">
+        <v>115</v>
+      </c>
+      <c r="H67">
         <v>7592</v>
       </c>
-      <c r="G67">
-        <v>2</v>
-      </c>
-      <c r="H67">
+      <c r="I67">
+        <v>2</v>
+      </c>
+      <c r="J67">
         <v>15</v>
       </c>
-      <c r="I67">
+      <c r="K67">
         <v>48842</v>
       </c>
-      <c r="J67">
+      <c r="L67">
         <v>3620</v>
       </c>
-      <c r="K67">
+      <c r="M67">
         <v>6465</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>82</v>
       </c>
@@ -3295,28 +3710,34 @@
         <v>113</v>
       </c>
       <c r="E68" t="s">
+        <v>113</v>
+      </c>
+      <c r="F68" t="s">
         <v>105</v>
       </c>
-      <c r="F68">
+      <c r="G68" t="s">
+        <v>115</v>
+      </c>
+      <c r="H68">
         <v>14969</v>
       </c>
-      <c r="G68">
+      <c r="I68">
         <v>5</v>
       </c>
-      <c r="H68">
+      <c r="J68">
         <v>33</v>
       </c>
-      <c r="I68">
+      <c r="K68">
         <v>9873</v>
       </c>
-      <c r="J68">
-        <v>0</v>
-      </c>
-      <c r="K68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L68">
+        <v>0</v>
+      </c>
+      <c r="M68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>83</v>
       </c>
@@ -3327,28 +3748,34 @@
         <v>127</v>
       </c>
       <c r="E69" t="s">
+        <v>130</v>
+      </c>
+      <c r="F69" t="s">
         <v>105</v>
       </c>
-      <c r="F69">
+      <c r="G69" t="s">
+        <v>115</v>
+      </c>
+      <c r="H69">
         <v>14968</v>
       </c>
-      <c r="G69">
-        <v>2</v>
-      </c>
-      <c r="H69">
+      <c r="I69">
+        <v>2</v>
+      </c>
+      <c r="J69">
         <v>40</v>
       </c>
-      <c r="I69">
+      <c r="K69">
         <v>540</v>
       </c>
-      <c r="J69">
+      <c r="L69">
         <v>263</v>
       </c>
-      <c r="K69">
+      <c r="M69">
         <v>999</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>84</v>
       </c>
@@ -3358,26 +3785,32 @@
       <c r="D70" t="s">
         <v>107</v>
       </c>
-      <c r="F70">
+      <c r="E70" t="s">
+        <v>129</v>
+      </c>
+      <c r="G70" t="s">
+        <v>115</v>
+      </c>
+      <c r="H70">
         <v>14967</v>
       </c>
-      <c r="G70">
+      <c r="I70">
         <v>6</v>
       </c>
-      <c r="H70">
+      <c r="J70">
         <v>35</v>
       </c>
-      <c r="I70">
+      <c r="K70">
         <v>2796</v>
       </c>
-      <c r="J70">
+      <c r="L70">
         <v>2795</v>
       </c>
-      <c r="K70">
+      <c r="M70">
         <v>68100</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>85</v>
       </c>
@@ -3388,28 +3821,34 @@
         <v>126</v>
       </c>
       <c r="E71" t="s">
+        <v>117</v>
+      </c>
+      <c r="F71" t="s">
         <v>105</v>
       </c>
-      <c r="F71">
+      <c r="G71" t="s">
+        <v>115</v>
+      </c>
+      <c r="H71">
         <v>125920</v>
       </c>
-      <c r="G71">
-        <v>2</v>
-      </c>
-      <c r="H71">
+      <c r="I71">
+        <v>2</v>
+      </c>
+      <c r="J71">
         <v>13</v>
       </c>
-      <c r="I71">
+      <c r="K71">
         <v>500</v>
       </c>
-      <c r="J71">
+      <c r="L71">
         <v>401</v>
       </c>
-      <c r="K71">
+      <c r="M71">
         <v>835</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>87</v>
       </c>
@@ -3419,26 +3858,32 @@
       <c r="D72" t="s">
         <v>107</v>
       </c>
-      <c r="F72">
+      <c r="E72" t="s">
+        <v>129</v>
+      </c>
+      <c r="G72" t="s">
+        <v>115</v>
+      </c>
+      <c r="H72">
         <v>125921</v>
       </c>
-      <c r="G72">
+      <c r="I72">
         <v>10</v>
       </c>
-      <c r="H72">
+      <c r="J72">
         <v>8</v>
       </c>
-      <c r="I72">
+      <c r="K72">
         <v>500</v>
       </c>
-      <c r="J72">
-        <v>0</v>
-      </c>
-      <c r="K72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>88</v>
       </c>
@@ -3448,26 +3893,32 @@
       <c r="D73" t="s">
         <v>107</v>
       </c>
-      <c r="F73">
+      <c r="E73" t="s">
+        <v>129</v>
+      </c>
+      <c r="G73" t="s">
+        <v>115</v>
+      </c>
+      <c r="H73">
         <v>125922</v>
       </c>
-      <c r="G73">
+      <c r="I73">
         <v>11</v>
       </c>
-      <c r="H73">
+      <c r="J73">
         <v>41</v>
       </c>
-      <c r="I73">
+      <c r="K73">
         <v>5500</v>
       </c>
-      <c r="J73">
-        <v>0</v>
-      </c>
-      <c r="K73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L73">
+        <v>0</v>
+      </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>89</v>
       </c>
@@ -3477,26 +3928,29 @@
       <c r="D74" t="s">
         <v>108</v>
       </c>
-      <c r="F74">
+      <c r="E74" t="s">
+        <v>108</v>
+      </c>
+      <c r="H74">
         <v>146607</v>
       </c>
-      <c r="G74">
-        <v>2</v>
-      </c>
-      <c r="H74">
+      <c r="I74">
+        <v>2</v>
+      </c>
+      <c r="J74">
         <v>123</v>
       </c>
-      <c r="I74">
+      <c r="K74">
         <v>8378</v>
       </c>
-      <c r="J74">
+      <c r="L74">
         <v>7330</v>
       </c>
-      <c r="K74">
+      <c r="M74">
         <v>18372</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>61</v>
       </c>
@@ -3506,26 +3960,29 @@
       <c r="D75" t="s">
         <v>108</v>
       </c>
-      <c r="F75">
+      <c r="E75" t="s">
+        <v>108</v>
+      </c>
+      <c r="H75">
         <v>9986</v>
       </c>
-      <c r="G75">
+      <c r="I75">
         <v>6</v>
       </c>
-      <c r="H75">
-        <v>129</v>
-      </c>
-      <c r="I75">
+      <c r="J75">
+        <v>129</v>
+      </c>
+      <c r="K75">
         <v>13910</v>
       </c>
-      <c r="J75">
-        <v>0</v>
-      </c>
-      <c r="K75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L75">
+        <v>0</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>53</v>
       </c>
@@ -3536,28 +3993,34 @@
         <v>117</v>
       </c>
       <c r="E76" t="s">
+        <v>117</v>
+      </c>
+      <c r="F76" t="s">
         <v>105</v>
       </c>
-      <c r="F76">
+      <c r="G76" t="s">
+        <v>115</v>
+      </c>
+      <c r="H76">
         <v>14965</v>
       </c>
-      <c r="G76">
-        <v>2</v>
-      </c>
-      <c r="H76">
+      <c r="I76">
+        <v>2</v>
+      </c>
+      <c r="J76">
         <v>17</v>
       </c>
-      <c r="I76">
+      <c r="K76">
         <v>45211</v>
       </c>
-      <c r="J76">
-        <v>0</v>
-      </c>
-      <c r="K76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L76">
+        <v>0</v>
+      </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>71</v>
       </c>
@@ -3568,28 +4031,34 @@
         <v>113</v>
       </c>
       <c r="E77" t="s">
+        <v>113</v>
+      </c>
+      <c r="F77" t="s">
         <v>105</v>
       </c>
-      <c r="F77">
+      <c r="G77" t="s">
+        <v>115</v>
+      </c>
+      <c r="H77">
         <v>9956</v>
       </c>
-      <c r="G77">
+      <c r="I77">
         <v>100</v>
       </c>
-      <c r="H77">
+      <c r="J77">
         <v>65</v>
       </c>
-      <c r="I77">
+      <c r="K77">
         <v>1599</v>
       </c>
-      <c r="J77">
-        <v>0</v>
-      </c>
-      <c r="K77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L77">
+        <v>0</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>81</v>
       </c>
@@ -3599,26 +4068,32 @@
       <c r="D78" t="s">
         <v>107</v>
       </c>
-      <c r="F78">
+      <c r="E78" t="s">
+        <v>129</v>
+      </c>
+      <c r="G78" t="s">
+        <v>115</v>
+      </c>
+      <c r="H78">
         <v>34537</v>
       </c>
-      <c r="G78">
-        <v>2</v>
-      </c>
-      <c r="H78">
+      <c r="I78">
+        <v>2</v>
+      </c>
+      <c r="J78">
         <v>31</v>
       </c>
-      <c r="I78">
+      <c r="K78">
         <v>11055</v>
       </c>
-      <c r="J78">
-        <v>0</v>
-      </c>
-      <c r="K78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L78">
+        <v>0</v>
+      </c>
+      <c r="M78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>90</v>
       </c>
@@ -3629,28 +4104,34 @@
         <v>113</v>
       </c>
       <c r="E79" t="s">
+        <v>113</v>
+      </c>
+      <c r="F79" t="s">
         <v>105</v>
       </c>
-      <c r="F79">
+      <c r="G79" t="s">
+        <v>105</v>
+      </c>
+      <c r="H79">
         <v>146195</v>
       </c>
-      <c r="G79">
+      <c r="I79">
         <v>3</v>
       </c>
-      <c r="H79">
+      <c r="J79">
         <v>43</v>
       </c>
-      <c r="I79">
+      <c r="K79">
         <v>67557</v>
       </c>
-      <c r="J79">
-        <v>0</v>
-      </c>
-      <c r="K79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L79">
+        <v>0</v>
+      </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>80</v>
       </c>
@@ -3664,28 +4145,34 @@
         <v>117</v>
       </c>
       <c r="E80" t="s">
+        <v>117</v>
+      </c>
+      <c r="F80" t="s">
         <v>105</v>
       </c>
-      <c r="F80">
+      <c r="G80" t="s">
+        <v>105</v>
+      </c>
+      <c r="H80">
         <v>34539</v>
       </c>
-      <c r="G80">
-        <v>2</v>
-      </c>
-      <c r="H80">
+      <c r="I80">
+        <v>2</v>
+      </c>
+      <c r="J80">
         <v>10</v>
       </c>
-      <c r="I80">
+      <c r="K80">
         <v>32769</v>
       </c>
-      <c r="J80">
-        <v>0</v>
-      </c>
-      <c r="K80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L80">
+        <v>0</v>
+      </c>
+      <c r="M80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>62</v>
       </c>
@@ -3695,26 +4182,29 @@
       <c r="D81" t="s">
         <v>108</v>
       </c>
-      <c r="F81">
+      <c r="E81" t="s">
+        <v>108</v>
+      </c>
+      <c r="H81">
         <v>14970</v>
       </c>
-      <c r="G81">
+      <c r="I81">
         <v>6</v>
       </c>
-      <c r="H81">
+      <c r="J81">
         <v>562</v>
       </c>
-      <c r="I81">
+      <c r="K81">
         <v>10299</v>
       </c>
-      <c r="J81">
-        <v>0</v>
-      </c>
-      <c r="K81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L81">
+        <v>0</v>
+      </c>
+      <c r="M81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>79</v>
       </c>
@@ -3724,26 +4214,29 @@
       <c r="D82" t="s">
         <v>108</v>
       </c>
-      <c r="F82">
+      <c r="E82" t="s">
+        <v>108</v>
+      </c>
+      <c r="H82">
         <v>14966</v>
       </c>
-      <c r="G82">
-        <v>2</v>
-      </c>
-      <c r="H82">
+      <c r="I82">
+        <v>2</v>
+      </c>
+      <c r="J82">
         <v>1777</v>
       </c>
-      <c r="I82">
+      <c r="K82">
         <v>3751</v>
       </c>
-      <c r="J82">
-        <v>0</v>
-      </c>
-      <c r="K82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L82">
+        <v>0</v>
+      </c>
+      <c r="M82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>86</v>
       </c>
@@ -3754,28 +4247,34 @@
         <v>117</v>
       </c>
       <c r="E83" t="s">
+        <v>117</v>
+      </c>
+      <c r="F83" t="s">
         <v>105</v>
       </c>
-      <c r="F83">
+      <c r="G83" t="s">
+        <v>105</v>
+      </c>
+      <c r="H83">
         <v>146606</v>
       </c>
-      <c r="G83">
-        <v>2</v>
-      </c>
-      <c r="H83">
+      <c r="I83">
+        <v>2</v>
+      </c>
+      <c r="J83">
         <v>29</v>
       </c>
-      <c r="I83">
+      <c r="K83">
         <v>98050</v>
       </c>
-      <c r="J83">
+      <c r="L83">
         <v>1</v>
       </c>
-      <c r="K83">
+      <c r="M83">
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>40</v>
       </c>
@@ -3785,26 +4284,29 @@
       <c r="D84" t="s">
         <v>108</v>
       </c>
-      <c r="F84">
+      <c r="E84" t="s">
+        <v>108</v>
+      </c>
+      <c r="H84">
         <v>3573</v>
       </c>
-      <c r="G84">
+      <c r="I84">
         <v>10</v>
       </c>
-      <c r="H84">
+      <c r="J84">
         <v>785</v>
       </c>
-      <c r="I84">
+      <c r="K84">
         <v>70000</v>
       </c>
-      <c r="J84">
-        <v>0</v>
-      </c>
-      <c r="K84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L84">
+        <v>0</v>
+      </c>
+      <c r="M84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>41</v>
       </c>
@@ -3814,26 +4316,29 @@
       <c r="D85" t="s">
         <v>108</v>
       </c>
-      <c r="F85">
+      <c r="E85" t="s">
+        <v>108</v>
+      </c>
+      <c r="H85">
         <v>3891</v>
       </c>
-      <c r="G85">
-        <v>2</v>
-      </c>
-      <c r="H85">
+      <c r="I85">
+        <v>2</v>
+      </c>
+      <c r="J85">
         <v>971</v>
       </c>
-      <c r="I85">
+      <c r="K85">
         <v>3468</v>
       </c>
-      <c r="J85">
-        <v>0</v>
-      </c>
-      <c r="K85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L85">
+        <v>0</v>
+      </c>
+      <c r="M85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -3843,26 +4348,29 @@
       <c r="D86" t="s">
         <v>108</v>
       </c>
-      <c r="F86">
+      <c r="E86" t="s">
+        <v>108</v>
+      </c>
+      <c r="H86">
         <v>3481</v>
       </c>
-      <c r="G86">
+      <c r="I86">
         <v>26</v>
       </c>
-      <c r="H86">
+      <c r="J86">
         <v>618</v>
       </c>
-      <c r="I86">
+      <c r="K86">
         <v>7797</v>
       </c>
-      <c r="J86">
-        <v>0</v>
-      </c>
-      <c r="K86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L86">
+        <v>0</v>
+      </c>
+      <c r="M86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>58</v>
       </c>
@@ -3872,26 +4380,29 @@
       <c r="D87" t="s">
         <v>108</v>
       </c>
-      <c r="F87">
+      <c r="E87" t="s">
+        <v>108</v>
+      </c>
+      <c r="H87">
         <v>9981</v>
       </c>
-      <c r="G87">
+      <c r="I87">
         <v>9</v>
       </c>
-      <c r="H87">
+      <c r="J87">
         <v>857</v>
       </c>
-      <c r="I87">
+      <c r="K87">
         <v>1080</v>
       </c>
-      <c r="J87">
-        <v>0</v>
-      </c>
-      <c r="K87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L87">
+        <v>0</v>
+      </c>
+      <c r="M87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>74</v>
       </c>
@@ -3901,26 +4412,29 @@
       <c r="D88" t="s">
         <v>108</v>
       </c>
-      <c r="F88">
+      <c r="E88" t="s">
+        <v>108</v>
+      </c>
+      <c r="H88">
         <v>9964</v>
       </c>
-      <c r="G88">
+      <c r="I88">
         <v>10</v>
       </c>
-      <c r="H88">
+      <c r="J88">
         <v>257</v>
       </c>
-      <c r="I88">
+      <c r="K88">
         <v>1593</v>
       </c>
-      <c r="J88">
-        <v>0</v>
-      </c>
-      <c r="K88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L88">
+        <v>0</v>
+      </c>
+      <c r="M88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>77</v>
       </c>
@@ -3930,26 +4444,29 @@
       <c r="D89" t="s">
         <v>108</v>
       </c>
-      <c r="F89">
+      <c r="E89" t="s">
+        <v>108</v>
+      </c>
+      <c r="H89">
         <v>9950</v>
       </c>
-      <c r="G89">
+      <c r="I89">
         <v>20</v>
       </c>
-      <c r="H89">
+      <c r="J89">
         <v>1301</v>
       </c>
-      <c r="I89">
+      <c r="K89">
         <v>571</v>
       </c>
-      <c r="J89">
-        <v>0</v>
-      </c>
-      <c r="K89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L89">
+        <v>0</v>
+      </c>
+      <c r="M89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>65</v>
       </c>
@@ -3959,26 +4476,29 @@
       <c r="D90" t="s">
         <v>108</v>
       </c>
-      <c r="F90">
+      <c r="E90" t="s">
+        <v>108</v>
+      </c>
+      <c r="H90">
         <v>9976</v>
       </c>
-      <c r="G90">
-        <v>2</v>
-      </c>
-      <c r="H90">
+      <c r="I90">
+        <v>2</v>
+      </c>
+      <c r="J90">
         <v>501</v>
       </c>
-      <c r="I90">
+      <c r="K90">
         <v>2600</v>
       </c>
-      <c r="J90">
-        <v>0</v>
-      </c>
-      <c r="K90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L90">
+        <v>0</v>
+      </c>
+      <c r="M90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>8</v>
       </c>
@@ -3988,26 +4508,29 @@
       <c r="D91" t="s">
         <v>108</v>
       </c>
-      <c r="F91">
+      <c r="E91" t="s">
+        <v>108</v>
+      </c>
+      <c r="H91">
         <v>20</v>
       </c>
-      <c r="G91">
+      <c r="I91">
         <v>10</v>
       </c>
-      <c r="H91">
+      <c r="J91">
         <v>241</v>
       </c>
-      <c r="I91">
+      <c r="K91">
         <v>2000</v>
       </c>
-      <c r="J91">
-        <v>0</v>
-      </c>
-      <c r="K91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L91">
+        <v>0</v>
+      </c>
+      <c r="M91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>49</v>
       </c>
@@ -4017,26 +4540,29 @@
       <c r="D92" t="s">
         <v>108</v>
       </c>
-      <c r="F92">
+      <c r="E92" t="s">
+        <v>108</v>
+      </c>
+      <c r="H92">
         <v>3946</v>
       </c>
-      <c r="G92">
-        <v>2</v>
-      </c>
-      <c r="H92">
+      <c r="I92">
+        <v>2</v>
+      </c>
+      <c r="J92">
         <v>231</v>
       </c>
-      <c r="I92">
+      <c r="K92">
         <v>50000</v>
       </c>
-      <c r="J92">
+      <c r="L92">
         <v>50000</v>
       </c>
-      <c r="K92">
+      <c r="M92">
         <v>8024152</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>50</v>
       </c>
@@ -4046,22 +4572,25 @@
       <c r="D93" t="s">
         <v>108</v>
       </c>
-      <c r="F93" s="2">
+      <c r="E93" t="s">
+        <v>108</v>
+      </c>
+      <c r="H93" s="2">
         <v>3948</v>
       </c>
-      <c r="G93">
-        <v>2</v>
-      </c>
-      <c r="H93">
+      <c r="I93">
+        <v>2</v>
+      </c>
+      <c r="J93">
         <v>231</v>
       </c>
-      <c r="I93">
+      <c r="K93">
         <v>50000</v>
       </c>
-      <c r="J93">
+      <c r="L93">
         <v>50000</v>
       </c>
-      <c r="K93">
+      <c r="M93">
         <v>8024152</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MS2 - Reintroduce mastery workflow
</commit_message>
<xml_diff>
--- a/benchmark/Configuration.xlsx
+++ b/benchmark/Configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\autem\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E513ADA-BE92-4628-B517-D9EC3516C97B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5809D5-259B-4B29-9DA6-46DF63B93EE0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="135">
   <si>
     <t>kr-vs-kp</t>
   </si>
@@ -431,6 +431,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>MA2</t>
   </si>
 </sst>
 </file>
@@ -1275,13 +1278,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M93"/>
+  <dimension ref="A1:N93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G79" sqref="G79"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1291,16 +1294,16 @@
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="7" width="17.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="37" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="37" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>98</v>
       </c>
@@ -1322,26 +1325,29 @@
       <c r="G1" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1357,26 +1363,29 @@
       <c r="G2" t="s">
         <v>115</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2">
         <v>37</v>
       </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
       <c r="J2">
+        <v>2</v>
+      </c>
+      <c r="K2">
         <v>9</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>768</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
@@ -1392,26 +1401,29 @@
       <c r="G3" t="s">
         <v>115</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3">
         <v>53</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>4</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>19</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>846</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
       <c r="M3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>91</v>
       </c>
@@ -1430,26 +1442,29 @@
       <c r="G4" t="s">
         <v>115</v>
       </c>
-      <c r="H4">
+      <c r="H4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4">
         <v>125923</v>
       </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
       <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
         <v>15</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>690</v>
       </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
       <c r="M4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1465,26 +1480,29 @@
       <c r="G5" t="s">
         <v>115</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5">
         <v>145804</v>
       </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
       <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
         <v>10</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>958</v>
       </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
       <c r="M5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -1500,26 +1518,29 @@
       <c r="G6" t="s">
         <v>115</v>
       </c>
-      <c r="H6">
+      <c r="H6" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6">
         <v>18</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>10</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>7</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>2000</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
       <c r="M6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1538,26 +1559,29 @@
       <c r="G7" t="s">
         <v>115</v>
       </c>
-      <c r="H7">
+      <c r="H7" t="s">
+        <v>105</v>
+      </c>
+      <c r="I7">
         <v>11</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>3</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>5</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>625</v>
       </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
       <c r="M7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1573,26 +1597,29 @@
       <c r="G8" t="s">
         <v>115</v>
       </c>
-      <c r="H8">
+      <c r="H8" t="s">
+        <v>105</v>
+      </c>
+      <c r="I8">
         <v>3021</v>
       </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
       <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
         <v>30</v>
-      </c>
-      <c r="K8">
-        <v>3772</v>
       </c>
       <c r="L8">
         <v>3772</v>
       </c>
       <c r="M8">
+        <v>3772</v>
+      </c>
+      <c r="N8">
         <v>6064</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1611,26 +1638,29 @@
       <c r="G9" t="s">
         <v>115</v>
       </c>
-      <c r="H9">
+      <c r="H9" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9">
         <v>29</v>
       </c>
-      <c r="I9">
-        <v>2</v>
-      </c>
       <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
         <v>16</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>690</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>37</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -1646,26 +1676,29 @@
       <c r="G10" t="s">
         <v>115</v>
       </c>
-      <c r="H10">
+      <c r="H10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I10">
         <v>41</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>19</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>36</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>683</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>121</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>2337</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -1681,26 +1714,29 @@
       <c r="G11" t="s">
         <v>115</v>
       </c>
-      <c r="H11">
+      <c r="H11" t="s">
+        <v>105</v>
+      </c>
+      <c r="I11">
         <v>1779</v>
       </c>
-      <c r="I11">
-        <v>2</v>
-      </c>
       <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
         <v>10</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>699</v>
-      </c>
-      <c r="L11">
-        <v>16</v>
       </c>
       <c r="M11">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1716,26 +1752,29 @@
       <c r="G12" t="s">
         <v>115</v>
       </c>
-      <c r="H12">
+      <c r="H12" t="s">
+        <v>105</v>
+      </c>
+      <c r="I12">
         <v>23</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>3</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>10</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>1473</v>
       </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
       <c r="M12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
@@ -1751,26 +1790,29 @@
       <c r="G13" t="s">
         <v>115</v>
       </c>
-      <c r="H13">
+      <c r="H13" t="s">
+        <v>105</v>
+      </c>
+      <c r="I13">
         <v>3561</v>
       </c>
-      <c r="I13">
-        <v>2</v>
-      </c>
       <c r="J13">
+        <v>2</v>
+      </c>
+      <c r="K13">
         <v>10</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>672</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>666</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>1200</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1786,26 +1828,29 @@
       <c r="G14" t="s">
         <v>115</v>
       </c>
-      <c r="H14">
+      <c r="H14" t="s">
+        <v>105</v>
+      </c>
+      <c r="I14">
         <v>1788</v>
       </c>
-      <c r="I14">
-        <v>2</v>
-      </c>
       <c r="J14">
+        <v>2</v>
+      </c>
+      <c r="K14">
         <v>23</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>8124</v>
-      </c>
-      <c r="L14">
-        <v>2480</v>
       </c>
       <c r="M14">
         <v>2480</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1821,26 +1866,29 @@
       <c r="G15" t="s">
         <v>115</v>
       </c>
-      <c r="H15">
+      <c r="H15" t="s">
+        <v>105</v>
+      </c>
+      <c r="I15">
         <v>28</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>10</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>65</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>5620</v>
       </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
       <c r="M15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1859,26 +1907,29 @@
       <c r="G16" t="s">
         <v>115</v>
       </c>
-      <c r="H16">
+      <c r="H16" t="s">
+        <v>105</v>
+      </c>
+      <c r="I16">
         <v>31</v>
       </c>
-      <c r="I16">
-        <v>2</v>
-      </c>
       <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16">
         <v>21</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>1000</v>
       </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
       <c r="M16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1894,26 +1945,29 @@
       <c r="G17" t="s">
         <v>115</v>
       </c>
-      <c r="H17">
+      <c r="H17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I17">
         <v>32</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>10</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>17</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>10992</v>
       </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
       <c r="M17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -1929,26 +1983,29 @@
       <c r="G18" t="s">
         <v>115</v>
       </c>
-      <c r="H18">
+      <c r="H18" t="s">
+        <v>105</v>
+      </c>
+      <c r="I18">
         <v>3</v>
       </c>
-      <c r="I18">
-        <v>2</v>
-      </c>
       <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18">
         <v>37</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>3196</v>
       </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
       <c r="M18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
@@ -1964,26 +2021,29 @@
       <c r="G19" t="s">
         <v>115</v>
       </c>
-      <c r="H19">
+      <c r="H19" t="s">
+        <v>105</v>
+      </c>
+      <c r="I19">
         <v>6</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>26</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>17</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>20000</v>
       </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
       <c r="M19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
@@ -1999,26 +2059,29 @@
       <c r="G20" t="s">
         <v>115</v>
       </c>
-      <c r="H20">
+      <c r="H20" t="s">
+        <v>105</v>
+      </c>
+      <c r="I20">
         <v>12</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>10</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>217</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>2000</v>
       </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
       <c r="M20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>4</v>
       </c>
@@ -2034,26 +2097,29 @@
       <c r="G21" t="s">
         <v>115</v>
       </c>
-      <c r="H21">
+      <c r="H21" t="s">
+        <v>105</v>
+      </c>
+      <c r="I21">
         <v>1778</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>10</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>77</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>2000</v>
       </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
       <c r="M21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
@@ -2069,26 +2135,29 @@
       <c r="G22" t="s">
         <v>115</v>
       </c>
-      <c r="H22">
+      <c r="H22" t="s">
+        <v>105</v>
+      </c>
+      <c r="I22">
         <v>16</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>10</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>65</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>2000</v>
       </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
       <c r="M22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -2104,26 +2173,29 @@
       <c r="G23" t="s">
         <v>115</v>
       </c>
-      <c r="H23">
+      <c r="H23" t="s">
+        <v>105</v>
+      </c>
+      <c r="I23">
         <v>22</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <v>10</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>48</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>2000</v>
       </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
       <c r="M23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
@@ -2139,26 +2211,29 @@
       <c r="G24" t="s">
         <v>115</v>
       </c>
-      <c r="H24">
+      <c r="H24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I24">
         <v>36</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>7</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>20</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>2310</v>
       </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
       <c r="M24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
@@ -2177,26 +2252,29 @@
       <c r="G25" t="s">
         <v>115</v>
       </c>
-      <c r="H25">
+      <c r="H25" t="s">
+        <v>105</v>
+      </c>
+      <c r="I25">
         <v>43</v>
       </c>
-      <c r="I25">
-        <v>2</v>
-      </c>
       <c r="J25">
+        <v>2</v>
+      </c>
+      <c r="K25">
         <v>58</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>4601</v>
       </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
       <c r="M25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
@@ -2212,26 +2290,29 @@
       <c r="G26" t="s">
         <v>115</v>
       </c>
-      <c r="H26">
+      <c r="H26" t="s">
+        <v>105</v>
+      </c>
+      <c r="I26">
         <v>45</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <v>3</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>62</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>3190</v>
       </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
       <c r="M26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
@@ -2247,26 +2328,29 @@
       <c r="G27" t="s">
         <v>115</v>
       </c>
-      <c r="H27">
+      <c r="H27" t="s">
+        <v>105</v>
+      </c>
+      <c r="I27">
         <v>58</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>3</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>41</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>5000</v>
       </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
       <c r="M27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -2282,26 +2366,29 @@
       <c r="G28" t="s">
         <v>115</v>
       </c>
-      <c r="H28">
+      <c r="H28" t="s">
+        <v>105</v>
+      </c>
+      <c r="I28">
         <v>2074</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>6</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>37</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>6430</v>
       </c>
-      <c r="L28">
-        <v>0</v>
-      </c>
       <c r="M28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -2323,26 +2410,29 @@
       <c r="G29" t="s">
         <v>115</v>
       </c>
-      <c r="H29">
+      <c r="H29" t="s">
+        <v>105</v>
+      </c>
+      <c r="I29">
         <v>2125</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>5</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>20</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>736</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <v>95</v>
       </c>
-      <c r="M29">
+      <c r="N29">
         <v>448</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -2358,26 +2448,29 @@
       <c r="G30" t="s">
         <v>115</v>
       </c>
-      <c r="H30">
+      <c r="H30" t="s">
+        <v>105</v>
+      </c>
+      <c r="I30">
         <v>3022</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>11</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>13</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>990</v>
       </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
       <c r="M30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -2393,26 +2486,29 @@
       <c r="G31" t="s">
         <v>115</v>
       </c>
-      <c r="H31">
+      <c r="H31" t="s">
+        <v>105</v>
+      </c>
+      <c r="I31">
         <v>3485</v>
       </c>
-      <c r="I31">
-        <v>2</v>
-      </c>
       <c r="J31">
+        <v>2</v>
+      </c>
+      <c r="K31">
         <v>300</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>2407</v>
       </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
       <c r="M31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
@@ -2431,26 +2527,29 @@
       <c r="G32" t="s">
         <v>115</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" t="s">
+        <v>105</v>
+      </c>
+      <c r="I32" s="2">
         <v>3492</v>
       </c>
-      <c r="I32">
-        <v>2</v>
-      </c>
       <c r="J32">
+        <v>2</v>
+      </c>
+      <c r="K32">
         <v>7</v>
       </c>
-      <c r="K32">
+      <c r="L32">
         <v>556</v>
       </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
       <c r="M32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>32</v>
       </c>
@@ -2469,26 +2568,29 @@
       <c r="G33" t="s">
         <v>115</v>
       </c>
-      <c r="H33">
+      <c r="H33" t="s">
+        <v>105</v>
+      </c>
+      <c r="I33">
         <v>3493</v>
       </c>
-      <c r="I33">
-        <v>2</v>
-      </c>
       <c r="J33">
+        <v>2</v>
+      </c>
+      <c r="K33">
         <v>7</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <v>601</v>
       </c>
-      <c r="L33">
-        <v>0</v>
-      </c>
       <c r="M33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
@@ -2507,26 +2609,29 @@
       <c r="G34" t="s">
         <v>115</v>
       </c>
-      <c r="H34">
+      <c r="H34" t="s">
+        <v>105</v>
+      </c>
+      <c r="I34">
         <v>3494</v>
       </c>
-      <c r="I34">
-        <v>2</v>
-      </c>
       <c r="J34">
+        <v>2</v>
+      </c>
+      <c r="K34">
         <v>7</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <v>554</v>
       </c>
-      <c r="L34">
-        <v>0</v>
-      </c>
       <c r="M34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -2542,26 +2647,29 @@
       <c r="G35" t="s">
         <v>115</v>
       </c>
-      <c r="H35">
+      <c r="H35" t="s">
+        <v>105</v>
+      </c>
+      <c r="I35">
         <v>4544</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <v>9</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <v>15</v>
       </c>
-      <c r="K35">
+      <c r="L35">
         <v>9961</v>
       </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
       <c r="M35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
@@ -2577,26 +2685,29 @@
       <c r="G36" t="s">
         <v>115</v>
       </c>
-      <c r="H36">
+      <c r="H36" t="s">
+        <v>105</v>
+      </c>
+      <c r="I36">
         <v>3512</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>6</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>62</v>
       </c>
-      <c r="K36">
+      <c r="L36">
         <v>600</v>
       </c>
-      <c r="L36">
-        <v>0</v>
-      </c>
       <c r="M36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
@@ -2612,26 +2723,29 @@
       <c r="G37" t="s">
         <v>115</v>
       </c>
-      <c r="H37">
+      <c r="H37" t="s">
+        <v>105</v>
+      </c>
+      <c r="I37">
         <v>3543</v>
       </c>
-      <c r="I37">
-        <v>2</v>
-      </c>
       <c r="J37">
+        <v>2</v>
+      </c>
+      <c r="K37">
         <v>6</v>
       </c>
-      <c r="K37">
+      <c r="L37">
         <v>500</v>
-      </c>
-      <c r="L37">
-        <v>32</v>
       </c>
       <c r="M37">
         <v>32</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
@@ -2647,26 +2761,29 @@
       <c r="G38" t="s">
         <v>115</v>
       </c>
-      <c r="H38">
+      <c r="H38" t="s">
+        <v>105</v>
+      </c>
+      <c r="I38">
         <v>3549</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <v>4</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>71</v>
       </c>
-      <c r="K38">
+      <c r="L38">
         <v>841</v>
       </c>
-      <c r="L38">
-        <v>0</v>
-      </c>
       <c r="M38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
@@ -2682,26 +2799,29 @@
       <c r="G39" t="s">
         <v>115</v>
       </c>
-      <c r="H39">
+      <c r="H39" t="s">
+        <v>105</v>
+      </c>
+      <c r="I39">
         <v>3560</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>6</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <v>5</v>
       </c>
-      <c r="K39">
+      <c r="L39">
         <v>797</v>
       </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
       <c r="M39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>42</v>
       </c>
@@ -2717,26 +2837,29 @@
       <c r="G40" t="s">
         <v>115</v>
       </c>
-      <c r="H40">
+      <c r="H40" t="s">
+        <v>105</v>
+      </c>
+      <c r="I40">
         <v>3899</v>
       </c>
-      <c r="I40">
-        <v>2</v>
-      </c>
       <c r="J40">
+        <v>2</v>
+      </c>
+      <c r="K40">
         <v>6</v>
       </c>
-      <c r="K40">
+      <c r="L40">
         <v>15545</v>
       </c>
-      <c r="L40">
-        <v>0</v>
-      </c>
       <c r="M40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>43</v>
       </c>
@@ -2752,26 +2875,29 @@
       <c r="G41" t="s">
         <v>115</v>
       </c>
-      <c r="H41">
+      <c r="H41" t="s">
+        <v>105</v>
+      </c>
+      <c r="I41">
         <v>3902</v>
       </c>
-      <c r="I41">
-        <v>2</v>
-      </c>
       <c r="J41">
+        <v>2</v>
+      </c>
+      <c r="K41">
         <v>38</v>
       </c>
-      <c r="K41">
+      <c r="L41">
         <v>1458</v>
       </c>
-      <c r="L41">
-        <v>0</v>
-      </c>
       <c r="M41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>44</v>
       </c>
@@ -2787,26 +2913,29 @@
       <c r="G42" t="s">
         <v>115</v>
       </c>
-      <c r="H42">
+      <c r="H42" t="s">
+        <v>105</v>
+      </c>
+      <c r="I42">
         <v>3903</v>
       </c>
-      <c r="I42">
-        <v>2</v>
-      </c>
       <c r="J42">
+        <v>2</v>
+      </c>
+      <c r="K42">
         <v>38</v>
       </c>
-      <c r="K42">
+      <c r="L42">
         <v>1563</v>
       </c>
-      <c r="L42">
-        <v>0</v>
-      </c>
       <c r="M42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>45</v>
       </c>
@@ -2822,26 +2951,29 @@
       <c r="G43" t="s">
         <v>115</v>
       </c>
-      <c r="H43">
+      <c r="H43" t="s">
+        <v>105</v>
+      </c>
+      <c r="I43">
         <v>3904</v>
       </c>
-      <c r="I43">
-        <v>2</v>
-      </c>
       <c r="J43">
+        <v>2</v>
+      </c>
+      <c r="K43">
         <v>22</v>
       </c>
-      <c r="K43">
+      <c r="L43">
         <v>10885</v>
       </c>
-      <c r="L43">
+      <c r="M43">
         <v>5</v>
       </c>
-      <c r="M43">
+      <c r="N43">
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>46</v>
       </c>
@@ -2857,26 +2989,29 @@
       <c r="G44" t="s">
         <v>115</v>
       </c>
-      <c r="H44">
+      <c r="H44" t="s">
+        <v>105</v>
+      </c>
+      <c r="I44">
         <v>3913</v>
       </c>
-      <c r="I44">
-        <v>2</v>
-      </c>
       <c r="J44">
+        <v>2</v>
+      </c>
+      <c r="K44">
         <v>22</v>
       </c>
-      <c r="K44">
+      <c r="L44">
         <v>522</v>
       </c>
-      <c r="L44">
-        <v>0</v>
-      </c>
       <c r="M44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>47</v>
       </c>
@@ -2892,26 +3027,29 @@
       <c r="G45" t="s">
         <v>115</v>
       </c>
-      <c r="H45">
+      <c r="H45" t="s">
+        <v>105</v>
+      </c>
+      <c r="I45">
         <v>3917</v>
       </c>
-      <c r="I45">
-        <v>2</v>
-      </c>
       <c r="J45">
+        <v>2</v>
+      </c>
+      <c r="K45">
         <v>22</v>
       </c>
-      <c r="K45">
+      <c r="L45">
         <v>2109</v>
       </c>
-      <c r="L45">
-        <v>0</v>
-      </c>
       <c r="M45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>48</v>
       </c>
@@ -2927,26 +3065,29 @@
       <c r="G46" t="s">
         <v>115</v>
       </c>
-      <c r="H46">
+      <c r="H46" t="s">
+        <v>105</v>
+      </c>
+      <c r="I46">
         <v>3918</v>
       </c>
-      <c r="I46">
-        <v>2</v>
-      </c>
       <c r="J46">
+        <v>2</v>
+      </c>
+      <c r="K46">
         <v>22</v>
       </c>
-      <c r="K46">
+      <c r="L46">
         <v>1109</v>
       </c>
-      <c r="L46">
-        <v>0</v>
-      </c>
       <c r="M46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
@@ -2965,26 +3106,29 @@
       <c r="G47" t="s">
         <v>115</v>
       </c>
-      <c r="H47">
+      <c r="H47" t="s">
+        <v>105</v>
+      </c>
+      <c r="I47">
         <v>3954</v>
       </c>
-      <c r="I47">
-        <v>2</v>
-      </c>
       <c r="J47">
+        <v>2</v>
+      </c>
+      <c r="K47">
         <v>12</v>
       </c>
-      <c r="K47">
+      <c r="L47">
         <v>19020</v>
       </c>
-      <c r="L47">
-        <v>0</v>
-      </c>
       <c r="M47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>52</v>
       </c>
@@ -3003,26 +3147,29 @@
       <c r="G48" t="s">
         <v>115</v>
       </c>
-      <c r="H48">
+      <c r="H48" t="s">
+        <v>105</v>
+      </c>
+      <c r="I48">
         <v>14964</v>
       </c>
-      <c r="I48">
+      <c r="J48">
         <v>10</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <v>8</v>
       </c>
-      <c r="K48">
+      <c r="L48">
         <v>10218</v>
       </c>
-      <c r="L48">
-        <v>0</v>
-      </c>
       <c r="M48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>25</v>
       </c>
@@ -3041,26 +3188,29 @@
       <c r="G49" t="s">
         <v>115</v>
       </c>
-      <c r="H49">
+      <c r="H49" t="s">
+        <v>105</v>
+      </c>
+      <c r="I49">
         <v>219</v>
       </c>
-      <c r="I49">
-        <v>2</v>
-      </c>
       <c r="J49">
+        <v>2</v>
+      </c>
+      <c r="K49">
         <v>9</v>
       </c>
-      <c r="K49">
+      <c r="L49">
         <v>45312</v>
       </c>
-      <c r="L49">
-        <v>0</v>
-      </c>
       <c r="M49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>54</v>
       </c>
@@ -3076,26 +3226,29 @@
       <c r="G50" t="s">
         <v>115</v>
       </c>
-      <c r="H50" s="2">
+      <c r="H50" t="s">
+        <v>105</v>
+      </c>
+      <c r="I50" s="2">
         <v>10093</v>
       </c>
-      <c r="I50">
-        <v>2</v>
-      </c>
       <c r="J50">
+        <v>2</v>
+      </c>
+      <c r="K50">
         <v>5</v>
       </c>
-      <c r="K50">
+      <c r="L50">
         <v>1372</v>
       </c>
-      <c r="L50">
-        <v>0</v>
-      </c>
       <c r="M50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
@@ -3111,26 +3264,29 @@
       <c r="G51" t="s">
         <v>115</v>
       </c>
-      <c r="H51">
+      <c r="H51" t="s">
+        <v>105</v>
+      </c>
+      <c r="I51">
         <v>10101</v>
       </c>
-      <c r="I51">
-        <v>2</v>
-      </c>
       <c r="J51">
+        <v>2</v>
+      </c>
+      <c r="K51">
         <v>5</v>
       </c>
-      <c r="K51">
+      <c r="L51">
         <v>748</v>
       </c>
-      <c r="L51">
-        <v>0</v>
-      </c>
       <c r="M51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>56</v>
       </c>
@@ -3146,26 +3302,29 @@
       <c r="G52" t="s">
         <v>115</v>
       </c>
-      <c r="H52">
+      <c r="H52" t="s">
+        <v>105</v>
+      </c>
+      <c r="I52">
         <v>9979</v>
       </c>
-      <c r="I52">
+      <c r="J52">
         <v>10</v>
       </c>
-      <c r="J52">
+      <c r="K52">
         <v>36</v>
       </c>
-      <c r="K52">
+      <c r="L52">
         <v>2126</v>
       </c>
-      <c r="L52">
-        <v>0</v>
-      </c>
       <c r="M52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>57</v>
       </c>
@@ -3181,26 +3340,29 @@
       <c r="G53" t="s">
         <v>115</v>
       </c>
-      <c r="H53">
+      <c r="H53" t="s">
+        <v>105</v>
+      </c>
+      <c r="I53">
         <v>9980</v>
       </c>
-      <c r="I53">
-        <v>2</v>
-      </c>
       <c r="J53">
+        <v>2</v>
+      </c>
+      <c r="K53">
         <v>21</v>
       </c>
-      <c r="K53">
+      <c r="L53">
         <v>540</v>
       </c>
-      <c r="L53">
-        <v>0</v>
-      </c>
       <c r="M53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
@@ -3216,26 +3378,29 @@
       <c r="G54" t="s">
         <v>115</v>
       </c>
-      <c r="H54">
+      <c r="H54" t="s">
+        <v>105</v>
+      </c>
+      <c r="I54">
         <v>9983</v>
       </c>
-      <c r="I54">
-        <v>2</v>
-      </c>
       <c r="J54">
+        <v>2</v>
+      </c>
+      <c r="K54">
         <v>15</v>
       </c>
-      <c r="K54">
+      <c r="L54">
         <v>14980</v>
       </c>
-      <c r="L54">
-        <v>0</v>
-      </c>
       <c r="M54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>60</v>
       </c>
@@ -3254,26 +3419,29 @@
       <c r="G55" t="s">
         <v>115</v>
       </c>
-      <c r="H55">
+      <c r="H55" t="s">
+        <v>105</v>
+      </c>
+      <c r="I55">
         <v>9985</v>
       </c>
-      <c r="I55">
+      <c r="J55">
         <v>6</v>
       </c>
-      <c r="J55">
+      <c r="K55">
         <v>52</v>
       </c>
-      <c r="K55">
+      <c r="L55">
         <v>6118</v>
       </c>
-      <c r="L55">
-        <v>0</v>
-      </c>
       <c r="M55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>63</v>
       </c>
@@ -3289,26 +3457,29 @@
       <c r="G56" t="s">
         <v>115</v>
       </c>
-      <c r="H56">
+      <c r="H56" t="s">
+        <v>105</v>
+      </c>
+      <c r="I56">
         <v>9970</v>
       </c>
-      <c r="I56">
-        <v>2</v>
-      </c>
       <c r="J56">
+        <v>2</v>
+      </c>
+      <c r="K56">
         <v>101</v>
       </c>
-      <c r="K56">
+      <c r="L56">
         <v>1212</v>
       </c>
-      <c r="L56">
-        <v>0</v>
-      </c>
       <c r="M56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>64</v>
       </c>
@@ -3324,26 +3495,29 @@
       <c r="G57" t="s">
         <v>115</v>
       </c>
-      <c r="H57">
+      <c r="H57" t="s">
+        <v>105</v>
+      </c>
+      <c r="I57">
         <v>9971</v>
       </c>
-      <c r="I57">
-        <v>2</v>
-      </c>
       <c r="J57">
+        <v>2</v>
+      </c>
+      <c r="K57">
         <v>11</v>
       </c>
-      <c r="K57">
+      <c r="L57">
         <v>583</v>
       </c>
-      <c r="L57">
-        <v>0</v>
-      </c>
       <c r="M57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>66</v>
       </c>
@@ -3359,26 +3533,26 @@
       <c r="E58" t="s">
         <v>108</v>
       </c>
-      <c r="H58">
+      <c r="I58">
         <v>9977</v>
       </c>
-      <c r="I58">
-        <v>2</v>
-      </c>
       <c r="J58">
+        <v>2</v>
+      </c>
+      <c r="K58">
         <v>119</v>
       </c>
-      <c r="K58">
+      <c r="L58">
         <v>34465</v>
       </c>
-      <c r="L58">
-        <v>0</v>
-      </c>
       <c r="M58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>67</v>
       </c>
@@ -3394,26 +3568,29 @@
       <c r="G59" t="s">
         <v>115</v>
       </c>
-      <c r="H59">
+      <c r="H59" t="s">
+        <v>105</v>
+      </c>
+      <c r="I59">
         <v>9978</v>
       </c>
-      <c r="I59">
-        <v>2</v>
-      </c>
       <c r="J59">
+        <v>2</v>
+      </c>
+      <c r="K59">
         <v>73</v>
       </c>
-      <c r="K59">
+      <c r="L59">
         <v>2534</v>
       </c>
-      <c r="L59">
-        <v>0</v>
-      </c>
       <c r="M59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>68</v>
       </c>
@@ -3429,26 +3606,29 @@
       <c r="G60" t="s">
         <v>115</v>
       </c>
-      <c r="H60">
+      <c r="H60" t="s">
+        <v>105</v>
+      </c>
+      <c r="I60">
         <v>9952</v>
       </c>
-      <c r="I60">
-        <v>2</v>
-      </c>
       <c r="J60">
+        <v>2</v>
+      </c>
+      <c r="K60">
         <v>6</v>
       </c>
-      <c r="K60">
+      <c r="L60">
         <v>5404</v>
       </c>
-      <c r="L60">
-        <v>0</v>
-      </c>
       <c r="M60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>69</v>
       </c>
@@ -3467,26 +3647,29 @@
       <c r="G61" t="s">
         <v>115</v>
       </c>
-      <c r="H61">
+      <c r="H61" t="s">
+        <v>105</v>
+      </c>
+      <c r="I61">
         <v>9954</v>
       </c>
-      <c r="I61">
+      <c r="J61">
         <v>100</v>
       </c>
-      <c r="J61">
+      <c r="K61">
         <v>65</v>
       </c>
-      <c r="K61">
+      <c r="L61">
         <v>1600</v>
       </c>
-      <c r="L61">
-        <v>0</v>
-      </c>
       <c r="M61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>70</v>
       </c>
@@ -3505,26 +3688,29 @@
       <c r="G62" t="s">
         <v>115</v>
       </c>
-      <c r="H62">
+      <c r="H62" t="s">
+        <v>105</v>
+      </c>
+      <c r="I62">
         <v>9955</v>
       </c>
-      <c r="I62">
+      <c r="J62">
         <v>100</v>
       </c>
-      <c r="J62">
+      <c r="K62">
         <v>65</v>
       </c>
-      <c r="K62">
+      <c r="L62">
         <v>1600</v>
       </c>
-      <c r="L62">
-        <v>0</v>
-      </c>
       <c r="M62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>72</v>
       </c>
@@ -3540,26 +3726,29 @@
       <c r="G63" t="s">
         <v>115</v>
       </c>
-      <c r="H63">
+      <c r="H63" t="s">
+        <v>105</v>
+      </c>
+      <c r="I63">
         <v>9957</v>
       </c>
-      <c r="I63">
-        <v>2</v>
-      </c>
       <c r="J63">
+        <v>2</v>
+      </c>
+      <c r="K63">
         <v>42</v>
       </c>
-      <c r="K63">
+      <c r="L63">
         <v>1055</v>
       </c>
-      <c r="L63">
-        <v>0</v>
-      </c>
       <c r="M63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>73</v>
       </c>
@@ -3575,26 +3764,29 @@
       <c r="G64" t="s">
         <v>115</v>
       </c>
-      <c r="H64">
+      <c r="H64" t="s">
+        <v>105</v>
+      </c>
+      <c r="I64">
         <v>9960</v>
       </c>
-      <c r="I64">
+      <c r="J64">
         <v>4</v>
       </c>
-      <c r="J64">
+      <c r="K64">
         <v>25</v>
       </c>
-      <c r="K64">
+      <c r="L64">
         <v>5456</v>
       </c>
-      <c r="L64">
-        <v>0</v>
-      </c>
       <c r="M64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>75</v>
       </c>
@@ -3610,26 +3802,29 @@
       <c r="G65" t="s">
         <v>115</v>
       </c>
-      <c r="H65">
+      <c r="H65" t="s">
+        <v>105</v>
+      </c>
+      <c r="I65">
         <v>9967</v>
       </c>
-      <c r="I65">
-        <v>2</v>
-      </c>
       <c r="J65">
+        <v>2</v>
+      </c>
+      <c r="K65">
         <v>34</v>
       </c>
-      <c r="K65">
+      <c r="L65">
         <v>1941</v>
       </c>
-      <c r="L65">
-        <v>0</v>
-      </c>
       <c r="M65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>76</v>
       </c>
@@ -3645,26 +3840,29 @@
       <c r="G66" t="s">
         <v>115</v>
       </c>
-      <c r="H66">
+      <c r="H66" t="s">
+        <v>105</v>
+      </c>
+      <c r="I66">
         <v>9946</v>
       </c>
-      <c r="I66">
-        <v>2</v>
-      </c>
       <c r="J66">
+        <v>2</v>
+      </c>
+      <c r="K66">
         <v>31</v>
       </c>
-      <c r="K66">
+      <c r="L66">
         <v>569</v>
       </c>
-      <c r="L66">
-        <v>0</v>
-      </c>
       <c r="M66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>78</v>
       </c>
@@ -3680,26 +3878,29 @@
       <c r="G67" t="s">
         <v>115</v>
       </c>
-      <c r="H67">
+      <c r="H67" t="s">
+        <v>105</v>
+      </c>
+      <c r="I67">
         <v>7592</v>
       </c>
-      <c r="I67">
-        <v>2</v>
-      </c>
       <c r="J67">
+        <v>2</v>
+      </c>
+      <c r="K67">
         <v>15</v>
       </c>
-      <c r="K67">
+      <c r="L67">
         <v>48842</v>
       </c>
-      <c r="L67">
+      <c r="M67">
         <v>3620</v>
       </c>
-      <c r="M67">
+      <c r="N67">
         <v>6465</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>82</v>
       </c>
@@ -3718,26 +3919,29 @@
       <c r="G68" t="s">
         <v>115</v>
       </c>
-      <c r="H68">
+      <c r="H68" t="s">
+        <v>105</v>
+      </c>
+      <c r="I68">
         <v>14969</v>
       </c>
-      <c r="I68">
+      <c r="J68">
         <v>5</v>
       </c>
-      <c r="J68">
+      <c r="K68">
         <v>33</v>
       </c>
-      <c r="K68">
+      <c r="L68">
         <v>9873</v>
       </c>
-      <c r="L68">
-        <v>0</v>
-      </c>
       <c r="M68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>83</v>
       </c>
@@ -3756,26 +3960,29 @@
       <c r="G69" t="s">
         <v>115</v>
       </c>
-      <c r="H69">
+      <c r="H69" t="s">
+        <v>105</v>
+      </c>
+      <c r="I69">
         <v>14968</v>
       </c>
-      <c r="I69">
-        <v>2</v>
-      </c>
       <c r="J69">
+        <v>2</v>
+      </c>
+      <c r="K69">
         <v>40</v>
       </c>
-      <c r="K69">
+      <c r="L69">
         <v>540</v>
       </c>
-      <c r="L69">
+      <c r="M69">
         <v>263</v>
       </c>
-      <c r="M69">
+      <c r="N69">
         <v>999</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>84</v>
       </c>
@@ -3791,26 +3998,29 @@
       <c r="G70" t="s">
         <v>115</v>
       </c>
-      <c r="H70">
+      <c r="H70" t="s">
+        <v>105</v>
+      </c>
+      <c r="I70">
         <v>14967</v>
       </c>
-      <c r="I70">
+      <c r="J70">
         <v>6</v>
       </c>
-      <c r="J70">
+      <c r="K70">
         <v>35</v>
       </c>
-      <c r="K70">
+      <c r="L70">
         <v>2796</v>
       </c>
-      <c r="L70">
+      <c r="M70">
         <v>2795</v>
       </c>
-      <c r="M70">
+      <c r="N70">
         <v>68100</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>85</v>
       </c>
@@ -3829,26 +4039,29 @@
       <c r="G71" t="s">
         <v>115</v>
       </c>
-      <c r="H71">
+      <c r="H71" t="s">
+        <v>105</v>
+      </c>
+      <c r="I71">
         <v>125920</v>
       </c>
-      <c r="I71">
-        <v>2</v>
-      </c>
       <c r="J71">
+        <v>2</v>
+      </c>
+      <c r="K71">
         <v>13</v>
       </c>
-      <c r="K71">
+      <c r="L71">
         <v>500</v>
       </c>
-      <c r="L71">
+      <c r="M71">
         <v>401</v>
       </c>
-      <c r="M71">
+      <c r="N71">
         <v>835</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>87</v>
       </c>
@@ -3864,26 +4077,29 @@
       <c r="G72" t="s">
         <v>115</v>
       </c>
-      <c r="H72">
+      <c r="H72" t="s">
+        <v>105</v>
+      </c>
+      <c r="I72">
         <v>125921</v>
       </c>
-      <c r="I72">
+      <c r="J72">
         <v>10</v>
       </c>
-      <c r="J72">
+      <c r="K72">
         <v>8</v>
       </c>
-      <c r="K72">
+      <c r="L72">
         <v>500</v>
       </c>
-      <c r="L72">
-        <v>0</v>
-      </c>
       <c r="M72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>88</v>
       </c>
@@ -3899,26 +4115,29 @@
       <c r="G73" t="s">
         <v>115</v>
       </c>
-      <c r="H73">
+      <c r="H73" t="s">
+        <v>105</v>
+      </c>
+      <c r="I73">
         <v>125922</v>
       </c>
-      <c r="I73">
+      <c r="J73">
         <v>11</v>
       </c>
-      <c r="J73">
+      <c r="K73">
         <v>41</v>
       </c>
-      <c r="K73">
+      <c r="L73">
         <v>5500</v>
       </c>
-      <c r="L73">
-        <v>0</v>
-      </c>
       <c r="M73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>89</v>
       </c>
@@ -3931,26 +4150,26 @@
       <c r="E74" t="s">
         <v>108</v>
       </c>
-      <c r="H74">
+      <c r="I74">
         <v>146607</v>
       </c>
-      <c r="I74">
-        <v>2</v>
-      </c>
       <c r="J74">
+        <v>2</v>
+      </c>
+      <c r="K74">
         <v>123</v>
       </c>
-      <c r="K74">
+      <c r="L74">
         <v>8378</v>
       </c>
-      <c r="L74">
+      <c r="M74">
         <v>7330</v>
       </c>
-      <c r="M74">
+      <c r="N74">
         <v>18372</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>61</v>
       </c>
@@ -3963,26 +4182,26 @@
       <c r="E75" t="s">
         <v>108</v>
       </c>
-      <c r="H75">
+      <c r="I75">
         <v>9986</v>
       </c>
-      <c r="I75">
+      <c r="J75">
         <v>6</v>
       </c>
-      <c r="J75">
-        <v>129</v>
-      </c>
       <c r="K75">
+        <v>129</v>
+      </c>
+      <c r="L75">
         <v>13910</v>
       </c>
-      <c r="L75">
-        <v>0</v>
-      </c>
       <c r="M75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>53</v>
       </c>
@@ -4001,26 +4220,29 @@
       <c r="G76" t="s">
         <v>115</v>
       </c>
-      <c r="H76">
+      <c r="H76" t="s">
+        <v>105</v>
+      </c>
+      <c r="I76">
         <v>14965</v>
       </c>
-      <c r="I76">
-        <v>2</v>
-      </c>
       <c r="J76">
+        <v>2</v>
+      </c>
+      <c r="K76">
         <v>17</v>
       </c>
-      <c r="K76">
+      <c r="L76">
         <v>45211</v>
       </c>
-      <c r="L76">
-        <v>0</v>
-      </c>
       <c r="M76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>71</v>
       </c>
@@ -4039,26 +4261,29 @@
       <c r="G77" t="s">
         <v>115</v>
       </c>
-      <c r="H77">
+      <c r="H77" t="s">
+        <v>105</v>
+      </c>
+      <c r="I77">
         <v>9956</v>
       </c>
-      <c r="I77">
+      <c r="J77">
         <v>100</v>
       </c>
-      <c r="J77">
+      <c r="K77">
         <v>65</v>
       </c>
-      <c r="K77">
+      <c r="L77">
         <v>1599</v>
       </c>
-      <c r="L77">
-        <v>0</v>
-      </c>
       <c r="M77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>81</v>
       </c>
@@ -4074,26 +4299,29 @@
       <c r="G78" t="s">
         <v>115</v>
       </c>
-      <c r="H78">
+      <c r="H78" t="s">
+        <v>105</v>
+      </c>
+      <c r="I78">
         <v>34537</v>
       </c>
-      <c r="I78">
-        <v>2</v>
-      </c>
       <c r="J78">
+        <v>2</v>
+      </c>
+      <c r="K78">
         <v>31</v>
       </c>
-      <c r="K78">
+      <c r="L78">
         <v>11055</v>
       </c>
-      <c r="L78">
-        <v>0</v>
-      </c>
       <c r="M78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>90</v>
       </c>
@@ -4112,26 +4340,29 @@
       <c r="G79" t="s">
         <v>105</v>
       </c>
-      <c r="H79">
+      <c r="H79" t="s">
+        <v>105</v>
+      </c>
+      <c r="I79">
         <v>146195</v>
       </c>
-      <c r="I79">
+      <c r="J79">
         <v>3</v>
       </c>
-      <c r="J79">
+      <c r="K79">
         <v>43</v>
       </c>
-      <c r="K79">
+      <c r="L79">
         <v>67557</v>
       </c>
-      <c r="L79">
-        <v>0</v>
-      </c>
       <c r="M79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>80</v>
       </c>
@@ -4153,26 +4384,29 @@
       <c r="G80" t="s">
         <v>105</v>
       </c>
-      <c r="H80">
+      <c r="H80" t="s">
+        <v>105</v>
+      </c>
+      <c r="I80">
         <v>34539</v>
       </c>
-      <c r="I80">
-        <v>2</v>
-      </c>
       <c r="J80">
+        <v>2</v>
+      </c>
+      <c r="K80">
         <v>10</v>
       </c>
-      <c r="K80">
+      <c r="L80">
         <v>32769</v>
       </c>
-      <c r="L80">
-        <v>0</v>
-      </c>
       <c r="M80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>62</v>
       </c>
@@ -4185,26 +4419,26 @@
       <c r="E81" t="s">
         <v>108</v>
       </c>
-      <c r="H81">
+      <c r="I81">
         <v>14970</v>
       </c>
-      <c r="I81">
+      <c r="J81">
         <v>6</v>
       </c>
-      <c r="J81">
+      <c r="K81">
         <v>562</v>
       </c>
-      <c r="K81">
+      <c r="L81">
         <v>10299</v>
       </c>
-      <c r="L81">
-        <v>0</v>
-      </c>
       <c r="M81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>79</v>
       </c>
@@ -4217,26 +4451,26 @@
       <c r="E82" t="s">
         <v>108</v>
       </c>
-      <c r="H82">
+      <c r="I82">
         <v>14966</v>
       </c>
-      <c r="I82">
-        <v>2</v>
-      </c>
       <c r="J82">
+        <v>2</v>
+      </c>
+      <c r="K82">
         <v>1777</v>
       </c>
-      <c r="K82">
+      <c r="L82">
         <v>3751</v>
       </c>
-      <c r="L82">
-        <v>0</v>
-      </c>
       <c r="M82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>86</v>
       </c>
@@ -4255,26 +4489,29 @@
       <c r="G83" t="s">
         <v>105</v>
       </c>
-      <c r="H83">
+      <c r="H83" t="s">
+        <v>105</v>
+      </c>
+      <c r="I83">
         <v>146606</v>
       </c>
-      <c r="I83">
-        <v>2</v>
-      </c>
       <c r="J83">
+        <v>2</v>
+      </c>
+      <c r="K83">
         <v>29</v>
       </c>
-      <c r="K83">
+      <c r="L83">
         <v>98050</v>
       </c>
-      <c r="L83">
+      <c r="M83">
         <v>1</v>
       </c>
-      <c r="M83">
+      <c r="N83">
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>40</v>
       </c>
@@ -4287,26 +4524,26 @@
       <c r="E84" t="s">
         <v>108</v>
       </c>
-      <c r="H84">
+      <c r="I84">
         <v>3573</v>
       </c>
-      <c r="I84">
+      <c r="J84">
         <v>10</v>
       </c>
-      <c r="J84">
+      <c r="K84">
         <v>785</v>
       </c>
-      <c r="K84">
+      <c r="L84">
         <v>70000</v>
       </c>
-      <c r="L84">
-        <v>0</v>
-      </c>
       <c r="M84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>41</v>
       </c>
@@ -4319,26 +4556,26 @@
       <c r="E85" t="s">
         <v>108</v>
       </c>
-      <c r="H85">
+      <c r="I85">
         <v>3891</v>
       </c>
-      <c r="I85">
-        <v>2</v>
-      </c>
       <c r="J85">
+        <v>2</v>
+      </c>
+      <c r="K85">
         <v>971</v>
       </c>
-      <c r="K85">
+      <c r="L85">
         <v>3468</v>
       </c>
-      <c r="L85">
-        <v>0</v>
-      </c>
       <c r="M85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>28</v>
       </c>
@@ -4351,26 +4588,26 @@
       <c r="E86" t="s">
         <v>108</v>
       </c>
-      <c r="H86">
+      <c r="I86">
         <v>3481</v>
       </c>
-      <c r="I86">
+      <c r="J86">
         <v>26</v>
       </c>
-      <c r="J86">
+      <c r="K86">
         <v>618</v>
       </c>
-      <c r="K86">
+      <c r="L86">
         <v>7797</v>
       </c>
-      <c r="L86">
-        <v>0</v>
-      </c>
       <c r="M86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>58</v>
       </c>
@@ -4383,26 +4620,26 @@
       <c r="E87" t="s">
         <v>108</v>
       </c>
-      <c r="H87">
+      <c r="I87">
         <v>9981</v>
       </c>
-      <c r="I87">
+      <c r="J87">
         <v>9</v>
       </c>
-      <c r="J87">
+      <c r="K87">
         <v>857</v>
       </c>
-      <c r="K87">
+      <c r="L87">
         <v>1080</v>
       </c>
-      <c r="L87">
-        <v>0</v>
-      </c>
       <c r="M87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>74</v>
       </c>
@@ -4415,26 +4652,26 @@
       <c r="E88" t="s">
         <v>108</v>
       </c>
-      <c r="H88">
+      <c r="I88">
         <v>9964</v>
       </c>
-      <c r="I88">
+      <c r="J88">
         <v>10</v>
       </c>
-      <c r="J88">
+      <c r="K88">
         <v>257</v>
       </c>
-      <c r="K88">
+      <c r="L88">
         <v>1593</v>
       </c>
-      <c r="L88">
-        <v>0</v>
-      </c>
       <c r="M88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>77</v>
       </c>
@@ -4447,26 +4684,26 @@
       <c r="E89" t="s">
         <v>108</v>
       </c>
-      <c r="H89">
+      <c r="I89">
         <v>9950</v>
       </c>
-      <c r="I89">
+      <c r="J89">
         <v>20</v>
       </c>
-      <c r="J89">
+      <c r="K89">
         <v>1301</v>
       </c>
-      <c r="K89">
+      <c r="L89">
         <v>571</v>
       </c>
-      <c r="L89">
-        <v>0</v>
-      </c>
       <c r="M89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>65</v>
       </c>
@@ -4479,26 +4716,26 @@
       <c r="E90" t="s">
         <v>108</v>
       </c>
-      <c r="H90">
+      <c r="I90">
         <v>9976</v>
       </c>
-      <c r="I90">
-        <v>2</v>
-      </c>
       <c r="J90">
+        <v>2</v>
+      </c>
+      <c r="K90">
         <v>501</v>
       </c>
-      <c r="K90">
+      <c r="L90">
         <v>2600</v>
       </c>
-      <c r="L90">
-        <v>0</v>
-      </c>
       <c r="M90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>8</v>
       </c>
@@ -4511,26 +4748,26 @@
       <c r="E91" t="s">
         <v>108</v>
       </c>
-      <c r="H91">
+      <c r="I91">
         <v>20</v>
       </c>
-      <c r="I91">
+      <c r="J91">
         <v>10</v>
       </c>
-      <c r="J91">
+      <c r="K91">
         <v>241</v>
       </c>
-      <c r="K91">
+      <c r="L91">
         <v>2000</v>
       </c>
-      <c r="L91">
-        <v>0</v>
-      </c>
       <c r="M91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>49</v>
       </c>
@@ -4543,26 +4780,26 @@
       <c r="E92" t="s">
         <v>108</v>
       </c>
-      <c r="H92">
+      <c r="I92">
         <v>3946</v>
       </c>
-      <c r="I92">
-        <v>2</v>
-      </c>
       <c r="J92">
+        <v>2</v>
+      </c>
+      <c r="K92">
         <v>231</v>
-      </c>
-      <c r="K92">
-        <v>50000</v>
       </c>
       <c r="L92">
         <v>50000</v>
       </c>
       <c r="M92">
+        <v>50000</v>
+      </c>
+      <c r="N92">
         <v>8024152</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>50</v>
       </c>
@@ -4575,22 +4812,22 @@
       <c r="E93" t="s">
         <v>108</v>
       </c>
-      <c r="H93" s="2">
+      <c r="I93" s="2">
         <v>3948</v>
       </c>
-      <c r="I93">
-        <v>2</v>
-      </c>
       <c r="J93">
+        <v>2</v>
+      </c>
+      <c r="K93">
         <v>231</v>
-      </c>
-      <c r="K93">
-        <v>50000</v>
       </c>
       <c r="L93">
         <v>50000</v>
       </c>
       <c r="M93">
+        <v>50000</v>
+      </c>
+      <c r="N93">
         <v>8024152</v>
       </c>
     </row>

</xml_diff>